<commit_message>
Update investigaciones, i121, Barrios Vivos, ficha V1
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -526,7 +526,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>202591004200100025E</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>OAP</t>
@@ -674,14 +678,28 @@
           <t>Sector Cultura</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Diseñar los indicadores que permitan hacer seguimiento a los procesos de formación en arte, cultura y patrimonio en el Distrito y su impacto a nivel de ciudad y localidades.</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>https://drive.google.com/drive/folders/1clr5wOumCR15k_x2ft_Ltyg1vDRlHBHK</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Formación, prácticas, cultura, patrimonio, arte</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Gisela Castrillón
+Diego Lemus
+Germán Urbina</t>
+        </is>
+      </c>
       <c r="N4" t="n">
         <v>2025</v>
       </c>
@@ -1898,7 +1916,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>202591004200100026E</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>Gobernanza - DALP</t>
@@ -1909,7 +1931,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1930,7 +1952,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Mauricio Ojeda</t>
+          <t>Mauricio Ojeda, Mábel Ayala</t>
         </is>
       </c>
       <c r="N24" t="n">
@@ -8494,7 +8516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E779"/>
+  <dimension ref="A1:E780"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19875,7 +19897,7 @@
       </c>
       <c r="C552" t="inlineStr">
         <is>
-          <t>Informe interactivo</t>
+          <t>Documento metodológico</t>
         </is>
       </c>
       <c r="D552" t="inlineStr">
@@ -19885,7 +19907,7 @@
       </c>
       <c r="E552" t="inlineStr">
         <is>
-          <t>https://observatoriocultura.github.io/observatorio/#/analisis-participaciones-plan-cultura-2038</t>
+          <t>https://drive.google.com/file/d/1UG7IUOwHocaP8Wkl5IA-8VUZtU16run1/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -19895,12 +19917,12 @@
       </c>
       <c r="B553" t="inlineStr">
         <is>
-          <t>Presentación</t>
+          <t>Visualización</t>
         </is>
       </c>
       <c r="C553" t="inlineStr">
         <is>
-          <t>Presentación de resultados</t>
+          <t>Tablero de resultados cuantitativos</t>
         </is>
       </c>
       <c r="D553" t="inlineStr">
@@ -19910,7 +19932,7 @@
       </c>
       <c r="E553" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1HKGcBc5WagGUkXbGurD0W5EICWnmGjvd/view?usp=drive_link</t>
+          <t>https://app.powerbi.com/view?r=eyJrIjoiMjdhMDk0ZjYtMDQwMi00ZTBmLThhODItNWExNzEwZGJiMjRjIiwidCI6IjRmNzkzOWM3LWFhNjAtNDliZC05YjdiLTZmODFjMzdkMWIzNyJ9</t>
         </is>
       </c>
     </row>
@@ -19920,12 +19942,12 @@
       </c>
       <c r="B554" t="inlineStr">
         <is>
-          <t>Visualización</t>
+          <t>Presentación</t>
         </is>
       </c>
       <c r="C554" t="inlineStr">
         <is>
-          <t>Tablero de resultados cuantitativos</t>
+          <t>Presentación de resultados</t>
         </is>
       </c>
       <c r="D554" t="inlineStr">
@@ -19935,7 +19957,7 @@
       </c>
       <c r="E554" t="inlineStr">
         <is>
-          <t>https://app.powerbi.com/view?r=eyJrIjoiMjdhMDk0ZjYtMDQwMi00ZTBmLThhODItNWExNzEwZGJiMjRjIiwidCI6IjRmNzkzOWM3LWFhNjAtNDliZC05YjdiLTZmODFjMzdkMWIzNyJ9</t>
+          <t>https://drive.google.com/file/d/1HKGcBc5WagGUkXbGurD0W5EICWnmGjvd/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -19950,7 +19972,7 @@
       </c>
       <c r="C555" t="inlineStr">
         <is>
-          <t>Documento metodológico</t>
+          <t>Informe interactivo</t>
         </is>
       </c>
       <c r="D555" t="inlineStr">
@@ -19960,7 +19982,7 @@
       </c>
       <c r="E555" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1UG7IUOwHocaP8Wkl5IA-8VUZtU16run1/view?usp=drive_link</t>
+          <t>https://observatoriocultura.github.io/observatorio/#/analisis-participaciones-plan-cultura-2038</t>
         </is>
       </c>
     </row>
@@ -19970,20 +19992,24 @@
       </c>
       <c r="B556" t="inlineStr">
         <is>
-          <t>Plan de trabajo</t>
+          <t>Base de datos</t>
         </is>
       </c>
       <c r="C556" t="inlineStr">
         <is>
-          <t>Plan de trabajo</t>
+          <t>Datos procesados y conclusiones</t>
         </is>
       </c>
       <c r="D556" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E556" t="inlineStr"/>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E556" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1I4Z2G_fY9HV45clwX1FWDf-O7SuD5P8b/edit?usp=drive_link&amp;ouid=114299960211627169695&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="557">
       <c r="A557" t="n">
@@ -19991,12 +20017,12 @@
       </c>
       <c r="B557" t="inlineStr">
         <is>
-          <t>Carpeta archivos</t>
+          <t>Plan de trabajo</t>
         </is>
       </c>
       <c r="C557" t="inlineStr">
         <is>
-          <t>Archivos de trabajo</t>
+          <t>Plan de trabajo</t>
         </is>
       </c>
       <c r="D557" t="inlineStr">
@@ -20008,11 +20034,23 @@
     </row>
     <row r="558">
       <c r="A558" t="n">
-        <v>101</v>
-      </c>
-      <c r="B558" t="inlineStr"/>
-      <c r="C558" t="inlineStr"/>
-      <c r="D558" t="inlineStr"/>
+        <v>100</v>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Carpeta archivos</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>Archivos de trabajo</t>
+        </is>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E558" t="inlineStr"/>
     </row>
     <row r="559">
@@ -20062,7 +20100,7 @@
     </row>
     <row r="564">
       <c r="A564" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B564" t="inlineStr"/>
       <c r="C564" t="inlineStr"/>
@@ -20116,7 +20154,7 @@
     </row>
     <row r="570">
       <c r="A570" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B570" t="inlineStr"/>
       <c r="C570" t="inlineStr"/>
@@ -20170,7 +20208,7 @@
     </row>
     <row r="576">
       <c r="A576" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B576" t="inlineStr"/>
       <c r="C576" t="inlineStr"/>
@@ -20224,7 +20262,7 @@
     </row>
     <row r="582">
       <c r="A582" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B582" t="inlineStr"/>
       <c r="C582" t="inlineStr"/>
@@ -20278,7 +20316,7 @@
     </row>
     <row r="588">
       <c r="A588" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B588" t="inlineStr"/>
       <c r="C588" t="inlineStr"/>
@@ -20332,7 +20370,7 @@
     </row>
     <row r="594">
       <c r="A594" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B594" t="inlineStr"/>
       <c r="C594" t="inlineStr"/>
@@ -20386,7 +20424,7 @@
     </row>
     <row r="600">
       <c r="A600" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B600" t="inlineStr"/>
       <c r="C600" t="inlineStr"/>
@@ -20440,7 +20478,7 @@
     </row>
     <row r="606">
       <c r="A606" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B606" t="inlineStr"/>
       <c r="C606" t="inlineStr"/>
@@ -20494,7 +20532,7 @@
     </row>
     <row r="612">
       <c r="A612" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B612" t="inlineStr"/>
       <c r="C612" t="inlineStr"/>
@@ -20548,7 +20586,7 @@
     </row>
     <row r="618">
       <c r="A618" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B618" t="inlineStr"/>
       <c r="C618" t="inlineStr"/>
@@ -20602,7 +20640,7 @@
     </row>
     <row r="624">
       <c r="A624" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B624" t="inlineStr"/>
       <c r="C624" t="inlineStr"/>
@@ -20656,7 +20694,7 @@
     </row>
     <row r="630">
       <c r="A630" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B630" t="inlineStr"/>
       <c r="C630" t="inlineStr"/>
@@ -20710,7 +20748,7 @@
     </row>
     <row r="636">
       <c r="A636" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B636" t="inlineStr"/>
       <c r="C636" t="inlineStr"/>
@@ -20764,7 +20802,7 @@
     </row>
     <row r="642">
       <c r="A642" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B642" t="inlineStr"/>
       <c r="C642" t="inlineStr"/>
@@ -20818,7 +20856,7 @@
     </row>
     <row r="648">
       <c r="A648" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B648" t="inlineStr"/>
       <c r="C648" t="inlineStr"/>
@@ -20872,7 +20910,7 @@
     </row>
     <row r="654">
       <c r="A654" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B654" t="inlineStr"/>
       <c r="C654" t="inlineStr"/>
@@ -20926,7 +20964,7 @@
     </row>
     <row r="660">
       <c r="A660" t="n">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B660" t="inlineStr"/>
       <c r="C660" t="inlineStr"/>
@@ -20980,7 +21018,7 @@
     </row>
     <row r="666">
       <c r="A666" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B666" t="inlineStr"/>
       <c r="C666" t="inlineStr"/>
@@ -21034,7 +21072,7 @@
     </row>
     <row r="672">
       <c r="A672" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B672" t="inlineStr"/>
       <c r="C672" t="inlineStr"/>
@@ -21088,7 +21126,7 @@
     </row>
     <row r="678">
       <c r="A678" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B678" t="inlineStr"/>
       <c r="C678" t="inlineStr"/>
@@ -21099,50 +21137,130 @@
       <c r="A679" t="n">
         <v>121</v>
       </c>
-      <c r="B679" t="inlineStr"/>
-      <c r="C679" t="inlineStr"/>
-      <c r="D679" t="inlineStr"/>
-      <c r="E679" t="inlineStr"/>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>Instrucciones sobre registro de información</t>
+        </is>
+      </c>
+      <c r="D679" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E679" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1gbIyrWH8cK07q00yoPBs9D8IWYNv4P2I/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="680">
       <c r="A680" t="n">
         <v>121</v>
       </c>
-      <c r="B680" t="inlineStr"/>
-      <c r="C680" t="inlineStr"/>
-      <c r="D680" t="inlineStr"/>
-      <c r="E680" t="inlineStr"/>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>Prototipo para registro</t>
+        </is>
+      </c>
+      <c r="D680" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E680" t="inlineStr">
+        <is>
+          <t>https://www.prototipos-sicc.com/app/barrios_vivos/explorar</t>
+        </is>
+      </c>
     </row>
     <row r="681">
       <c r="A681" t="n">
         <v>121</v>
       </c>
-      <c r="B681" t="inlineStr"/>
-      <c r="C681" t="inlineStr"/>
-      <c r="D681" t="inlineStr"/>
-      <c r="E681" t="inlineStr"/>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>Tablero de seguimiento</t>
+        </is>
+      </c>
+      <c r="D681" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E681" t="inlineStr">
+        <is>
+          <t>https://lookerstudio.google.com/reporting/a1e266a6-ed1a-4500-8776-58e82d1d7746/page/p_pjg06p6njd</t>
+        </is>
+      </c>
     </row>
     <row r="682">
       <c r="A682" t="n">
         <v>121</v>
       </c>
-      <c r="B682" t="inlineStr"/>
-      <c r="C682" t="inlineStr"/>
-      <c r="D682" t="inlineStr"/>
-      <c r="E682" t="inlineStr"/>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Audiovisual</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>Vídeo tutoriales para registro</t>
+        </is>
+      </c>
+      <c r="D682" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E682" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1Cuy0w3cr883zTx_4X1n4TquCUCnheBRm</t>
+        </is>
+      </c>
     </row>
     <row r="683">
       <c r="A683" t="n">
         <v>121</v>
       </c>
-      <c r="B683" t="inlineStr"/>
-      <c r="C683" t="inlineStr"/>
-      <c r="D683" t="inlineStr"/>
-      <c r="E683" t="inlineStr"/>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>Tablero Encuesta</t>
+        </is>
+      </c>
+      <c r="D683" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E683" t="inlineStr">
+        <is>
+          <t>https://lookerstudio.google.com/reporting/ccbecff5-f250-4a21-b1f8-5290632c1187/page/p_shhgwuepsd</t>
+        </is>
+      </c>
     </row>
     <row r="684">
       <c r="A684" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B684" t="inlineStr"/>
       <c r="C684" t="inlineStr"/>
@@ -21196,7 +21314,7 @@
     </row>
     <row r="690">
       <c r="A690" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B690" t="inlineStr"/>
       <c r="C690" t="inlineStr"/>
@@ -21250,7 +21368,7 @@
     </row>
     <row r="696">
       <c r="A696" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B696" t="inlineStr"/>
       <c r="C696" t="inlineStr"/>
@@ -21304,7 +21422,7 @@
     </row>
     <row r="702">
       <c r="A702" t="n">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B702" t="inlineStr"/>
       <c r="C702" t="inlineStr"/>
@@ -21358,7 +21476,7 @@
     </row>
     <row r="708">
       <c r="A708" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B708" t="inlineStr"/>
       <c r="C708" t="inlineStr"/>
@@ -21412,7 +21530,7 @@
     </row>
     <row r="714">
       <c r="A714" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B714" t="inlineStr"/>
       <c r="C714" t="inlineStr"/>
@@ -21466,7 +21584,7 @@
     </row>
     <row r="720">
       <c r="A720" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B720" t="inlineStr"/>
       <c r="C720" t="inlineStr"/>
@@ -21520,7 +21638,7 @@
     </row>
     <row r="726">
       <c r="A726" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B726" t="inlineStr"/>
       <c r="C726" t="inlineStr"/>
@@ -21574,7 +21692,7 @@
     </row>
     <row r="732">
       <c r="A732" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B732" t="inlineStr"/>
       <c r="C732" t="inlineStr"/>
@@ -21628,7 +21746,7 @@
     </row>
     <row r="738">
       <c r="A738" t="n">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B738" t="inlineStr"/>
       <c r="C738" t="inlineStr"/>
@@ -21682,7 +21800,7 @@
     </row>
     <row r="744">
       <c r="A744" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B744" t="inlineStr"/>
       <c r="C744" t="inlineStr"/>
@@ -21736,7 +21854,7 @@
     </row>
     <row r="750">
       <c r="A750" t="n">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B750" t="inlineStr"/>
       <c r="C750" t="inlineStr"/>
@@ -21790,7 +21908,7 @@
     </row>
     <row r="756">
       <c r="A756" t="n">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B756" t="inlineStr"/>
       <c r="C756" t="inlineStr"/>
@@ -21844,7 +21962,7 @@
     </row>
     <row r="762">
       <c r="A762" t="n">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B762" t="inlineStr"/>
       <c r="C762" t="inlineStr"/>
@@ -21898,7 +22016,7 @@
     </row>
     <row r="768">
       <c r="A768" t="n">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B768" t="inlineStr"/>
       <c r="C768" t="inlineStr"/>
@@ -21952,7 +22070,7 @@
     </row>
     <row r="774">
       <c r="A774" t="n">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B774" t="inlineStr"/>
       <c r="C774" t="inlineStr"/>
@@ -21972,10 +22090,26 @@
       <c r="A776" t="n">
         <v>137</v>
       </c>
-      <c r="B776" t="inlineStr"/>
-      <c r="C776" t="inlineStr"/>
-      <c r="D776" t="inlineStr"/>
-      <c r="E776" t="inlineStr"/>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>Tablero de resultados</t>
+        </is>
+      </c>
+      <c r="D776" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E776" t="inlineStr">
+        <is>
+          <t>https://lookerstudio.google.com/u/0/reporting/ff02ed3a-dd61-4f17-b3aa-9aa8b9cbc9c4/page/p_pjg06p6njd</t>
+        </is>
+      </c>
     </row>
     <row r="777">
       <c r="A777" t="n">
@@ -22003,6 +22137,15 @@
       <c r="C779" t="inlineStr"/>
       <c r="D779" t="inlineStr"/>
       <c r="E779" t="inlineStr"/>
+    </row>
+    <row r="780">
+      <c r="A780" t="n">
+        <v>137</v>
+      </c>
+      <c r="B780" t="inlineStr"/>
+      <c r="C780" t="inlineStr"/>
+      <c r="D780" t="inlineStr"/>
+      <c r="E780" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -26899,11 +27042,11 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>La metodología basada en análisis de lenguaje natural permitió identificar patrones semánticos, emocionales y argumentativos en más de 12.000 intervenciones. Esta apuesta innovadora traduce conversaciones ciudadanas en insumos de política, superando métodos tradicionales y fortaleciendo la escucha activa del Estado.</t>
+          <t>La metodología basada en análisis de lenguaje natural permitió identificar patrones semánticos, emocionales y argumentativos en más de 6.539 intervenciones. Esta apuesta innovadora traduce conversaciones ciudadanas en insumos de política, superando métodos tradicionales y fortaleciendo la escucha activa del Estado.</t>
         </is>
       </c>
       <c r="E276" t="n">
-        <v>12000</v>
+        <v>6.539</v>
       </c>
       <c r="F276" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update investigaciones, i081 Horarios nocturnos
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -2975,7 +2975,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>4 Entregada</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -3771,7 +3771,11 @@
           <t>Encuesta de Cultura Ambiental</t>
         </is>
       </c>
-      <c r="K57" t="inlineStr"/>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1LKhmDMxLL6nUDgtL8UjkmK_Tu4nAwgsi</t>
+        </is>
+      </c>
       <c r="L57" t="inlineStr">
         <is>
           <t>Comportamientos ambientales, protección animal, biodoversidad, cuidado del agua, infraestructura ecológica, ebc, encuesta bienal de culturas</t>
@@ -4083,7 +4087,7 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>79. ExperimentoFacturaEAAB</t>
+          <t>https://drive.google.com/open?id=12YHdekUPRzm2kD3clAAL3g5IUH2vf2pl&amp;usp=drive_fs</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
@@ -4429,7 +4433,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>deep, 24 horas</t>
+          <t>deep, 24 horas, economía cultural, consumo cultural, bogotá 24 horas, nocturno, noche, rumba</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
@@ -8570,7 +8574,11 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1Y_hXUsLkupgoUzaXuba0pvEQiAD9zr9f/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -11186,8 +11194,16 @@
           <t>Informe final</t>
         </is>
       </c>
-      <c r="C135" t="inlineStr"/>
-      <c r="D135" t="inlineStr"/>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Informe Final Diagnóstico</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E135" t="inlineStr"/>
     </row>
     <row r="136">
@@ -11245,10 +11261,26 @@
       <c r="A139" t="n">
         <v>77</v>
       </c>
-      <c r="B139" t="inlineStr"/>
-      <c r="C139" t="inlineStr"/>
-      <c r="D139" t="inlineStr"/>
-      <c r="E139" t="inlineStr"/>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Tablero de resultados ECA 2024</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>https://app.powerbi.com/view?r=eyJrIjoiMTdjZjQ5NDgtMjA1YS00YWMxLTk3NjMtM2VmZGNhMGVkZWE4IiwidCI6IjRmNzkzOWM3LWFhNjAtNDliZC05YjdiLTZmODFjMzdkMWIzNyJ9&amp;pageName=69b48348ad3ee2b5bec5</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -11607,8 +11639,16 @@
           <t>Informe de análisis encuesta Bogotá 24 horas</t>
         </is>
       </c>
-      <c r="D167" t="inlineStr"/>
-      <c r="E167" t="inlineStr"/>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1DDdOZG9H4IuBsiT9gQZ6KA1XmWxFevxd/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -11624,8 +11664,16 @@
           <t>Presentación resultados de la encuesta Bogotá 24 horas</t>
         </is>
       </c>
-      <c r="D168" t="inlineStr"/>
-      <c r="E168" t="inlineStr"/>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1SVDBhK3Lyx73mTV4txTEpO78WH0qK4AU/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -11638,11 +11686,19 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Encuesta_Bogotá_24_horas_Anonimizada</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr"/>
-      <c r="E169" t="inlineStr"/>
+          <t>Datos detallados de la encuesta</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1eezXFrTXJ6aBeE6eiUvJcByCQ82KhE5e/edit?usp=drive_link&amp;ouid=114299960211627169695&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -12393,7 +12449,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1WQeVJHbCsxac2P3icIDRzmvZnjLsYZ5VV</t>
+          <t>https://docs.google.com/spreadsheets/d/1u7_3ubCoOLwI5Qz_NL7m7w0765p9OVZNey1h4s070_s/edit?gid=168305545#gid=168305545</t>
         </is>
       </c>
     </row>
@@ -22464,7 +22520,9 @@
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
+      <c r="A16" t="n">
+        <v>63</v>
+      </c>
       <c r="B16" t="n">
         <v>1</v>
       </c>
@@ -22943,7 +23001,9 @@
       <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr"/>
+      <c r="A39" t="n">
+        <v>71</v>
+      </c>
       <c r="B39" t="n">
         <v>5</v>
       </c>
@@ -23004,7 +23064,9 @@
       <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
+      <c r="A42" t="n">
+        <v>75</v>
+      </c>
       <c r="B42" t="n">
         <v>2</v>
       </c>
@@ -23467,7 +23529,9 @@
       <c r="F65" t="inlineStr"/>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr"/>
+      <c r="A66" t="n">
+        <v>85</v>
+      </c>
       <c r="B66" t="n">
         <v>3</v>
       </c>
@@ -23485,7 +23549,9 @@
       <c r="F66" t="inlineStr"/>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr"/>
+      <c r="A67" t="n">
+        <v>85</v>
+      </c>
       <c r="B67" t="n">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Update investigaciones, i076 Espacio publico
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -3680,7 +3680,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Levantar una línea base sobre apropiación del espacio público e identidades del espacio público el cual contempla el levantamiento de un estado del arte, instrumentos cualitativos y cuantitativos para comprender la problemática y tener datos de base para el diseño de las estrategias de transformación cultural.</t>
+          <t>Línea base sobre apropiación del espacio público e identidades del espacio público, levantamiento de un estado del arte, instrumentos cualitativos y cuantitativos para comprender la problemática y tener datos de base para el diseño de las estrategias de transformación cultural.</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4394,7 +4394,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Levantar información cuantitativa a través de una encuesta sobre factores socioculturales que impiden que los ciudadanos habiten la ciudad en la noche, en puntos priorizados por la Dirección de Economía de la SCRD.</t>
+          <t>Encuesta sobre factores socioculturales que impiden que los ciudadanos habiten la ciudad en la noche, en puntos priorizados por la Dirección de Economía de la Secretaría de Cultura, Recreación y Deporte.</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -11014,7 +11014,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>https://docs.google.com/document/d/1P50IBnn096GO3TUeM_ZTOYKccJOlc-KQ/edit#heading=h.ihv636</t>
+          <t>https://drive.google.com/file/d/1167ghozNKQfSCGO52qNEbbz4IFZDq5Nq/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -11060,7 +11060,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>https://docs.google.com/spreadsheets/d/1kU8kdOtoCSom-amkPBPRidzKc-NyUDtt/edit?usp=sharing&amp;ouid=105090632649587320414&amp;rtpof=true&amp;sd=true</t>
+          <t>https://docs.google.com/spreadsheets/d/1102eDRaQDspY3lfV8f9WqSnwDHf2icfb/edit?usp=drive_link&amp;ouid=114299960211627169695&amp;rtpof=true&amp;sd=true</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update investigaciones, enero 2025
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -607,7 +607,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -617,8 +617,8 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Realizar un análisis de la información recolectada en los formularios aplicados a las ESALES 2024 y 2025, en terminos de oferta de valor, estructura organizacional y herramientas de sostenibilidad.
-Objetivo especifico: Continuar con el apoyo a la recolección de información de las ESALES registradas por la SCRD.</t>
+          <t xml:space="preserve">Realizar un análisis de la información recolectada en los formularios aplicados a las ESALES 2024 y 2025, en términos de oferta de valor, estructura organizacional y herramientas de sostenibilidad.
+</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -659,7 +659,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>202591004200100029E</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>DACP</t>
@@ -670,7 +674,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -695,9 +699,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Gisela Castrillón
-Diego Lemus
-Germán Urbina</t>
+          <t>Gisela Castrillón, Diego Lemus, Germán Urbina</t>
         </is>
       </c>
       <c r="N4" t="n">
@@ -739,7 +741,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -806,7 +808,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -872,7 +874,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -939,7 +941,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1001,7 +1003,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1056,7 +1058,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1122,7 +1124,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1189,7 +1191,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1251,7 +1253,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1294,7 +1296,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Caracterización de la asociatividad y sostenibilidad de agentes del sector</t>
+          <t>Caracterización de la asociatividad y sostenibilidad de agentes del sector. No se llegó a difinir la investigaicón que reemplazaría. Se marca como cancelda.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1317,7 +1319,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1 Sin iniciar</t>
+          <t>9 Cancelada</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1376,7 +1378,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1401,7 +1403,7 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Viviana Rodríguez, Carlos Suárez </t>
+          <t>Viviana Rodríguez</t>
         </is>
       </c>
       <c r="N15" t="n">
@@ -1442,7 +1444,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1508,7 +1510,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1574,7 +1576,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1 Sin iniciar</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1589,7 +1591,11 @@
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Julian Chavez,Laura Lozano</t>
+        </is>
+      </c>
       <c r="N18" t="n">
         <v>2025</v>
       </c>
@@ -1628,7 +1634,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1649,7 +1655,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Giovani Moreno ,Laura Lozano</t>
+          <t>Julian Chavez,Laura Lozano</t>
         </is>
       </c>
       <c r="N19" t="n">
@@ -1690,7 +1696,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1 Sin iniciar</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1704,10 +1710,14 @@
           <t>https://drive.google.com/drive/folders/1idDw2zgYulv3RPefcC3pTTU0KPWe-E-A</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr"/>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Gobernanza del deporte; ecosistema deportivo; actores institucionales; política pública del deporte; caracterización de actores; sistema de información.</t>
+        </is>
+      </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Giovani Moreno ,Laura Lozano</t>
+          <t>Andrea García,Laura Lozano</t>
         </is>
       </c>
       <c r="N20" t="n">
@@ -1748,7 +1758,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1763,7 +1773,11 @@
         </is>
       </c>
       <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Carlos Suárez,Todo el equipo</t>
+        </is>
+      </c>
       <c r="N21" t="n">
         <v>2025</v>
       </c>
@@ -1803,7 +1817,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1869,7 +1883,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1903,7 +1917,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Registro y seguimiento Barrios Vivos</t>
+          <t>Herramienta para el registro y seguimiento Barrios Vivos 2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1978,7 +1992,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>202591004200100030E</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr">
         <is>
           <t>SCCGC - DRAC</t>
@@ -1989,7 +2007,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2032,7 +2050,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>202591004200100002E</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>SCCGC - DTC</t>
@@ -2043,7 +2065,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2064,7 +2086,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Mónica Mora</t>
+          <t>Jhonatan Rosas</t>
         </is>
       </c>
       <c r="N26" t="n">
@@ -2082,7 +2104,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Realizar una investigación sobre el consumo de agua en barrios focalizados de Bogotá, analizando factores culturales, comportamentales y ambientales que afectan su uso</t>
+          <t>Realizar un sondeo sobre el consumo de agua  en dos zonas de Bogotá analizando factores culturales, comportamentales y ambientales que afectan su uso</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2090,7 +2112,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>202491004200100018E</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>SCCGC - DTC</t>
@@ -2101,7 +2127,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2122,7 +2148,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Mónica Mora</t>
+          <t>Jhonatan Rosas</t>
         </is>
       </c>
       <c r="N27" t="n">
@@ -2148,7 +2174,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>202591004200100031E</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
           <t>Gobernanza - DEEP</t>
@@ -2159,7 +2189,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1 Sin iniciar</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2174,7 +2204,11 @@
         </is>
       </c>
       <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Jhonatan Rosas</t>
+        </is>
+      </c>
       <c r="N28" t="n">
         <v>2025</v>
       </c>
@@ -2190,7 +2224,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Diagnóstico sobre xenofobia para proyecto de cambio cultural y de comportamiento  y seguimiento a la línea de base de la estrategia SOMOS.</t>
+          <t>Caracterización sobre xenofobia para proyecto de cambio cultural y de comportamiento  y seguimiento a la línea de base de la estrategia SOMOS.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2198,7 +2232,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>202591004200100032E</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
           <t>SCCGC - DTC</t>
@@ -2209,7 +2247,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1 Sin iniciar</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2252,7 +2290,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>202591004200100033E</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr">
         <is>
           <t>SCCGC - DTC</t>
@@ -2263,7 +2305,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2293,12 +2335,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Futuros culturales</t>
+          <t>Caracterización de Hacedores de Oficios Artesanales 2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Identificar las percepciones y expectativas de la ciudadanía sobre el futuro de Bogotá</t>
+          <t>PENDIENTE DESCRIPCIÓN</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2306,7 +2348,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>202591004200100014E</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>DACP</t>
@@ -2317,12 +2363,12 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1 Sin iniciar</t>
+          <t>2 En ejecución</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Cultura Ciudadana</t>
+          <t>Sector Cultura</t>
         </is>
       </c>
       <c r="J31" t="inlineStr"/>
@@ -2332,7 +2378,11 @@
         </is>
       </c>
       <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Viviana Rodriguez</t>
+        </is>
+      </c>
       <c r="N31" t="n">
         <v>2025</v>
       </c>
@@ -2356,7 +2406,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>202591004200100034E</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
           <t>DACP</t>
@@ -2367,7 +2421,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2460,7 +2514,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>202591004200100035E</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
           <t>SCCGC</t>
@@ -2471,7 +2529,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1 Sin iniciar</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2486,7 +2544,11 @@
         </is>
       </c>
       <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Jhonatan Rosas</t>
+        </is>
+      </c>
       <c r="N34" t="n">
         <v>2025</v>
       </c>
@@ -2510,7 +2572,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>202591004200100036E</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
           <t>SCCGC</t>
@@ -2521,7 +2587,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2536,7 +2602,11 @@
         </is>
       </c>
       <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Jhonatan Rosas</t>
+        </is>
+      </c>
       <c r="N35" t="n">
         <v>2025</v>
       </c>
@@ -2560,7 +2630,11 @@
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>202591004200100037E</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
           <t>SCCGC</t>
@@ -2571,7 +2645,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2740,7 +2814,11 @@
           <t>Sector</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>202591004200100027E</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="n">
         <v>1</v>
@@ -2761,7 +2839,11 @@
           <t>https://drive.google.com/drive/folders/1Oevcfhqb2fsyzMSPchXqH7WxkIbqvNw_</t>
         </is>
       </c>
-      <c r="L40" t="inlineStr"/>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>transporte, movilidad, transmilenio, estaciones, colados</t>
+        </is>
+      </c>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="n">
         <v>2025</v>
@@ -8520,7 +8602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E780"/>
+  <dimension ref="A1:E781"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20004,7 +20086,7 @@
       </c>
       <c r="E553" t="inlineStr">
         <is>
-          <t>https://app.powerbi.com/view?r=eyJrIjoiMjdhMDk0ZjYtMDQwMi00ZTBmLThhODItNWExNzEwZGJiMjRjIiwidCI6IjRmNzkzOWM3LWFhNjAtNDliZC05YjdiLTZmODFjMzdkMWIzNyJ9</t>
+          <t>https://app.powerbi.com/view?r=eyJrIjoiMjdhMDk0ZjYtMDQwMi00ZTBmLThhODItNWExNzEwZGJiMjRjIiwidCI6IjRmNzkzOWM3LWFhNjAtNDliZC05YjdiLTZmODFjMzdkMWIzNyJ9&amp;pageName=72a8ef23337c4b8b34e4</t>
         </is>
       </c>
     </row>
@@ -20129,7 +20211,11 @@
       <c r="A559" t="n">
         <v>101</v>
       </c>
-      <c r="B559" t="inlineStr"/>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
       <c r="C559" t="inlineStr"/>
       <c r="D559" t="inlineStr"/>
       <c r="E559" t="inlineStr"/>
@@ -20183,68 +20269,152 @@
       <c r="A565" t="n">
         <v>102</v>
       </c>
-      <c r="B565" t="inlineStr"/>
-      <c r="C565" t="inlineStr"/>
-      <c r="D565" t="inlineStr"/>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Base de datos</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>5. Base Encuesta_Ecosistema_247_Asistentes_CHAPINERO TEUSAQUILLO CANDELARIA Anonimizada.xlsx</t>
+        </is>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E565" t="inlineStr"/>
     </row>
     <row r="566">
       <c r="A566" t="n">
         <v>102</v>
       </c>
-      <c r="B566" t="inlineStr"/>
-      <c r="C566" t="inlineStr"/>
-      <c r="D566" t="inlineStr"/>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Base de datos</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>6. Base Ecosistema_Cultural_247_Oferta_Anonimizada.xlsx</t>
+        </is>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E566" t="inlineStr"/>
     </row>
     <row r="567">
       <c r="A567" t="n">
         <v>102</v>
       </c>
-      <c r="B567" t="inlineStr"/>
-      <c r="C567" t="inlineStr"/>
-      <c r="D567" t="inlineStr"/>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>1. Resul_247_Chap_Teusa_Cande Asistentes.xlsx</t>
+        </is>
+      </c>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E567" t="inlineStr"/>
     </row>
     <row r="568">
       <c r="A568" t="n">
         <v>102</v>
       </c>
-      <c r="B568" t="inlineStr"/>
-      <c r="C568" t="inlineStr"/>
-      <c r="D568" t="inlineStr"/>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>1_Resultados_Ecosistema_Cultural_247_Oferta.xls</t>
+        </is>
+      </c>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E568" t="inlineStr"/>
     </row>
     <row r="569">
       <c r="A569" t="n">
         <v>102</v>
       </c>
-      <c r="B569" t="inlineStr"/>
-      <c r="C569" t="inlineStr"/>
-      <c r="D569" t="inlineStr"/>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Otro</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>2. Ficha_Técnica_247 Asistentes</t>
+        </is>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E569" t="inlineStr"/>
     </row>
     <row r="570">
       <c r="A570" t="n">
         <v>102</v>
       </c>
-      <c r="B570" t="inlineStr"/>
-      <c r="C570" t="inlineStr"/>
-      <c r="D570" t="inlineStr"/>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Otro</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>3_Ficha_Técnica_Oferta_247</t>
+        </is>
+      </c>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E570" t="inlineStr"/>
     </row>
     <row r="571">
       <c r="A571" t="n">
-        <v>103</v>
-      </c>
-      <c r="B571" t="inlineStr"/>
-      <c r="C571" t="inlineStr"/>
-      <c r="D571" t="inlineStr"/>
+        <v>102</v>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>Informe Resultados Sondeo Ecosistema 24/7</t>
+        </is>
+      </c>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E571" t="inlineStr"/>
     </row>
     <row r="572">
       <c r="A572" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B572" t="inlineStr"/>
       <c r="C572" t="inlineStr"/>
@@ -20255,55 +20425,151 @@
       <c r="A573" t="n">
         <v>103</v>
       </c>
-      <c r="B573" t="inlineStr"/>
-      <c r="C573" t="inlineStr"/>
-      <c r="D573" t="inlineStr"/>
-      <c r="E573" t="inlineStr"/>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>Tabla de resultados Encuesta Consumo audioviual</t>
+        </is>
+      </c>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E573" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1mAuKVQ4jwBYEmHdb5ya2D0SniLhAqFpv/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="574">
       <c r="A574" t="n">
         <v>103</v>
       </c>
-      <c r="B574" t="inlineStr"/>
-      <c r="C574" t="inlineStr"/>
-      <c r="D574" t="inlineStr"/>
-      <c r="E574" t="inlineStr"/>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>Formulario encuesta Consumo audiovisual</t>
+        </is>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E574" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1-BM1IvKPZo7YQwHIR85wtFpZjGG9MY3a/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="575">
       <c r="A575" t="n">
         <v>103</v>
       </c>
-      <c r="B575" t="inlineStr"/>
-      <c r="C575" t="inlineStr"/>
-      <c r="D575" t="inlineStr"/>
-      <c r="E575" t="inlineStr"/>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>Guía metodológica Talleres Consumo Audiovisual de Audiencias Infantiles</t>
+        </is>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E575" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1GAARHYoLPuQK5kpz3GmsuhQXiOLa5Mcx/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="576">
       <c r="A576" t="n">
         <v>103</v>
       </c>
-      <c r="B576" t="inlineStr"/>
-      <c r="C576" t="inlineStr"/>
-      <c r="D576" t="inlineStr"/>
-      <c r="E576" t="inlineStr"/>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>Presentación resultados encuesta consumo audiovisual</t>
+        </is>
+      </c>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E576" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1H-gGZzkXd1x4NUFnUjlHJsbv2SNMHxa3/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="577">
       <c r="A577" t="n">
-        <v>104</v>
-      </c>
-      <c r="B577" t="inlineStr"/>
-      <c r="C577" t="inlineStr"/>
-      <c r="D577" t="inlineStr"/>
-      <c r="E577" t="inlineStr"/>
+        <v>103</v>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>Informe Consumo audiovisual</t>
+        </is>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E577" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1HGPpuS1Qhl-Udv-KC6DqisNNNB8_C8Ta/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="578">
       <c r="A578" t="n">
         <v>104</v>
       </c>
-      <c r="B578" t="inlineStr"/>
-      <c r="C578" t="inlineStr"/>
-      <c r="D578" t="inlineStr"/>
-      <c r="E578" t="inlineStr"/>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>Informe Festival Monumentum 2025</t>
+        </is>
+      </c>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E578" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1VNIkQ3a3hetNE0tCChMkmlcdGIUJ_ttA/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="579">
       <c r="A579" t="n">
@@ -20343,7 +20609,7 @@
     </row>
     <row r="583">
       <c r="A583" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B583" t="inlineStr"/>
       <c r="C583" t="inlineStr"/>
@@ -20354,7 +20620,11 @@
       <c r="A584" t="n">
         <v>105</v>
       </c>
-      <c r="B584" t="inlineStr"/>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
       <c r="C584" t="inlineStr"/>
       <c r="D584" t="inlineStr"/>
       <c r="E584" t="inlineStr"/>
@@ -20363,41 +20633,105 @@
       <c r="A585" t="n">
         <v>105</v>
       </c>
-      <c r="B585" t="inlineStr"/>
-      <c r="C585" t="inlineStr"/>
-      <c r="D585" t="inlineStr"/>
-      <c r="E585" t="inlineStr"/>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Anexo</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>Diseño muestral sondeo Libro al Viento</t>
+        </is>
+      </c>
+      <c r="D585" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E585" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1tIxsn32YTgQ9cvPyeP_ho9d-OwP3YCV8/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="586">
       <c r="A586" t="n">
         <v>105</v>
       </c>
-      <c r="B586" t="inlineStr"/>
-      <c r="C586" t="inlineStr"/>
-      <c r="D586" t="inlineStr"/>
-      <c r="E586" t="inlineStr"/>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tabla de resultado del sondeo </t>
+        </is>
+      </c>
+      <c r="D586" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E586" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1J8Fv4c1h5AkSY6r_YDdZq_K79nWYvCYT/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="587">
       <c r="A587" t="n">
         <v>105</v>
       </c>
-      <c r="B587" t="inlineStr"/>
-      <c r="C587" t="inlineStr"/>
-      <c r="D587" t="inlineStr"/>
-      <c r="E587" t="inlineStr"/>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>Formulario sondeo Libro al Viento</t>
+        </is>
+      </c>
+      <c r="D587" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E587" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1P9elZDJUfHrZ2cl3Siscf2HpGD60haGl/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="588">
       <c r="A588" t="n">
         <v>105</v>
       </c>
-      <c r="B588" t="inlineStr"/>
-      <c r="C588" t="inlineStr"/>
-      <c r="D588" t="inlineStr"/>
-      <c r="E588" t="inlineStr"/>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>Presentación resultados sondeo Libro al Viento</t>
+        </is>
+      </c>
+      <c r="D588" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E588" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1mXwj0vvK-rgG5796HaLg6bbJU7tt62xG/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="589">
       <c r="A589" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B589" t="inlineStr"/>
       <c r="C589" t="inlineStr"/>
@@ -20408,19 +20742,51 @@
       <c r="A590" t="n">
         <v>106</v>
       </c>
-      <c r="B590" t="inlineStr"/>
-      <c r="C590" t="inlineStr"/>
-      <c r="D590" t="inlineStr"/>
-      <c r="E590" t="inlineStr"/>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>Informe Premio Luis Caballero 2025</t>
+        </is>
+      </c>
+      <c r="D590" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E590" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1bwHUP2WQlU55fpvnMYn6gs-02lHoYDrR/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="591">
       <c r="A591" t="n">
         <v>106</v>
       </c>
-      <c r="B591" t="inlineStr"/>
-      <c r="C591" t="inlineStr"/>
-      <c r="D591" t="inlineStr"/>
-      <c r="E591" t="inlineStr"/>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>Presentación resultados Premio Luis Caballero 2025</t>
+        </is>
+      </c>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E591" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1RJzTRw-lxF_ZvQ08fhfsIohq1XHwRm7J/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="592">
       <c r="A592" t="n">
@@ -20451,7 +20817,7 @@
     </row>
     <row r="595">
       <c r="A595" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B595" t="inlineStr"/>
       <c r="C595" t="inlineStr"/>
@@ -20462,109 +20828,297 @@
       <c r="A596" t="n">
         <v>107</v>
       </c>
-      <c r="B596" t="inlineStr"/>
-      <c r="C596" t="inlineStr"/>
-      <c r="D596" t="inlineStr"/>
-      <c r="E596" t="inlineStr"/>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Base de datos</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>Base de datos Encuesta Circo</t>
+        </is>
+      </c>
+      <c r="D596" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E596" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1ujCFF1ZXlrfccgNw__yXUrzhtMpAiEya/edit?usp=drive_link&amp;ouid=105090632649587320414&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="597">
       <c r="A597" t="n">
         <v>107</v>
       </c>
-      <c r="B597" t="inlineStr"/>
-      <c r="C597" t="inlineStr"/>
-      <c r="D597" t="inlineStr"/>
-      <c r="E597" t="inlineStr"/>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>Tabla de resultados cuantitativos</t>
+        </is>
+      </c>
+      <c r="D597" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E597" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1B55s6qmoQu8Bya1h17h2RlICtcbL17Ns/edit?usp=drive_link&amp;ouid=105090632649587320414&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="598">
       <c r="A598" t="n">
         <v>107</v>
       </c>
-      <c r="B598" t="inlineStr"/>
-      <c r="C598" t="inlineStr"/>
-      <c r="D598" t="inlineStr"/>
-      <c r="E598" t="inlineStr"/>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Otro</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>Ficha técnica</t>
+        </is>
+      </c>
+      <c r="D598" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E598" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1qkYwDb3Jn7-aGmvK6Qc75ZMzSy3olOSP/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="599">
       <c r="A599" t="n">
         <v>107</v>
       </c>
-      <c r="B599" t="inlineStr"/>
-      <c r="C599" t="inlineStr"/>
-      <c r="D599" t="inlineStr"/>
-      <c r="E599" t="inlineStr"/>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>Formulario Encuesta Circo</t>
+        </is>
+      </c>
+      <c r="D599" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E599" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1svEtTUFS_BRDUv5P4Nq1NMPEHh6wCBMT/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="600">
       <c r="A600" t="n">
         <v>107</v>
       </c>
-      <c r="B600" t="inlineStr"/>
-      <c r="C600" t="inlineStr"/>
-      <c r="D600" t="inlineStr"/>
-      <c r="E600" t="inlineStr"/>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>Informe Final Caracterización Sector Circo - Fase 2</t>
+        </is>
+      </c>
+      <c r="D600" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E600" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1ysvsCPGJOfu0iRaVnhZLyxQlDeI4MJ2_/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="601">
       <c r="A601" t="n">
-        <v>108</v>
-      </c>
-      <c r="B601" t="inlineStr"/>
-      <c r="C601" t="inlineStr"/>
-      <c r="D601" t="inlineStr"/>
-      <c r="E601" t="inlineStr"/>
+        <v>107</v>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>Presentación Resultados Caracterización Sector Circo - Fase 2</t>
+        </is>
+      </c>
+      <c r="D601" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E601" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1zFYtNPqms3OkOZw6b-waNURvYySD2r8E/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="602">
       <c r="A602" t="n">
-        <v>108</v>
-      </c>
-      <c r="B602" t="inlineStr"/>
+        <v>107</v>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Anexo</t>
+        </is>
+      </c>
       <c r="C602" t="inlineStr"/>
-      <c r="D602" t="inlineStr"/>
-      <c r="E602" t="inlineStr"/>
+      <c r="D602" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E602" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/11ncAWgzQdVg1cGWEaPH4m4pKgU7YvP-L/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="603">
       <c r="A603" t="n">
         <v>108</v>
       </c>
-      <c r="B603" t="inlineStr"/>
-      <c r="C603" t="inlineStr"/>
-      <c r="D603" t="inlineStr"/>
-      <c r="E603" t="inlineStr"/>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>Informe Festival Joropo al Parque</t>
+        </is>
+      </c>
+      <c r="D603" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E603" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1lM0-Lxiox-ceikmrbzga-XoDbSS7BH5D/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="604">
       <c r="A604" t="n">
         <v>108</v>
       </c>
-      <c r="B604" t="inlineStr"/>
-      <c r="C604" t="inlineStr"/>
-      <c r="D604" t="inlineStr"/>
-      <c r="E604" t="inlineStr"/>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>Informe Festival Rock al Parque</t>
+        </is>
+      </c>
+      <c r="D604" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E604" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1tk6baWkyzn5SE-xR-67sOIlt4QUdT037/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="605">
       <c r="A605" t="n">
         <v>108</v>
       </c>
-      <c r="B605" t="inlineStr"/>
-      <c r="C605" t="inlineStr"/>
-      <c r="D605" t="inlineStr"/>
-      <c r="E605" t="inlineStr"/>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>Informe Festival Vallenato al Parque</t>
+        </is>
+      </c>
+      <c r="D605" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E605" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1F_mgYGnqD8wB0tGdAc1u9O-sYDLxyK8U/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="606">
       <c r="A606" t="n">
         <v>108</v>
       </c>
-      <c r="B606" t="inlineStr"/>
-      <c r="C606" t="inlineStr"/>
-      <c r="D606" t="inlineStr"/>
-      <c r="E606" t="inlineStr"/>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>Informe Festival Colombia al Parque</t>
+        </is>
+      </c>
+      <c r="D606" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E606" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1_XKbAYuvHAz0ietoVzj7wfnc8bLhaEqQ/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="607">
       <c r="A607" t="n">
-        <v>109</v>
-      </c>
-      <c r="B607" t="inlineStr"/>
-      <c r="C607" t="inlineStr"/>
-      <c r="D607" t="inlineStr"/>
-      <c r="E607" t="inlineStr"/>
+        <v>108</v>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>Informe Festival Jazz al Parque</t>
+        </is>
+      </c>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E607" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1VvHVdta58v22Q9aiSJwLr2H87fpU4L4P/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="608">
       <c r="A608" t="n">
@@ -20613,7 +21167,7 @@
     </row>
     <row r="613">
       <c r="A613" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B613" t="inlineStr"/>
       <c r="C613" t="inlineStr"/>
@@ -20622,52 +21176,132 @@
     </row>
     <row r="614">
       <c r="A614" t="n">
-        <v>110</v>
-      </c>
-      <c r="B614" t="inlineStr"/>
-      <c r="C614" t="inlineStr"/>
-      <c r="D614" t="inlineStr"/>
-      <c r="E614" t="inlineStr"/>
+        <v>108</v>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>Informe Festival Popular al Parque</t>
+        </is>
+      </c>
+      <c r="D614" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E614" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1zsEUS_LEdC8ZP8xY3ak_UbwJZecKesIv/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="615">
       <c r="A615" t="n">
-        <v>110</v>
-      </c>
-      <c r="B615" t="inlineStr"/>
-      <c r="C615" t="inlineStr"/>
-      <c r="D615" t="inlineStr"/>
-      <c r="E615" t="inlineStr"/>
+        <v>108</v>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>Informe Festival Hip Hop al Parque</t>
+        </is>
+      </c>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E615" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1ghYaEKtpBcgNKdjpzzHwnkJ7DwgZwKNO/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="616">
       <c r="A616" t="n">
-        <v>110</v>
-      </c>
-      <c r="B616" t="inlineStr"/>
-      <c r="C616" t="inlineStr"/>
-      <c r="D616" t="inlineStr"/>
-      <c r="E616" t="inlineStr"/>
+        <v>108</v>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>Informe Festival Salsa al Parque</t>
+        </is>
+      </c>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E616" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1UorO-F_CNULkKdJ0SOnc536TyhaC4006/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="617">
       <c r="A617" t="n">
         <v>110</v>
       </c>
-      <c r="B617" t="inlineStr"/>
-      <c r="C617" t="inlineStr"/>
-      <c r="D617" t="inlineStr"/>
-      <c r="E617" t="inlineStr"/>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>Informe Festival Patrimonios en Ruana 2025</t>
+        </is>
+      </c>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E617" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1wvZVJDVHbqK5dHnGP3YmZgPAUOh17Dxg/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="618">
       <c r="A618" t="n">
         <v>110</v>
       </c>
-      <c r="B618" t="inlineStr"/>
-      <c r="C618" t="inlineStr"/>
-      <c r="D618" t="inlineStr"/>
-      <c r="E618" t="inlineStr"/>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>Informe Noche de Museos 2025</t>
+        </is>
+      </c>
+      <c r="D618" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E618" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1pFLvJdEzUI-VNyrHRMUQCrJQpZAkapIx/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="619">
       <c r="A619" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B619" t="inlineStr"/>
       <c r="C619" t="inlineStr"/>
@@ -20721,7 +21355,7 @@
     </row>
     <row r="625">
       <c r="A625" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B625" t="inlineStr"/>
       <c r="C625" t="inlineStr"/>
@@ -20732,158 +21366,426 @@
       <c r="A626" t="n">
         <v>112</v>
       </c>
-      <c r="B626" t="inlineStr"/>
-      <c r="C626" t="inlineStr"/>
-      <c r="D626" t="inlineStr"/>
-      <c r="E626" t="inlineStr"/>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>Presentación Resultados Investigación Creación Colectiva - Fase 2</t>
+        </is>
+      </c>
+      <c r="D626" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E626" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/19KOuSHmJGiaB8rqfygKyihJJLWemAeCX/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="627">
       <c r="A627" t="n">
         <v>112</v>
       </c>
-      <c r="B627" t="inlineStr"/>
-      <c r="C627" t="inlineStr"/>
-      <c r="D627" t="inlineStr"/>
-      <c r="E627" t="inlineStr"/>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>Análisis metodología cualitativa Grupos CCC</t>
+        </is>
+      </c>
+      <c r="D627" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E627" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1JSvyqU8ju5qkFYokzXZfe_qEt3P8URC6/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="628">
       <c r="A628" t="n">
         <v>112</v>
       </c>
-      <c r="B628" t="inlineStr"/>
-      <c r="C628" t="inlineStr"/>
-      <c r="D628" t="inlineStr"/>
-      <c r="E628" t="inlineStr"/>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Otro</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>Sintesis comparativa dimensiones y categorias  Creación Colectiva</t>
+        </is>
+      </c>
+      <c r="D628" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E628" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1sOYo9HPDZyUy9zipBazRl1cVBo8794_o/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="629">
       <c r="A629" t="n">
         <v>112</v>
       </c>
-      <c r="B629" t="inlineStr"/>
-      <c r="C629" t="inlineStr"/>
-      <c r="D629" t="inlineStr"/>
-      <c r="E629" t="inlineStr"/>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Otro</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>Formato de entrevistas para caracterización de grupos de creación colectiva</t>
+        </is>
+      </c>
+      <c r="D629" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E629" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1JZTCvv1048dhsTBMol6Cbb3G2FeTAbzX/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="630">
       <c r="A630" t="n">
         <v>112</v>
       </c>
-      <c r="B630" t="inlineStr"/>
-      <c r="C630" t="inlineStr"/>
-      <c r="D630" t="inlineStr"/>
-      <c r="E630" t="inlineStr"/>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Otro</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>Metodología CCC para caracterización de grupos de creación colectiva</t>
+        </is>
+      </c>
+      <c r="D630" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E630" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1GCPgWSoPSoWiAtSW35TI2V8noKMigJqd/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="631">
       <c r="A631" t="n">
-        <v>113</v>
-      </c>
-      <c r="B631" t="inlineStr"/>
-      <c r="C631" t="inlineStr"/>
-      <c r="D631" t="inlineStr"/>
+        <v>112</v>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Base de datos</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>Directorio de identificación de grupos de teatro practicantes de creación colectiva en Bogotá</t>
+        </is>
+      </c>
+      <c r="D631" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E631" t="inlineStr"/>
     </row>
     <row r="632">
       <c r="A632" t="n">
         <v>113</v>
       </c>
-      <c r="B632" t="inlineStr"/>
-      <c r="C632" t="inlineStr"/>
-      <c r="D632" t="inlineStr"/>
-      <c r="E632" t="inlineStr"/>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>Formulario Final EBC LEO</t>
+        </is>
+      </c>
+      <c r="D632" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E632" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/16W6G5tRSMAk7F6SDasy_0yM92zpbwTbq/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="633">
       <c r="A633" t="n">
-        <v>113</v>
-      </c>
-      <c r="B633" t="inlineStr"/>
-      <c r="C633" t="inlineStr"/>
-      <c r="D633" t="inlineStr"/>
-      <c r="E633" t="inlineStr"/>
+        <v>114</v>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>Instrumento de recolección Espacios de Lectura</t>
+        </is>
+      </c>
+      <c r="D633" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E633" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/16W6G5tRSMAk7F6SDasy_0yM92zpbwTbq/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="634">
       <c r="A634" t="n">
-        <v>113</v>
-      </c>
-      <c r="B634" t="inlineStr"/>
-      <c r="C634" t="inlineStr"/>
-      <c r="D634" t="inlineStr"/>
-      <c r="E634" t="inlineStr"/>
+        <v>114</v>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>Sondeo Visitantes Biblioteca Pública Usaquén - Servitá</t>
+        </is>
+      </c>
+      <c r="D634" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E634" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1FRWQBJGGoZZttLVMLwagnXXYShR2lFqi/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="635">
       <c r="A635" t="n">
-        <v>113</v>
-      </c>
-      <c r="B635" t="inlineStr"/>
-      <c r="C635" t="inlineStr"/>
-      <c r="D635" t="inlineStr"/>
-      <c r="E635" t="inlineStr"/>
+        <v>114</v>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>Sondeo Visitantes Biblioteca Pública La Peña</t>
+        </is>
+      </c>
+      <c r="D635" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E635" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1RwsGRlcn7XYuXJ1rtmYJUnWj69aEpyMV/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="636">
       <c r="A636" t="n">
-        <v>113</v>
-      </c>
-      <c r="B636" t="inlineStr"/>
-      <c r="C636" t="inlineStr"/>
-      <c r="D636" t="inlineStr"/>
-      <c r="E636" t="inlineStr"/>
+        <v>114</v>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>Sondeo Visitantes Biblioteca Pública FUGA</t>
+        </is>
+      </c>
+      <c r="D636" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E636" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1DYP4zsQhzkx8PH-yydqgAloHd_DCEsTV/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="637">
       <c r="A637" t="n">
         <v>114</v>
       </c>
-      <c r="B637" t="inlineStr"/>
-      <c r="C637" t="inlineStr"/>
-      <c r="D637" t="inlineStr"/>
-      <c r="E637" t="inlineStr"/>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>Sondeo Visitantes Biblioteca Pública Virgilio Barco</t>
+        </is>
+      </c>
+      <c r="D637" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E637" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1caNM182qy71k48IqO5Mzv168P1KIbDs-/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="638">
       <c r="A638" t="n">
         <v>114</v>
       </c>
-      <c r="B638" t="inlineStr"/>
-      <c r="C638" t="inlineStr"/>
-      <c r="D638" t="inlineStr"/>
-      <c r="E638" t="inlineStr"/>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>Sondeo Visitantes Biblioteca Pública Caros E. Restrepo</t>
+        </is>
+      </c>
+      <c r="D638" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E638" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/19dgvioy6RYxY0oUSvS7HrWGkCn6Bdcve/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="639">
       <c r="A639" t="n">
         <v>114</v>
       </c>
-      <c r="B639" t="inlineStr"/>
-      <c r="C639" t="inlineStr"/>
-      <c r="D639" t="inlineStr"/>
-      <c r="E639" t="inlineStr"/>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>Sondeo Visitantes Biblioteca Pública Francisco José de Caldas</t>
+        </is>
+      </c>
+      <c r="D639" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E639" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1Xdo-9N2TnWtBpoKVhiMIb3Cwj2SYmDWR/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="640">
       <c r="A640" t="n">
         <v>114</v>
       </c>
-      <c r="B640" t="inlineStr"/>
-      <c r="C640" t="inlineStr"/>
-      <c r="D640" t="inlineStr"/>
-      <c r="E640" t="inlineStr"/>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>Sondeo Visitantes Biblioteca Pública Gabriel García Márquez - El Tunal</t>
+        </is>
+      </c>
+      <c r="D640" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E640" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1-_wpdpR7e4SMEdEdCVZQNFsVSxxFf7Yn/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="641">
       <c r="A641" t="n">
         <v>114</v>
       </c>
-      <c r="B641" t="inlineStr"/>
-      <c r="C641" t="inlineStr"/>
-      <c r="D641" t="inlineStr"/>
-      <c r="E641" t="inlineStr"/>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>Sondeo Visitantes Biblioteca Pública Julio Mario Santodomingo</t>
+        </is>
+      </c>
+      <c r="D641" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E641" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/19-EGROjB7Se6H5BC7lQ-5kcioDv17Aj8/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="642">
       <c r="A642" t="n">
         <v>114</v>
       </c>
-      <c r="B642" t="inlineStr"/>
-      <c r="C642" t="inlineStr"/>
-      <c r="D642" t="inlineStr"/>
-      <c r="E642" t="inlineStr"/>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>Sondeo Visitantes Biblioteca Pública Manuel Zapata Olivella - El Tintal</t>
+        </is>
+      </c>
+      <c r="D642" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E642" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1smpXVkZNK0D0NVvXTpaToUpQYbnUsJ2X/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="643">
       <c r="A643" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B643" t="inlineStr"/>
       <c r="C643" t="inlineStr"/>
@@ -20894,50 +21796,130 @@
       <c r="A644" t="n">
         <v>115</v>
       </c>
-      <c r="B644" t="inlineStr"/>
-      <c r="C644" t="inlineStr"/>
-      <c r="D644" t="inlineStr"/>
-      <c r="E644" t="inlineStr"/>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>Informe Espacios de actividad física</t>
+        </is>
+      </c>
+      <c r="D644" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E644" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1d3w0unHW47dgfCZ6IMcGCLINTQKRglPO/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="645">
       <c r="A645" t="n">
         <v>115</v>
       </c>
-      <c r="B645" t="inlineStr"/>
-      <c r="C645" t="inlineStr"/>
-      <c r="D645" t="inlineStr"/>
-      <c r="E645" t="inlineStr"/>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>Presentación resultados programas de Espacios de actividad física</t>
+        </is>
+      </c>
+      <c r="D645" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E645" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1qlsGIDoE8xuZRs0DD2wbob15tro_VEMX/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="646">
       <c r="A646" t="n">
         <v>115</v>
       </c>
-      <c r="B646" t="inlineStr"/>
-      <c r="C646" t="inlineStr"/>
-      <c r="D646" t="inlineStr"/>
-      <c r="E646" t="inlineStr"/>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>Tablas de resultado Espacios de actividad física</t>
+        </is>
+      </c>
+      <c r="D646" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E646" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1PeAnosF7Ne2O-rSJHyJNPYU_8VyKObOM/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="647">
       <c r="A647" t="n">
         <v>115</v>
       </c>
-      <c r="B647" t="inlineStr"/>
-      <c r="C647" t="inlineStr"/>
-      <c r="D647" t="inlineStr"/>
-      <c r="E647" t="inlineStr"/>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Base de datos</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>Base de datos Espacios de actividad física</t>
+        </is>
+      </c>
+      <c r="D647" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E647" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1pkjosapWgOR6hhHYZF-HqbqKBJZlYhtM/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="648">
       <c r="A648" t="n">
         <v>115</v>
       </c>
-      <c r="B648" t="inlineStr"/>
-      <c r="C648" t="inlineStr"/>
-      <c r="D648" t="inlineStr"/>
-      <c r="E648" t="inlineStr"/>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>Instrumento de recolección Espacios de actividad física</t>
+        </is>
+      </c>
+      <c r="D648" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E648" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1u4nc5ifpincy8njQifsXd-QfzDxYlwR8/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="649">
       <c r="A649" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B649" t="inlineStr"/>
       <c r="C649" t="inlineStr"/>
@@ -20948,109 +21930,302 @@
       <c r="A650" t="n">
         <v>116</v>
       </c>
-      <c r="B650" t="inlineStr"/>
-      <c r="C650" t="inlineStr"/>
-      <c r="D650" t="inlineStr"/>
-      <c r="E650" t="inlineStr"/>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Carpeta archivos</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>Bases de datos depuras Ciclovía y Escuela de la Bici</t>
+        </is>
+      </c>
+      <c r="D650" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E650" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1E04LKSNgVLJxshdGwwWy8BQRzbJwMkGs/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="651">
       <c r="A651" t="n">
         <v>116</v>
       </c>
-      <c r="B651" t="inlineStr"/>
-      <c r="C651" t="inlineStr"/>
-      <c r="D651" t="inlineStr"/>
-      <c r="E651" t="inlineStr"/>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>Informe presentación resultados programas de Ciclovía y Escuela de la bici</t>
+        </is>
+      </c>
+      <c r="D651" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E651" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1vW5sSAFWII3dQByOxN53S71Rj_aNYBgG/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="652">
       <c r="A652" t="n">
         <v>116</v>
       </c>
-      <c r="B652" t="inlineStr"/>
-      <c r="C652" t="inlineStr"/>
-      <c r="D652" t="inlineStr"/>
-      <c r="E652" t="inlineStr"/>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>Tabla de resultado Escuela de la Bici</t>
+        </is>
+      </c>
+      <c r="D652" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E652" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1zQZjjzdyGr9BkltBh0Xu5ntzvtJ1siUK/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="653">
       <c r="A653" t="n">
         <v>116</v>
       </c>
-      <c r="B653" t="inlineStr"/>
-      <c r="C653" t="inlineStr"/>
-      <c r="D653" t="inlineStr"/>
-      <c r="E653" t="inlineStr"/>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>Tabla de resultado Ciclovía 2025</t>
+        </is>
+      </c>
+      <c r="D653" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E653" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/16ZpRSW0DGRb8JPE9QCzrLu2VyFN2IXTt/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="654">
       <c r="A654" t="n">
         <v>116</v>
       </c>
-      <c r="B654" t="inlineStr"/>
-      <c r="C654" t="inlineStr"/>
-      <c r="D654" t="inlineStr"/>
-      <c r="E654" t="inlineStr"/>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>Instrumento de recolección Escuela de la Bici</t>
+        </is>
+      </c>
+      <c r="D654" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E654" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1j44f0nt3hcD7HjD-Ya48stCgjyv2gPDm/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="655">
       <c r="A655" t="n">
-        <v>117</v>
-      </c>
-      <c r="B655" t="inlineStr"/>
-      <c r="C655" t="inlineStr"/>
-      <c r="D655" t="inlineStr"/>
-      <c r="E655" t="inlineStr"/>
+        <v>116</v>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>Instrumento de recolección Ciclovía 2025</t>
+        </is>
+      </c>
+      <c r="D655" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E655" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1uwG-2pHQMS6-t0GhwSTGLJ3fWap6L6Y6/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="656">
       <c r="A656" t="n">
         <v>117</v>
       </c>
-      <c r="B656" t="inlineStr"/>
-      <c r="C656" t="inlineStr"/>
-      <c r="D656" t="inlineStr"/>
-      <c r="E656" t="inlineStr"/>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>Docuento metodológico</t>
+        </is>
+      </c>
+      <c r="D656" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E656" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1h8ZkIRLLynb8caE2rR8zZagF76_ChE1P/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="657">
       <c r="A657" t="n">
         <v>117</v>
       </c>
-      <c r="B657" t="inlineStr"/>
-      <c r="C657" t="inlineStr"/>
-      <c r="D657" t="inlineStr"/>
-      <c r="E657" t="inlineStr"/>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>Instrumento de recolección</t>
+        </is>
+      </c>
+      <c r="D657" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E657" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1VZIqZvzrUOBhPEVGF_n98ZthOb8RmV4V/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="658">
       <c r="A658" t="n">
         <v>117</v>
       </c>
-      <c r="B658" t="inlineStr"/>
-      <c r="C658" t="inlineStr"/>
-      <c r="D658" t="inlineStr"/>
-      <c r="E658" t="inlineStr"/>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Anexo</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>Matriz de revisión de literatura</t>
+        </is>
+      </c>
+      <c r="D658" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E658" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1U5vso-3VmBTA0uPp6Jwz3zolvbWR17sT/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="659">
       <c r="A659" t="n">
         <v>117</v>
       </c>
-      <c r="B659" t="inlineStr"/>
-      <c r="C659" t="inlineStr"/>
-      <c r="D659" t="inlineStr"/>
-      <c r="E659" t="inlineStr"/>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Anexo</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matriz de tipología de actores
+</t>
+        </is>
+      </c>
+      <c r="D659" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E659" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1HQUAEOPZWxBtWc-dexksGmXsqH3VLyB3/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="660">
       <c r="A660" t="n">
         <v>117</v>
       </c>
-      <c r="B660" t="inlineStr"/>
-      <c r="C660" t="inlineStr"/>
-      <c r="D660" t="inlineStr"/>
-      <c r="E660" t="inlineStr"/>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Anexo</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>Matriz de esquema interpretativo de la gobernanza del deporte</t>
+        </is>
+      </c>
+      <c r="D660" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E660" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/16EFX41hHQvz_pSfEG86A1RV2KQ969hzt/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="661">
       <c r="A661" t="n">
-        <v>118</v>
-      </c>
-      <c r="B661" t="inlineStr"/>
-      <c r="C661" t="inlineStr"/>
-      <c r="D661" t="inlineStr"/>
-      <c r="E661" t="inlineStr"/>
+        <v>117</v>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Plan de trabajo</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>Plan de trabajo</t>
+        </is>
+      </c>
+      <c r="D661" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E661" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1t70D31QSK9xXUEgVSMhUzuwxOwgYAfyO/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="662">
       <c r="A662" t="n">
@@ -21099,7 +22274,7 @@
     </row>
     <row r="667">
       <c r="A667" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B667" t="inlineStr"/>
       <c r="C667" t="inlineStr"/>
@@ -21110,10 +22285,26 @@
       <c r="A668" t="n">
         <v>119</v>
       </c>
-      <c r="B668" t="inlineStr"/>
-      <c r="C668" t="inlineStr"/>
-      <c r="D668" t="inlineStr"/>
-      <c r="E668" t="inlineStr"/>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>Informe Festival de Verano 2025</t>
+        </is>
+      </c>
+      <c r="D668" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E668" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1CTZIeR2jRkd_dxriQ3C8acUqnYvBlI6k/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="669">
       <c r="A669" t="n">
@@ -21153,7 +22344,7 @@
     </row>
     <row r="673">
       <c r="A673" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B673" t="inlineStr"/>
       <c r="C673" t="inlineStr"/>
@@ -21164,19 +22355,51 @@
       <c r="A674" t="n">
         <v>120</v>
       </c>
-      <c r="B674" t="inlineStr"/>
-      <c r="C674" t="inlineStr"/>
-      <c r="D674" t="inlineStr"/>
-      <c r="E674" t="inlineStr"/>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>Informe Concurso Internacional de Violín 2025</t>
+        </is>
+      </c>
+      <c r="D674" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E674" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1om-sh_zxWJhBidcMWVCsb1psSg8gwLXr/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="675">
       <c r="A675" t="n">
         <v>120</v>
       </c>
-      <c r="B675" t="inlineStr"/>
-      <c r="C675" t="inlineStr"/>
-      <c r="D675" t="inlineStr"/>
-      <c r="E675" t="inlineStr"/>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>Informe Bienal Internacional de Arte y Ciudad BOG25</t>
+        </is>
+      </c>
+      <c r="D675" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E675" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/19W6ZP0kAGHIjQJfGd3cAnFvG1Cmo4qtu/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="676">
       <c r="A676" t="n">
@@ -21207,28 +22430,12 @@
     </row>
     <row r="679">
       <c r="A679" t="n">
-        <v>121</v>
-      </c>
-      <c r="B679" t="inlineStr">
-        <is>
-          <t>Presentación</t>
-        </is>
-      </c>
-      <c r="C679" t="inlineStr">
-        <is>
-          <t>Instrucciones sobre registro de información</t>
-        </is>
-      </c>
-      <c r="D679" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="E679" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1gbIyrWH8cK07q00yoPBs9D8IWYNv4P2I/view?usp=drive_link</t>
-        </is>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="B679" t="inlineStr"/>
+      <c r="C679" t="inlineStr"/>
+      <c r="D679" t="inlineStr"/>
+      <c r="E679" t="inlineStr"/>
     </row>
     <row r="680">
       <c r="A680" t="n">
@@ -21236,12 +22443,12 @@
       </c>
       <c r="B680" t="inlineStr">
         <is>
-          <t>Instrumento recolección</t>
+          <t>Presentación</t>
         </is>
       </c>
       <c r="C680" t="inlineStr">
         <is>
-          <t>Prototipo para registro</t>
+          <t>Instrucciones sobre registro de información</t>
         </is>
       </c>
       <c r="D680" t="inlineStr">
@@ -21251,7 +22458,7 @@
       </c>
       <c r="E680" t="inlineStr">
         <is>
-          <t>https://www.prototipos-sicc.com/app/barrios_vivos/explorar</t>
+          <t>https://drive.google.com/file/d/1gbIyrWH8cK07q00yoPBs9D8IWYNv4P2I/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21261,12 +22468,12 @@
       </c>
       <c r="B681" t="inlineStr">
         <is>
-          <t>Visualización</t>
+          <t>Instrumento recolección</t>
         </is>
       </c>
       <c r="C681" t="inlineStr">
         <is>
-          <t>Tablero de seguimiento</t>
+          <t>Prototipo para registro</t>
         </is>
       </c>
       <c r="D681" t="inlineStr">
@@ -21276,7 +22483,7 @@
       </c>
       <c r="E681" t="inlineStr">
         <is>
-          <t>https://lookerstudio.google.com/reporting/a1e266a6-ed1a-4500-8776-58e82d1d7746/page/p_pjg06p6njd</t>
+          <t>https://www.prototipos-sicc.com/app/barrios_vivos/explorar</t>
         </is>
       </c>
     </row>
@@ -21286,12 +22493,12 @@
       </c>
       <c r="B682" t="inlineStr">
         <is>
-          <t>Audiovisual</t>
+          <t>Visualización</t>
         </is>
       </c>
       <c r="C682" t="inlineStr">
         <is>
-          <t>Vídeo tutoriales para registro</t>
+          <t>Tablero de seguimiento</t>
         </is>
       </c>
       <c r="D682" t="inlineStr">
@@ -21301,7 +22508,7 @@
       </c>
       <c r="E682" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1Cuy0w3cr883zTx_4X1n4TquCUCnheBRm</t>
+          <t>https://lookerstudio.google.com/reporting/a1e266a6-ed1a-4500-8776-58e82d1d7746/page/p_pjg06p6njd</t>
         </is>
       </c>
     </row>
@@ -21311,12 +22518,12 @@
       </c>
       <c r="B683" t="inlineStr">
         <is>
-          <t>Visualización</t>
+          <t>Audiovisual</t>
         </is>
       </c>
       <c r="C683" t="inlineStr">
         <is>
-          <t>Tablero Encuesta</t>
+          <t>Vídeo tutoriales para registro</t>
         </is>
       </c>
       <c r="D683" t="inlineStr">
@@ -21326,7 +22533,7 @@
       </c>
       <c r="E683" t="inlineStr">
         <is>
-          <t>https://lookerstudio.google.com/reporting/ccbecff5-f250-4a21-b1f8-5290632c1187/page/p_shhgwuepsd</t>
+          <t>https://drive.google.com/drive/folders/1Cuy0w3cr883zTx_4X1n4TquCUCnheBRm</t>
         </is>
       </c>
     </row>
@@ -21334,14 +22541,30 @@
       <c r="A684" t="n">
         <v>121</v>
       </c>
-      <c r="B684" t="inlineStr"/>
-      <c r="C684" t="inlineStr"/>
-      <c r="D684" t="inlineStr"/>
-      <c r="E684" t="inlineStr"/>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>Tablero Encuesta</t>
+        </is>
+      </c>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E684" t="inlineStr">
+        <is>
+          <t>https://lookerstudio.google.com/reporting/ccbecff5-f250-4a21-b1f8-5290632c1187/page/p_shhgwuepsd</t>
+        </is>
+      </c>
     </row>
     <row r="685">
       <c r="A685" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B685" t="inlineStr"/>
       <c r="C685" t="inlineStr"/>
@@ -21395,7 +22618,7 @@
     </row>
     <row r="691">
       <c r="A691" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B691" t="inlineStr"/>
       <c r="C691" t="inlineStr"/>
@@ -21406,7 +22629,11 @@
       <c r="A692" t="n">
         <v>123</v>
       </c>
-      <c r="B692" t="inlineStr"/>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
       <c r="C692" t="inlineStr"/>
       <c r="D692" t="inlineStr"/>
       <c r="E692" t="inlineStr"/>
@@ -21449,7 +22676,7 @@
     </row>
     <row r="697">
       <c r="A697" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B697" t="inlineStr"/>
       <c r="C697" t="inlineStr"/>
@@ -21469,8 +22696,16 @@
       <c r="A699" t="n">
         <v>124</v>
       </c>
-      <c r="B699" t="inlineStr"/>
-      <c r="C699" t="inlineStr"/>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Otro</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>Diseño de experimento económico</t>
+        </is>
+      </c>
       <c r="D699" t="inlineStr"/>
       <c r="E699" t="inlineStr"/>
     </row>
@@ -21478,8 +22713,16 @@
       <c r="A700" t="n">
         <v>124</v>
       </c>
-      <c r="B700" t="inlineStr"/>
-      <c r="C700" t="inlineStr"/>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>Cálculo de consumo de agua en ducha por factura</t>
+        </is>
+      </c>
       <c r="D700" t="inlineStr"/>
       <c r="E700" t="inlineStr"/>
     </row>
@@ -21487,8 +22730,16 @@
       <c r="A701" t="n">
         <v>124</v>
       </c>
-      <c r="B701" t="inlineStr"/>
-      <c r="C701" t="inlineStr"/>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Base de datos</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>Datos EAAB por Barrio para experimento</t>
+        </is>
+      </c>
       <c r="D701" t="inlineStr"/>
       <c r="E701" t="inlineStr"/>
     </row>
@@ -21496,17 +22747,33 @@
       <c r="A702" t="n">
         <v>124</v>
       </c>
-      <c r="B702" t="inlineStr"/>
-      <c r="C702" t="inlineStr"/>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Infografía</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>Datos de hitos Barrios Vivos Agua</t>
+        </is>
+      </c>
       <c r="D702" t="inlineStr"/>
       <c r="E702" t="inlineStr"/>
     </row>
     <row r="703">
       <c r="A703" t="n">
-        <v>125</v>
-      </c>
-      <c r="B703" t="inlineStr"/>
-      <c r="C703" t="inlineStr"/>
+        <v>124</v>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Plan de trabajo</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>Cronograma Investigación Agua</t>
+        </is>
+      </c>
       <c r="D703" t="inlineStr"/>
       <c r="E703" t="inlineStr"/>
     </row>
@@ -21523,8 +22790,16 @@
       <c r="A705" t="n">
         <v>125</v>
       </c>
-      <c r="B705" t="inlineStr"/>
-      <c r="C705" t="inlineStr"/>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>Tablas de salida</t>
+        </is>
+      </c>
       <c r="D705" t="inlineStr"/>
       <c r="E705" t="inlineStr"/>
     </row>
@@ -21532,8 +22807,16 @@
       <c r="A706" t="n">
         <v>125</v>
       </c>
-      <c r="B706" t="inlineStr"/>
-      <c r="C706" t="inlineStr"/>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Carpeta archivos</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>ICC Distritos Creativos 2025</t>
+        </is>
+      </c>
       <c r="D706" t="inlineStr"/>
       <c r="E706" t="inlineStr"/>
     </row>
@@ -21541,8 +22824,16 @@
       <c r="A707" t="n">
         <v>125</v>
       </c>
-      <c r="B707" t="inlineStr"/>
-      <c r="C707" t="inlineStr"/>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>Formulario ICC Distritos Creativos 2025</t>
+        </is>
+      </c>
       <c r="D707" t="inlineStr"/>
       <c r="E707" t="inlineStr"/>
     </row>
@@ -21550,17 +22841,33 @@
       <c r="A708" t="n">
         <v>125</v>
       </c>
-      <c r="B708" t="inlineStr"/>
-      <c r="C708" t="inlineStr"/>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Plan de trabajo</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>Cronograma ICC Distritos Creativos</t>
+        </is>
+      </c>
       <c r="D708" t="inlineStr"/>
       <c r="E708" t="inlineStr"/>
     </row>
     <row r="709">
       <c r="A709" t="n">
-        <v>126</v>
-      </c>
-      <c r="B709" t="inlineStr"/>
-      <c r="C709" t="inlineStr"/>
+        <v>125</v>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>Documento Distritos Creativos</t>
+        </is>
+      </c>
       <c r="D709" t="inlineStr"/>
       <c r="E709" t="inlineStr"/>
     </row>
@@ -21611,7 +22918,7 @@
     </row>
     <row r="715">
       <c r="A715" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B715" t="inlineStr"/>
       <c r="C715" t="inlineStr"/>
@@ -21665,7 +22972,7 @@
     </row>
     <row r="721">
       <c r="A721" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B721" t="inlineStr"/>
       <c r="C721" t="inlineStr"/>
@@ -21676,28 +22983,52 @@
       <c r="A722" t="n">
         <v>128</v>
       </c>
-      <c r="B722" t="inlineStr"/>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
       <c r="C722" t="inlineStr"/>
       <c r="D722" t="inlineStr"/>
-      <c r="E722" t="inlineStr"/>
+      <c r="E722" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1NsVGUlWsADXoKnEO31ub8Cp0Krp9Aig3/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="723">
       <c r="A723" t="n">
         <v>128</v>
       </c>
-      <c r="B723" t="inlineStr"/>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Anexo</t>
+        </is>
+      </c>
       <c r="C723" t="inlineStr"/>
       <c r="D723" t="inlineStr"/>
-      <c r="E723" t="inlineStr"/>
+      <c r="E723" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1yZIHrgUGq2Lu0TFlzzyGvCS7RXjuxd1M/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="724">
       <c r="A724" t="n">
         <v>128</v>
       </c>
-      <c r="B724" t="inlineStr"/>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
       <c r="C724" t="inlineStr"/>
       <c r="D724" t="inlineStr"/>
-      <c r="E724" t="inlineStr"/>
+      <c r="E724" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1AVJBnJQld7Uyna3WW04TEPkFOQQqFlQl/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="725">
       <c r="A725" t="n">
@@ -21719,7 +23050,7 @@
     </row>
     <row r="727">
       <c r="A727" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B727" t="inlineStr"/>
       <c r="C727" t="inlineStr"/>
@@ -21773,7 +23104,7 @@
     </row>
     <row r="733">
       <c r="A733" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B733" t="inlineStr"/>
       <c r="C733" t="inlineStr"/>
@@ -21827,7 +23158,7 @@
     </row>
     <row r="739">
       <c r="A739" t="n">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B739" t="inlineStr"/>
       <c r="C739" t="inlineStr"/>
@@ -21881,7 +23212,7 @@
     </row>
     <row r="745">
       <c r="A745" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B745" t="inlineStr"/>
       <c r="C745" t="inlineStr"/>
@@ -21935,10 +23266,18 @@
     </row>
     <row r="751">
       <c r="A751" t="n">
-        <v>133</v>
-      </c>
-      <c r="B751" t="inlineStr"/>
-      <c r="C751" t="inlineStr"/>
+        <v>132</v>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>Cultura Metro - Estado del Arte</t>
+        </is>
+      </c>
       <c r="D751" t="inlineStr"/>
       <c r="E751" t="inlineStr"/>
     </row>
@@ -21989,7 +23328,7 @@
     </row>
     <row r="757">
       <c r="A757" t="n">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B757" t="inlineStr"/>
       <c r="C757" t="inlineStr"/>
@@ -22043,12 +23382,28 @@
     </row>
     <row r="763">
       <c r="A763" t="n">
-        <v>135</v>
-      </c>
-      <c r="B763" t="inlineStr"/>
-      <c r="C763" t="inlineStr"/>
-      <c r="D763" t="inlineStr"/>
-      <c r="E763" t="inlineStr"/>
+        <v>134</v>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>Tablero invitados ECCI 2025 - Seguimiento</t>
+        </is>
+      </c>
+      <c r="D763" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E763" t="inlineStr">
+        <is>
+          <t>https://lookerstudio.google.com/reporting/49195a24-bd9a-4773-af8a-966bb697f78b/page/p_pjg06p6njd</t>
+        </is>
+      </c>
     </row>
     <row r="764">
       <c r="A764" t="n">
@@ -22097,7 +23452,7 @@
     </row>
     <row r="769">
       <c r="A769" t="n">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B769" t="inlineStr"/>
       <c r="C769" t="inlineStr"/>
@@ -22151,55 +23506,87 @@
     </row>
     <row r="775">
       <c r="A775" t="n">
-        <v>137</v>
-      </c>
-      <c r="B775" t="inlineStr"/>
-      <c r="C775" t="inlineStr"/>
-      <c r="D775" t="inlineStr"/>
-      <c r="E775" t="inlineStr"/>
+        <v>136</v>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Mapa/Geovisor</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>Geovisor Movilidad</t>
+        </is>
+      </c>
+      <c r="D775" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E775" t="inlineStr">
+        <is>
+          <t>https://www.arcgis.com/apps/dashboards/3a8a858de18047528174d7bc158b4b42</t>
+        </is>
+      </c>
     </row>
     <row r="776">
       <c r="A776" t="n">
         <v>137</v>
       </c>
-      <c r="B776" t="inlineStr">
-        <is>
-          <t>Visualización</t>
-        </is>
-      </c>
-      <c r="C776" t="inlineStr">
-        <is>
-          <t>Tablero de resultados</t>
-        </is>
-      </c>
-      <c r="D776" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="E776" t="inlineStr">
-        <is>
-          <t>https://lookerstudio.google.com/u/0/reporting/ff02ed3a-dd61-4f17-b3aa-9aa8b9cbc9c4/page/p_pjg06p6njd</t>
-        </is>
-      </c>
+      <c r="B776" t="inlineStr"/>
+      <c r="C776" t="inlineStr"/>
+      <c r="D776" t="inlineStr"/>
+      <c r="E776" t="inlineStr"/>
     </row>
     <row r="777">
       <c r="A777" t="n">
         <v>137</v>
       </c>
-      <c r="B777" t="inlineStr"/>
-      <c r="C777" t="inlineStr"/>
-      <c r="D777" t="inlineStr"/>
-      <c r="E777" t="inlineStr"/>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>Tablero de resultados</t>
+        </is>
+      </c>
+      <c r="D777" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E777" t="inlineStr">
+        <is>
+          <t>https://app.powerbi.com/view?r=eyJrIjoiOWYwOThhMjMtOTBjZC00ZGY5LThhYjktMTY5OWYzYWI0ZDJjIiwidCI6IjRmNzkzOWM3LWFhNjAtNDliZC05YjdiLTZmODFjMzdkMWIzNyJ9&amp;pageName=ef377ed828063259b15e</t>
+        </is>
+      </c>
     </row>
     <row r="778">
       <c r="A778" t="n">
         <v>137</v>
       </c>
-      <c r="B778" t="inlineStr"/>
-      <c r="C778" t="inlineStr"/>
-      <c r="D778" t="inlineStr"/>
-      <c r="E778" t="inlineStr"/>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Base de datos</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>Datos de encuestas</t>
+        </is>
+      </c>
+      <c r="D778" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E778" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1rX2RfuDon4SukoBpHxRg7m9fnL6_1Jw2/edit?usp=drive_link&amp;ouid=114299960211627169695&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="779">
       <c r="A779" t="n">
@@ -22218,6 +23605,15 @@
       <c r="C780" t="inlineStr"/>
       <c r="D780" t="inlineStr"/>
       <c r="E780" t="inlineStr"/>
+    </row>
+    <row r="781">
+      <c r="A781" t="n">
+        <v>137</v>
+      </c>
+      <c r="B781" t="inlineStr"/>
+      <c r="C781" t="inlineStr"/>
+      <c r="D781" t="inlineStr"/>
+      <c r="E781" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -22230,7 +23626,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F279"/>
+  <dimension ref="A1:F306"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27127,8 +28523,10 @@
           <t>La metodología basada en análisis de lenguaje natural permitió identificar patrones semánticos, emocionales y argumentativos en más de 6.539 intervenciones. Esta apuesta innovadora traduce conversaciones ciudadanas en insumos de política, superando métodos tradicionales y fortaleciendo la escucha activa del Estado.</t>
         </is>
       </c>
-      <c r="E276" t="n">
-        <v>6.539</v>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>6.539</t>
+        </is>
       </c>
       <c r="F276" t="inlineStr">
         <is>
@@ -27195,6 +28593,583 @@
       </c>
       <c r="E279" t="inlineStr"/>
       <c r="F279" t="inlineStr"/>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>103</v>
+      </c>
+      <c r="B280" t="n">
+        <v>1</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Reconocimiento y acceso a los canales en la ciudad</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Los resultados de la encuesta muestran que los principales retos de los canales se relacionan con su nivel de reconocimiento y visibilidad, más que con dificultades de acceso a la señal. En Bogotá, el 54,6% de la población afirma conocer Canal Capital, mientras que Eureka es reconocido por el 10,9%. No obstante, entre quienes identifican los canales, la percepción sobre el acceso es ampliamente favorable: el 89,6% considera que Canal Capital es de fácil acceso y, en el caso de Eureka, esta valoración positiva supera el 82%. Estos datos indican que, una vez conocidos, ambos canales son percibidos como accesibles para la ciudadanía.
+Este hallazgo confirma que los desafíos principales se ubican en el plano del posicionamiento, la recordación y el reconocimiento dentro del conjunto de la ciudadanía.
+</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>54,60%</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>Población</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>103</v>
+      </c>
+      <c r="B281" t="n">
+        <v>2</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Imagen de marca y recordación de la programación</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Las asociaciones espontáneas y las valoraciones recogidas muestran que Canal Capital es reconocido por su vínculo con la ciudad, la cultura y la información de interés público. No obstante, la recordación de programas específicos es parcial y se concentra en algunos contenidos puntuales. Aun así, la valoración general del canal es ampliamente positiva, más del 85% de quienes lo conocen reconoce su aporte cultural e informativo. 
+Esta solidez en la imagen de marca constituye un activo relevante, que puede aprovecharse para fortalecer la recordación de la programación y profundizar la conexión con las audiencias.
+</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>Quienes conocen</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>103</v>
+      </c>
+      <c r="B282" t="n">
+        <v>3</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Consumo audiovisual infantil mayoritariamente solitario</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Los talleres participativos permitieron identificar que los hábitos de consumo audiovisual de niños y niñas se configuran principalmente en el ámbito doméstico y bajo lógicas de intimidad y rutina cotidiana. El consumo se representa mayoritariamente como una práctica individual, lo que sugiere una relación directa y personalizada con los contenidos audiovisuales. No obstante, esta experiencia solitaria convive con formas de acompañamiento familiar, especialmente con hermanos y madres, lo que indica que el consumo audiovisual también cumple una función relacional dentro del hogar, aunque de manera secundaria. La baja presencia de figuras adultas como el padre y de otros acompañantes refuerza la idea de una práctica centrada en la autonomía infantil y en dinámicas propias del tiempo libre.
+</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr"/>
+      <c r="F282" t="inlineStr"/>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>103</v>
+      </c>
+      <c r="B283" t="n">
+        <v>4</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Los niños y niñas se vinculan frente a los contenidos audiovisuales principalmente alrededor de los mensajes que transmiten, y su propia experiencia personal</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El análisis de las preferencias frente a los contenidos del canal Eureka muestra que las opiniones infantiles se expresan principalmente a través de valoraciones afectivas y apreciaciones temáticas. Las categorías emergentes con mayor frecuencia corresponden a sensaciones como gusto, aburrimiento, interés o miedo, así como a referencias directas a los temas abordados por los programas. Esto sugiere que la recepción se construye desde una experiencia inmediata y emocional del visionado, más que desde una reflexión técnica o narrativa elaborada. Los elementos técnicos y las referencias explícitas a la experiencia personal aparecen de manera marginal, lo que indica que, en este contexto metodológico, los niños y niñas priorizan la reacción emocional y el contenido del mensaje.
+</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr"/>
+      <c r="F283" t="inlineStr"/>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>105</v>
+      </c>
+      <c r="B284" t="n">
+        <v>1</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Libro al Viento como encuentro ocasional con la lectura</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Los resultados muestran que Libro al Viento funciona principalmente como una oportunidad ocasional de encuentro con la lectura, más que como un sistema de préstamo frecuente. La mayoría de las personas que toman libros accede a pocos ejemplares y lo hace de manera puntual. Esta característica es coherente con el diseño del programa y con su presencia en el espacio público, donde el acceso es abierto, espontáneo y no mediado por trámites o registros.</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr"/>
+      <c r="F284" t="inlineStr"/>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>105</v>
+      </c>
+      <c r="B285" t="n">
+        <v>2</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Experiencia de lectura, disfrute, utilidad y apropiación
+</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">La experiencia asociada a los libros de Libro al Viento combina el disfrute con usos prácticos. La lectura aparece vinculada principalmente a la diversión, pero también al trabajo, al aprendizaje y al enriquecimiento cultural, con variaciones según el tipo de entorno. Además, los efectos simbólicos son claros entre quienes conocen el programa: orgullo por su existencia, disfrute de la lectura y reconocimiento de que leer no es solo para especialistas. Estos impactos, aunque concentrados en un grupo reducido, son intensos y significativos.
+</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr"/>
+      <c r="F285" t="inlineStr"/>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>105</v>
+      </c>
+      <c r="B286" t="n">
+        <v>3</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>Presencia urbana y valor cultural del programa</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Libro al Viento es percibido como un proyecto cultural con presencia en múltiples espacios de la ciudad, lo que refuerza su carácter de política cultural urbana. Su circulación por bibliotecas, parques, eventos culturales, instituciones educativas y espacios de tránsito cotidiano lo posiciona como una iniciativa accesible, cercana y reconocible, que trasciende los espacios tradicionales de lectura y se integra a la vida urbana.</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr"/>
+      <c r="F286" t="inlineStr"/>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>105</v>
+      </c>
+      <c r="B287" t="n">
+        <v>4</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Circulación extendida y apropiación simbólica de los libros</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>La manera en que los libros circulan muestra que su valor no se agota en el punto de entrega ni en la regla de devolución. Al conservarlos, regalarlos o compartirlos, las personas expresan una fuerte apropiación simbólica. Esta circulación extendida refuerza la presencia del programa en la vida cotidiana y lo inscribe en trayectorias personales y sociales diversas, aunque también plantea retos para la disponibilidad y sostenibilidad del sistema de dispensadores.</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr"/>
+      <c r="F287" t="inlineStr"/>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>105</v>
+      </c>
+      <c r="B288" t="n">
+        <v>5</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El libro como objeto social situado: inserción comunitaria y política cultural </t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Las cartografías sociales evidencian que los libros del programa Libro al Viento se integran a prácticas sociales concretas y territorialmente situadas, más allá de su simple circulación física. Los libros se insertan en dinámicas comunitarias, educativas y cotidianas, adquiriendo sentidos diversos según los contextos sociales y territoriales de cada taller. En este sentido, Libro al Viento se configura como una política cultural situada, cuyos efectos dependen de las relaciones sociales que median la apropiación del libro. Las cartografías complementan el sondeo cuantitativo al mostrar cómo los libros se anclan, circulan y se resignifican en la vida cotidiana, dando lugar a circuitos múltiples y no lineales de uso. 
+</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr"/>
+      <c r="F288" t="inlineStr"/>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>112</v>
+      </c>
+      <c r="B289" t="n">
+        <v>1</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Naturaleza de la creación colectiva
+</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>La creación colectiva se caracteriza por su profunda vocación de horizontalidad, solidaridad y libertad. Más que centrarse en la obtención de un producto final, privilegia el proceso como un espacio vivo de exploración, diálogo y construcción conjunta. En este sentido, se configura como un ejercicio humano y político que desafía las jerarquías tradicionales, redistribuye el poder creativo y habilita formas alternativas de relación y producción cultural.</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr"/>
+      <c r="F289" t="inlineStr"/>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>112</v>
+      </c>
+      <c r="B290" t="n">
+        <v>2</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Metodologías, roles y autoría</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>En los procesos de creación colectiva, las metodologías se construyen desde la participación activa y la co-decisión. Los roles no se imponen de antemano, sino que emergen en función de las necesidades y momentos del proceso, lo que promueve dinámicas más flexibles y colaborativas. El liderazgo se concibe como un acompañamiento empático y orientador, antes que como una instancia de dirección jerárquica. La dramaturgia, por su parte, surge de la investigación, la improvisación y la apertura estructural, y aunque la documentación es una herramienta valiosa, suele ser poco sistemática debido a la naturaleza orgánica del trabajo.</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr"/>
+      <c r="F290" t="inlineStr"/>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>112</v>
+      </c>
+      <c r="B291" t="n">
+        <v>3</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>Interdisciplinariedad y articulación de saberes</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>La creación colectiva se nutre de una integración natural y fluida de múltiples artes, oficios y conocimientos. La apertura metodológica facilita aportes espontáneos entre disciplinas y la incorporación de especialistas externos, enriqueciendo el proceso. La tecnología también se incorpora como recurso creativo y expresivo, privilegiando enfoques de cultura libre y acceso abierto, lo que amplía las posibilidades estéticas y fomenta la innovación en los lenguajes escénicos.</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr"/>
+      <c r="F291" t="inlineStr"/>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>112</v>
+      </c>
+      <c r="B292" t="n">
+        <v>4</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Sostenibilidad e impacto sociocultural</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>La sostenibilidad de estos procesos depende, ante todo, de los vínculos humanos, la confianza entre los participantes y la claridad de un propósito común. En este modelo, la comunidad no es solo receptora, sino coproductora activa del proceso y sus resultados. Esta dinámica favorece transformaciones significativas tanto en el plano personal como en el territorial, fortaleciendo el sentido de pertenencia, la identidad colectiva y los procesos de memoria y cuidado de los territorios.</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr"/>
+      <c r="F292" t="inlineStr"/>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>115</v>
+      </c>
+      <c r="B293" t="n">
+        <v>1</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Patrones de uso y acompañamiento social</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Los resultados muestran que los parques estructurantes priorizados presentan patrones de uso regular, con predominio de visitas semanales y diarias. La asistencia se realiza mayoritariamente en compañía de familiares, y el horario de uso se concentra principalmente en la franja de la mañana. La práctica de deporte o actividad física es la actividad reportada con mayor frecuencia en todos los parques, seguida por usos asociados al acompañamiento y al tránsito cotidiano</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr"/>
+      <c r="F293" t="inlineStr"/>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>115</v>
+      </c>
+      <c r="B294" t="n">
+        <v>2</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Valoración del estado físico y la seguridad</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t xml:space="preserve">La mayoría de las personas encuestadas califica el estado físico y el mantenimiento de los parques como “bueno” o “excelente”. De igual forma, una alta proporción de usuarios manifiesta sentirse segura al visitar estos espacios. No obstante, una parte de la población reporta percepciones de inseguridad, especialmente asociadas a condiciones como la iluminación, lo que coincide con los aspectos físicos señalados como susceptibles de mejora.
+</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr"/>
+      <c r="F294" t="inlineStr"/>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>115</v>
+      </c>
+      <c r="B295" t="n">
+        <v>3</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Reconocimiento comunitario del parque</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Los parques son reconocidos por la mayoría de los usuarios como espacios importantes para su comunidad o barrio. Este reconocimiento se presenta de manera consistente en los cinco parques analizados, lo que describe el papel de estos escenarios como referentes del entorno social y del uso cotidiano del espacio público.
+</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr"/>
+      <c r="F295" t="inlineStr"/>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>115</v>
+      </c>
+      <c r="B296" t="n">
+        <v>4</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Diferencia entre participación reportada e interés declarado</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Los resultados evidencian que la proporción de personas que reporta haber participado en actividades organizadas en los parques es menor que la proporción de usuarios que manifiesta interés en participar en actividades deportivas, recreativas, culturales o comunitarias. Esta diferencia describe una brecha entre la participación efectiva y la disposición declarada por la ciudadanía.
+</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr"/>
+      <c r="F296" t="inlineStr"/>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>115</v>
+      </c>
+      <c r="B297" t="n">
+        <v>5</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Barreras y condiciones para el aprovechamiento</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>La falta de tiempo es la barrera más reportada para el uso y aprovechamiento de los parques, seguida por la percepción de inseguridad y la falta de información sobre la oferta de actividades. Estas barreras se presentan en todos los parques, con variaciones en su magnitud relativa según el escenario.</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr"/>
+      <c r="F297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>116</v>
+      </c>
+      <c r="B298" t="n">
+        <v>1</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">La motivación existe. 
+Las barreras son estructurales y de contexto
+</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ciclovía: la mayoría sabe montar bicicleta y reconoce beneficios claros (ahorro de tiempo/dinero, autonomía).
+Escuela de la Bici: el principal obstáculo inicial no es el desinterés, sino no saber montar, la inseguridad y la falta de confianza.
+</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr"/>
+      <c r="F298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>116</v>
+      </c>
+      <c r="B299" t="n">
+        <v>2</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Los programas generan percepción de impacto, pero de forma diferenciada</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Ciclovía: alta recurrencia y masividad; impacto percibido en actividad física, motivación semanal y uso recreativo de la bicicleta.
+Escuela de la Bici: impacto percibido en aprendizaje, confianza, bienestar emocional y cambio personal, aunque con menor uso posterior por barreras materiales.</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr"/>
+      <c r="F299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>116</v>
+      </c>
+      <c r="B300" t="n">
+        <v>3</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>La bicicleta transforma la vida cotidiana más que la identidad colectiva</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>La sociabilidad se expresa principalmente en vínculos cercanos (familia, amigos) más que en colectivos organizados.
+El principal beneficio percibido es práctico (ahorro de tiempo/dinero, autonomía), seguido de salud y bienestar.</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr"/>
+      <c r="F300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>117</v>
+      </c>
+      <c r="B301" t="n">
+        <v>1</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Comprender la gobernanza deportiva como un sistema complejo, multinivel y en evolución</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Los hallazgos de esta investigación muestran que la gobernanza del deporte, la recreación y la actividad física en Bogotá debería entenderse como un sistema complejo en el que convergen actores públicos, privados, comunitarios y académicos con distintos niveles de autoridad, capacidades y responsabilidades. La revisión de literatura confirma que los modelos contemporáneos de gobernanza combinan mecanismos jerárquicos, colaborativos e híbridos, lo cual coincide con la configuración del ecosistema distrital. Esta perspectiva permite reconocer tanto el valor de las estructuras formales del Sistema Nacional del Deporte como la importancia de los vínculos territoriales, las redes sociales y las prácticas comunitarias que sostienen el funcionamiento cotidiano del sistema.</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr"/>
+      <c r="F301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>117</v>
+      </c>
+      <c r="B302" t="n">
+        <v>2</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Clarificar el papel de los actores como base para mejorar la articulación y corresponsabilidad</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Se considera necesario seguir avanzando en mecanismos que fortalezcan la corresponsabilidad entre niveles de gobierno, organizaciones deportivas, sector privado, ciudadanía y academia. La claridad en los roles y la comprensión de las relaciones entre actores son condiciones esenciales para que la política deportiva distrital evolucione hacia formas más consistentes de cooperación, planificación conjunta y toma de decisiones basada en evidencia, la tipología de actores es un punto de partida para esta definición.</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr"/>
+      <c r="F302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>117</v>
+      </c>
+      <c r="B303" t="n">
+        <v>3</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Aplicar la medición para caracterizar a los actores y fortalecer el sistema de información</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>El desarrollo de las categorías analíticas, del formulario cuantitativo y de la propuesta metodológica cualitativa constituye un insumo clave para avanzar hacia un sistema de información más sólido y útil para la toma de decisiones. La aplicación de estos instrumentos permitirá caracterizar de manera rigurosa a los actores del ecosistema deportivo y facilitará una comprensión más completa, contextualizada y accionable sobre el funcionamiento real del ecosistema deportivo y sobre las oportunidades para fortalecer su gobernanza.</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr"/>
+      <c r="F303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>117</v>
+      </c>
+      <c r="B304" t="n">
+        <v>4</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Usar el instrumento como herramienta progresiva para la mejora de la política pública</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Se recomienda concebir el instrumento desarrollado no como un ejercicio aislado de levantamiento de información, sino como una herramienta estratégica de uso progresivo para el fortalecimiento de la política pública del deporte en Bogotá. Su aplicación periódica y su articulación con otros sistemas de información permitirán identificar brechas, monitorear avances en la articulación institucional y ajustar intervenciones de manera gradual. En este sentido, el instrumento ofrece una base para avanzar hacia procesos de planeación, seguimiento y evaluación más coherentes, orientados al aprendizaje institucional y a la generación de valor público en el ecosistema deportivo.
+En este marco, el instrumento constituye una base para promover procesos de aprendizaje institucional, mejorar la coordinación entre actores y fortalecer la generación de valor público en el ecosistema deportivo, a partir de decisiones informadas y basadas en evidencia.
+</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr"/>
+      <c r="F304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>121</v>
+      </c>
+      <c r="B305" t="n">
+        <v>4</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Mucho orgullo, confianza aún frágil</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>La encuesta muestra un considerable orgullo por Bogotá, pero una confianza interpersonal limitada: la mayoría dice poder confiar en menos de la mitad de las personas. Esta brecha sugiere que el sentido de pertenencia no se traduce automáticamente en cooperación cotidiana. Para cerrarla, los laboratorios deben priorizar mediaciones comunitarias, pedagogía de cuidado del espacio público y acciones que incrementen encuentros repetidos y seguros entre vecinos. Deporte, juego y arte son palancas idóneas para “hacer juntos” con bajas barreras de entrada. Medir confianza barrial antes y después de cada ciclo permitirá verificar si las intervenciones logran convertir orgullo en vínculos efectivos.</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr"/>
+      <c r="F305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>121</v>
+      </c>
+      <c r="B306" t="n">
+        <v>5</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Gobernanza compartida con palancas culturales</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Los hallazgos apuntan a corresponsabilidad distribuida: fuerza pública, entidades distritales, vecinos y JAL son percibidos como actores clave según el tipo de problema. Esta lectura respalda una gobernanza compartida, con roles claros y coordinación por barrio, donde cultura ciudadana, bibliotecas y arte urbano actúan como catalizadores. La priorización debe enfocarse en inseguridad y basuras, conectando intervenciones de seguridad situacional con cuidado del entorno y gestión de residuos. Diseñar participación flexible (horarios extendidos, micro-tareas, reconocimiento simbólico) reduce barreras para ese tercio que no puede involucrarse. Con tableros de seguimiento por barrio, la estrategia podrá iterar con evidencia y escalar lo que funciona.</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr"/>
+      <c r="F306" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update investigaciones, 133 seguridad y justica
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -784,8 +784,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Se desarrollarán dos componentes complementarios: una actualización de la medición sobre hábitos y tendencias de consumo audiovisual en Bogotá, y una investigación cualitativa sobre percepciones ciudadanas respecto a contenidos del canal Eureka. Se busca consolidar información estratégica sobre las audiencias de Canal Capital y su relación con los contenidos infantiles, culturales y educativos del canal.
-</t>
+          <t>La investigación analiza la percepción, el reconocimiento y los hábitos de consumo de contenidos audiovisuales de las audiencias de Bogotá, con énfasis en Canal Capital y Eureka. A partir de un enfoque mixto que combina una encuesta de hogares y talleres con audiencias infantiles, el estudio caracteriza las formas de acceso, uso e integración de los contenidos audiovisuales en la vida cotidiana de públicos adultos y de niños, niñas, jóvenes y adolescentes. Los resultados ofrecen un panorama actualizado de la relación de la ciudadanía con ambos canales y aportan insumos estratégicos para fortalecer su visibilidad, posicionamiento y vínculo con las audiencias.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -851,7 +850,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Evaluar los impactos sociales, culturales y económicos de festivales organizados por la FUGA en el centro de Bogotá.</t>
+          <t>Evaluación de los impactos sociales, culturales y económicos de festivales organizados por la FUGA en el centro de Bogotá.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -895,7 +894,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>FUGA - Monumentum - Centro - Música - Festivales</t>
+          <t>FUGA - Monumentum - Centro - Música - Festivales, fundación gilberto alzate avendaño, centro, eventos, economía cultural</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -918,7 +917,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sondeo conmemorativo que recoge percepciones ciudadanas sobre la trayectoria, pertinencia y transformaciones del Programa Libro al Viento, a propósito de sus 20 años.</t>
+          <t>La investigación analiza los usos sociales del Programa Libro al Viento en Bogotá, a partir de un enfoque mixto que combina herramientas cuantitativas y cualitativas para comprender las prácticas de lectura en el espacio público. El estudio se centra en las formas de conocimiento, apropiación y circulación de los libros, así como en los sentidos que la ciudadanía atribuye al programa en su vida cotidiana. Los resultados permiten caracterizar a Libro al Viento como una experiencia de encuentro con la lectura integrada a la dinámica urbana, e identificar tanto sus aportes simbólicos como los principales retos para su visibilidad y sostenibilidad.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1553,7 +1552,8 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Análisis del acceso a parques, canchas y ciclovías en zonas de alta densidad poblacional y sectores de bajos recursos, incorporando variables geoespaciales y revisión de políticas públicas.</t>
+          <t xml:space="preserve">La investigación analiza el uso, la apropiación y el aprovechamiento de cinco parques estructurantes de Bogotá a partir de información recolectada mediante encuestas presenciales a personas usuarias. El estudio caracteriza los perfiles de uso, los horarios, las actividades realizadas, con énfasis en la práctica de actividad física, y las formas de acompañamiento, así como las percepciones sobre el estado físico, el mantenimiento y la seguridad de los espacios. Los resultados identifican barreras y oportunidades para fortalecer el uso de los parques y evidencian una brecha entre el interés declarado y la participación efectiva en actividades culturales y recreativas.
+</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Identificar los productos, saberes y tradiciones que definen la gastronomía de Bogotá, con el fin de fortalecer su apropiación, difusión y valor cultural, promoviendo el orgullo por lo local.</t>
+          <t>Identificación de los productos, saberes y tradiciones que definen la gastronomía de Bogotá, con el fin de fortalecer su apropiación, difusión y valor cultural, promoviendo el orgullo por lo local.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>cultura, oferta cultural, gastronomía, restaurantes, comida</t>
+          <t>cultura, oferta cultural, gastronomía, restaurantes, comida, sabor bogotá</t>
         </is>
       </c>
       <c r="M25" t="inlineStr"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>ambiente, residuos, espacio público, recicladores, basuras, reciclaje</t>
+          <t>ambiente, residuos, espacio público, recicladores, basuras, reciclaje, ambiental</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2104,7 +2104,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Realizar un sondeo sobre el consumo de agua  en dos zonas de Bogotá analizando factores culturales, comportamentales y ambientales que afectan su uso</t>
+          <t>Realizar un sondeo sobre el consumo de agua en dos zonas de Bogotá analizando factores culturales, comportamentales y ambientales que afectan su uso</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Investigación centrada en el centro histórico de Bogotá, que explore la relación de la ciudadanía con el espacio público desde un enfoque de género, los imaginarios y representaciones sociales sobre este territorio, así como la relación de las personas con los bienes muebles de carácter patrimonial y las motivaciones que impulsan las intervenciones gráficas en el espacio</t>
+          <t>Exploración de la relación de la ciudadanía con el espacio público desde un enfoque de género, los imaginarios y representaciones sociales sobre este territorio, así como la relación de las personas con los bienes muebles de carácter patrimonial y las motivaciones que impulsan las intervenciones gráficas en el espacio. Investigación centrada en el centro histórico de Bogotá.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2319,7 +2319,11 @@
           <t>https://drive.google.com/drive/folders/1vVogB5CLhZRhice-_J7af0PcyNBkby7C</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr"/>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>género enfoque espacio público centro de bogotá</t>
+        </is>
+      </c>
       <c r="M30" t="inlineStr">
         <is>
           <t>Daniel Galeano</t>
@@ -2622,7 +2626,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Encuesta de Seguridad, justicia y convivencia. Diagnosticar posibles barreras para la denuncia y el acceso a la justicia así como los principales facilitadores que podrían promover una mayor confianza y uso del sistema judicial.</t>
+          <t>Encuesta de Seguridad, justicia y convivencia. Diagnóstico de posibles barreras para la denuncia y el acceso a la justicia así como los principales facilitadores que podrían promover una mayor confianza y uso del sistema judicial.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2659,7 +2663,11 @@
           <t>https://drive.google.com/drive/folders/1MWFewR9L0BNvHjLM7eObX-qfanPu4MYj</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr"/>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>seguridad, mujer, justicia, género, enfoque, confianza institucional, masculinidad y violencia sexual, violencia sexual en adolescentes, jóvenes ofensores sexuales, masculinidades hegemónicas, violencia sexual intrafamiliar, violencia basada en género, cultura de la violación, consentimiento y poder, factores psicosociales de la violencia sexual, educación sexual integral, justicia restaurativa con hombres, prevención de violencia sexual</t>
+        </is>
+      </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="n">
         <v>2025</v>
@@ -20625,9 +20633,21 @@
           <t>Informe final</t>
         </is>
       </c>
-      <c r="C584" t="inlineStr"/>
-      <c r="D584" t="inlineStr"/>
-      <c r="E584" t="inlineStr"/>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>Informe Libro al Viento 2025</t>
+        </is>
+      </c>
+      <c r="D584" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E584" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1gEDdQ_9ggb2qbkisdnS3h-SixumLgwVD/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="585">
       <c r="A585" t="n">
@@ -20733,10 +20753,26 @@
       <c r="A589" t="n">
         <v>105</v>
       </c>
-      <c r="B589" t="inlineStr"/>
-      <c r="C589" t="inlineStr"/>
-      <c r="D589" t="inlineStr"/>
-      <c r="E589" t="inlineStr"/>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>Guía metodológica Talleres Consumo Audiovisual de Audiencias Infantiles</t>
+        </is>
+      </c>
+      <c r="D589" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E589" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1tAdGD8sp6Rzn-d8_J6FLIEpZ7KexawEk/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="590">
       <c r="A590" t="n">
@@ -23285,10 +23321,26 @@
       <c r="A752" t="n">
         <v>133</v>
       </c>
-      <c r="B752" t="inlineStr"/>
-      <c r="C752" t="inlineStr"/>
-      <c r="D752" t="inlineStr"/>
-      <c r="E752" t="inlineStr"/>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="D752" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E752" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/16AYD-Y9HF8O45rYDxH6a_pgEbUjv_Ofo/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="753">
       <c r="A753" t="n">
@@ -23626,7 +23678,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F306"/>
+  <dimension ref="A1:F311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29171,6 +29223,106 @@
       <c r="E306" t="inlineStr"/>
       <c r="F306" t="inlineStr"/>
     </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>133</v>
+      </c>
+      <c r="B307" t="n">
+        <v>1</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>La violencia sexual no es un desvío, es un mandato aprendido</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>La investigación evidencia que la violencia sexual no aparece como un hecho aislado o accidental, sino como una expresión coherente de la masculinidad hegemónica aprendida en distintos entornos sociales. El ejercicio de la violencia se asocia a expectativas de poder, control, dominación y validación identitaria masculina. Estas prácticas son reforzadas por la familia, los pares, los medios y, en ocasiones, por la ausencia de una educación sexual integral. La violencia se convierte así en un mecanismo para “demostrar hombría”, más que en una desviación individual.</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr"/>
+      <c r="F307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>133</v>
+      </c>
+      <c r="B308" t="n">
+        <v>2</v>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>El hogar es el principal escenario de riesgo y silenciamiento</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Una proporción significativa de los hechos de violencia sexual ocurre en la vivienda y es ejercida por personas cercanas a la víctima. El entorno familiar, lejos de ser siempre un espacio protector, puede funcionar como un escenario de encubrimiento, negación o minimización del daño. Esta dinámica dificulta la denuncia, la intervención temprana y la activación de rutas de protección. La naturalización del abuso dentro del hogar refuerza el silencio y perpetúa la violencia.</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr"/>
+      <c r="F308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>133</v>
+      </c>
+      <c r="B309" t="n">
+        <v>3</v>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Negar, minimizar y justificar: la principal barrera para la responsabilidad</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Tanto los ofensores como sus familias tienden a negar, minimizar o justificar la violencia sexual, lo que constituye una barrera estructural para los procesos de responsabilización y reparación. Estas narrativas desplazan la culpa hacia las víctimas, apelan a la cercanía afectiva o normalizan el abuso como “error” o “juego”. Esta falta de reconocimiento del daño limita la efectividad de las sanciones y de los procesos restaurativos. Sin responsabilidad no hay transformación posible.</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr"/>
+      <c r="F309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>133</v>
+      </c>
+      <c r="B310" t="n">
+        <v>4</v>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>La sexualidad se aprende sin consentimiento ni empatía</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Los hallazgos muestran que muchos jóvenes adquieren conocimientos sobre sexualidad a través de pares, pornografía y medios, sin mediación crítica ni enfoque ético. Esto produce ideas distorsionadas sobre el consentimiento, la reciprocidad y el deseo, normalizando la cosificación y la dominación. La ausencia de educación sexual integral favorece prácticas sexuales violentas y dificulta el desarrollo de empatía hacia las víctimas. La sexualidad se configura más como ejercicio de poder que como relación.</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr"/>
+      <c r="F310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>133</v>
+      </c>
+      <c r="B311" t="n">
+        <v>5</v>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Transformar las masculinidades es clave para prevenir la violencia</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>La erradicación de la violencia sexual requiere intervenir directamente en la construcción social de las masculinidades. El estudio muestra que trabajar únicamente sobre las víctimas o desde una lógica punitiva es insuficiente. Se necesitan estrategias preventivas, educativas, culturales y restaurativas que involucren activamente a los hombres, desde la infancia hasta la adultez. Promover masculinidades no violentas es una condición central para la justicia, la convivencia y la transformación cultural.</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr"/>
+      <c r="F311" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update investigaciones, sabor bogota
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -575,39 +575,35 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Caracterización de Entidades Sin Ánimo de Lucro 2025</t>
+          <t xml:space="preserve">Impactos de la transformación digital en la cultura: </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Segunda etapa del estudio sectorial iniciado en 2024, enfocado en actualizar y profundizar la caracterización de las Entidades Sin Ánimo de Lucro (ESAL) adscritas a la SCRD, abordando aspectos de infraestructura, oferta de valor, sostenibilidad financiera y modelos de gestión.</t>
+          <t>Estudio comparativo de los impactos de la transformación digital en la cultura en tres ciudades de Iberoamérica: Bogotá, Ciudad de México y Río de Janeiro.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SCRD</t>
+          <t>Sector</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>202591004200100004E</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Gobernanza - DPJ</t>
-        </is>
-      </c>
+          <t>202591004200100024E</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>5 Finalizada</t>
+          <t>2 En ejecución</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -615,93 +611,68 @@
           <t>Sector Cultura</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Realizar un análisis de la información recolectada en los formularios aplicados a las ESALES 2024 y 2025, en términos de oferta de valor, estructura organizacional y herramientas de sostenibilidad.
-</t>
-        </is>
-      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1GPyUMdbxqqJ-fja7DNFswVLKyoucNKao</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Dirección de Personas Juridicas, ESALES Culturales, Oferta de Valor, Infraestructura, Sostenibilidad, economía</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Giovani Moreno,Carlos Suárez </t>
-        </is>
-      </c>
+          <t>https://drive.google.com/drive/folders/1UCBoZjmBtwVBZ7LWWCh_1djcuAc4g4rc</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Indicadores del Sistema Distrital de Formación Artística y Cultural - SIDFAC</t>
+          <t>Cultura ciudadana en TransMilenio: confianza y orgullo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Diseño de una batería de indicadores basada en fuentes existentes, como la Encuesta Bienal de Culturas y el Índice de Derechos Culturales, para evaluar variables asociadas a la formación artística, cultural y patrimonial. Los resultados servirán como insumo técnico para la actualización normativa del SIDFAC.</t>
+          <t>Medición de las percepciones ciudadanas de confianza, orgullo y apropiación en el sistema TransMilenio. A partir de una encuesta aplicada a personas usuarias en estaciones y portales priorizados, el estudio analiza estas dimensiones junto con emociones y comportamientos asociados al uso del sistema, con el objetivo de generar evidencia para comprender la experiencia cotidiana, evaluar procesos de transformación cultural y orientar acciones de cultura ciudadana basadas en datos.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>SCRD</t>
+          <t>Sector</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>202591004200100029E</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>DACP</t>
-        </is>
-      </c>
+          <t>202591004200100027E</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>5 Finalizada</t>
+          <t>2 En ejecución</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Diseñar los indicadores que permitan hacer seguimiento a los procesos de formación en arte, cultura y patrimonio en el Distrito y su impacto a nivel de ciudad y localidades.</t>
-        </is>
-      </c>
+          <t>Cultura Ciudadana</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1clr5wOumCR15k_x2ft_Ltyg1vDRlHBHK</t>
+          <t>https://drive.google.com/drive/folders/1Oevcfhqb2fsyzMSPchXqH7WxkIbqvNw_</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Formación, prácticas, cultura, patrimonio, arte</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Gisela Castrillón, Diego Lemus, Germán Urbina</t>
-        </is>
-      </c>
+          <t>transporte, movilidad, transmilenio, estaciones, colados, confianza, orgullo, apropiación, confianza en TransMilenio, orgullo ciudadano, apropiación del sistema de transporte, cultura ciudadana Bogotá, percepción ciudadana transporte público, convivencia en TransMilenio, emociones y comportamiento ciudadano, investigación cultura ciudadana, medición de percepción ciudadana, transformación cultural urbana</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
         <v>2025</v>
       </c>
@@ -841,31 +812,31 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Impacto de festivales de gran formato en el Centro de Bogotá</t>
+          <t>Caracterización de Entidades Sin Ánimo de Lucro 2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Evaluación de los impactos sociales, culturales y económicos de festivales organizados por la FUGA en el centro de Bogotá.</t>
+          <t>Segunda etapa del estudio sectorial iniciado en 2024, enfocado en actualizar y profundizar la caracterización de las Entidades Sin Ánimo de Lucro (ESAL) adscritas a la SCRD, abordando aspectos de infraestructura, oferta de valor, sostenibilidad financiera y modelos de gestión.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FUGA</t>
+          <t>SCRD</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>202591004200100007E</t>
+          <t>202591004200100004E</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FUGA SGCB</t>
+          <t>Gobernanza - DPJ</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -883,306 +854,306 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
+          <t xml:space="preserve">Realizar un análisis de la información recolectada en los formularios aplicados a las ESALES 2024 y 2025, en términos de oferta de valor, estructura organizacional y herramientas de sostenibilidad.
+</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1GPyUMdbxqqJ-fja7DNFswVLKyoucNKao</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Dirección de Personas Juridicas, ESALES Culturales, Oferta de Valor, Infraestructura, Sostenibilidad, economía</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Giovani Moreno,Carlos Suárez </t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>101</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Indicadores del Sistema Distrital de Formación Artística y Cultural - SIDFAC</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Diseño de una batería de indicadores basada en fuentes existentes, como la Encuesta Bienal de Culturas y el Índice de Derechos Culturales, para evaluar variables asociadas a la formación artística, cultural y patrimonial. Los resultados servirán como insumo técnico para la actualización normativa del SIDFAC.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>SCRD</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>202591004200100029E</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>DACP</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Diseñar los indicadores que permitan hacer seguimiento a los procesos de formación en arte, cultura y patrimonio en el Distrito y su impacto a nivel de ciudad y localidades.</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1clr5wOumCR15k_x2ft_Ltyg1vDRlHBHK</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Formación, prácticas, cultura, patrimonio, arte</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Gisela Castrillón, Diego Lemus, Germán Urbina</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>105</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Sondeo sobre el Programa Libro al Viento</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>La investigación analiza los usos sociales del Programa Libro al Viento en Bogotá, a partir de un enfoque mixto que combina herramientas cuantitativas y cualitativas para comprender las prácticas de lectura en el espacio público. El estudio se centra en las formas de conocimiento, apropiación y circulación de los libros, así como en los sentidos que la ciudadanía atribuye al programa en su vida cotidiana. Los resultados permiten caracterizar a Libro al Viento como una experiencia de encuentro con la lectura integrada a la dinámica urbana, e identificar tanto sus aportes simbólicos como los principales retos para su visibilidad y sostenibilidad.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>IDARTES</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>202591004200100008E</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>IDARTES G Literatura</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1m2paVRCF0WLmM6GCJXbDKsrppfiwtB73</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>lectura, literatura, aniversario, leo</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Carlos Suárez, Giovani Moreno</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>104</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Impacto de festivales de gran formato en el Centro de Bogotá</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Evaluación de los impactos sociales, culturales y económicos de festivales organizados por la FUGA en el centro de Bogotá.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>FUGA</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>202591004200100007E</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>FUGA SGCB</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
           <t xml:space="preserve">Medir el impacto económico, sociocultural y ambiental de los eventos relacionados con cultura, patrimonio, recreación y deporte  de la ciudad de Bogotá.
 </t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>https://drive.google.com/drive/folders/1C_bdCxznPjXK63YsleE-hDTOQ1zmjfuB</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>FUGA - Monumentum - Centro - Música - Festivales, fundación gilberto alzate avendaño, centro, eventos, economía cultural</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>Viviana Rodríguez, Laura Lozano, Giovani Moreno, Diego Lemus</t>
         </is>
       </c>
-      <c r="N7" t="n">
+      <c r="N10" t="n">
         <v>2025</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>105</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Sondeo sobre el Programa Libro al Viento</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>La investigación analiza los usos sociales del Programa Libro al Viento en Bogotá, a partir de un enfoque mixto que combina herramientas cuantitativas y cualitativas para comprender las prácticas de lectura en el espacio público. El estudio se centra en las formas de conocimiento, apropiación y circulación de los libros, así como en los sentidos que la ciudadanía atribuye al programa en su vida cotidiana. Los resultados permiten caracterizar a Libro al Viento como una experiencia de encuentro con la lectura integrada a la dinámica urbana, e identificar tanto sus aportes simbólicos como los principales retos para su visibilidad y sostenibilidad.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="n">
+        <v>106</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Percepción ciudadana sobre el Premio Luis Caballero</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Medir la percepción del público visitante sobre el Premio Luis Caballero, valorando conocimientos, emociones y sentido otorgado a las exposiciones, para orientar futuras ediciones y estrategias de mediación.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>IDARTES</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>202591004200100008E</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>IDARTES G Literatura</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>202591004200100009E</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>IDARTES G Plásticas</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>5 Finalizada</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Sector Cultura</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1m2paVRCF0WLmM6GCJXbDKsrppfiwtB73</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>lectura, literatura, aniversario, leo</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Carlos Suárez, Giovani Moreno</t>
-        </is>
-      </c>
-      <c r="N8" t="n">
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1qEkfdB8IzvAAAQS-Q6Dbmi1B1iui7bhP</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="n">
         <v>2025</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>106</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Percepción ciudadana sobre el Premio Luis Caballero</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Medir la percepción del público visitante sobre el Premio Luis Caballero, valorando conocimientos, emociones y sentido otorgado a las exposiciones, para orientar futuras ediciones y estrategias de mediación.</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>IDARTES</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>202591004200100009E</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>IDARTES G Plásticas</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1qEkfdB8IzvAAAQS-Q6Dbmi1B1iui7bhP</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="12">
+      <c r="A12" t="n">
         <v>107</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Caracterización del sector circo – Fase 2</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve">Segunda fase del diagnóstico del sector circense en Bogotá, que ampliará el inventario georreferenciado de agentes y espacios, e incluirá un análisis de las condiciones técnicas, económicas y de oferta para fortalecer estrategias de apoyo al sector.
 </t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>IDARTES</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>202591004200100010E</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>IDARTES G Dramático</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Profundizar en el conocimiento de las características, necesidades y distribución territorial del sector circense en Bogotá, con el fin de fortalecer los lineamientos para la formulación de políticas públicas y programas que respondan de manera pertinente a su realidad e incidencia en las localidades de la ciudad.</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1hf4-sbaDvKEyxKOBEDUutNLalZjrUZbp</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Circo - Prácticas circenses - georreferenciación - Caracterización espacios y actores</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Viviana Rodríguez, Carlos Suárez </t>
-        </is>
-      </c>
-      <c r="N10" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>108</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Festivales al Parque</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Caracterizar las percepciones, prácticas y valoraciones de la ciudadanía frente a los Festivales al Parque, mediante técnicas cualitativas y cuantitativas, con especial énfasis en los 30 años de Rock al Parque.</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>IDARTES</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>202591004200100011E</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>IDARTES G Música</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Medir el impacto económico, sociocultural y ambiental de los eventos relacionados con cultura, patrimonio, recreación y deporte  de la ciudad de Bogotá.
-</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/196DgrWaLJDfw8elriPEi0BkqesPoofkQ</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Festival - Música - Asistentes - Emprendedores - Artistas</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>VivianaRodríguez, Laura Lozano, Giovani Moreno, Diego Lemus</t>
-        </is>
-      </c>
-      <c r="N11" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>109</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Percepciones sobre el Festival Centro 2025</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Análisis de las percepciones de asistentes y actores vinculados al Festival Centro 2025, con base en la información ya recolectada, para identificar oportunidades de mejora y fortalecer futuras ediciones.</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>FUGA</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>202591004200100012E</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>FUGA - Artística</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -1200,20 +1171,24 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Realizar el análisis de resultados de la medición del Festival Centro 2025, centrada en la aplicaicón del instrumento orientado a asistentes</t>
+          <t>Profundizar en el conocimiento de las características, necesidades y distribución territorial del sector circense en Bogotá, con el fin de fortalecer los lineamientos para la formulación de políticas públicas y programas que respondan de manera pertinente a su realidad e incidencia en las localidades de la ciudad.</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1btfJ10uYqzIsb9OBp_9cS1u-KQ_WPMr8</t>
+          <t>https://drive.google.com/drive/folders/1hf4-sbaDvKEyxKOBEDUutNLalZjrUZbp</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Festival - Música - Centro - Asistentes</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr"/>
+          <t>Circo - Prácticas circenses - georreferenciación - Caracterización espacios y actores</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Viviana Rodríguez, Carlos Suárez </t>
+        </is>
+      </c>
       <c r="N12" t="n">
         <v>2025</v>
       </c>
@@ -1344,32 +1319,31 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Teatro de creación colectiva</t>
+          <t>Festivales al Parque</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Continuación del proceso de identificación y caracterización de grupos y espacios vinculados al teatro de creación colectiva en localidades de Bogotá, con priorización territorial y fases sucesivas de aplicación y sistematización.
-</t>
+          <t>Caracterizar las percepciones, prácticas y valoraciones de la ciudadanía frente a los Festivales al Parque, mediante técnicas cualitativas y cuantitativas, con especial énfasis en los 30 años de Rock al Parque.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>IDPC</t>
+          <t>IDARTES</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>202591004200100015E</t>
+          <t>202591004200100011E</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>IDPC Divulgación</t>
+          <t>IDARTES G Música</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1387,22 +1361,23 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Avanzar en la ejecución de las fases 2 y 3 del proyecto, mediante el levantamiento, sistematización y análisis de información sobre grupos, colectivos, organizaciones y espacios en las distintas localidades de la ciudad, con el fin de fortalecer el directorio de actores, aplicar instrumentos de caracterización en territorios priorizados y divulgar los resultados en el marco del Colectivo de la Salvaguardia.</t>
+          <t xml:space="preserve">Medir el impacto económico, sociocultural y ambiental de los eventos relacionados con cultura, patrimonio, recreación y deporte  de la ciudad de Bogotá.
+</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/13jmKoZRuSXFpQfQpwt5x18N_T5o5Quzs</t>
+          <t>https://drive.google.com/drive/folders/196DgrWaLJDfw8elriPEi0BkqesPoofkQ</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Creación colectiva - Teatro - Agrupaciones teatrales</t>
+          <t>Festival - Música - Asistentes - Emprendedores - Artistas</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Viviana Rodríguez</t>
+          <t>VivianaRodríguez, Laura Lozano, Giovani Moreno, Diego Lemus</t>
         </is>
       </c>
       <c r="N15" t="n">
@@ -1411,31 +1386,31 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>EBC - LEO 2025</t>
+          <t>Percepciones sobre el Festival Centro 2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Diseño, aplicación y análisis del módulo de Lectura, Escritura y Oralidad en la Encuesta Bienal de Culturas 2025, en articulación con la Dirección de Lectura y Bibliotecas. Incluye trabajo de campo por muestreo probabilístico, procesamiento de datos y análisis de resultados.</t>
+          <t>Análisis de las percepciones de asistentes y actores vinculados al Festival Centro 2025, con base en la información ya recolectada, para identificar oportunidades de mejora y fortalecer futuras ediciones.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>SCRD</t>
+          <t>FUGA</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>202591004200100016E</t>
+          <t>202591004200100012E</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>SCCGC</t>
+          <t>FUGA - Artística</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1453,24 +1428,20 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Obtener información que permita hacer seguimiento a la política pública LEO y caracterizar los hábitos de lectura, escritura y oralidad. Recoge los conocimientos, actitudes, valoraciones, emociones y percepciones frente a la lectura, la escritura y la oralidad.</t>
+          <t>Realizar el análisis de resultados de la medición del Festival Centro 2025, centrada en la aplicaicón del instrumento orientado a asistentes</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1sTNCho5MGwcW5BVNJa4KYzMzVgdYCLeG</t>
+          <t>https://drive.google.com/drive/folders/1btfJ10uYqzIsb9OBp_9cS1u-KQ_WPMr8</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Lectura - Escritura - Oralidad -EBC</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>Viviana Rodríguez, Carlos Suárez, Giovani Moreno, Laura Lozano</t>
-        </is>
-      </c>
+          <t>Festival - Música - Centro - Asistentes</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
         <v>2025</v>
       </c>
@@ -1611,7 +1582,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Evaluar el impacto de las iniciativas Ciclovía y Escuela de la Bici en la actividad física y los hábitos de movilidad de los bogotanos.</t>
+          <t>La investigación presenta los principales resultados y hallazgos sobre la percepción ciudadana del aporte de los programas Ciclovía y Escuela de la Bici a los hábitos de movilidad y actividad física en Bogotá. El análisis muestra el papel de la bicicleta como práctica cotidiana asociada a la movilidad sostenible, la actividad física y el fortalecimiento de vínculos sociales, así como las barreras percibidas para una participación equitativa, especialmente en términos de seguridad y cargas de cuidado. En este marco, la Escuela de la Bici se reconoce como un programa complementario que acompaña a personas interesadas en usar la bicicleta, pero que enfrentan barreras de aprendizaje y confianza, y que contribuye a la incorporación de esta práctica en la vida cotidiana, aunque persisten limitaciones materiales para su uso fuera del programa.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1673,7 +1644,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Análisis de modelos de colaboración entre el sector público, privado y organizaciones sociales en el desarrollo del deporte en Bogotá, con énfasis en el apoyo a deportistas de alto rendimiento.</t>
+          <t>La investigación documenta el proceso de diseño de insumos metodológicos para la medición y caracterización del ecosistema de gobernanza del deporte, la recreación y la actividad física en Bogotá. A partir de la revisión de literatura, el análisis de esquemas de gobernanza y la identificación de actores clave, el estudio construye categorías analíticas, instrumentos de recolección de información y orientaciones metodológicas que constituyen una base conceptual y operativa. Los resultados aportan insumos para fortalecer el sistema de información del sector y apoyar procesos de planeación, articulación institucional y toma de decisiones orientadas a la generación de valor público.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1851,31 +1822,32 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Medición de eventos culturales de gran formato de la SCRD</t>
+          <t>Teatro de creación colectiva</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Evaluar el impacto cultural, social y económico de los principales eventos de gran formato organizados por la SCRD, incluyendo el Concurso Internacional de Violín, la Feria de Navidad, el Encuentro de Cultura en Iberoamérica y la Bienal de Arte y Ciudad.</t>
+          <t xml:space="preserve">Continuación del proceso de identificación y caracterización de grupos y espacios vinculados al teatro de creación colectiva en localidades de Bogotá, con priorización territorial y fases sucesivas de aplicación y sistematización.
+</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>SCRD</t>
+          <t>IDPC</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>202591004200100023E</t>
+          <t>202591004200100015E</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>SCCGC</t>
+          <t>IDPC Divulgación</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1893,18 +1865,22 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Realizar las mediciones para la evaluación del impacto cultural, social y económico de los principales eventos de gran formato organizados por la SCRD, (el Concurso Internacional de Violín, la Feria de Navidad, el Encuentro de Cultura en Iberoamérica y la Bienal de Arte y Ciudad.)</t>
+          <t>Avanzar en la ejecución de las fases 2 y 3 del proyecto, mediante el levantamiento, sistematización y análisis de información sobre grupos, colectivos, organizaciones y espacios en las distintas localidades de la ciudad, con el fin de fortalecer el directorio de actores, aplicar instrumentos de caracterización en territorios priorizados y divulgar los resultados en el marco del Colectivo de la Salvaguardia.</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1eoJ-Dh54kQxI4zIwJ-tAeGnd9IOTOUD_</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr"/>
+          <t>https://drive.google.com/drive/folders/13jmKoZRuSXFpQfQpwt5x18N_T5o5Quzs</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Creación colectiva - Teatro - Agrupaciones teatrales</t>
+        </is>
+      </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Viviana Rodríguez, Carlos Suárez, Giovani Moreno, Laura Lozano</t>
+          <t>Viviana Rodríguez</t>
         </is>
       </c>
       <c r="N23" t="n">
@@ -1913,16 +1889,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Herramienta para el registro y seguimiento Barrios Vivos 2025</t>
+          <t>EBC - LEO 2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Diseñar un mecanismo de registro de información de la ejecución de los laboratorios de la Estrategia Barrios Vivos en 2025, útil para la caracterización de los laboratorios, personas asociadas, actividades, conclusiones, relación de contenidos y productos.</t>
+          <t>Diseño, aplicación y análisis del módulo de Lectura, Escritura y Oralidad en la Encuesta Bienal de Culturas 2025, en articulación con la Dirección de Lectura y Bibliotecas. Incluye trabajo de campo por muestreo probabilístico, procesamiento de datos y análisis de resultados.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1932,12 +1908,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>202591004200100026E</t>
+          <t>202591004200100016E</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Gobernanza - DALP</t>
+          <t>SCCGC</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1950,23 +1926,27 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Cultura Ciudadana</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr"/>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Obtener información que permita hacer seguimiento a la política pública LEO y caracterizar los hábitos de lectura, escritura y oralidad. Recoge los conocimientos, actitudes, valoraciones, emociones y percepciones frente a la lectura, la escritura y la oralidad.</t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1g23Z2SwPIT7u3nLxuX75n9eSk7T93FP3</t>
+          <t>https://drive.google.com/drive/folders/1sTNCho5MGwcW5BVNJa4KYzMzVgdYCLeG</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>barrios vivos, territorial, sistemas de información, cronograma, actividades, descripción, seguimiento, monitoreo</t>
+          <t>Lectura - Escritura - Oralidad -EBC</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Mauricio Ojeda, Mábel Ayala</t>
+          <t>Viviana Rodríguez, Carlos Suárez, Giovani Moreno, Laura Lozano</t>
         </is>
       </c>
       <c r="N24" t="n">
@@ -1975,16 +1955,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Sabores y productos de identidad gastronómica</t>
+          <t>Herramienta para el registro y seguimiento Barrios Vivos 2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Identificación de los productos, saberes y tradiciones que definen la gastronomía de Bogotá, con el fin de fortalecer su apropiación, difusión y valor cultural, promoviendo el orgullo por lo local.</t>
+          <t>Diseñar un mecanismo de registro de información de la ejecución de los laboratorios de la Estrategia Barrios Vivos en 2025, útil para la caracterización de los laboratorios, personas asociadas, actividades, conclusiones, relación de contenidos y productos.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1994,12 +1974,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>202591004200100030E</t>
+          <t>202591004200100026E</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>SCCGC - DRAC</t>
+          <t>Gobernanza - DALP</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -2018,31 +1998,35 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1fFoEhz2VqUqD_9s0k7Zs7bqcoiev2ZBu</t>
+          <t>https://drive.google.com/drive/folders/1g23Z2SwPIT7u3nLxuX75n9eSk7T93FP3</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>cultura, oferta cultural, gastronomía, restaurantes, comida, sabor bogotá</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr"/>
+          <t>barrios vivos, territorial, sistemas de información, cronograma, actividades, descripción, seguimiento, monitoreo</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Mauricio Ojeda, Mábel Ayala</t>
+        </is>
+      </c>
       <c r="N25" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Comportamiento y factores culturales en la gestión de residuos en Bogotá</t>
+          <t>Medición de eventos culturales de gran formato de la SCRD</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Analizar factores culturales y comportamentales en las dinámicas de recolección y disposición de residuos en Bogotá y evaluar intervenciones de cultura ciudadana realizadas en el marco de la estrategia.</t>
+          <t>Evaluar el impacto cultural, social y económico de los principales eventos de gran formato organizados por la SCRD, incluyendo el Concurso Internacional de Violín, la Feria de Navidad, el Encuentro de Cultura en Iberoamérica y la Bienal de Arte y Ciudad.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2052,12 +2036,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>202591004200100002E</t>
+          <t>202591004200100023E</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>SCCGC - DTC</t>
+          <t>SCCGC</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -2070,23 +2054,23 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Cultura Ciudadana</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr"/>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Realizar las mediciones para la evaluación del impacto cultural, social y económico de los principales eventos de gran formato organizados por la SCRD, (el Concurso Internacional de Violín, la Feria de Navidad, el Encuentro de Cultura en Iberoamérica y la Bienal de Arte y Ciudad.)</t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1HKEB8rfgtEPbbb4LS2AUt2-q1qlZBJZH</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>ambiente, residuos, espacio público, recicladores, basuras, reciclaje, ambiental</t>
-        </is>
-      </c>
+          <t>https://drive.google.com/drive/folders/1eoJ-Dh54kQxI4zIwJ-tAeGnd9IOTOUD_</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Jhonatan Rosas</t>
+          <t>Viviana Rodríguez, Carlos Suárez, Giovani Moreno, Laura Lozano</t>
         </is>
       </c>
       <c r="N26" t="n">
@@ -2095,16 +2079,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Factores culturales, comportamentales y ambientales que inciden en el  ahorro y consumo de agua</t>
+          <t>Sabores y productos de identidad gastronómica</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Realizar un sondeo sobre el consumo de agua en dos zonas de Bogotá analizando factores culturales, comportamentales y ambientales que afectan su uso</t>
+          <t>Identificación de los productos, saberes y tradiciones que definen la gastronomía de Bogotá, con el fin de fortalecer su apropiación, difusión y valor cultural, promoviendo el orgullo por lo local.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2114,12 +2098,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>202491004200100018E</t>
+          <t>202591004200100030E</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>SCCGC - DTC</t>
+          <t>SCCGC - DRAC</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -2138,35 +2122,31 @@
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1w_BWFPcr1o0TkxlngZiWXFI86WUw-l6q</t>
+          <t>https://drive.google.com/drive/folders/1fFoEhz2VqUqD_9s0k7Zs7bqcoiev2ZBu</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>agua, ambiente</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>Jhonatan Rosas</t>
-        </is>
-      </c>
+          <t>cultura, oferta cultural, gastronomía, restaurantes, comida, sabor bogotá, pan, panaderías, emocional</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr"/>
       <c r="N27" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Actualización de indicadores sobre comportamiento cívico y participación ciudadana en los distritos creativos</t>
+          <t>Comportamiento y factores culturales en la gestión de residuos en Bogotá</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Actualización del Índice de Cultura Ciudadana en Distritos Creativos y análisis de relaciones entre agentes culturales. Aporta al seguimiento de la Política de Economía Cultural y Creativa.</t>
+          <t>Análisis de los factores culturales y comportamentales en las dinámicas de recolección y disposición de residuos en Bogotá y evaluación de intervenciones de cultura ciudadana realizadas en el marco de la estrategia de espacio úblico y ambiente.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2176,12 +2156,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>202591004200100031E</t>
+          <t>202591004200100002E</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Gobernanza - DEEP</t>
+          <t>SCCGC - DTC</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -2200,10 +2180,14 @@
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1YSI4dSNBDGnUfUJTvZxdvN-3fhMP8Dns</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr"/>
+          <t>https://drive.google.com/drive/folders/1HKEB8rfgtEPbbb4LS2AUt2-q1qlZBJZH</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>ambiente, residuos, espacio público, recicladores, basuras, reciclaje, ambiental</t>
+        </is>
+      </c>
       <c r="M28" t="inlineStr">
         <is>
           <t>Jhonatan Rosas</t>
@@ -2335,16 +2319,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Caracterización de Hacedores de Oficios Artesanales 2025</t>
+          <t>Factores culturales, comportamentales y ambientales que inciden en el  ahorro y consumo de agua</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>PENDIENTE DESCRIPCIÓN</t>
+          <t>Realizar un sondeo sobre el consumo de agua en dos zonas de Bogotá analizando factores culturales, comportamentales y ambientales que afectan su uso</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2354,12 +2338,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>202591004200100014E</t>
+          <t>202491004200100018E</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>DACP</t>
+          <t>SCCGC - DTC</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -2367,24 +2351,28 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Sector Cultura</t>
+          <t>Cultura Ciudadana</t>
         </is>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1g-Ptwuv3NOni721gkCwjjAUaKCfBs_Zf</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr"/>
+          <t>https://drive.google.com/drive/folders/1w_BWFPcr1o0TkxlngZiWXFI86WUw-l6q</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>agua, ambiente</t>
+        </is>
+      </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Viviana Rodriguez</t>
+          <t>Jhonatan Rosas</t>
         </is>
       </c>
       <c r="N31" t="n">
@@ -2393,16 +2381,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Medición laboratorios EstarBien</t>
+          <t>Actualización de indicadores sobre comportamiento cívico y participación ciudadana en los distritos creativos</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Dar cuenta de los efectos de los laboratorios de cultura para el bienestar y la salud EstarBien.</t>
+          <t>Actualización del Índice de Cultura Ciudadana en Distritos Creativos y análisis de relaciones entre agentes culturales. Aporta al seguimiento de la Política de Economía Cultural y Creativa.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2412,12 +2400,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>202591004200100034E</t>
+          <t>202591004200100031E</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>DACP</t>
+          <t>Gobernanza - DEEP</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -2436,13 +2424,13 @@
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/11Zm0JlM-6ii_q8G0Cpd_Bs5qzRdcVMcn</t>
+          <t>https://drive.google.com/drive/folders/1YSI4dSNBDGnUfUJTvZxdvN-3fhMP8Dns</t>
         </is>
       </c>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Daniel Galeano</t>
+          <t>Jhonatan Rosas</t>
         </is>
       </c>
       <c r="N32" t="n">
@@ -2451,27 +2439,31 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Encuesta de Cultura Ciudadana y Garantía de Derechos - EBC 2025</t>
+          <t>Medición laboratorios EstarBien</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Diseño y recolección de la Encuesta de Indicadores de Cultura Ciudadana y Garantía de Derechos 2025, como módulo de la Encuesta Bienal de Culturas</t>
+          <t>Dar cuenta de los efectos de los laboratorios de cultura para el bienestar y la salud EstarBien.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Sector</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>SCRD</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>202591004200100034E</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>DACP</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -2479,7 +2471,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1 Sin iniciar</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2490,27 +2482,31 @@
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1Y1WHEMuOfoGbnoQf08Yzt9szXfpZ8BJi</t>
+          <t>https://drive.google.com/drive/folders/11Zm0JlM-6ii_q8G0Cpd_Bs5qzRdcVMcn</t>
         </is>
       </c>
       <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Daniel Galeano</t>
+        </is>
+      </c>
       <c r="N33" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Confianza y orgullo en la Ciudad</t>
+          <t>Caracterización de Hacedores de Oficios Artesanales 2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Medición de la confianza y el orgullo en Bogotá desde un enfoque cultural y comportamental.</t>
+          <t>PENDIENTE DESCRIPCIÓN</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2520,12 +2516,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>202591004200100035E</t>
+          <t>202591004200100014E</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>SCCGC</t>
+          <t>DACP</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -2533,24 +2529,24 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>5 Finalizada</t>
+          <t>2 En ejecución</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Cultura Ciudadana</t>
+          <t>Sector Cultura</t>
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1vdhaS15fUDp51h8d3JEwlHnHXKnjypyz</t>
+          <t>https://drive.google.com/drive/folders/1g-Ptwuv3NOni721gkCwjjAUaKCfBs_Zf</t>
         </is>
       </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Jhonatan Rosas</t>
+          <t>Viviana Rodriguez</t>
         </is>
       </c>
       <c r="N34" t="n">
@@ -2559,31 +2555,27 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Bogotá se Prepara para el Metro</t>
+          <t>Encuesta de Cultura Ciudadana y Garantía de Derechos - EBC 2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Estudio para anticipar comportamientos de los futuros usuarios y diseñar intervenciones de cultura ciudadana basados en evidencia.</t>
+          <t>Diseño y recolección de la Encuesta de Indicadores de Cultura Ciudadana y Garantía de Derechos 2025, como módulo de la Encuesta Bienal de Culturas</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>SCRD</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>202591004200100036E</t>
-        </is>
-      </c>
+          <t>Sector</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>SCCGC</t>
+          <t>General</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -2591,7 +2583,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>5 Finalizada</t>
+          <t>1 Sin iniciar</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2602,31 +2594,31 @@
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1CYdTe2QA8XN8vX4ufStphxfANS5wVveM</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>Jhonatan Rosas</t>
-        </is>
-      </c>
+          <t>https://drive.google.com/drive/folders/1Y1WHEMuOfoGbnoQf08Yzt9szXfpZ8BJi</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>cultura ciudadana, indicadores, variables, monitoreo, seguimiento, política, ambiente, participación, género, política</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr"/>
       <c r="N35" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Seguridad, justicia y convivencia: Masculinidad y Delito</t>
+          <t>Confianza y orgullo en la Ciudad</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Encuesta de Seguridad, justicia y convivencia. Diagnóstico de posibles barreras para la denuncia y el acceso a la justicia así como los principales facilitadores que podrían promover una mayor confianza y uso del sistema judicial.</t>
+          <t>Medición de la confianza y el orgullo en Bogotá desde un enfoque cultural y comportamental.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2636,7 +2628,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>202591004200100037E</t>
+          <t>202591004200100035E</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2660,64 +2652,72 @@
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1MWFewR9L0BNvHjLM7eObX-qfanPu4MYj</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>seguridad, mujer, justicia, género, enfoque, confianza institucional, masculinidad y violencia sexual, violencia sexual en adolescentes, jóvenes ofensores sexuales, masculinidades hegemónicas, violencia sexual intrafamiliar, violencia basada en género, cultura de la violación, consentimiento y poder, factores psicosociales de la violencia sexual, educación sexual integral, justicia restaurativa con hombres, prevención de violencia sexual</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr"/>
+          <t>https://drive.google.com/drive/folders/1vdhaS15fUDp51h8d3JEwlHnHXKnjypyz</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Jhonatan Rosas</t>
+        </is>
+      </c>
       <c r="N36" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Impactos de la transformación digital en la cultura: </t>
+          <t>Seguridad, justicia y convivencia: Masculinidad y Delito</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Estudio comparativo de los impactos de la transformación digital en la cultura en tres ciudades de Iberoamérica: Bogotá, Ciudad de México y Río de Janeiro.</t>
+          <t>Encuesta de Seguridad, justicia y convivencia. Diagnóstico de posibles barreras para la denuncia y el acceso a la justicia así como los principales facilitadores que podrían promover una mayor confianza y uso del sistema judicial.</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Sector</t>
+          <t>SCRD</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>202591004200100024E</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr"/>
+          <t>202591004200100037E</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>SCCGC</t>
+        </is>
+      </c>
       <c r="G37" t="n">
         <v>1</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Sector Cultura</t>
+          <t>Cultura Ciudadana</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1UCBoZjmBtwVBZ7LWWCh_1djcuAc4g4rc</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr"/>
+          <t>https://drive.google.com/drive/folders/1MWFewR9L0BNvHjLM7eObX-qfanPu4MYj</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>seguridad, mujer, justicia, género, enfoque, confianza institucional, masculinidad y violencia sexual, violencia sexual en adolescentes, jóvenes ofensores sexuales, masculinidades hegemónicas, violencia sexual intrafamiliar, violencia basada en género, cultura de la violación, consentimiento y poder, factores psicosociales de la violencia sexual, educación sexual integral, justicia restaurativa con hombres, prevención de violencia sexual</t>
+        </is>
+      </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="n">
         <v>2025</v>
@@ -2725,27 +2725,39 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Índice de condiciones de reconciliación en Bogotá D.C.</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr"/>
+          <t>Bogotá se Prepara para el Metro</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Estudio para anticipar comportamientos de los futuros usuarios y diseñar intervenciones de cultura ciudadana basados en evidencia.</t>
+        </is>
+      </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Sector</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
+          <t>SCRD</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>202591004200100036E</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>SCCGC</t>
+        </is>
+      </c>
       <c r="G38" t="n">
         <v>1</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2756,22 +2768,26 @@
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/10j435Vr1CiTkDTwG6OuGfJ3F-aPvD1g1</t>
+          <t>https://drive.google.com/drive/folders/1CYdTe2QA8XN8vX4ufStphxfANS5wVveM</t>
         </is>
       </c>
       <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Jhonatan Rosas</t>
+        </is>
+      </c>
       <c r="N38" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Convenio Movilidad</t>
+          <t>Índice de condiciones de reconciliación en Bogotá D.C.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
@@ -2798,7 +2814,7 @@
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1eUtyQUKC5Z12LRdniWYYgx18GxkvKH9M</t>
+          <t>https://drive.google.com/drive/folders/10j435Vr1CiTkDTwG6OuGfJ3F-aPvD1g1</t>
         </is>
       </c>
       <c r="L39" t="inlineStr"/>
@@ -2809,11 +2825,11 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Convenio Transmilenio</t>
+          <t>Convenio Movilidad</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -2822,11 +2838,7 @@
           <t>Sector</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>202591004200100027E</t>
-        </is>
-      </c>
+      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="n">
         <v>1</v>
@@ -2844,14 +2856,10 @@
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1Oevcfhqb2fsyzMSPchXqH7WxkIbqvNw_</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>transporte, movilidad, transmilenio, estaciones, colados</t>
-        </is>
-      </c>
+          <t>https://drive.google.com/drive/folders/1eUtyQUKC5Z12LRdniWYYgx18GxkvKH9M</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="n">
         <v>2025</v>
@@ -21883,7 +21891,7 @@
       </c>
       <c r="D647" t="inlineStr">
         <is>
-          <t>Sí</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E647" t="inlineStr">
@@ -22625,10 +22633,26 @@
       <c r="A688" t="n">
         <v>122</v>
       </c>
-      <c r="B688" t="inlineStr"/>
-      <c r="C688" t="inlineStr"/>
-      <c r="D688" t="inlineStr"/>
-      <c r="E688" t="inlineStr"/>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>Presentación final</t>
+        </is>
+      </c>
+      <c r="D688" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E688" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1f6sPy_pAB5aZpB_kvra4Qy4YiKsiGjgR/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="689">
       <c r="A689" t="n">
@@ -22684,18 +22708,46 @@
           <t>Presentación</t>
         </is>
       </c>
-      <c r="C694" t="inlineStr"/>
-      <c r="D694" t="inlineStr"/>
-      <c r="E694" t="inlineStr"/>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>Presentación final</t>
+        </is>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E694" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/presentation/d/1BogTIIMdH15s1-pa4Z9qN-RIW_VTct_g/edit?slide=id.p1#slide=id.p1</t>
+        </is>
+      </c>
     </row>
     <row r="695">
       <c r="A695" t="n">
         <v>123</v>
       </c>
-      <c r="B695" t="inlineStr"/>
-      <c r="C695" t="inlineStr"/>
-      <c r="D695" t="inlineStr"/>
-      <c r="E695" t="inlineStr"/>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Anexo</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>Anexo resultados comparativos</t>
+        </is>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E695" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/11YGZTE7pzMI4lDBZmvYiq5Xq9TwCE1z4/edit?usp=drive_link&amp;ouid=114299960211627169695&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="696">
       <c r="A696" t="n">
@@ -23599,10 +23651,26 @@
       <c r="A778" t="n">
         <v>137</v>
       </c>
-      <c r="B778" t="inlineStr"/>
-      <c r="C778" t="inlineStr"/>
-      <c r="D778" t="inlineStr"/>
-      <c r="E778" t="inlineStr"/>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>Informe final de mediciones</t>
+        </is>
+      </c>
+      <c r="D778" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E778" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1liHn1t_9w1D5ry0UIfT6kxLszVuyErB_/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="779">
       <c r="A779" t="n">

</xml_diff>

<commit_message>
Update investigaciones, pendientes Cultura Ciudadana
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -575,35 +575,39 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Impactos de la transformación digital en la cultura: </t>
+          <t>Sondeo sobre el Programa Libro al Viento</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Estudio comparativo de los impactos de la transformación digital en la cultura en tres ciudades de Iberoamérica: Bogotá, Ciudad de México y Río de Janeiro.</t>
+          <t>Análisis de los usos sociales del Programa Libro al Viento en Bogotá, a partir de un enfoque mixto que combina herramientas cuantitativas y cualitativas para comprender las prácticas de lectura en el espacio público. El estudio se centra en las formas de conocimiento, apropiación y circulación de los libros, así como en los sentidos que la ciudadanía atribuye al programa en su vida cotidiana. Los resultados permiten caracterizar a Libro al Viento como una experiencia de encuentro con la lectura integrada a la dinámica urbana, e identificar tanto sus aportes simbólicos como los principales retos para su visibilidad y sostenibilidad.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sector</t>
+          <t>IDARTES</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>202591004200100024E</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>202591004200100008E</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>IDARTES G Literatura</t>
+        </is>
+      </c>
       <c r="G3" t="n">
         <v>2</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -614,11 +618,19 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1UCBoZjmBtwVBZ7LWWCh_1djcuAc4g4rc</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
+          <t>https://drive.google.com/drive/folders/1m2paVRCF0WLmM6GCJXbDKsrppfiwtB73</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>lectura, literatura, aniversario, leo, Libro al Viento; lectura en el espacio público; usos sociales de la lectura; apropiación simbólica; políticas culturales; circulación de libros.</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Carlos Suárez, Giovani Moreno</t>
+        </is>
+      </c>
       <c r="N3" t="n">
         <v>2025</v>
       </c>
@@ -653,7 +665,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -679,426 +691,402 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>122</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Sabores y productos de identidad gastronómica</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Identificación de los productos, saberes y tradiciones que definen la gastronomía de Bogotá, con el fin de fortalecer su apropiación, difusión y valor cultural, promoviendo el orgullo por lo local.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>SCRD</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>202591004200100030E</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>SCCGC - DRAC</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Cultura Ciudadana</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1fFoEhz2VqUqD_9s0k7Zs7bqcoiev2ZBu</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>cultura, oferta cultural, gastronomía, restaurantes, comida, sabor bogotá, pan, panaderías, emocional</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>123</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Comportamiento y factores culturales en la gestión de residuos en Bogotá</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Análisis de los factores culturales y comportamentales en las dinámicas de recolección y disposición de residuos en Bogotá y evaluación de intervenciones de cultura ciudadana realizadas en el marco de la estrategia de espacio úblico y ambiente.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>SCRD</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>202591004200100002E</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>SCCGC - DTC</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Cultura Ciudadana</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1HKEB8rfgtEPbbb4LS2AUt2-q1qlZBJZH</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>ambiente, residuos, espacio público, recicladores, basuras, reciclaje, ambiental</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Jhonatan Rosas</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>134</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Impactos de la transformación digital en la cultura: </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Estudio comparativo de los impactos de la transformación digital en la cultura en tres ciudades de Iberoamérica: Bogotá, Ciudad de México y Río de Janeiro.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sector</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>202591004200100024E</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1UCBoZjmBtwVBZ7LWWCh_1djcuAc4g4rc</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>99</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Caracterización de Entidades Sin Ánimo de Lucro 2025</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Segunda etapa del estudio sectorial iniciado en 2024, enfocado en actualizar y profundizar la caracterización de las Entidades Sin Ánimo de Lucro (ESAL) adscritas a la SCRD, abordando aspectos de infraestructura, oferta de valor, sostenibilidad financiera y modelos de gestión.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>SCRD</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>202591004200100004E</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Gobernanza - DPJ</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Realizar un análisis de la información recolectada en los formularios aplicados a las ESALES 2024 y 2025, en términos de oferta de valor, estructura organizacional y herramientas de sostenibilidad.
+</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1GPyUMdbxqqJ-fja7DNFswVLKyoucNKao</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Dirección de Personas Juridicas, ESALES Culturales, Oferta de Valor, Infraestructura, Sostenibilidad, economía</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Giovani Moreno,Carlos Suárez </t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>104</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Impacto de festivales de gran formato en el Centro de Bogotá</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Evaluación de los impactos sociales, culturales y económicos de festivales organizados por la FUGA en el centro de Bogotá.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>FUGA</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>202591004200100007E</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>FUGA SGCB</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Medir el impacto económico, sociocultural y ambiental de los eventos relacionados con cultura, patrimonio, recreación y deporte  de la ciudad de Bogotá.
+</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1C_bdCxznPjXK63YsleE-hDTOQ1zmjfuB</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>FUGA - Monumentum - Centro - Música - Festivales, fundación gilberto alzate avendaño, centro, eventos, economía cultural</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Viviana Rodríguez, Laura Lozano, Giovani Moreno, Diego Lemus</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>103</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Hábitos y tendencias de consumo audiovisual</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>La investigación analiza la percepción, el reconocimiento y los hábitos de consumo de contenidos audiovisuales de las audiencias de Bogotá, con énfasis en Canal Capital y Eureka. A partir de un enfoque mixto que combina una encuesta de hogares y talleres con audiencias infantiles, el estudio caracteriza las formas de acceso, uso e integración de los contenidos audiovisuales en la vida cotidiana de públicos adultos y de niños, niñas, jóvenes y adolescentes. Los resultados ofrecen un panorama actualizado de la relación de la ciudadanía con ambos canales y aportan insumos estratégicos para fortalecer su visibilidad, posicionamiento y vínculo con las audiencias.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Canal Capital</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>202591004200100006E</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>CC Planeación</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Realizar un estudio para conocer el reconocimiento de Canal Capital y Eureka, asi como la percepción y habitos de consumo de contenidos de las audiencias de estos canales a partir de la aplicación de instrumentos metodológicos que permitan levantar la información relevante a nivel distrital, y que permitan abordar tanto públicos adultos como de NNJA.  </t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1qHfHWjozziDeNN6Q1oN8MKFr7-J-GMvD</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Canal Capital - Audiencias - Eureka, consumo cultural, televisión</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Carlos Suárez, Giovani Moreno, Laura Lozano</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>102</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Ecosistema cultural 24/7</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve">Caracterización de la oferta cultural en horarios no convencionales, con énfasis en públicos, franjas horarias e impactos. Incluye un módulo sobre estímulos e hitos 24/7 del sector.
 </t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>SCRD</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>202591004200100005E</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Gobernanza - DEEP</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Realizar plan piloto para mapear y caracterizar la oferta y la demanda del ecosistema cultural de Bogotá, reconociendo las necesidades, aspiraciones y factores culturales de la ciudadanía para viabilizar un ecosistema cultural activo, sostenible y diverso, con especial énfasis en el aprovechamiento de la noche como un espacio vital para la vida cultural y social de la ciudad, hacia una Bogotá 24/7.</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1JqeXwSxSbL_4Zqoij_tRwE1U6RAIMIks</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Ecosistema cultural, oferta artística nocturna, 24/7, noche, oferta cultural, economía</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Viviana Rodríguez, Carlos Suárez, Giovani Moreno,  Laura Lozano</t>
-        </is>
-      </c>
-      <c r="N5" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>103</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Hábitos y tendencias de consumo audiovisual</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>La investigación analiza la percepción, el reconocimiento y los hábitos de consumo de contenidos audiovisuales de las audiencias de Bogotá, con énfasis en Canal Capital y Eureka. A partir de un enfoque mixto que combina una encuesta de hogares y talleres con audiencias infantiles, el estudio caracteriza las formas de acceso, uso e integración de los contenidos audiovisuales en la vida cotidiana de públicos adultos y de niños, niñas, jóvenes y adolescentes. Los resultados ofrecen un panorama actualizado de la relación de la ciudadanía con ambos canales y aportan insumos estratégicos para fortalecer su visibilidad, posicionamiento y vínculo con las audiencias.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Canal Capital</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>202591004200100006E</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>CC Planeación</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Realizar un estudio para conocer el reconocimiento de Canal Capital y Eureka, asi como la percepción y habitos de consumo de contenidos de las audiencias de estos canales a partir de la aplicación de instrumentos metodológicos que permitan levantar la información relevante a nivel distrital, y que permitan abordar tanto públicos adultos como de NNJA.  </t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1qHfHWjozziDeNN6Q1oN8MKFr7-J-GMvD</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Canal Capital - Audiencias - Eureka, consumo cultural, televisión</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Carlos Suárez, Giovani Moreno, Laura Lozano</t>
-        </is>
-      </c>
-      <c r="N6" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>99</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Caracterización de Entidades Sin Ánimo de Lucro 2025</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Segunda etapa del estudio sectorial iniciado en 2024, enfocado en actualizar y profundizar la caracterización de las Entidades Sin Ánimo de Lucro (ESAL) adscritas a la SCRD, abordando aspectos de infraestructura, oferta de valor, sostenibilidad financiera y modelos de gestión.</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>SCRD</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>202591004200100004E</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Gobernanza - DPJ</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Realizar un análisis de la información recolectada en los formularios aplicados a las ESALES 2024 y 2025, en términos de oferta de valor, estructura organizacional y herramientas de sostenibilidad.
-</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1GPyUMdbxqqJ-fja7DNFswVLKyoucNKao</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Dirección de Personas Juridicas, ESALES Culturales, Oferta de Valor, Infraestructura, Sostenibilidad, economía</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Giovani Moreno,Carlos Suárez </t>
-        </is>
-      </c>
-      <c r="N7" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>101</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Indicadores del Sistema Distrital de Formación Artística y Cultural - SIDFAC</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Diseño de una batería de indicadores basada en fuentes existentes, como la Encuesta Bienal de Culturas y el Índice de Derechos Culturales, para evaluar variables asociadas a la formación artística, cultural y patrimonial. Los resultados servirán como insumo técnico para la actualización normativa del SIDFAC.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>SCRD</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>202591004200100029E</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>DACP</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Diseñar los indicadores que permitan hacer seguimiento a los procesos de formación en arte, cultura y patrimonio en el Distrito y su impacto a nivel de ciudad y localidades.</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1clr5wOumCR15k_x2ft_Ltyg1vDRlHBHK</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Formación, prácticas, cultura, patrimonio, arte</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Gisela Castrillón, Diego Lemus, Germán Urbina</t>
-        </is>
-      </c>
-      <c r="N8" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>105</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Sondeo sobre el Programa Libro al Viento</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>La investigación analiza los usos sociales del Programa Libro al Viento en Bogotá, a partir de un enfoque mixto que combina herramientas cuantitativas y cualitativas para comprender las prácticas de lectura en el espacio público. El estudio se centra en las formas de conocimiento, apropiación y circulación de los libros, así como en los sentidos que la ciudadanía atribuye al programa en su vida cotidiana. Los resultados permiten caracterizar a Libro al Viento como una experiencia de encuentro con la lectura integrada a la dinámica urbana, e identificar tanto sus aportes simbólicos como los principales retos para su visibilidad y sostenibilidad.</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>IDARTES</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>202591004200100008E</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>IDARTES G Literatura</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1m2paVRCF0WLmM6GCJXbDKsrppfiwtB73</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>lectura, literatura, aniversario, leo</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Carlos Suárez, Giovani Moreno</t>
-        </is>
-      </c>
-      <c r="N9" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>104</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Impacto de festivales de gran formato en el Centro de Bogotá</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Evaluación de los impactos sociales, culturales y económicos de festivales organizados por la FUGA en el centro de Bogotá.</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>FUGA</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>202591004200100007E</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>FUGA SGCB</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Medir el impacto económico, sociocultural y ambiental de los eventos relacionados con cultura, patrimonio, recreación y deporte  de la ciudad de Bogotá.
-</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1C_bdCxznPjXK63YsleE-hDTOQ1zmjfuB</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>FUGA - Monumentum - Centro - Música - Festivales, fundación gilberto alzate avendaño, centro, eventos, economía cultural</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Viviana Rodríguez, Laura Lozano, Giovani Moreno, Diego Lemus</t>
-        </is>
-      </c>
-      <c r="N10" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>106</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Percepción ciudadana sobre el Premio Luis Caballero</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Medir la percepción del público visitante sobre el Premio Luis Caballero, valorando conocimientos, emociones y sentido otorgado a las exposiciones, para orientar futuras ediciones y estrategias de mediación.</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>IDARTES</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>202591004200100009E</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>IDARTES G Plásticas</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -1114,178 +1102,178 @@
           <t>Sector Cultura</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Realizar plan piloto para mapear y caracterizar la oferta y la demanda del ecosistema cultural de Bogotá, reconociendo las necesidades, aspiraciones y factores culturales de la ciudadanía para viabilizar un ecosistema cultural activo, sostenible y diverso, con especial énfasis en el aprovechamiento de la noche como un espacio vital para la vida cultural y social de la ciudad, hacia una Bogotá 24/7.</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1qEkfdB8IzvAAAQS-Q6Dbmi1B1iui7bhP</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
+          <t>https://drive.google.com/drive/folders/1JqeXwSxSbL_4Zqoij_tRwE1U6RAIMIks</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Ecosistema cultural, oferta artística nocturna, 24/7, noche, oferta cultural, economía</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Viviana Rodríguez, Carlos Suárez, Giovani Moreno,  Laura Lozano</t>
+        </is>
+      </c>
       <c r="N11" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
+        <v>101</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Indicadores del Sistema Distrital de Formación Artística y Cultural - SIDFAC</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Diseño de una batería de indicadores basada en fuentes existentes, como la Encuesta Bienal de Culturas y el Índice de Derechos Culturales, para evaluar variables asociadas a la formación artística, cultural y patrimonial. Los resultados servirán como insumo técnico para la actualización normativa del SIDFAC.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>SCRD</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>202591004200100029E</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>DACP</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Diseñar los indicadores que permitan hacer seguimiento a los procesos de formación en arte, cultura y patrimonio en el Distrito y su impacto a nivel de ciudad y localidades.</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1clr5wOumCR15k_x2ft_Ltyg1vDRlHBHK</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Formación, prácticas, cultura, patrimonio, arte</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Gisela Castrillón, Diego Lemus, Germán Urbina</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>106</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Percepción ciudadana sobre el Premio Luis Caballero</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Medir la percepción del público visitante sobre el Premio Luis Caballero, valorando conocimientos, emociones y sentido otorgado a las exposiciones, para orientar futuras ediciones y estrategias de mediación.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>IDARTES</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>202591004200100009E</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>IDARTES G Plásticas</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>5 Finalizada</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1qEkfdB8IzvAAAQS-Q6Dbmi1B1iui7bhP</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>107</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Caracterización del sector circo – Fase 2</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve">Segunda fase del diagnóstico del sector circense en Bogotá, que ampliará el inventario georreferenciado de agentes y espacios, e incluirá un análisis de las condiciones técnicas, económicas y de oferta para fortalecer estrategias de apoyo al sector.
 </t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>IDARTES</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>202591004200100010E</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>IDARTES G Dramático</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Profundizar en el conocimiento de las características, necesidades y distribución territorial del sector circense en Bogotá, con el fin de fortalecer los lineamientos para la formulación de políticas públicas y programas que respondan de manera pertinente a su realidad e incidencia en las localidades de la ciudad.</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1hf4-sbaDvKEyxKOBEDUutNLalZjrUZbp</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Circo - Prácticas circenses - georreferenciación - Caracterización espacios y actores</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Viviana Rodríguez, Carlos Suárez </t>
-        </is>
-      </c>
-      <c r="N12" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>110</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Noche de Museos y Noche Iberoamericana de Museos</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Investigación dirigida a caracterizar los públicos y recoger percepciones sobre los eventos culturales de gran formato del IDPC, incluyendo la Noche de Museos, la Noche Iberoamericana de Museos y el Festival de Patrimonios en Ruana.</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>IDPC</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>202591004200100013E</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>IDPC Divulgación</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>5 Finalizada</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Realizar el diseño metodologico y aplicación de las mediciones tres eventos organizados por el IDPC (noche de museos, noche Iberoamercana de Museos y Festival de Patrimonios en Ruana)</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/drive/folders/1xjocKAYz8q0DO-L6hTN_wWcd077f-n3V</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>Noches de Museos, IDPC, Museos, Patrimonio Cultural, Bogotá nocturna.</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>Giovani Moreno ,todo el equipo</t>
-        </is>
-      </c>
-      <c r="N13" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>111</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PENDIENTE REEMPLAZA AGENTES</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Caracterización de la asociatividad y sostenibilidad de agentes del sector. No se llegó a difinir la investigaicón que reemplazaría. Se marca como cancelda.</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>SCRD</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>202591004200100014E</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Gobernanza - Fomento</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -1293,26 +1281,34 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>9 Cancelada</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Cultura Ciudadana</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Profundizar en el conocimiento de las características, necesidades y distribución territorial del sector circense en Bogotá, con el fin de fortalecer los lineamientos para la formulación de políticas públicas y programas que respondan de manera pertinente a su realidad e incidencia en las localidades de la ciudad.</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1S-Bf8soIeS71sk3a5vco8X45vVaUNM3l</t>
+          <t>https://drive.google.com/drive/folders/1hf4-sbaDvKEyxKOBEDUutNLalZjrUZbp</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Asociatividad agentes, Fomento, </t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr"/>
+          <t>Circo - Prácticas circenses - georreferenciación - Caracterización espacios y actores</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Viviana Rodríguez, Carlos Suárez </t>
+        </is>
+      </c>
       <c r="N14" t="n">
         <v>2025</v>
       </c>
@@ -1697,31 +1693,31 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Encuesta Bienal de Culturas - Encuesta de Prácticas Artísticas, Creativas y Patrimoniales.</t>
+          <t>Noche de Museos y Noche Iberoamericana de Museos</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Diseño, recolección y análisis del módulo de prácticas artísticas, culturales, creativas y patrimoniales, como parte de la Encuesta Bienal de Culturas 2025. Esta medición permite observar tendencias de largo plazo, caracterizar el ecosistema cultural y generar evidencia clave para la formulación de políticas sectoriales.</t>
+          <t>Investigación dirigida a caracterizar los públicos y recoger percepciones sobre los eventos culturales de gran formato del IDPC, incluyendo la Noche de Museos, la Noche Iberoamericana de Museos y el Festival de Patrimonios en Ruana.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Sector</t>
+          <t>IDPC</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>202591004200100021E</t>
+          <t>202591004200100013E</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>IDPC Divulgación</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1737,16 +1733,24 @@
           <t>Sector Cultura</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Realizar el diseño metodologico y aplicación de las mediciones tres eventos organizados por el IDPC (noche de museos, noche Iberoamercana de Museos y Festival de Patrimonios en Ruana)</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1E1FXuQmN_CvD-RBsZYfpTCuGpKCtbdv6</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr"/>
+          <t>https://drive.google.com/drive/folders/1xjocKAYz8q0DO-L6hTN_wWcd077f-n3V</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Noches de Museos, IDPC, Museos, Patrimonio Cultural, Bogotá nocturna.</t>
+        </is>
+      </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Carlos Suárez,Todo el equipo</t>
+          <t>Giovani Moreno ,todo el equipo</t>
         </is>
       </c>
       <c r="N21" t="n">
@@ -1755,32 +1759,31 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Medición del Festival de Verano - IDRD</t>
+          <t>PENDIENTE REEMPLAZA AGENTES</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Evaluar los impactos culturales, sociales y económicos del Festival de Verano, incluyendo la caracterización de públicos, satisfacción, consumo, percepción de marca y aportes al posicionamiento de Bogotá como ciudad de grandes eventos.
-</t>
+          <t>Caracterización de la asociatividad y sostenibilidad de agentes del sector. No se llegó a difinir la investigaicón que reemplazaría. Se marca como cancelda.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>IDRD</t>
+          <t>SCRD</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>202591004200100022E</t>
+          <t>202591004200100014E</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>IDRD</t>
+          <t>Gobernanza - Fomento</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1788,34 +1791,26 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>5 Finalizada</t>
+          <t>9 Cancelada</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Sector Cultura</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Conocer las percepciones y opiniones de los asistentes y otros agentes participantes  frente a los aspectos socioculturales y económicos de algunos eventos organizados por el IDRD para 2025</t>
-        </is>
-      </c>
+          <t>Cultura Ciudadana</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1hQe7h8f_dk0atsR0Ga8AWGrWuAyB-sGV</t>
+          <t>https://drive.google.com/drive/folders/1S-Bf8soIeS71sk3a5vco8X45vVaUNM3l</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Festival de Verano, IDRD, Actividad Fisica, Prácticas Deportivas, Recreación.</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>Giovani Moreno ,todo el equipo</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Asociatividad agentes, Fomento, </t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
         <v>2025</v>
       </c>
@@ -2079,31 +2074,32 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sabores y productos de identidad gastronómica</t>
+          <t>Medición del Festival de Verano - IDRD</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Identificación de los productos, saberes y tradiciones que definen la gastronomía de Bogotá, con el fin de fortalecer su apropiación, difusión y valor cultural, promoviendo el orgullo por lo local.</t>
+          <t xml:space="preserve">Evaluar los impactos culturales, sociales y económicos del Festival de Verano, incluyendo la caracterización de públicos, satisfacción, consumo, percepción de marca y aportes al posicionamiento de Bogotá como ciudad de grandes eventos.
+</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>SCRD</t>
+          <t>IDRD</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>202591004200100030E</t>
+          <t>202591004200100022E</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>SCCGC - DRAC</t>
+          <t>IDRD</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -2116,52 +2112,60 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Cultura Ciudadana</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr"/>
+          <t>Sector Cultura</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Conocer las percepciones y opiniones de los asistentes y otros agentes participantes  frente a los aspectos socioculturales y económicos de algunos eventos organizados por el IDRD para 2025</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1fFoEhz2VqUqD_9s0k7Zs7bqcoiev2ZBu</t>
+          <t>https://drive.google.com/drive/folders/1hQe7h8f_dk0atsR0Ga8AWGrWuAyB-sGV</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>cultura, oferta cultural, gastronomía, restaurantes, comida, sabor bogotá, pan, panaderías, emocional</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr"/>
+          <t>Festival de Verano, IDRD, Actividad Fisica, Prácticas Deportivas, Recreación.</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Giovani Moreno ,todo el equipo</t>
+        </is>
+      </c>
       <c r="N27" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Comportamiento y factores culturales en la gestión de residuos en Bogotá</t>
+          <t>Encuesta Bienal de Culturas - Encuesta de Prácticas Artísticas, Creativas y Patrimoniales.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Análisis de los factores culturales y comportamentales en las dinámicas de recolección y disposición de residuos en Bogotá y evaluación de intervenciones de cultura ciudadana realizadas en el marco de la estrategia de espacio úblico y ambiente.</t>
+          <t>Diseño, recolección y análisis del módulo de prácticas artísticas, culturales, creativas y patrimoniales, como parte de la Encuesta Bienal de Culturas 2025. Esta medición permite observar tendencias de largo plazo, caracterizar el ecosistema cultural y generar evidencia clave para la formulación de políticas sectoriales.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>SCRD</t>
+          <t>Sector</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>202591004200100002E</t>
+          <t>202591004200100021E</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>SCCGC - DTC</t>
+          <t>General</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -2174,23 +2178,19 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Cultura Ciudadana</t>
+          <t>Sector Cultura</t>
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1HKEB8rfgtEPbbb4LS2AUt2-q1qlZBJZH</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>ambiente, residuos, espacio público, recicladores, basuras, reciclaje, ambiental</t>
-        </is>
-      </c>
+          <t>https://drive.google.com/drive/folders/1E1FXuQmN_CvD-RBsZYfpTCuGpKCtbdv6</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Jhonatan Rosas</t>
+          <t>Carlos Suárez,Todo el equipo</t>
         </is>
       </c>
       <c r="N28" t="n">
@@ -2803,7 +2803,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -8616,7 +8616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E783"/>
+  <dimension ref="A1:E730"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20247,7 +20247,11 @@
         </is>
       </c>
       <c r="C561" t="inlineStr"/>
-      <c r="D561" t="inlineStr"/>
+      <c r="D561" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E561" t="inlineStr"/>
     </row>
     <row r="562">
@@ -22622,16 +22626,32 @@
     </row>
     <row r="687">
       <c r="A687" t="n">
-        <v>121</v>
-      </c>
-      <c r="B687" t="inlineStr"/>
-      <c r="C687" t="inlineStr"/>
-      <c r="D687" t="inlineStr"/>
-      <c r="E687" t="inlineStr"/>
+        <v>122</v>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>Presentación final</t>
+        </is>
+      </c>
+      <c r="D687" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E687" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1f6sPy_pAB5aZpB_kvra4Qy4YiKsiGjgR/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="688">
       <c r="A688" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B688" t="inlineStr">
         <is>
@@ -22650,377 +22670,605 @@
       </c>
       <c r="E688" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1f6sPy_pAB5aZpB_kvra4Qy4YiKsiGjgR/view?usp=drive_link</t>
+          <t>https://docs.google.com/presentation/d/1BogTIIMdH15s1-pa4Z9qN-RIW_VTct_g/edit?slide=id.p1#slide=id.p1</t>
         </is>
       </c>
     </row>
     <row r="689">
       <c r="A689" t="n">
-        <v>122</v>
-      </c>
-      <c r="B689" t="inlineStr"/>
-      <c r="C689" t="inlineStr"/>
-      <c r="D689" t="inlineStr"/>
-      <c r="E689" t="inlineStr"/>
+        <v>123</v>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Anexo</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>Anexo resultados comparativos</t>
+        </is>
+      </c>
+      <c r="D689" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E689" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/11YGZTE7pzMI4lDBZmvYiq5Xq9TwCE1z4/edit?usp=drive_link&amp;ouid=114299960211627169695&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="690">
       <c r="A690" t="n">
-        <v>122</v>
-      </c>
-      <c r="B690" t="inlineStr"/>
-      <c r="C690" t="inlineStr"/>
-      <c r="D690" t="inlineStr"/>
-      <c r="E690" t="inlineStr"/>
+        <v>124</v>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Infografía</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>Presentación final</t>
+        </is>
+      </c>
+      <c r="D690" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E690" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1VhroKpPxgqcqQso3fwqBLmJ5zbwmJ8od/view?usp=share_link</t>
+        </is>
+      </c>
     </row>
     <row r="691">
       <c r="A691" t="n">
-        <v>122</v>
-      </c>
-      <c r="B691" t="inlineStr"/>
-      <c r="C691" t="inlineStr"/>
-      <c r="D691" t="inlineStr"/>
+        <v>124</v>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Otro</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>Diseño de experimento económico</t>
+        </is>
+      </c>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E691" t="inlineStr"/>
     </row>
     <row r="692">
       <c r="A692" t="n">
-        <v>122</v>
-      </c>
-      <c r="B692" t="inlineStr"/>
-      <c r="C692" t="inlineStr"/>
-      <c r="D692" t="inlineStr"/>
+        <v>124</v>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>Cálculo de consumo de agua en ducha por factura</t>
+        </is>
+      </c>
+      <c r="D692" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E692" t="inlineStr"/>
     </row>
     <row r="693">
       <c r="A693" t="n">
-        <v>122</v>
-      </c>
-      <c r="B693" t="inlineStr"/>
-      <c r="C693" t="inlineStr"/>
-      <c r="D693" t="inlineStr"/>
+        <v>124</v>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Base de datos</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>Datos EAAB por Barrio para experimento</t>
+        </is>
+      </c>
+      <c r="D693" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E693" t="inlineStr"/>
     </row>
     <row r="694">
       <c r="A694" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B694" t="inlineStr">
         <is>
-          <t>Presentación</t>
+          <t>Infografía</t>
         </is>
       </c>
       <c r="C694" t="inlineStr">
         <is>
-          <t>Presentación final</t>
+          <t>Datos de hitos Barrios Vivos Agua</t>
         </is>
       </c>
       <c r="D694" t="inlineStr">
         <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="E694" t="inlineStr">
-        <is>
-          <t>https://docs.google.com/presentation/d/1BogTIIMdH15s1-pa4Z9qN-RIW_VTct_g/edit?slide=id.p1#slide=id.p1</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E694" t="inlineStr"/>
     </row>
     <row r="695">
       <c r="A695" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B695" t="inlineStr">
         <is>
-          <t>Anexo</t>
+          <t>Plan de trabajo</t>
         </is>
       </c>
       <c r="C695" t="inlineStr">
         <is>
-          <t>Anexo resultados comparativos</t>
+          <t>Cronograma Investigación Agua</t>
         </is>
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="E695" t="inlineStr">
-        <is>
-          <t>https://docs.google.com/spreadsheets/d/11YGZTE7pzMI4lDBZmvYiq5Xq9TwCE1z4/edit?usp=drive_link&amp;ouid=114299960211627169695&amp;rtpof=true&amp;sd=true</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E695" t="inlineStr"/>
     </row>
     <row r="696">
       <c r="A696" t="n">
-        <v>123</v>
-      </c>
-      <c r="B696" t="inlineStr"/>
-      <c r="C696" t="inlineStr"/>
-      <c r="D696" t="inlineStr"/>
-      <c r="E696" t="inlineStr"/>
+        <v>125</v>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>Presentación final</t>
+        </is>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E696" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1KnbyFYzDxdGfLHJqZDXjhrrUnvwF8O0D/view?usp=share_link</t>
+        </is>
+      </c>
     </row>
     <row r="697">
       <c r="A697" t="n">
-        <v>123</v>
-      </c>
-      <c r="B697" t="inlineStr"/>
-      <c r="C697" t="inlineStr"/>
-      <c r="D697" t="inlineStr"/>
+        <v>125</v>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>Tablas de salida</t>
+        </is>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E697" t="inlineStr"/>
     </row>
     <row r="698">
       <c r="A698" t="n">
-        <v>123</v>
-      </c>
-      <c r="B698" t="inlineStr"/>
-      <c r="C698" t="inlineStr"/>
-      <c r="D698" t="inlineStr"/>
+        <v>125</v>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Carpeta archivos</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>ICC Distritos Creativos 2025</t>
+        </is>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E698" t="inlineStr"/>
     </row>
     <row r="699">
       <c r="A699" t="n">
-        <v>123</v>
-      </c>
-      <c r="B699" t="inlineStr"/>
-      <c r="C699" t="inlineStr"/>
-      <c r="D699" t="inlineStr"/>
+        <v>125</v>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>Formulario ICC Distritos Creativos 2025</t>
+        </is>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E699" t="inlineStr"/>
     </row>
     <row r="700">
       <c r="A700" t="n">
-        <v>124</v>
-      </c>
-      <c r="B700" t="inlineStr"/>
-      <c r="C700" t="inlineStr"/>
-      <c r="D700" t="inlineStr"/>
+        <v>125</v>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Plan de trabajo</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>Cronograma ICC Distritos Creativos</t>
+        </is>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E700" t="inlineStr"/>
     </row>
     <row r="701">
       <c r="A701" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B701" t="inlineStr">
         <is>
-          <t>Otro</t>
+          <t>Informe final</t>
         </is>
       </c>
       <c r="C701" t="inlineStr">
         <is>
-          <t>Diseño de experimento económico</t>
-        </is>
-      </c>
-      <c r="D701" t="inlineStr"/>
-      <c r="E701" t="inlineStr"/>
+          <t>Informe de caracterización con fuentes secundarias</t>
+        </is>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E701" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1nqXIcpjznaD1Dn8fjBR_fg7L2XdFwKsg/view?usp=share_link</t>
+        </is>
+      </c>
     </row>
     <row r="702">
       <c r="A702" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B702" t="inlineStr">
         <is>
-          <t>Informe cuantitativo</t>
+          <t>Visualización</t>
         </is>
       </c>
       <c r="C702" t="inlineStr">
         <is>
-          <t>Cálculo de consumo de agua en ducha por factura</t>
-        </is>
-      </c>
-      <c r="D702" t="inlineStr"/>
-      <c r="E702" t="inlineStr"/>
+          <t xml:space="preserve">Tablero de recorrido por espacio púbilco del centro </t>
+        </is>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E702" t="inlineStr">
+        <is>
+          <t>https://sdcrd.maps.arcgis.com/apps/dashboards/f5ba03060ca94dfa8d4fee25f0de6d7f</t>
+        </is>
+      </c>
     </row>
     <row r="703">
       <c r="A703" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B703" t="inlineStr">
         <is>
-          <t>Base de datos</t>
+          <t>Informe final</t>
         </is>
       </c>
       <c r="C703" t="inlineStr">
         <is>
-          <t>Datos EAAB por Barrio para experimento</t>
-        </is>
-      </c>
-      <c r="D703" t="inlineStr"/>
+          <t xml:space="preserve">Tablero de recorrido por espacio púbilco del centro </t>
+        </is>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E703" t="inlineStr"/>
     </row>
     <row r="704">
       <c r="A704" t="n">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B704" t="inlineStr">
         <is>
-          <t>Infografía</t>
-        </is>
-      </c>
-      <c r="C704" t="inlineStr">
-        <is>
-          <t>Datos de hitos Barrios Vivos Agua</t>
-        </is>
-      </c>
-      <c r="D704" t="inlineStr"/>
-      <c r="E704" t="inlineStr"/>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr"/>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E704" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1NsVGUlWsADXoKnEO31ub8Cp0Krp9Aig3/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="705">
       <c r="A705" t="n">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B705" t="inlineStr">
         <is>
-          <t>Plan de trabajo</t>
-        </is>
-      </c>
-      <c r="C705" t="inlineStr">
-        <is>
-          <t>Cronograma Investigación Agua</t>
-        </is>
-      </c>
-      <c r="D705" t="inlineStr"/>
-      <c r="E705" t="inlineStr"/>
+          <t>Anexo</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr"/>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E705" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1yZIHrgUGq2Lu0TFlzzyGvCS7RXjuxd1M/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="706">
       <c r="A706" t="n">
-        <v>125</v>
-      </c>
-      <c r="B706" t="inlineStr"/>
+        <v>128</v>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
       <c r="C706" t="inlineStr"/>
-      <c r="D706" t="inlineStr"/>
-      <c r="E706" t="inlineStr"/>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E706" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1AVJBnJQld7Uyna3WW04TEPkFOQQqFlQl/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="707">
       <c r="A707" t="n">
-        <v>125</v>
-      </c>
-      <c r="B707" t="inlineStr">
-        <is>
-          <t>Informe cuantitativo</t>
-        </is>
-      </c>
-      <c r="C707" t="inlineStr">
-        <is>
-          <t>Tablas de salida</t>
-        </is>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B707" t="inlineStr"/>
+      <c r="C707" t="inlineStr"/>
       <c r="D707" t="inlineStr"/>
       <c r="E707" t="inlineStr"/>
     </row>
     <row r="708">
       <c r="A708" t="n">
-        <v>125</v>
-      </c>
-      <c r="B708" t="inlineStr">
-        <is>
-          <t>Carpeta archivos</t>
-        </is>
-      </c>
-      <c r="C708" t="inlineStr">
-        <is>
-          <t>ICC Distritos Creativos 2025</t>
-        </is>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B708" t="inlineStr"/>
+      <c r="C708" t="inlineStr"/>
       <c r="D708" t="inlineStr"/>
       <c r="E708" t="inlineStr"/>
     </row>
     <row r="709">
       <c r="A709" t="n">
-        <v>125</v>
-      </c>
-      <c r="B709" t="inlineStr">
-        <is>
-          <t>Instrumento recolección</t>
-        </is>
-      </c>
-      <c r="C709" t="inlineStr">
-        <is>
-          <t>Formulario ICC Distritos Creativos 2025</t>
-        </is>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B709" t="inlineStr"/>
+      <c r="C709" t="inlineStr"/>
       <c r="D709" t="inlineStr"/>
       <c r="E709" t="inlineStr"/>
     </row>
     <row r="710">
       <c r="A710" t="n">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B710" t="inlineStr">
         <is>
-          <t>Plan de trabajo</t>
+          <t>Informe final</t>
         </is>
       </c>
       <c r="C710" t="inlineStr">
         <is>
-          <t>Cronograma ICC Distritos Creativos</t>
-        </is>
-      </c>
-      <c r="D710" t="inlineStr"/>
-      <c r="E710" t="inlineStr"/>
+          <t xml:space="preserve">Análisis de impacto de la implementación de los Laboratorios de Bienestar a adolescentes: Comparación de encuestas pre y post de la implementación del laboratorio: “El Viaje Hacia Dentro de Mi” - Estrategia EstarBien Bogotá </t>
+        </is>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E710" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1R8tXuWA5XQrs_U1P2LAakV8WjHZp-Hyc/view?usp=share_link</t>
+        </is>
+      </c>
     </row>
     <row r="711">
       <c r="A711" t="n">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B711" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Plan de trabajo</t>
         </is>
       </c>
       <c r="C711" t="inlineStr">
         <is>
-          <t>Documento Distritos Creativos</t>
-        </is>
-      </c>
-      <c r="D711" t="inlineStr"/>
+          <t>Plan de investigación</t>
+        </is>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E711" t="inlineStr"/>
     </row>
     <row r="712">
       <c r="A712" t="n">
-        <v>126</v>
-      </c>
-      <c r="B712" t="inlineStr"/>
-      <c r="C712" t="inlineStr"/>
-      <c r="D712" t="inlineStr"/>
-      <c r="E712" t="inlineStr"/>
+        <v>130</v>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>Matriz de preguntas de la EBC</t>
+        </is>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E712" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1DBDvo9ZxCKI-N5iG-XNns-ILD2S1UEMe/view?usp=share_link</t>
+        </is>
+      </c>
     </row>
     <row r="713">
       <c r="A713" t="n">
-        <v>126</v>
-      </c>
-      <c r="B713" t="inlineStr"/>
-      <c r="C713" t="inlineStr"/>
-      <c r="D713" t="inlineStr"/>
-      <c r="E713" t="inlineStr"/>
+        <v>131</v>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>Presentación final</t>
+        </is>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E713" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1Ez5bU0fGKborxl5_zyUc27muZZizMtFC/view?usp=share_link</t>
+        </is>
+      </c>
     </row>
     <row r="714">
       <c r="A714" t="n">
-        <v>126</v>
-      </c>
-      <c r="B714" t="inlineStr"/>
-      <c r="C714" t="inlineStr"/>
-      <c r="D714" t="inlineStr"/>
+        <v>131</v>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>Encuesta de recolección de fuentes primarias</t>
+        </is>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E714" t="inlineStr"/>
     </row>
     <row r="715">
       <c r="A715" t="n">
-        <v>126</v>
-      </c>
-      <c r="B715" t="inlineStr"/>
-      <c r="C715" t="inlineStr"/>
-      <c r="D715" t="inlineStr"/>
-      <c r="E715" t="inlineStr"/>
+        <v>132</v>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>Cultura Metro - Estado del Arte</t>
+        </is>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E715" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/document/d/1TvqbXkunNvyWYuMDu2TZ_rwJeAI2fjFR/edit?usp=sharing&amp;ouid=100772003525119686921&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="716">
       <c r="A716" t="n">
-        <v>126</v>
-      </c>
-      <c r="B716" t="inlineStr"/>
-      <c r="C716" t="inlineStr"/>
-      <c r="D716" t="inlineStr"/>
-      <c r="E716" t="inlineStr"/>
+        <v>133</v>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Presentación Final </t>
+        </is>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E716" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/16AYD-Y9HF8O45rYDxH6a_pgEbUjv_Ofo/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="717">
       <c r="A717" t="n">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B717" t="inlineStr"/>
       <c r="C717" t="inlineStr"/>
@@ -23029,7 +23277,7 @@
     </row>
     <row r="718">
       <c r="A718" t="n">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B718" t="inlineStr"/>
       <c r="C718" t="inlineStr"/>
@@ -23038,7 +23286,7 @@
     </row>
     <row r="719">
       <c r="A719" t="n">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B719" t="inlineStr"/>
       <c r="C719" t="inlineStr"/>
@@ -23047,7 +23295,7 @@
     </row>
     <row r="720">
       <c r="A720" t="n">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B720" t="inlineStr"/>
       <c r="C720" t="inlineStr"/>
@@ -23056,7 +23304,7 @@
     </row>
     <row r="721">
       <c r="A721" t="n">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B721" t="inlineStr"/>
       <c r="C721" t="inlineStr"/>
@@ -23065,689 +23313,226 @@
     </row>
     <row r="722">
       <c r="A722" t="n">
-        <v>127</v>
-      </c>
-      <c r="B722" t="inlineStr"/>
-      <c r="C722" t="inlineStr"/>
-      <c r="D722" t="inlineStr"/>
-      <c r="E722" t="inlineStr"/>
+        <v>134</v>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>Tablero invitados ECCI 2025 - Seguimiento</t>
+        </is>
+      </c>
+      <c r="D722" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E722" t="inlineStr">
+        <is>
+          <t>https://lookerstudio.google.com/reporting/49195a24-bd9a-4773-af8a-966bb697f78b/page/p_pjg06p6njd</t>
+        </is>
+      </c>
     </row>
     <row r="723">
       <c r="A723" t="n">
-        <v>127</v>
-      </c>
-      <c r="B723" t="inlineStr"/>
-      <c r="C723" t="inlineStr"/>
-      <c r="D723" t="inlineStr"/>
-      <c r="E723" t="inlineStr"/>
+        <v>135</v>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>Marco conceptual</t>
+        </is>
+      </c>
+      <c r="D723" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E723" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/12I-YN44-_0suC2dpHX3vOLYgHwHTHA-E/view?usp=share_link</t>
+        </is>
+      </c>
     </row>
     <row r="724">
       <c r="A724" t="n">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B724" t="inlineStr">
         <is>
-          <t>Informe final</t>
-        </is>
-      </c>
-      <c r="C724" t="inlineStr"/>
-      <c r="D724" t="inlineStr"/>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t xml:space="preserve">índice de reconciliación y paz </t>
+        </is>
+      </c>
+      <c r="D724" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E724" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1NsVGUlWsADXoKnEO31ub8Cp0Krp9Aig3/view?usp=drive_link</t>
+          <t>https://drive.google.com/file/d/1ySdEC1LyX43LPMZdqi2vBiSWXoQRieJH/view?usp=share_link</t>
         </is>
       </c>
     </row>
     <row r="725">
       <c r="A725" t="n">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B725" t="inlineStr">
         <is>
-          <t>Anexo</t>
-        </is>
-      </c>
-      <c r="C725" t="inlineStr"/>
-      <c r="D725" t="inlineStr"/>
-      <c r="E725" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1yZIHrgUGq2Lu0TFlzzyGvCS7RXjuxd1M/view?usp=drive_link</t>
-        </is>
-      </c>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Documento Desarrollo Técnico Normativo y misional del enfoque de Cultura Ciudadana para la movilidad
+</t>
+        </is>
+      </c>
+      <c r="D725" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E725" t="inlineStr"/>
     </row>
     <row r="726">
       <c r="A726" t="n">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B726" t="inlineStr">
         <is>
-          <t>Instrumento recolección</t>
-        </is>
-      </c>
-      <c r="C726" t="inlineStr"/>
-      <c r="D726" t="inlineStr"/>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estado del arte y de la práctica sobre problemáticas relacionadas a cultura ciudadana y movilidad 
+</t>
+        </is>
+      </c>
+      <c r="D726" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
       <c r="E726" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1AVJBnJQld7Uyna3WW04TEPkFOQQqFlQl/view?usp=drive_link</t>
+          <t>https://drive.google.com/file/d/1l3CBDIXbCVbiG153wP35kkD4Q44DZbI1/view?usp=share_link</t>
         </is>
       </c>
     </row>
     <row r="727">
       <c r="A727" t="n">
-        <v>128</v>
-      </c>
-      <c r="B727" t="inlineStr"/>
-      <c r="C727" t="inlineStr"/>
-      <c r="D727" t="inlineStr"/>
-      <c r="E727" t="inlineStr"/>
+        <v>136</v>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Mapa/Geovisor</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>Geovisor Movilidad</t>
+        </is>
+      </c>
+      <c r="D727" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E727" t="inlineStr">
+        <is>
+          <t>https://www.arcgis.com/apps/dashboards/3a8a858de18047528174d7bc158b4b42</t>
+        </is>
+      </c>
     </row>
     <row r="728">
       <c r="A728" t="n">
-        <v>128</v>
-      </c>
-      <c r="B728" t="inlineStr"/>
-      <c r="C728" t="inlineStr"/>
-      <c r="D728" t="inlineStr"/>
-      <c r="E728" t="inlineStr"/>
+        <v>137</v>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>Informe final de mediciones</t>
+        </is>
+      </c>
+      <c r="D728" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E728" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1liHn1t_9w1D5ry0UIfT6kxLszVuyErB_/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="729">
       <c r="A729" t="n">
-        <v>128</v>
-      </c>
-      <c r="B729" t="inlineStr"/>
-      <c r="C729" t="inlineStr"/>
-      <c r="D729" t="inlineStr"/>
-      <c r="E729" t="inlineStr"/>
+        <v>137</v>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>Tablero de resultados</t>
+        </is>
+      </c>
+      <c r="D729" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E729" t="inlineStr">
+        <is>
+          <t>https://app.powerbi.com/view?r=eyJrIjoiOWYwOThhMjMtOTBjZC00ZGY5LThhYjktMTY5OWYzYWI0ZDJjIiwidCI6IjRmNzkzOWM3LWFhNjAtNDliZC05YjdiLTZmODFjMzdkMWIzNyJ9&amp;pageName=ef377ed828063259b15e</t>
+        </is>
+      </c>
     </row>
     <row r="730">
       <c r="A730" t="n">
-        <v>129</v>
-      </c>
-      <c r="B730" t="inlineStr"/>
-      <c r="C730" t="inlineStr"/>
-      <c r="D730" t="inlineStr"/>
-      <c r="E730" t="inlineStr"/>
-    </row>
-    <row r="731">
-      <c r="A731" t="n">
-        <v>129</v>
-      </c>
-      <c r="B731" t="inlineStr"/>
-      <c r="C731" t="inlineStr"/>
-      <c r="D731" t="inlineStr"/>
-      <c r="E731" t="inlineStr"/>
-    </row>
-    <row r="732">
-      <c r="A732" t="n">
-        <v>129</v>
-      </c>
-      <c r="B732" t="inlineStr"/>
-      <c r="C732" t="inlineStr"/>
-      <c r="D732" t="inlineStr"/>
-      <c r="E732" t="inlineStr"/>
-    </row>
-    <row r="733">
-      <c r="A733" t="n">
-        <v>129</v>
-      </c>
-      <c r="B733" t="inlineStr"/>
-      <c r="C733" t="inlineStr"/>
-      <c r="D733" t="inlineStr"/>
-      <c r="E733" t="inlineStr"/>
-    </row>
-    <row r="734">
-      <c r="A734" t="n">
-        <v>129</v>
-      </c>
-      <c r="B734" t="inlineStr"/>
-      <c r="C734" t="inlineStr"/>
-      <c r="D734" t="inlineStr"/>
-      <c r="E734" t="inlineStr"/>
-    </row>
-    <row r="735">
-      <c r="A735" t="n">
-        <v>129</v>
-      </c>
-      <c r="B735" t="inlineStr"/>
-      <c r="C735" t="inlineStr"/>
-      <c r="D735" t="inlineStr"/>
-      <c r="E735" t="inlineStr"/>
-    </row>
-    <row r="736">
-      <c r="A736" t="n">
-        <v>130</v>
-      </c>
-      <c r="B736" t="inlineStr"/>
-      <c r="C736" t="inlineStr"/>
-      <c r="D736" t="inlineStr"/>
-      <c r="E736" t="inlineStr"/>
-    </row>
-    <row r="737">
-      <c r="A737" t="n">
-        <v>130</v>
-      </c>
-      <c r="B737" t="inlineStr"/>
-      <c r="C737" t="inlineStr"/>
-      <c r="D737" t="inlineStr"/>
-      <c r="E737" t="inlineStr"/>
-    </row>
-    <row r="738">
-      <c r="A738" t="n">
-        <v>130</v>
-      </c>
-      <c r="B738" t="inlineStr"/>
-      <c r="C738" t="inlineStr"/>
-      <c r="D738" t="inlineStr"/>
-      <c r="E738" t="inlineStr"/>
-    </row>
-    <row r="739">
-      <c r="A739" t="n">
-        <v>130</v>
-      </c>
-      <c r="B739" t="inlineStr"/>
-      <c r="C739" t="inlineStr"/>
-      <c r="D739" t="inlineStr"/>
-      <c r="E739" t="inlineStr"/>
-    </row>
-    <row r="740">
-      <c r="A740" t="n">
-        <v>130</v>
-      </c>
-      <c r="B740" t="inlineStr"/>
-      <c r="C740" t="inlineStr"/>
-      <c r="D740" t="inlineStr"/>
-      <c r="E740" t="inlineStr"/>
-    </row>
-    <row r="741">
-      <c r="A741" t="n">
-        <v>130</v>
-      </c>
-      <c r="B741" t="inlineStr"/>
-      <c r="C741" t="inlineStr"/>
-      <c r="D741" t="inlineStr"/>
-      <c r="E741" t="inlineStr"/>
-    </row>
-    <row r="742">
-      <c r="A742" t="n">
-        <v>131</v>
-      </c>
-      <c r="B742" t="inlineStr"/>
-      <c r="C742" t="inlineStr"/>
-      <c r="D742" t="inlineStr"/>
-      <c r="E742" t="inlineStr"/>
-    </row>
-    <row r="743">
-      <c r="A743" t="n">
-        <v>131</v>
-      </c>
-      <c r="B743" t="inlineStr"/>
-      <c r="C743" t="inlineStr"/>
-      <c r="D743" t="inlineStr"/>
-      <c r="E743" t="inlineStr"/>
-    </row>
-    <row r="744">
-      <c r="A744" t="n">
-        <v>131</v>
-      </c>
-      <c r="B744" t="inlineStr"/>
-      <c r="C744" t="inlineStr"/>
-      <c r="D744" t="inlineStr"/>
-      <c r="E744" t="inlineStr"/>
-    </row>
-    <row r="745">
-      <c r="A745" t="n">
-        <v>131</v>
-      </c>
-      <c r="B745" t="inlineStr"/>
-      <c r="C745" t="inlineStr"/>
-      <c r="D745" t="inlineStr"/>
-      <c r="E745" t="inlineStr"/>
-    </row>
-    <row r="746">
-      <c r="A746" t="n">
-        <v>131</v>
-      </c>
-      <c r="B746" t="inlineStr"/>
-      <c r="C746" t="inlineStr"/>
-      <c r="D746" t="inlineStr"/>
-      <c r="E746" t="inlineStr"/>
-    </row>
-    <row r="747">
-      <c r="A747" t="n">
-        <v>131</v>
-      </c>
-      <c r="B747" t="inlineStr"/>
-      <c r="C747" t="inlineStr"/>
-      <c r="D747" t="inlineStr"/>
-      <c r="E747" t="inlineStr"/>
-    </row>
-    <row r="748">
-      <c r="A748" t="n">
-        <v>132</v>
-      </c>
-      <c r="B748" t="inlineStr"/>
-      <c r="C748" t="inlineStr"/>
-      <c r="D748" t="inlineStr"/>
-      <c r="E748" t="inlineStr"/>
-    </row>
-    <row r="749">
-      <c r="A749" t="n">
-        <v>132</v>
-      </c>
-      <c r="B749" t="inlineStr"/>
-      <c r="C749" t="inlineStr"/>
-      <c r="D749" t="inlineStr"/>
-      <c r="E749" t="inlineStr"/>
-    </row>
-    <row r="750">
-      <c r="A750" t="n">
-        <v>132</v>
-      </c>
-      <c r="B750" t="inlineStr"/>
-      <c r="C750" t="inlineStr"/>
-      <c r="D750" t="inlineStr"/>
-      <c r="E750" t="inlineStr"/>
-    </row>
-    <row r="751">
-      <c r="A751" t="n">
-        <v>132</v>
-      </c>
-      <c r="B751" t="inlineStr"/>
-      <c r="C751" t="inlineStr"/>
-      <c r="D751" t="inlineStr"/>
-      <c r="E751" t="inlineStr"/>
-    </row>
-    <row r="752">
-      <c r="A752" t="n">
-        <v>132</v>
-      </c>
-      <c r="B752" t="inlineStr"/>
-      <c r="C752" t="inlineStr"/>
-      <c r="D752" t="inlineStr"/>
-      <c r="E752" t="inlineStr"/>
-    </row>
-    <row r="753">
-      <c r="A753" t="n">
-        <v>132</v>
-      </c>
-      <c r="B753" t="inlineStr">
-        <is>
-          <t>Informe final</t>
-        </is>
-      </c>
-      <c r="C753" t="inlineStr">
-        <is>
-          <t>Cultura Metro - Estado del Arte</t>
-        </is>
-      </c>
-      <c r="D753" t="inlineStr"/>
-      <c r="E753" t="inlineStr"/>
-    </row>
-    <row r="754">
-      <c r="A754" t="n">
-        <v>133</v>
-      </c>
-      <c r="B754" t="inlineStr">
-        <is>
-          <t>Presentación</t>
-        </is>
-      </c>
-      <c r="C754" t="inlineStr">
-        <is>
-          <t>Presentación</t>
-        </is>
-      </c>
-      <c r="D754" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="E754" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/16AYD-Y9HF8O45rYDxH6a_pgEbUjv_Ofo/view?usp=drive_link</t>
-        </is>
-      </c>
-    </row>
-    <row r="755">
-      <c r="A755" t="n">
-        <v>133</v>
-      </c>
-      <c r="B755" t="inlineStr"/>
-      <c r="C755" t="inlineStr"/>
-      <c r="D755" t="inlineStr"/>
-      <c r="E755" t="inlineStr"/>
-    </row>
-    <row r="756">
-      <c r="A756" t="n">
-        <v>133</v>
-      </c>
-      <c r="B756" t="inlineStr"/>
-      <c r="C756" t="inlineStr"/>
-      <c r="D756" t="inlineStr"/>
-      <c r="E756" t="inlineStr"/>
-    </row>
-    <row r="757">
-      <c r="A757" t="n">
-        <v>133</v>
-      </c>
-      <c r="B757" t="inlineStr"/>
-      <c r="C757" t="inlineStr"/>
-      <c r="D757" t="inlineStr"/>
-      <c r="E757" t="inlineStr"/>
-    </row>
-    <row r="758">
-      <c r="A758" t="n">
-        <v>133</v>
-      </c>
-      <c r="B758" t="inlineStr"/>
-      <c r="C758" t="inlineStr"/>
-      <c r="D758" t="inlineStr"/>
-      <c r="E758" t="inlineStr"/>
-    </row>
-    <row r="759">
-      <c r="A759" t="n">
-        <v>133</v>
-      </c>
-      <c r="B759" t="inlineStr"/>
-      <c r="C759" t="inlineStr"/>
-      <c r="D759" t="inlineStr"/>
-      <c r="E759" t="inlineStr"/>
-    </row>
-    <row r="760">
-      <c r="A760" t="n">
-        <v>134</v>
-      </c>
-      <c r="B760" t="inlineStr"/>
-      <c r="C760" t="inlineStr"/>
-      <c r="D760" t="inlineStr"/>
-      <c r="E760" t="inlineStr"/>
-    </row>
-    <row r="761">
-      <c r="A761" t="n">
-        <v>134</v>
-      </c>
-      <c r="B761" t="inlineStr"/>
-      <c r="C761" t="inlineStr"/>
-      <c r="D761" t="inlineStr"/>
-      <c r="E761" t="inlineStr"/>
-    </row>
-    <row r="762">
-      <c r="A762" t="n">
-        <v>134</v>
-      </c>
-      <c r="B762" t="inlineStr"/>
-      <c r="C762" t="inlineStr"/>
-      <c r="D762" t="inlineStr"/>
-      <c r="E762" t="inlineStr"/>
-    </row>
-    <row r="763">
-      <c r="A763" t="n">
-        <v>134</v>
-      </c>
-      <c r="B763" t="inlineStr"/>
-      <c r="C763" t="inlineStr"/>
-      <c r="D763" t="inlineStr"/>
-      <c r="E763" t="inlineStr"/>
-    </row>
-    <row r="764">
-      <c r="A764" t="n">
-        <v>134</v>
-      </c>
-      <c r="B764" t="inlineStr"/>
-      <c r="C764" t="inlineStr"/>
-      <c r="D764" t="inlineStr"/>
-      <c r="E764" t="inlineStr"/>
-    </row>
-    <row r="765">
-      <c r="A765" t="n">
-        <v>134</v>
-      </c>
-      <c r="B765" t="inlineStr">
-        <is>
-          <t>Visualización</t>
-        </is>
-      </c>
-      <c r="C765" t="inlineStr">
-        <is>
-          <t>Tablero invitados ECCI 2025 - Seguimiento</t>
-        </is>
-      </c>
-      <c r="D765" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E765" t="inlineStr">
-        <is>
-          <t>https://lookerstudio.google.com/reporting/49195a24-bd9a-4773-af8a-966bb697f78b/page/p_pjg06p6njd</t>
-        </is>
-      </c>
-    </row>
-    <row r="766">
-      <c r="A766" t="n">
-        <v>135</v>
-      </c>
-      <c r="B766" t="inlineStr"/>
-      <c r="C766" t="inlineStr"/>
-      <c r="D766" t="inlineStr"/>
-      <c r="E766" t="inlineStr"/>
-    </row>
-    <row r="767">
-      <c r="A767" t="n">
-        <v>135</v>
-      </c>
-      <c r="B767" t="inlineStr"/>
-      <c r="C767" t="inlineStr"/>
-      <c r="D767" t="inlineStr"/>
-      <c r="E767" t="inlineStr"/>
-    </row>
-    <row r="768">
-      <c r="A768" t="n">
-        <v>135</v>
-      </c>
-      <c r="B768" t="inlineStr"/>
-      <c r="C768" t="inlineStr"/>
-      <c r="D768" t="inlineStr"/>
-      <c r="E768" t="inlineStr"/>
-    </row>
-    <row r="769">
-      <c r="A769" t="n">
-        <v>135</v>
-      </c>
-      <c r="B769" t="inlineStr"/>
-      <c r="C769" t="inlineStr"/>
-      <c r="D769" t="inlineStr"/>
-      <c r="E769" t="inlineStr"/>
-    </row>
-    <row r="770">
-      <c r="A770" t="n">
-        <v>135</v>
-      </c>
-      <c r="B770" t="inlineStr"/>
-      <c r="C770" t="inlineStr"/>
-      <c r="D770" t="inlineStr"/>
-      <c r="E770" t="inlineStr"/>
-    </row>
-    <row r="771">
-      <c r="A771" t="n">
-        <v>135</v>
-      </c>
-      <c r="B771" t="inlineStr"/>
-      <c r="C771" t="inlineStr"/>
-      <c r="D771" t="inlineStr"/>
-      <c r="E771" t="inlineStr"/>
-    </row>
-    <row r="772">
-      <c r="A772" t="n">
-        <v>136</v>
-      </c>
-      <c r="B772" t="inlineStr"/>
-      <c r="C772" t="inlineStr"/>
-      <c r="D772" t="inlineStr"/>
-      <c r="E772" t="inlineStr"/>
-    </row>
-    <row r="773">
-      <c r="A773" t="n">
-        <v>136</v>
-      </c>
-      <c r="B773" t="inlineStr"/>
-      <c r="C773" t="inlineStr"/>
-      <c r="D773" t="inlineStr"/>
-      <c r="E773" t="inlineStr"/>
-    </row>
-    <row r="774">
-      <c r="A774" t="n">
-        <v>136</v>
-      </c>
-      <c r="B774" t="inlineStr"/>
-      <c r="C774" t="inlineStr"/>
-      <c r="D774" t="inlineStr"/>
-      <c r="E774" t="inlineStr"/>
-    </row>
-    <row r="775">
-      <c r="A775" t="n">
-        <v>136</v>
-      </c>
-      <c r="B775" t="inlineStr"/>
-      <c r="C775" t="inlineStr"/>
-      <c r="D775" t="inlineStr"/>
-      <c r="E775" t="inlineStr"/>
-    </row>
-    <row r="776">
-      <c r="A776" t="n">
-        <v>136</v>
-      </c>
-      <c r="B776" t="inlineStr"/>
-      <c r="C776" t="inlineStr"/>
-      <c r="D776" t="inlineStr"/>
-      <c r="E776" t="inlineStr"/>
-    </row>
-    <row r="777">
-      <c r="A777" t="n">
-        <v>136</v>
-      </c>
-      <c r="B777" t="inlineStr">
-        <is>
-          <t>Mapa/Geovisor</t>
-        </is>
-      </c>
-      <c r="C777" t="inlineStr">
-        <is>
-          <t>Geovisor Movilidad</t>
-        </is>
-      </c>
-      <c r="D777" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E777" t="inlineStr">
-        <is>
-          <t>https://www.arcgis.com/apps/dashboards/3a8a858de18047528174d7bc158b4b42</t>
-        </is>
-      </c>
-    </row>
-    <row r="778">
-      <c r="A778" t="n">
         <v>137</v>
       </c>
-      <c r="B778" t="inlineStr">
-        <is>
-          <t>Informe final</t>
-        </is>
-      </c>
-      <c r="C778" t="inlineStr">
-        <is>
-          <t>Informe final de mediciones</t>
-        </is>
-      </c>
-      <c r="D778" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="E778" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1liHn1t_9w1D5ry0UIfT6kxLszVuyErB_/view?usp=drive_link</t>
-        </is>
-      </c>
-    </row>
-    <row r="779">
-      <c r="A779" t="n">
-        <v>137</v>
-      </c>
-      <c r="B779" t="inlineStr">
-        <is>
-          <t>Visualización</t>
-        </is>
-      </c>
-      <c r="C779" t="inlineStr">
-        <is>
-          <t>Tablero de resultados</t>
-        </is>
-      </c>
-      <c r="D779" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="E779" t="inlineStr">
-        <is>
-          <t>https://app.powerbi.com/view?r=eyJrIjoiOWYwOThhMjMtOTBjZC00ZGY5LThhYjktMTY5OWYzYWI0ZDJjIiwidCI6IjRmNzkzOWM3LWFhNjAtNDliZC05YjdiLTZmODFjMzdkMWIzNyJ9&amp;pageName=ef377ed828063259b15e</t>
-        </is>
-      </c>
-    </row>
-    <row r="780">
-      <c r="A780" t="n">
-        <v>137</v>
-      </c>
-      <c r="B780" t="inlineStr">
+      <c r="B730" t="inlineStr">
         <is>
           <t>Base de datos</t>
         </is>
       </c>
-      <c r="C780" t="inlineStr">
+      <c r="C730" t="inlineStr">
         <is>
           <t>Datos de encuestas</t>
         </is>
       </c>
-      <c r="D780" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="E780" t="inlineStr">
+      <c r="D730" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E730" t="inlineStr">
         <is>
           <t>https://docs.google.com/spreadsheets/d/1rX2RfuDon4SukoBpHxRg7m9fnL6_1Jw2/edit?usp=drive_link&amp;ouid=114299960211627169695&amp;rtpof=true&amp;sd=true</t>
         </is>
       </c>
-    </row>
-    <row r="781">
-      <c r="A781" t="n">
-        <v>137</v>
-      </c>
-      <c r="B781" t="inlineStr"/>
-      <c r="C781" t="inlineStr"/>
-      <c r="D781" t="inlineStr"/>
-      <c r="E781" t="inlineStr"/>
-    </row>
-    <row r="782">
-      <c r="A782" t="n">
-        <v>137</v>
-      </c>
-      <c r="B782" t="inlineStr"/>
-      <c r="C782" t="inlineStr"/>
-      <c r="D782" t="inlineStr"/>
-      <c r="E782" t="inlineStr"/>
-    </row>
-    <row r="783">
-      <c r="A783" t="n">
-        <v>137</v>
-      </c>
-      <c r="B783" t="inlineStr"/>
-      <c r="C783" t="inlineStr"/>
-      <c r="D783" t="inlineStr"/>
-      <c r="E783" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update investigaciones, pendientes Sector Cultura
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -2506,7 +2506,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PENDIENTE DESCRIPCIÓN</t>
+          <t>Caracterización de los hacedores y hacedoras de oficios artesanales que realizan aprovechamiento económico del espacio público en Bogotá. A partir de los aprendizajes del piloto realizado en 2024 y del marco normativo definido por el Decreto 315 de 2024 y la Resolución 500 de 2025, el estudio ajusta su objetivo, redefine la población de interés y actualiza el instrumento de recolección. Los resultados buscan aportar una comprensión más precisa de las condiciones de trabajo, los oficios, la cadena de valor y la relación de estas prácticas con el espacio público, como insumo para la gestión y formulación de políticas públicas.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -20020,19 +20020,52 @@
       <c r="A548" t="n">
         <v>99</v>
       </c>
-      <c r="B548" t="inlineStr"/>
-      <c r="C548" t="inlineStr"/>
-      <c r="D548" t="inlineStr"/>
-      <c r="E548" t="inlineStr"/>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Informe final Caracterización de las ESALES culturales de Bogotá 2025
+</t>
+        </is>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E548" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1V2LcYxrrvtQrwyVv-PxQ9jHBnJp-Q5lX/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="549">
       <c r="A549" t="n">
         <v>99</v>
       </c>
-      <c r="B549" t="inlineStr"/>
-      <c r="C549" t="inlineStr"/>
-      <c r="D549" t="inlineStr"/>
-      <c r="E549" t="inlineStr"/>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>Formulario ESALES 2025</t>
+        </is>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E549" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1MzaFzKFri8-Y3gbOaECJEpN3dTcbHzKV/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="550">
       <c r="A550" t="n">
@@ -20246,19 +20279,31 @@
           <t>Instrumento recolección</t>
         </is>
       </c>
-      <c r="C561" t="inlineStr"/>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>Formulario EBC - PACCP Final Indicadores Formación</t>
+        </is>
+      </c>
       <c r="D561" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E561" t="inlineStr"/>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E561" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1FdjJSejVqDjcXO3k5xNzxpCU2Gv_V3er/edit?usp=sharing&amp;ouid=105090632649587320414&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="562">
       <c r="A562" t="n">
         <v>101</v>
       </c>
-      <c r="B562" t="inlineStr"/>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Base de datos</t>
+        </is>
+      </c>
       <c r="C562" t="inlineStr"/>
       <c r="D562" t="inlineStr"/>
       <c r="E562" t="inlineStr"/>
@@ -20267,7 +20312,11 @@
       <c r="A563" t="n">
         <v>101</v>
       </c>
-      <c r="B563" t="inlineStr"/>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
       <c r="C563" t="inlineStr"/>
       <c r="D563" t="inlineStr"/>
       <c r="E563" t="inlineStr"/>
@@ -20310,7 +20359,7 @@
       </c>
       <c r="C567" t="inlineStr">
         <is>
-          <t>5. Base Encuesta_Ecosistema_247_Asistentes_CHAPINERO TEUSAQUILLO CANDELARIA Anonimizada.xlsx</t>
+          <t>Base anonimizada Ecosistema Cultural 24/7 Asistentes</t>
         </is>
       </c>
       <c r="D567" t="inlineStr">
@@ -20318,7 +20367,11 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="E567" t="inlineStr"/>
+      <c r="E567" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1robWu-87K25n70k06owJuRggNwMVnXLF/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="568">
       <c r="A568" t="n">
@@ -20331,7 +20384,7 @@
       </c>
       <c r="C568" t="inlineStr">
         <is>
-          <t>6. Base Ecosistema_Cultural_247_Oferta_Anonimizada.xlsx</t>
+          <t xml:space="preserve">Base anonimizada Ecosistema Cultural 24/7 Oferta </t>
         </is>
       </c>
       <c r="D568" t="inlineStr">
@@ -20339,7 +20392,11 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="E568" t="inlineStr"/>
+      <c r="E568" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1JTi5z-x1PgmRrGThTV8H0w86uOk3pDdd/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="569">
       <c r="A569" t="n">
@@ -20352,7 +20409,7 @@
       </c>
       <c r="C569" t="inlineStr">
         <is>
-          <t>1. Resul_247_Chap_Teusa_Cande Asistentes.xlsx</t>
+          <t>Resultados Asistentes</t>
         </is>
       </c>
       <c r="D569" t="inlineStr">
@@ -20360,7 +20417,11 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="E569" t="inlineStr"/>
+      <c r="E569" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1Haze9wH0-YlSDY1bHrWDfXJjMwc1LD7J/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="570">
       <c r="A570" t="n">
@@ -20373,7 +20434,7 @@
       </c>
       <c r="C570" t="inlineStr">
         <is>
-          <t>1_Resultados_Ecosistema_Cultural_247_Oferta.xls</t>
+          <t>Resultados Oferta</t>
         </is>
       </c>
       <c r="D570" t="inlineStr">
@@ -20381,7 +20442,11 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="E570" t="inlineStr"/>
+      <c r="E570" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1eL-kvZajGI8undcq5WGwmKI7cSji0iyJ/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="571">
       <c r="A571" t="n">
@@ -20394,7 +20459,7 @@
       </c>
       <c r="C571" t="inlineStr">
         <is>
-          <t>2. Ficha_Técnica_247 Asistentes</t>
+          <t>FichaTécnica Asistentes</t>
         </is>
       </c>
       <c r="D571" t="inlineStr">
@@ -20402,7 +20467,11 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="E571" t="inlineStr"/>
+      <c r="E571" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1BPmvMkVgSMtofKkz65LdTUdby-e0nI66/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="572">
       <c r="A572" t="n">
@@ -20415,7 +20484,7 @@
       </c>
       <c r="C572" t="inlineStr">
         <is>
-          <t>3_Ficha_Técnica_Oferta_247</t>
+          <t>Ficha Técnica Oferta</t>
         </is>
       </c>
       <c r="D572" t="inlineStr">
@@ -20423,7 +20492,11 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="E572" t="inlineStr"/>
+      <c r="E572" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/121wFHZbwRLw_NGTkQ8UjMg0rsYtFQ3yl/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="573">
       <c r="A573" t="n">
@@ -20444,7 +20517,11 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="E573" t="inlineStr"/>
+      <c r="E573" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1QIL_a1eOSFhjpKgln0XgVpFeVcFhCG1n/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="574">
       <c r="A574" t="n">
@@ -21186,19 +21263,51 @@
       <c r="A610" t="n">
         <v>109</v>
       </c>
-      <c r="B610" t="inlineStr"/>
-      <c r="C610" t="inlineStr"/>
-      <c r="D610" t="inlineStr"/>
-      <c r="E610" t="inlineStr"/>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>Informe Festival Centro 2025</t>
+        </is>
+      </c>
+      <c r="D610" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E610" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1OFk4HXgTpXjngSXZwFWsEeZxJvkpUpdI/view?usp=drive_link</t>
+        </is>
+      </c>
     </row>
     <row r="611">
       <c r="A611" t="n">
         <v>109</v>
       </c>
-      <c r="B611" t="inlineStr"/>
-      <c r="C611" t="inlineStr"/>
-      <c r="D611" t="inlineStr"/>
-      <c r="E611" t="inlineStr"/>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>Tablas de salida Festival Centro</t>
+        </is>
+      </c>
+      <c r="D611" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E611" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1e2ga-N1piD18x0W9kwcv0lMJDrROL_dW/edit?usp=drive_link&amp;ouid=114639277514087565011&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="612">
       <c r="A612" t="n">
@@ -22293,16 +22402,36 @@
       <c r="A664" t="n">
         <v>118</v>
       </c>
-      <c r="B664" t="inlineStr"/>
-      <c r="C664" t="inlineStr"/>
-      <c r="D664" t="inlineStr"/>
-      <c r="E664" t="inlineStr"/>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>Formulario EBC - PACCP Final</t>
+        </is>
+      </c>
+      <c r="D664" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E664" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/1qsclq1ogNVWTc6Sh7swGgV-k7DZr-Wnj/edit?usp=drive_link&amp;ouid=105090632649587320414&amp;rtpof=true&amp;sd=true</t>
+        </is>
+      </c>
     </row>
     <row r="665">
       <c r="A665" t="n">
         <v>118</v>
       </c>
-      <c r="B665" t="inlineStr"/>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Base de datos</t>
+        </is>
+      </c>
       <c r="C665" t="inlineStr"/>
       <c r="D665" t="inlineStr"/>
       <c r="E665" t="inlineStr"/>
@@ -22311,7 +22440,11 @@
       <c r="A666" t="n">
         <v>118</v>
       </c>
-      <c r="B666" t="inlineStr"/>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Informe cuantitativo</t>
+        </is>
+      </c>
       <c r="C666" t="inlineStr"/>
       <c r="D666" t="inlineStr"/>
       <c r="E666" t="inlineStr"/>
@@ -23545,7 +23678,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F311"/>
+  <dimension ref="A1:F324"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28407,87 +28540,111 @@
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B275" t="n">
         <v>1</v>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>Una ciudad que imagina y actúa desde el reconocimiento</t>
+          <t xml:space="preserve">Áreas de actuación y alcance territorial: alta concentración urbana y fuerte orientación formativa–escénica
+</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>El análisis evidenció un deseo colectivo por una Bogotá que valore lo diverso, propicie el reconocimiento de identidades y fomente el cuidado mutuo. Las voces de la ciudadanía expresaron aspiraciones de convivencia, inclusión y justicia, ubicando la cultura como eje fundamental de transformación social.</t>
-        </is>
-      </c>
-      <c r="E275" t="inlineStr"/>
-      <c r="F275" t="inlineStr"/>
+          <t xml:space="preserve">El diagnóstico evidencia que las ESALES culturales en Bogotá desarrollan mayoritariamente su actividad en entornos urbanos y con una concentración territorial en localidades centrales como Teusaquillo (8,2%), Chapinero (7,7%), La Candelaria (6,4%) y Santa Fe (6,4%). Aunque una proporción relevante de entidades reporta alcance nacional y metropolitano (41,6% en cada uno de estos niveles), el anclaje operativo y organizativo sigue siendo predominantemente local y urbano, como lo confirma el hecho de que el 76,1% desarrolla sus actividades en ámbito urbano y el 97,9% tiene su ciudad de residencia en Bogotá. 
+</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>76,10%</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>ESALES que desarrollan sus actividades en el ámbito urbano</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B276" t="n">
         <v>2</v>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>El lenguaje cotidiano como insumo de política pública</t>
+          <t>Fortalezas estructurales: organizaciones consolidadas pero con alta concentración de funciones</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>La metodología basada en análisis de lenguaje natural permitió identificar patrones semánticos, emocionales y argumentativos en más de 6.539 intervenciones. Esta apuesta innovadora traduce conversaciones ciudadanas en insumos de política, superando métodos tradicionales y fortaleciendo la escucha activa del Estado.</t>
+          <t xml:space="preserve">El sector se caracteriza por una base de entidades con trayectorias medias y largas, dado que el 30,3% tiene entre 10 y 20 años de existencia y el 28,2% supera los 20 años de constitución jurídica. No obstante, esta fortaleza convive con una alta concentración de roles en una misma persona, particularmente en la figura del representante legal, quien en el 100% de los casos cumple simultáneamente funciones de dirección o gerencia y, también en el 100%, asume múltiples roles dentro de la organización. 
+</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>6.539</t>
+          <t>28,20%</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>intervenciones</t>
+          <t>ESALESs con más de 20 años de constitución jurídica</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B277" t="n">
         <v>3</v>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>La cocreación como motor de sentido colectivo</t>
+          <t xml:space="preserve">Financiamiento: dependencia del recurso público con avances relevantes en ingresos propios
+</t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Los espacios de participación propiciaron no solo el acopio de opiniones, sino la construcción conjunta de visiones de futuro. La diversidad de actores y territorios involucrados fortaleció la legitimidad del proceso y dio lugar a un horizonte compartido: una Bogotá culturalmente viva, incluyente y consciente.</t>
-        </is>
-      </c>
-      <c r="E277" t="inlineStr"/>
-      <c r="F277" t="inlineStr"/>
+          <t xml:space="preserve">En materia de sostenibilidad económica, el diagnóstico muestra como principal fortaleza la capacidad de acceso a recursos públicos, utilizados por el 68,3% de las ESALES y que representan, en promedio, el 39,4% del total de su financiamiento. A ello se suma un avance en la venta de productos y/o servicios, reportada por el 57,0% de las entidades y que aporta en promedio el 38,7% de sus ingresos, lo que indica procesos incipientes pero relevantes de autogeneración de recursos. La empresa privada participa como fuente de financiamiento en el 40,9% de los casos, con un peso promedio del 15,0%. Sin embargo, persiste una baja diversificación financiera, evidenciada en la escasa participación de la cooperación internacional (9,2% de las entidades; 2,9% del financiamiento promedio) y de los créditos comerciales o internos (7,0%; 4,0% del promedio).
+Esta estructura financiera refuerza la estabilidad de corto plazo, pero mantiene al sector expuesto a riesgos asociados a la variabilidad de la inversión pública y a las limitaciones en capacidades comerciales y de negociación, en un contexto donde el 68,3% de las entidades reporta ingresos anuales inferiores a $100 millones.
+</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>68,30%</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>ESALES que acceden a recursos públicos</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B278" t="n">
         <v>4</v>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>Tecnología al servicio de lo humano</t>
+          <t xml:space="preserve">Perspectivas de mejora: consenso en la necesidad de fortalecer sostenibilidad y capacidades estratégicas
+</t>
         </is>
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>El uso de herramientas como IA, análisis de sentimientos y clasificación temática automatizada demostró cómo la tecnología puede potenciar la comprensión de lo social, sin reemplazar la interpretación crítica. Esta hibridación metodológica plantea nuevas posibilidades para la investigación pública y participativa.</t>
+          <t xml:space="preserve">Las ESALES culturales presentan una notable convergencia en sus perspectivas de futuro, al identificar como retos prioritarios la mejora de la sostenibilidad financiera (97,9% la considera importante o muy importante), el fortalecimiento organizacional (94,4%) y el aumento del número de beneficiarios o personas impactadas (94,4%). Este consenso se complementa con un interés creciente en la incorporación de herramientas digitales y tecnológicas, señaladas como innovación futura por el 42,3% de las entidades, así como en el fortalecimiento de capacidades relacionadas con la contratación pública (57,8%) y las alianzas estratégicas (57,0%) como temas prioritarios de capacitación. Al mismo tiempo, la baja definición de innovaciones futuras en el 44,4% de las organizaciones (Ns/Nr) sugiere la necesidad de procesos de acompañamiento estratégico que permitan traducir estas aspiraciones en planes concretos de desarrollo, diversificación territorial y ampliación del alcance cultural.
+</t>
         </is>
       </c>
       <c r="E278" t="inlineStr"/>
@@ -28498,16 +28655,16 @@
         <v>100</v>
       </c>
       <c r="B279" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>Metodologías que transforman la gestión pública</t>
+          <t>Una ciudad que imagina y actúa desde el reconocimiento</t>
         </is>
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Más allá de los resultados, la principal innovación fue metodológica: convertir un proceso de planeación en un ejercicio de escucha plural, analizado con rigor técnico y sensibilidad ética. Este enfoque fortalece la capacidad del Estado para actuar desde el conocimiento colectivo y en clave de transformación cultural.</t>
+          <t>El análisis evidenció un deseo colectivo por una Bogotá que valore lo diverso, propicie el reconocimiento de identidades y fomente el cuidado mutuo. Las voces de la ciudadanía expresaron aspiraciones de convivencia, inclusión y justicia, ubicando la cultura como eje fundamental de transformación social.</t>
         </is>
       </c>
       <c r="E279" t="inlineStr"/>
@@ -28515,680 +28672,953 @@
     </row>
     <row r="280">
       <c r="A280" t="n">
+        <v>100</v>
+      </c>
+      <c r="B280" t="n">
+        <v>2</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>El lenguaje cotidiano como insumo de política pública</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>La metodología basada en análisis de lenguaje natural permitió identificar patrones semánticos, emocionales y argumentativos en más de 6.539 intervenciones. Esta apuesta innovadora traduce conversaciones ciudadanas en insumos de política, superando métodos tradicionales y fortaleciendo la escucha activa del Estado.</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>6.539</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>intervenciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>100</v>
+      </c>
+      <c r="B281" t="n">
+        <v>3</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>La cocreación como motor de sentido colectivo</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Los espacios de participación propiciaron no solo el acopio de opiniones, sino la construcción conjunta de visiones de futuro. La diversidad de actores y territorios involucrados fortaleció la legitimidad del proceso y dio lugar a un horizonte compartido: una Bogotá culturalmente viva, incluyente y consciente.</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr"/>
+      <c r="F281" t="inlineStr"/>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>100</v>
+      </c>
+      <c r="B282" t="n">
+        <v>4</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Tecnología al servicio de lo humano</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>El uso de herramientas como IA, análisis de sentimientos y clasificación temática automatizada demostró cómo la tecnología puede potenciar la comprensión de lo social, sin reemplazar la interpretación crítica. Esta hibridación metodológica plantea nuevas posibilidades para la investigación pública y participativa.</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr"/>
+      <c r="F282" t="inlineStr"/>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>100</v>
+      </c>
+      <c r="B283" t="n">
+        <v>5</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Metodologías que transforman la gestión pública</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Más allá de los resultados, la principal innovación fue metodológica: convertir un proceso de planeación en un ejercicio de escucha plural, analizado con rigor técnico y sensibilidad ética. Este enfoque fortalece la capacidad del Estado para actuar desde el conocimiento colectivo y en clave de transformación cultural.</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr"/>
+      <c r="F283" t="inlineStr"/>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>102</v>
+      </c>
+      <c r="B284" t="n">
+        <v>1</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>El ecosistema cultural nocturno en Bogotá presenta condiciones para una ampliación horaria gradual</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Si bien una proporción de establecimientos opera en la franja nocturna temprana y la ciudadanía manifiesta alta disposición a asistir a actividades en la noche, la operación sostenida en horarios extendidos y de madrugada es limitada, tanto en la práctica como en la disposición declarada.</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr"/>
+      <c r="F284" t="inlineStr"/>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>102</v>
+      </c>
+      <c r="B285" t="n">
+        <v>2</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Existe una desalineación entre la disposición de la demanda y las capacidades operativas de la oferta</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Mientras la ciudadanía expresa altos niveles de interés y disposición a asistir con frecuencia regular a eventos nocturnos, la oferta presenta limitaciones asociadas a protocolos, articulación entre actores y gestión del riesgo, lo que condiciona su capacidad de responder a dicha demanda.</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr"/>
+      <c r="F285" t="inlineStr"/>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>102</v>
+      </c>
+      <c r="B286" t="n">
+        <v>3</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>La estrategia Ecosistema Cultural 24/7 presenta una baja apropiación desde la ciudadanía, pese a una valoración mayoritariamente positiva del enfoque</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>El bajo nivel de conocimiento de la estrategia contrasta con la aceptación general de la ampliación de la oferta nocturna, lo que sugiere una brecha entre el diseño institucional y su posicionamiento público.</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr"/>
+      <c r="F286" t="inlineStr"/>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>102</v>
+      </c>
+      <c r="B287" t="n">
+        <v>4</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Las barreras para la operación y el consumo nocturno son principalmente de carácter urbano y estructural</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>La seguridad y la movilidad emergen como los principales factores que condicionan tanto la decisión de los establecimientos para ampliar horarios como la disposición de la ciudadanía para asistir, por encima de restricciones normativas o culturales.</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr"/>
+      <c r="F287" t="inlineStr"/>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>102</v>
+      </c>
+      <c r="B288" t="n">
+        <v>5</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>El ecosistema se compone mayoritariamente de establecimientos de pequeña y mediana escala, con formas de operación que tienden a desarrollarse de manera individual y localizada</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Este perfil favorece dinámicas de consumo de cercanía y experiencias de menor escala, especialmente en franjas horarias extendidas, aunque también plantea desafíos para la articulación entre actores y la construcción de ofertas nocturnas integrales, particularmente en ausencia de mecanismos de coordinación o acompañamiento institucional.</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr"/>
+      <c r="F288" t="inlineStr"/>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
         <v>103</v>
       </c>
-      <c r="B280" t="n">
+      <c r="B289" t="n">
         <v>1</v>
       </c>
-      <c r="C280" t="inlineStr">
+      <c r="C289" t="inlineStr">
         <is>
           <t>Reconocimiento y acceso a los canales en la ciudad</t>
         </is>
       </c>
-      <c r="D280" t="inlineStr">
+      <c r="D289" t="inlineStr">
         <is>
           <t xml:space="preserve">Los resultados de la encuesta muestran que los principales retos de los canales se relacionan con su nivel de reconocimiento y visibilidad, más que con dificultades de acceso a la señal. En Bogotá, el 54,6% de la población afirma conocer Canal Capital, mientras que Eureka es reconocido por el 10,9%. No obstante, entre quienes identifican los canales, la percepción sobre el acceso es ampliamente favorable: el 89,6% considera que Canal Capital es de fácil acceso y, en el caso de Eureka, esta valoración positiva supera el 82%. Estos datos indican que, una vez conocidos, ambos canales son percibidos como accesibles para la ciudadanía.
 Este hallazgo confirma que los desafíos principales se ubican en el plano del posicionamiento, la recordación y el reconocimiento dentro del conjunto de la ciudadanía.
 </t>
         </is>
       </c>
-      <c r="E280" t="inlineStr">
+      <c r="E289" t="inlineStr">
         <is>
           <t>54,60%</t>
         </is>
       </c>
-      <c r="F280" t="inlineStr">
+      <c r="F289" t="inlineStr">
         <is>
           <t>Población</t>
         </is>
       </c>
     </row>
-    <row r="281">
-      <c r="A281" t="n">
+    <row r="290">
+      <c r="A290" t="n">
         <v>103</v>
       </c>
-      <c r="B281" t="n">
+      <c r="B290" t="n">
         <v>2</v>
       </c>
-      <c r="C281" t="inlineStr">
+      <c r="C290" t="inlineStr">
         <is>
           <t>Imagen de marca y recordación de la programación</t>
         </is>
       </c>
-      <c r="D281" t="inlineStr">
+      <c r="D290" t="inlineStr">
         <is>
           <t xml:space="preserve">Las asociaciones espontáneas y las valoraciones recogidas muestran que Canal Capital es reconocido por su vínculo con la ciudad, la cultura y la información de interés público. No obstante, la recordación de programas específicos es parcial y se concentra en algunos contenidos puntuales. Aun así, la valoración general del canal es ampliamente positiva, más del 85% de quienes lo conocen reconoce su aporte cultural e informativo. 
 Esta solidez en la imagen de marca constituye un activo relevante, que puede aprovecharse para fortalecer la recordación de la programación y profundizar la conexión con las audiencias.
 </t>
         </is>
       </c>
-      <c r="E281" t="inlineStr">
+      <c r="E290" t="inlineStr">
         <is>
           <t>85%</t>
         </is>
       </c>
-      <c r="F281" t="inlineStr">
+      <c r="F290" t="inlineStr">
         <is>
           <t>Quienes conocen</t>
         </is>
       </c>
     </row>
-    <row r="282">
-      <c r="A282" t="n">
+    <row r="291">
+      <c r="A291" t="n">
         <v>103</v>
       </c>
-      <c r="B282" t="n">
+      <c r="B291" t="n">
         <v>3</v>
       </c>
-      <c r="C282" t="inlineStr">
+      <c r="C291" t="inlineStr">
         <is>
           <t>Consumo audiovisual infantil mayoritariamente solitario</t>
         </is>
       </c>
-      <c r="D282" t="inlineStr">
+      <c r="D291" t="inlineStr">
         <is>
           <t xml:space="preserve">Los talleres participativos permitieron identificar que los hábitos de consumo audiovisual de niños y niñas se configuran principalmente en el ámbito doméstico y bajo lógicas de intimidad y rutina cotidiana. El consumo se representa mayoritariamente como una práctica individual, lo que sugiere una relación directa y personalizada con los contenidos audiovisuales. No obstante, esta experiencia solitaria convive con formas de acompañamiento familiar, especialmente con hermanos y madres, lo que indica que el consumo audiovisual también cumple una función relacional dentro del hogar, aunque de manera secundaria. La baja presencia de figuras adultas como el padre y de otros acompañantes refuerza la idea de una práctica centrada en la autonomía infantil y en dinámicas propias del tiempo libre.
 </t>
         </is>
       </c>
-      <c r="E282" t="inlineStr"/>
-      <c r="F282" t="inlineStr"/>
-    </row>
-    <row r="283">
-      <c r="A283" t="n">
+      <c r="E291" t="inlineStr"/>
+      <c r="F291" t="inlineStr"/>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
         <v>103</v>
       </c>
-      <c r="B283" t="n">
+      <c r="B292" t="n">
         <v>4</v>
       </c>
-      <c r="C283" t="inlineStr">
+      <c r="C292" t="inlineStr">
         <is>
           <t>Los niños y niñas se vinculan frente a los contenidos audiovisuales principalmente alrededor de los mensajes que transmiten, y su propia experiencia personal</t>
         </is>
       </c>
-      <c r="D283" t="inlineStr">
+      <c r="D292" t="inlineStr">
         <is>
           <t xml:space="preserve">El análisis de las preferencias frente a los contenidos del canal Eureka muestra que las opiniones infantiles se expresan principalmente a través de valoraciones afectivas y apreciaciones temáticas. Las categorías emergentes con mayor frecuencia corresponden a sensaciones como gusto, aburrimiento, interés o miedo, así como a referencias directas a los temas abordados por los programas. Esto sugiere que la recepción se construye desde una experiencia inmediata y emocional del visionado, más que desde una reflexión técnica o narrativa elaborada. Los elementos técnicos y las referencias explícitas a la experiencia personal aparecen de manera marginal, lo que indica que, en este contexto metodológico, los niños y niñas priorizan la reacción emocional y el contenido del mensaje.
 </t>
         </is>
       </c>
-      <c r="E283" t="inlineStr"/>
-      <c r="F283" t="inlineStr"/>
-    </row>
-    <row r="284">
-      <c r="A284" t="n">
+      <c r="E292" t="inlineStr"/>
+      <c r="F292" t="inlineStr"/>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
         <v>105</v>
       </c>
-      <c r="B284" t="n">
+      <c r="B293" t="n">
         <v>1</v>
       </c>
-      <c r="C284" t="inlineStr">
+      <c r="C293" t="inlineStr">
         <is>
           <t>Libro al Viento como encuentro ocasional con la lectura</t>
         </is>
       </c>
-      <c r="D284" t="inlineStr">
+      <c r="D293" t="inlineStr">
         <is>
           <t>Los resultados muestran que Libro al Viento funciona principalmente como una oportunidad ocasional de encuentro con la lectura, más que como un sistema de préstamo frecuente. La mayoría de las personas que toman libros accede a pocos ejemplares y lo hace de manera puntual. Esta característica es coherente con el diseño del programa y con su presencia en el espacio público, donde el acceso es abierto, espontáneo y no mediado por trámites o registros.</t>
         </is>
       </c>
-      <c r="E284" t="inlineStr"/>
-      <c r="F284" t="inlineStr"/>
-    </row>
-    <row r="285">
-      <c r="A285" t="n">
+      <c r="E293" t="inlineStr"/>
+      <c r="F293" t="inlineStr"/>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
         <v>105</v>
       </c>
-      <c r="B285" t="n">
+      <c r="B294" t="n">
         <v>2</v>
       </c>
-      <c r="C285" t="inlineStr">
+      <c r="C294" t="inlineStr">
         <is>
           <t xml:space="preserve">Experiencia de lectura, disfrute, utilidad y apropiación
 </t>
         </is>
       </c>
-      <c r="D285" t="inlineStr">
+      <c r="D294" t="inlineStr">
         <is>
           <t xml:space="preserve">La experiencia asociada a los libros de Libro al Viento combina el disfrute con usos prácticos. La lectura aparece vinculada principalmente a la diversión, pero también al trabajo, al aprendizaje y al enriquecimiento cultural, con variaciones según el tipo de entorno. Además, los efectos simbólicos son claros entre quienes conocen el programa: orgullo por su existencia, disfrute de la lectura y reconocimiento de que leer no es solo para especialistas. Estos impactos, aunque concentrados en un grupo reducido, son intensos y significativos.
 </t>
         </is>
       </c>
-      <c r="E285" t="inlineStr"/>
-      <c r="F285" t="inlineStr"/>
-    </row>
-    <row r="286">
-      <c r="A286" t="n">
+      <c r="E294" t="inlineStr"/>
+      <c r="F294" t="inlineStr"/>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
         <v>105</v>
       </c>
-      <c r="B286" t="n">
+      <c r="B295" t="n">
         <v>3</v>
       </c>
-      <c r="C286" t="inlineStr">
+      <c r="C295" t="inlineStr">
         <is>
           <t>Presencia urbana y valor cultural del programa</t>
         </is>
       </c>
-      <c r="D286" t="inlineStr">
+      <c r="D295" t="inlineStr">
         <is>
           <t>Libro al Viento es percibido como un proyecto cultural con presencia en múltiples espacios de la ciudad, lo que refuerza su carácter de política cultural urbana. Su circulación por bibliotecas, parques, eventos culturales, instituciones educativas y espacios de tránsito cotidiano lo posiciona como una iniciativa accesible, cercana y reconocible, que trasciende los espacios tradicionales de lectura y se integra a la vida urbana.</t>
         </is>
       </c>
-      <c r="E286" t="inlineStr"/>
-      <c r="F286" t="inlineStr"/>
-    </row>
-    <row r="287">
-      <c r="A287" t="n">
+      <c r="E295" t="inlineStr"/>
+      <c r="F295" t="inlineStr"/>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
         <v>105</v>
       </c>
-      <c r="B287" t="n">
+      <c r="B296" t="n">
         <v>4</v>
       </c>
-      <c r="C287" t="inlineStr">
+      <c r="C296" t="inlineStr">
         <is>
           <t>Circulación extendida y apropiación simbólica de los libros</t>
         </is>
       </c>
-      <c r="D287" t="inlineStr">
+      <c r="D296" t="inlineStr">
         <is>
           <t>La manera en que los libros circulan muestra que su valor no se agota en el punto de entrega ni en la regla de devolución. Al conservarlos, regalarlos o compartirlos, las personas expresan una fuerte apropiación simbólica. Esta circulación extendida refuerza la presencia del programa en la vida cotidiana y lo inscribe en trayectorias personales y sociales diversas, aunque también plantea retos para la disponibilidad y sostenibilidad del sistema de dispensadores.</t>
         </is>
       </c>
-      <c r="E287" t="inlineStr"/>
-      <c r="F287" t="inlineStr"/>
-    </row>
-    <row r="288">
-      <c r="A288" t="n">
+      <c r="E296" t="inlineStr"/>
+      <c r="F296" t="inlineStr"/>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
         <v>105</v>
       </c>
-      <c r="B288" t="n">
+      <c r="B297" t="n">
         <v>5</v>
       </c>
-      <c r="C288" t="inlineStr">
+      <c r="C297" t="inlineStr">
         <is>
           <t xml:space="preserve">El libro como objeto social situado: inserción comunitaria y política cultural </t>
         </is>
       </c>
-      <c r="D288" t="inlineStr">
+      <c r="D297" t="inlineStr">
         <is>
           <t xml:space="preserve">Las cartografías sociales evidencian que los libros del programa Libro al Viento se integran a prácticas sociales concretas y territorialmente situadas, más allá de su simple circulación física. Los libros se insertan en dinámicas comunitarias, educativas y cotidianas, adquiriendo sentidos diversos según los contextos sociales y territoriales de cada taller. En este sentido, Libro al Viento se configura como una política cultural situada, cuyos efectos dependen de las relaciones sociales que median la apropiación del libro. Las cartografías complementan el sondeo cuantitativo al mostrar cómo los libros se anclan, circulan y se resignifican en la vida cotidiana, dando lugar a circuitos múltiples y no lineales de uso. 
 </t>
         </is>
       </c>
-      <c r="E288" t="inlineStr"/>
-      <c r="F288" t="inlineStr"/>
-    </row>
-    <row r="289">
-      <c r="A289" t="n">
+      <c r="E297" t="inlineStr"/>
+      <c r="F297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>109</v>
+      </c>
+      <c r="B298" t="n">
+        <v>1</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>El Festival activa dinámicas económicas y de sosenibilidad cultural</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aunque el apoyo a emprendimientos culturales, la compra de productos o el intercambio con melómanos no constituyen el principal motivo de asistencia en ninguno de los escenarios, sí aparecen de manera consistente en todos ellos como motivaciones complementarias. Este patrón sugiere que el Festival Centro no solo funciona como un espacio de circulación artística, sino también como un dispositivo que contribuye a la sostenibilidad económica del ecosistema cultural, al activar prácticas de consumo cultural, visibilización de agentes y circulación de bienes simbólicos asociados a la música y las artes.
+Así, se podría seguir fortaleciendo de manera estratégica los componentes de circulación económica y visibilización de emprendimientos culturales, especialmente en aquellos escenarios con mayor afluencia y diversidad de públicos, sin desdibujar el eje artístico del Festival.
+</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr"/>
+      <c r="F298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>109</v>
+      </c>
+      <c r="B299" t="n">
+        <v>2</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>El Festival no genera mayores impactos negativos en el espacio público</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t xml:space="preserve">En los cuatro escenarios analizados, la percepción mayoritaria de los asistentes indica que la realización del Festival no modifica sustancialmente problemáticas asociadas al espacio público, como el arrojo de basuras, el parqueo en zonas prohibidas o la contaminación auditiva y visual. 
+Por otro lado, en algunos casos, como el Muelle de la FUGA y La Media Torta, se registra una mayor percepción de incremento en la presencia de vendedores informales o en el turismo; sin embargo, estos fenómenos coexisten con una valoración positiva del evento y no se asocian a un deterioro de la convivencia en la zona.
+</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr"/>
+      <c r="F299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>109</v>
+      </c>
+      <c r="B300" t="n">
+        <v>3</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>El Festival articula los desplazamientos, recorridos y consumos culturales en el centro</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>En todos los escenarios, una proporción mayoritaria de asistentes declaró haber visitado o tener previsto visitar otros espacios del centro antes o después del evento. Los recorridos se concentraron principalmente en equipamientos culturales, cafés, restaurantes, bares, teatros, salas de arte y museos, lo que evidencia una alta capacidad del Festival para articular la oferta cultural, gastronómica y comercial del centro de Bogotá. Este comportamiento refuerza el papel del Festival Centro como dinamizador territorial y como nodo de conexión entre la programación cultural pública y otras actividades económicas y simbólicas del área.</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr"/>
+      <c r="F300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>109</v>
+      </c>
+      <c r="B301" t="n">
+        <v>4</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t xml:space="preserve">La oferta musical y artística es el principal motivo de asistencia
+</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>En todos los escenarios, los motivos de asistencia se concentran de manera consistente en la presencia de los grupos y artistas, el interés por conocer nuevas propuestas musicales y el reconocimiento previo de algunos de los artistas participantes. El Festival Centro opera simultáneamente como un espacio de encuentro entre artistas y sus audiencias y como una plataforma para el descubrimiento de nuevas propuestas, lo que explica la coexistencia de públicos con trayectoria en el Festival y de personas que asisten por primera vez.</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr"/>
+      <c r="F301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
         <v>112</v>
       </c>
-      <c r="B289" t="n">
+      <c r="B302" t="n">
         <v>1</v>
       </c>
-      <c r="C289" t="inlineStr">
+      <c r="C302" t="inlineStr">
         <is>
           <t xml:space="preserve">Naturaleza de la creación colectiva
 </t>
         </is>
       </c>
-      <c r="D289" t="inlineStr">
+      <c r="D302" t="inlineStr">
         <is>
           <t>La creación colectiva se caracteriza por su profunda vocación de horizontalidad, solidaridad y libertad. Más que centrarse en la obtención de un producto final, privilegia el proceso como un espacio vivo de exploración, diálogo y construcción conjunta. En este sentido, se configura como un ejercicio humano y político que desafía las jerarquías tradicionales, redistribuye el poder creativo y habilita formas alternativas de relación y producción cultural.</t>
         </is>
       </c>
-      <c r="E289" t="inlineStr"/>
-      <c r="F289" t="inlineStr"/>
-    </row>
-    <row r="290">
-      <c r="A290" t="n">
+      <c r="E302" t="inlineStr"/>
+      <c r="F302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
         <v>112</v>
       </c>
-      <c r="B290" t="n">
+      <c r="B303" t="n">
         <v>2</v>
       </c>
-      <c r="C290" t="inlineStr">
+      <c r="C303" t="inlineStr">
         <is>
           <t>Metodologías, roles y autoría</t>
         </is>
       </c>
-      <c r="D290" t="inlineStr">
+      <c r="D303" t="inlineStr">
         <is>
           <t>En los procesos de creación colectiva, las metodologías se construyen desde la participación activa y la co-decisión. Los roles no se imponen de antemano, sino que emergen en función de las necesidades y momentos del proceso, lo que promueve dinámicas más flexibles y colaborativas. El liderazgo se concibe como un acompañamiento empático y orientador, antes que como una instancia de dirección jerárquica. La dramaturgia, por su parte, surge de la investigación, la improvisación y la apertura estructural, y aunque la documentación es una herramienta valiosa, suele ser poco sistemática debido a la naturaleza orgánica del trabajo.</t>
         </is>
       </c>
-      <c r="E290" t="inlineStr"/>
-      <c r="F290" t="inlineStr"/>
-    </row>
-    <row r="291">
-      <c r="A291" t="n">
+      <c r="E303" t="inlineStr"/>
+      <c r="F303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
         <v>112</v>
       </c>
-      <c r="B291" t="n">
+      <c r="B304" t="n">
         <v>3</v>
       </c>
-      <c r="C291" t="inlineStr">
+      <c r="C304" t="inlineStr">
         <is>
           <t>Interdisciplinariedad y articulación de saberes</t>
         </is>
       </c>
-      <c r="D291" t="inlineStr">
+      <c r="D304" t="inlineStr">
         <is>
           <t>La creación colectiva se nutre de una integración natural y fluida de múltiples artes, oficios y conocimientos. La apertura metodológica facilita aportes espontáneos entre disciplinas y la incorporación de especialistas externos, enriqueciendo el proceso. La tecnología también se incorpora como recurso creativo y expresivo, privilegiando enfoques de cultura libre y acceso abierto, lo que amplía las posibilidades estéticas y fomenta la innovación en los lenguajes escénicos.</t>
         </is>
       </c>
-      <c r="E291" t="inlineStr"/>
-      <c r="F291" t="inlineStr"/>
-    </row>
-    <row r="292">
-      <c r="A292" t="n">
+      <c r="E304" t="inlineStr"/>
+      <c r="F304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
         <v>112</v>
       </c>
-      <c r="B292" t="n">
+      <c r="B305" t="n">
         <v>4</v>
       </c>
-      <c r="C292" t="inlineStr">
+      <c r="C305" t="inlineStr">
         <is>
           <t>Sostenibilidad e impacto sociocultural</t>
         </is>
       </c>
-      <c r="D292" t="inlineStr">
+      <c r="D305" t="inlineStr">
         <is>
           <t>La sostenibilidad de estos procesos depende, ante todo, de los vínculos humanos, la confianza entre los participantes y la claridad de un propósito común. En este modelo, la comunidad no es solo receptora, sino coproductora activa del proceso y sus resultados. Esta dinámica favorece transformaciones significativas tanto en el plano personal como en el territorial, fortaleciendo el sentido de pertenencia, la identidad colectiva y los procesos de memoria y cuidado de los territorios.</t>
         </is>
       </c>
-      <c r="E292" t="inlineStr"/>
-      <c r="F292" t="inlineStr"/>
-    </row>
-    <row r="293">
-      <c r="A293" t="n">
+      <c r="E305" t="inlineStr"/>
+      <c r="F305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
         <v>115</v>
       </c>
-      <c r="B293" t="n">
+      <c r="B306" t="n">
         <v>1</v>
       </c>
-      <c r="C293" t="inlineStr">
+      <c r="C306" t="inlineStr">
         <is>
           <t>Patrones de uso y acompañamiento social</t>
         </is>
       </c>
-      <c r="D293" t="inlineStr">
+      <c r="D306" t="inlineStr">
         <is>
           <t>Los resultados muestran que los parques estructurantes priorizados presentan patrones de uso regular, con predominio de visitas semanales y diarias. La asistencia se realiza mayoritariamente en compañía de familiares, y el horario de uso se concentra principalmente en la franja de la mañana. La práctica de deporte o actividad física es la actividad reportada con mayor frecuencia en todos los parques, seguida por usos asociados al acompañamiento y al tránsito cotidiano</t>
         </is>
       </c>
-      <c r="E293" t="inlineStr"/>
-      <c r="F293" t="inlineStr"/>
-    </row>
-    <row r="294">
-      <c r="A294" t="n">
+      <c r="E306" t="inlineStr"/>
+      <c r="F306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
         <v>115</v>
       </c>
-      <c r="B294" t="n">
+      <c r="B307" t="n">
         <v>2</v>
       </c>
-      <c r="C294" t="inlineStr">
+      <c r="C307" t="inlineStr">
         <is>
           <t>Valoración del estado físico y la seguridad</t>
         </is>
       </c>
-      <c r="D294" t="inlineStr">
+      <c r="D307" t="inlineStr">
         <is>
           <t xml:space="preserve">La mayoría de las personas encuestadas califica el estado físico y el mantenimiento de los parques como “bueno” o “excelente”. De igual forma, una alta proporción de usuarios manifiesta sentirse segura al visitar estos espacios. No obstante, una parte de la población reporta percepciones de inseguridad, especialmente asociadas a condiciones como la iluminación, lo que coincide con los aspectos físicos señalados como susceptibles de mejora.
 </t>
         </is>
       </c>
-      <c r="E294" t="inlineStr"/>
-      <c r="F294" t="inlineStr"/>
-    </row>
-    <row r="295">
-      <c r="A295" t="n">
+      <c r="E307" t="inlineStr"/>
+      <c r="F307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
         <v>115</v>
       </c>
-      <c r="B295" t="n">
+      <c r="B308" t="n">
         <v>3</v>
       </c>
-      <c r="C295" t="inlineStr">
+      <c r="C308" t="inlineStr">
         <is>
           <t>Reconocimiento comunitario del parque</t>
         </is>
       </c>
-      <c r="D295" t="inlineStr">
+      <c r="D308" t="inlineStr">
         <is>
           <t xml:space="preserve">Los parques son reconocidos por la mayoría de los usuarios como espacios importantes para su comunidad o barrio. Este reconocimiento se presenta de manera consistente en los cinco parques analizados, lo que describe el papel de estos escenarios como referentes del entorno social y del uso cotidiano del espacio público.
 </t>
         </is>
       </c>
-      <c r="E295" t="inlineStr"/>
-      <c r="F295" t="inlineStr"/>
-    </row>
-    <row r="296">
-      <c r="A296" t="n">
+      <c r="E308" t="inlineStr"/>
+      <c r="F308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
         <v>115</v>
       </c>
-      <c r="B296" t="n">
+      <c r="B309" t="n">
         <v>4</v>
       </c>
-      <c r="C296" t="inlineStr">
+      <c r="C309" t="inlineStr">
         <is>
           <t>Diferencia entre participación reportada e interés declarado</t>
         </is>
       </c>
-      <c r="D296" t="inlineStr">
+      <c r="D309" t="inlineStr">
         <is>
           <t xml:space="preserve">Los resultados evidencian que la proporción de personas que reporta haber participado en actividades organizadas en los parques es menor que la proporción de usuarios que manifiesta interés en participar en actividades deportivas, recreativas, culturales o comunitarias. Esta diferencia describe una brecha entre la participación efectiva y la disposición declarada por la ciudadanía.
 </t>
         </is>
       </c>
-      <c r="E296" t="inlineStr"/>
-      <c r="F296" t="inlineStr"/>
-    </row>
-    <row r="297">
-      <c r="A297" t="n">
+      <c r="E309" t="inlineStr"/>
+      <c r="F309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
         <v>115</v>
       </c>
-      <c r="B297" t="n">
+      <c r="B310" t="n">
         <v>5</v>
       </c>
-      <c r="C297" t="inlineStr">
+      <c r="C310" t="inlineStr">
         <is>
           <t>Barreras y condiciones para el aprovechamiento</t>
         </is>
       </c>
-      <c r="D297" t="inlineStr">
+      <c r="D310" t="inlineStr">
         <is>
           <t>La falta de tiempo es la barrera más reportada para el uso y aprovechamiento de los parques, seguida por la percepción de inseguridad y la falta de información sobre la oferta de actividades. Estas barreras se presentan en todos los parques, con variaciones en su magnitud relativa según el escenario.</t>
         </is>
       </c>
-      <c r="E297" t="inlineStr"/>
-      <c r="F297" t="inlineStr"/>
-    </row>
-    <row r="298">
-      <c r="A298" t="n">
+      <c r="E310" t="inlineStr"/>
+      <c r="F310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
         <v>116</v>
       </c>
-      <c r="B298" t="n">
+      <c r="B311" t="n">
         <v>1</v>
       </c>
-      <c r="C298" t="inlineStr">
+      <c r="C311" t="inlineStr">
         <is>
           <t xml:space="preserve">La motivación existe. 
 Las barreras son estructurales y de contexto
 </t>
         </is>
       </c>
-      <c r="D298" t="inlineStr">
+      <c r="D311" t="inlineStr">
         <is>
           <t xml:space="preserve">Ciclovía: la mayoría sabe montar bicicleta y reconoce beneficios claros (ahorro de tiempo/dinero, autonomía).
 Escuela de la Bici: el principal obstáculo inicial no es el desinterés, sino no saber montar, la inseguridad y la falta de confianza.
 </t>
         </is>
       </c>
-      <c r="E298" t="inlineStr"/>
-      <c r="F298" t="inlineStr"/>
-    </row>
-    <row r="299">
-      <c r="A299" t="n">
+      <c r="E311" t="inlineStr"/>
+      <c r="F311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
         <v>116</v>
       </c>
-      <c r="B299" t="n">
+      <c r="B312" t="n">
         <v>2</v>
       </c>
-      <c r="C299" t="inlineStr">
+      <c r="C312" t="inlineStr">
         <is>
           <t>Los programas generan percepción de impacto, pero de forma diferenciada</t>
         </is>
       </c>
-      <c r="D299" t="inlineStr">
+      <c r="D312" t="inlineStr">
         <is>
           <t>Ciclovía: alta recurrencia y masividad; impacto percibido en actividad física, motivación semanal y uso recreativo de la bicicleta.
 Escuela de la Bici: impacto percibido en aprendizaje, confianza, bienestar emocional y cambio personal, aunque con menor uso posterior por barreras materiales.</t>
         </is>
       </c>
-      <c r="E299" t="inlineStr"/>
-      <c r="F299" t="inlineStr"/>
-    </row>
-    <row r="300">
-      <c r="A300" t="n">
+      <c r="E312" t="inlineStr"/>
+      <c r="F312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
         <v>116</v>
       </c>
-      <c r="B300" t="n">
+      <c r="B313" t="n">
         <v>3</v>
       </c>
-      <c r="C300" t="inlineStr">
+      <c r="C313" t="inlineStr">
         <is>
           <t>La bicicleta transforma la vida cotidiana más que la identidad colectiva</t>
         </is>
       </c>
-      <c r="D300" t="inlineStr">
+      <c r="D313" t="inlineStr">
         <is>
           <t>La sociabilidad se expresa principalmente en vínculos cercanos (familia, amigos) más que en colectivos organizados.
 El principal beneficio percibido es práctico (ahorro de tiempo/dinero, autonomía), seguido de salud y bienestar.</t>
         </is>
       </c>
-      <c r="E300" t="inlineStr"/>
-      <c r="F300" t="inlineStr"/>
-    </row>
-    <row r="301">
-      <c r="A301" t="n">
+      <c r="E313" t="inlineStr"/>
+      <c r="F313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
         <v>117</v>
       </c>
-      <c r="B301" t="n">
+      <c r="B314" t="n">
         <v>1</v>
       </c>
-      <c r="C301" t="inlineStr">
+      <c r="C314" t="inlineStr">
         <is>
           <t>Comprender la gobernanza deportiva como un sistema complejo, multinivel y en evolución</t>
         </is>
       </c>
-      <c r="D301" t="inlineStr">
+      <c r="D314" t="inlineStr">
         <is>
           <t>Los hallazgos de esta investigación muestran que la gobernanza del deporte, la recreación y la actividad física en Bogotá debería entenderse como un sistema complejo en el que convergen actores públicos, privados, comunitarios y académicos con distintos niveles de autoridad, capacidades y responsabilidades. La revisión de literatura confirma que los modelos contemporáneos de gobernanza combinan mecanismos jerárquicos, colaborativos e híbridos, lo cual coincide con la configuración del ecosistema distrital. Esta perspectiva permite reconocer tanto el valor de las estructuras formales del Sistema Nacional del Deporte como la importancia de los vínculos territoriales, las redes sociales y las prácticas comunitarias que sostienen el funcionamiento cotidiano del sistema.</t>
         </is>
       </c>
-      <c r="E301" t="inlineStr"/>
-      <c r="F301" t="inlineStr"/>
-    </row>
-    <row r="302">
-      <c r="A302" t="n">
+      <c r="E314" t="inlineStr"/>
+      <c r="F314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
         <v>117</v>
       </c>
-      <c r="B302" t="n">
+      <c r="B315" t="n">
         <v>2</v>
       </c>
-      <c r="C302" t="inlineStr">
+      <c r="C315" t="inlineStr">
         <is>
           <t>Clarificar el papel de los actores como base para mejorar la articulación y corresponsabilidad</t>
         </is>
       </c>
-      <c r="D302" t="inlineStr">
+      <c r="D315" t="inlineStr">
         <is>
           <t>Se considera necesario seguir avanzando en mecanismos que fortalezcan la corresponsabilidad entre niveles de gobierno, organizaciones deportivas, sector privado, ciudadanía y academia. La claridad en los roles y la comprensión de las relaciones entre actores son condiciones esenciales para que la política deportiva distrital evolucione hacia formas más consistentes de cooperación, planificación conjunta y toma de decisiones basada en evidencia, la tipología de actores es un punto de partida para esta definición.</t>
         </is>
       </c>
-      <c r="E302" t="inlineStr"/>
-      <c r="F302" t="inlineStr"/>
-    </row>
-    <row r="303">
-      <c r="A303" t="n">
+      <c r="E315" t="inlineStr"/>
+      <c r="F315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
         <v>117</v>
       </c>
-      <c r="B303" t="n">
+      <c r="B316" t="n">
         <v>3</v>
       </c>
-      <c r="C303" t="inlineStr">
+      <c r="C316" t="inlineStr">
         <is>
           <t>Aplicar la medición para caracterizar a los actores y fortalecer el sistema de información</t>
         </is>
       </c>
-      <c r="D303" t="inlineStr">
+      <c r="D316" t="inlineStr">
         <is>
           <t>El desarrollo de las categorías analíticas, del formulario cuantitativo y de la propuesta metodológica cualitativa constituye un insumo clave para avanzar hacia un sistema de información más sólido y útil para la toma de decisiones. La aplicación de estos instrumentos permitirá caracterizar de manera rigurosa a los actores del ecosistema deportivo y facilitará una comprensión más completa, contextualizada y accionable sobre el funcionamiento real del ecosistema deportivo y sobre las oportunidades para fortalecer su gobernanza.</t>
         </is>
       </c>
-      <c r="E303" t="inlineStr"/>
-      <c r="F303" t="inlineStr"/>
-    </row>
-    <row r="304">
-      <c r="A304" t="n">
+      <c r="E316" t="inlineStr"/>
+      <c r="F316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
         <v>117</v>
       </c>
-      <c r="B304" t="n">
+      <c r="B317" t="n">
         <v>4</v>
       </c>
-      <c r="C304" t="inlineStr">
+      <c r="C317" t="inlineStr">
         <is>
           <t>Usar el instrumento como herramienta progresiva para la mejora de la política pública</t>
         </is>
       </c>
-      <c r="D304" t="inlineStr">
+      <c r="D317" t="inlineStr">
         <is>
           <t xml:space="preserve">Se recomienda concebir el instrumento desarrollado no como un ejercicio aislado de levantamiento de información, sino como una herramienta estratégica de uso progresivo para el fortalecimiento de la política pública del deporte en Bogotá. Su aplicación periódica y su articulación con otros sistemas de información permitirán identificar brechas, monitorear avances en la articulación institucional y ajustar intervenciones de manera gradual. En este sentido, el instrumento ofrece una base para avanzar hacia procesos de planeación, seguimiento y evaluación más coherentes, orientados al aprendizaje institucional y a la generación de valor público en el ecosistema deportivo.
 En este marco, el instrumento constituye una base para promover procesos de aprendizaje institucional, mejorar la coordinación entre actores y fortalecer la generación de valor público en el ecosistema deportivo, a partir de decisiones informadas y basadas en evidencia.
 </t>
         </is>
       </c>
-      <c r="E304" t="inlineStr"/>
-      <c r="F304" t="inlineStr"/>
-    </row>
-    <row r="305">
-      <c r="A305" t="n">
+      <c r="E317" t="inlineStr"/>
+      <c r="F317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
         <v>121</v>
       </c>
-      <c r="B305" t="n">
+      <c r="B318" t="n">
         <v>4</v>
       </c>
-      <c r="C305" t="inlineStr">
+      <c r="C318" t="inlineStr">
         <is>
           <t>Mucho orgullo, confianza aún frágil</t>
         </is>
       </c>
-      <c r="D305" t="inlineStr">
+      <c r="D318" t="inlineStr">
         <is>
           <t>La encuesta muestra un considerable orgullo por Bogotá, pero una confianza interpersonal limitada: la mayoría dice poder confiar en menos de la mitad de las personas. Esta brecha sugiere que el sentido de pertenencia no se traduce automáticamente en cooperación cotidiana. Para cerrarla, los laboratorios deben priorizar mediaciones comunitarias, pedagogía de cuidado del espacio público y acciones que incrementen encuentros repetidos y seguros entre vecinos. Deporte, juego y arte son palancas idóneas para “hacer juntos” con bajas barreras de entrada. Medir confianza barrial antes y después de cada ciclo permitirá verificar si las intervenciones logran convertir orgullo en vínculos efectivos.</t>
         </is>
       </c>
-      <c r="E305" t="inlineStr"/>
-      <c r="F305" t="inlineStr"/>
-    </row>
-    <row r="306">
-      <c r="A306" t="n">
+      <c r="E318" t="inlineStr"/>
+      <c r="F318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
         <v>121</v>
       </c>
-      <c r="B306" t="n">
+      <c r="B319" t="n">
         <v>5</v>
       </c>
-      <c r="C306" t="inlineStr">
+      <c r="C319" t="inlineStr">
         <is>
           <t>Gobernanza compartida con palancas culturales</t>
         </is>
       </c>
-      <c r="D306" t="inlineStr">
+      <c r="D319" t="inlineStr">
         <is>
           <t>Los hallazgos apuntan a corresponsabilidad distribuida: fuerza pública, entidades distritales, vecinos y JAL son percibidos como actores clave según el tipo de problema. Esta lectura respalda una gobernanza compartida, con roles claros y coordinación por barrio, donde cultura ciudadana, bibliotecas y arte urbano actúan como catalizadores. La priorización debe enfocarse en inseguridad y basuras, conectando intervenciones de seguridad situacional con cuidado del entorno y gestión de residuos. Diseñar participación flexible (horarios extendidos, micro-tareas, reconocimiento simbólico) reduce barreras para ese tercio que no puede involucrarse. Con tableros de seguimiento por barrio, la estrategia podrá iterar con evidencia y escalar lo que funciona.</t>
         </is>
       </c>
-      <c r="E306" t="inlineStr"/>
-      <c r="F306" t="inlineStr"/>
-    </row>
-    <row r="307">
-      <c r="A307" t="n">
+      <c r="E319" t="inlineStr"/>
+      <c r="F319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
         <v>133</v>
       </c>
-      <c r="B307" t="n">
+      <c r="B320" t="n">
         <v>1</v>
       </c>
-      <c r="C307" t="inlineStr">
+      <c r="C320" t="inlineStr">
         <is>
           <t>La violencia sexual no es un desvío, es un mandato aprendido</t>
         </is>
       </c>
-      <c r="D307" t="inlineStr">
+      <c r="D320" t="inlineStr">
         <is>
           <t>La investigación evidencia que la violencia sexual no aparece como un hecho aislado o accidental, sino como una expresión coherente de la masculinidad hegemónica aprendida en distintos entornos sociales. El ejercicio de la violencia se asocia a expectativas de poder, control, dominación y validación identitaria masculina. Estas prácticas son reforzadas por la familia, los pares, los medios y, en ocasiones, por la ausencia de una educación sexual integral. La violencia se convierte así en un mecanismo para “demostrar hombría”, más que en una desviación individual.</t>
         </is>
       </c>
-      <c r="E307" t="inlineStr"/>
-      <c r="F307" t="inlineStr"/>
-    </row>
-    <row r="308">
-      <c r="A308" t="n">
+      <c r="E320" t="inlineStr"/>
+      <c r="F320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
         <v>133</v>
       </c>
-      <c r="B308" t="n">
+      <c r="B321" t="n">
         <v>2</v>
       </c>
-      <c r="C308" t="inlineStr">
+      <c r="C321" t="inlineStr">
         <is>
           <t>El hogar es el principal escenario de riesgo y silenciamiento</t>
         </is>
       </c>
-      <c r="D308" t="inlineStr">
+      <c r="D321" t="inlineStr">
         <is>
           <t>Una proporción significativa de los hechos de violencia sexual ocurre en la vivienda y es ejercida por personas cercanas a la víctima. El entorno familiar, lejos de ser siempre un espacio protector, puede funcionar como un escenario de encubrimiento, negación o minimización del daño. Esta dinámica dificulta la denuncia, la intervención temprana y la activación de rutas de protección. La naturalización del abuso dentro del hogar refuerza el silencio y perpetúa la violencia.</t>
         </is>
       </c>
-      <c r="E308" t="inlineStr"/>
-      <c r="F308" t="inlineStr"/>
-    </row>
-    <row r="309">
-      <c r="A309" t="n">
+      <c r="E321" t="inlineStr"/>
+      <c r="F321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
         <v>133</v>
       </c>
-      <c r="B309" t="n">
+      <c r="B322" t="n">
         <v>3</v>
       </c>
-      <c r="C309" t="inlineStr">
+      <c r="C322" t="inlineStr">
         <is>
           <t>Negar, minimizar y justificar: la principal barrera para la responsabilidad</t>
         </is>
       </c>
-      <c r="D309" t="inlineStr">
+      <c r="D322" t="inlineStr">
         <is>
           <t>Tanto los ofensores como sus familias tienden a negar, minimizar o justificar la violencia sexual, lo que constituye una barrera estructural para los procesos de responsabilización y reparación. Estas narrativas desplazan la culpa hacia las víctimas, apelan a la cercanía afectiva o normalizan el abuso como “error” o “juego”. Esta falta de reconocimiento del daño limita la efectividad de las sanciones y de los procesos restaurativos. Sin responsabilidad no hay transformación posible.</t>
         </is>
       </c>
-      <c r="E309" t="inlineStr"/>
-      <c r="F309" t="inlineStr"/>
-    </row>
-    <row r="310">
-      <c r="A310" t="n">
+      <c r="E322" t="inlineStr"/>
+      <c r="F322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
         <v>133</v>
       </c>
-      <c r="B310" t="n">
+      <c r="B323" t="n">
         <v>4</v>
       </c>
-      <c r="C310" t="inlineStr">
+      <c r="C323" t="inlineStr">
         <is>
           <t>La sexualidad se aprende sin consentimiento ni empatía</t>
         </is>
       </c>
-      <c r="D310" t="inlineStr">
+      <c r="D323" t="inlineStr">
         <is>
           <t>Los hallazgos muestran que muchos jóvenes adquieren conocimientos sobre sexualidad a través de pares, pornografía y medios, sin mediación crítica ni enfoque ético. Esto produce ideas distorsionadas sobre el consentimiento, la reciprocidad y el deseo, normalizando la cosificación y la dominación. La ausencia de educación sexual integral favorece prácticas sexuales violentas y dificulta el desarrollo de empatía hacia las víctimas. La sexualidad se configura más como ejercicio de poder que como relación.</t>
         </is>
       </c>
-      <c r="E310" t="inlineStr"/>
-      <c r="F310" t="inlineStr"/>
-    </row>
-    <row r="311">
-      <c r="A311" t="n">
+      <c r="E323" t="inlineStr"/>
+      <c r="F323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
         <v>133</v>
       </c>
-      <c r="B311" t="n">
+      <c r="B324" t="n">
         <v>5</v>
       </c>
-      <c r="C311" t="inlineStr">
+      <c r="C324" t="inlineStr">
         <is>
           <t>Transformar las masculinidades es clave para prevenir la violencia</t>
         </is>
       </c>
-      <c r="D311" t="inlineStr">
+      <c r="D324" t="inlineStr">
         <is>
           <t>La erradicación de la violencia sexual requiere intervenir directamente en la construcción social de las masculinidades. El estudio muestra que trabajar únicamente sobre las víctimas o desde una lógica punitiva es insuficiente. Se necesitan estrategias preventivas, educativas, culturales y restaurativas que involucren activamente a los hombres, desde la infancia hasta la adultez. Promover masculinidades no violentas es una condición central para la justicia, la convivencia y la transformación cultural.</t>
         </is>
       </c>
-      <c r="E311" t="inlineStr"/>
-      <c r="F311" t="inlineStr"/>
+      <c r="E324" t="inlineStr"/>
+      <c r="F324" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update investigaciones, pendientes Sector Cultura, LauLoz
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -2529,7 +2529,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2 En ejecución</t>
+          <t>5 Finalizada</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -20071,10 +20071,26 @@
       <c r="A550" t="n">
         <v>99</v>
       </c>
-      <c r="B550" t="inlineStr"/>
-      <c r="C550" t="inlineStr"/>
-      <c r="D550" t="inlineStr"/>
-      <c r="E550" t="inlineStr"/>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>Tablero de resultados cuantitativos</t>
+        </is>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E550" t="inlineStr">
+        <is>
+          <t>https://lookerstudio.google.com/u/0/reporting/4a928fd5-3d5a-4de3-a655-943ad2da4e6e/page/p_d6cfr52jwd</t>
+        </is>
+      </c>
     </row>
     <row r="551">
       <c r="A551" t="n">
@@ -20527,10 +20543,26 @@
       <c r="A574" t="n">
         <v>102</v>
       </c>
-      <c r="B574" t="inlineStr"/>
-      <c r="C574" t="inlineStr"/>
-      <c r="D574" t="inlineStr"/>
-      <c r="E574" t="inlineStr"/>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>Tablero de resultados cuantitativos</t>
+        </is>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E574" t="inlineStr">
+        <is>
+          <t>https://lookerstudio.google.com/reporting/f0ca73ce-6555-49ec-9219-1ee6b4e60428</t>
+        </is>
+      </c>
     </row>
     <row r="575">
       <c r="A575" t="n">
@@ -20623,7 +20655,7 @@
       </c>
       <c r="D578" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Sí</t>
         </is>
       </c>
       <c r="E578" t="inlineStr">
@@ -20653,7 +20685,7 @@
       </c>
       <c r="E579" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1HGPpuS1Qhl-Udv-KC6DqisNNNB8_C8Ta/view?usp=drive_link</t>
+          <t>https://drive.google.com/file/d/1zSXYH6cCKPEoIcuur0PuPncZ0IaOLo8E/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -20686,10 +20718,26 @@
       <c r="A581" t="n">
         <v>104</v>
       </c>
-      <c r="B581" t="inlineStr"/>
-      <c r="C581" t="inlineStr"/>
-      <c r="D581" t="inlineStr"/>
-      <c r="E581" t="inlineStr"/>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>Presentación resultados Festival Monumentum 2025</t>
+        </is>
+      </c>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E581" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1xJO1lFA1uh52DD5A-mAYv6s-glGlN2jZ/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="582">
       <c r="A582" t="n">
@@ -21122,7 +21170,11 @@
           <t>Anexo</t>
         </is>
       </c>
-      <c r="C604" t="inlineStr"/>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>Anexo 1. Análisis de las preguntas espaciales</t>
+        </is>
+      </c>
       <c r="D604" t="inlineStr">
         <is>
           <t>Sí</t>
@@ -21145,7 +21197,7 @@
       </c>
       <c r="C605" t="inlineStr">
         <is>
-          <t>Informe Festival Joropo al Parque</t>
+          <t>Productos finales Festival Joropo al Parque</t>
         </is>
       </c>
       <c r="D605" t="inlineStr">
@@ -21155,7 +21207,7 @@
       </c>
       <c r="E605" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1lM0-Lxiox-ceikmrbzga-XoDbSS7BH5D/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/1Lcu0iYLFoiXHMX8f8ivPgJPF5XDn-IYx?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21170,7 +21222,7 @@
       </c>
       <c r="C606" t="inlineStr">
         <is>
-          <t>Informe Festival Rock al Parque</t>
+          <t>Productos finales Festival Rock al Parque</t>
         </is>
       </c>
       <c r="D606" t="inlineStr">
@@ -21180,7 +21232,7 @@
       </c>
       <c r="E606" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1tk6baWkyzn5SE-xR-67sOIlt4QUdT037/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/1rccxA6SFUSsKbjgRKqWnvEbok0SpWS9t?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21195,7 +21247,7 @@
       </c>
       <c r="C607" t="inlineStr">
         <is>
-          <t>Informe Festival Vallenato al Parque</t>
+          <t>Productos finales Festival Vallenato al Parque</t>
         </is>
       </c>
       <c r="D607" t="inlineStr">
@@ -21205,7 +21257,7 @@
       </c>
       <c r="E607" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1F_mgYGnqD8wB0tGdAc1u9O-sYDLxyK8U/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/1BchZfxR7zuYYbkgIH8qE8fdgQ1y1EYZk?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21220,7 +21272,7 @@
       </c>
       <c r="C608" t="inlineStr">
         <is>
-          <t>Informe Festival Colombia al Parque</t>
+          <t>Productos finales Festival Colombia al Parque</t>
         </is>
       </c>
       <c r="D608" t="inlineStr">
@@ -21230,7 +21282,7 @@
       </c>
       <c r="E608" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1_XKbAYuvHAz0ietoVzj7wfnc8bLhaEqQ/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/1HBmOWH-hQDqwj0mDiTDqlVdSUVcQkhYt?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21245,7 +21297,7 @@
       </c>
       <c r="C609" t="inlineStr">
         <is>
-          <t>Informe Festival Jazz al Parque</t>
+          <t>Productos finales Festival Jazz al Parque</t>
         </is>
       </c>
       <c r="D609" t="inlineStr">
@@ -21255,7 +21307,7 @@
       </c>
       <c r="E609" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1VvHVdta58v22Q9aiSJwLr2H87fpU4L4P/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/1SSz2sXnITpz_lT4g5-n2AR3M8Ed3LsnM?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21356,7 +21408,7 @@
       </c>
       <c r="C616" t="inlineStr">
         <is>
-          <t>Informe Festival Popular al Parque</t>
+          <t>Productos finales Festival Popular al Parque</t>
         </is>
       </c>
       <c r="D616" t="inlineStr">
@@ -21366,7 +21418,7 @@
       </c>
       <c r="E616" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1zsEUS_LEdC8ZP8xY3ak_UbwJZecKesIv/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/14CmZAQrG8eHOh7xDTf8ypS7TweGA5Df_?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21381,7 +21433,7 @@
       </c>
       <c r="C617" t="inlineStr">
         <is>
-          <t>Informe Festival Hip Hop al Parque</t>
+          <t>Productos finales Festival Hip Hop al Parque</t>
         </is>
       </c>
       <c r="D617" t="inlineStr">
@@ -21391,7 +21443,7 @@
       </c>
       <c r="E617" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1ghYaEKtpBcgNKdjpzzHwnkJ7DwgZwKNO/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/19PXuTzH3C_Nfl5Gj8LO1_XHUgBfjb4b4?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21406,7 +21458,7 @@
       </c>
       <c r="C618" t="inlineStr">
         <is>
-          <t>Informe Festival Salsa al Parque</t>
+          <t>Productos finales Festival Salsa al Parque</t>
         </is>
       </c>
       <c r="D618" t="inlineStr">
@@ -21416,7 +21468,7 @@
       </c>
       <c r="E618" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1UorO-F_CNULkKdJ0SOnc536TyhaC4006/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/1DwWfpUiZRNgalk9jBxS-hFLcAWPqdcap?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21474,19 +21526,51 @@
       <c r="A621" t="n">
         <v>110</v>
       </c>
-      <c r="B621" t="inlineStr"/>
-      <c r="C621" t="inlineStr"/>
-      <c r="D621" t="inlineStr"/>
-      <c r="E621" t="inlineStr"/>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>Presentación Festival Patrimonios en Ruana 2025</t>
+        </is>
+      </c>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E621" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1CaHBM28hdOyauLNWrACrgLpvdPbUDqch/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="622">
       <c r="A622" t="n">
-        <v>111</v>
-      </c>
-      <c r="B622" t="inlineStr"/>
-      <c r="C622" t="inlineStr"/>
-      <c r="D622" t="inlineStr"/>
-      <c r="E622" t="inlineStr"/>
+        <v>110</v>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>Presentación Noche de Museos 2025</t>
+        </is>
+      </c>
+      <c r="D622" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E622" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1CaHBM28hdOyauLNWrACrgLpvdPbUDqch/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="623">
       <c r="A623" t="n">
@@ -22497,7 +22581,7 @@
       </c>
       <c r="E670" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1CTZIeR2jRkd_dxriQ3C8acUqnYvBlI6k/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/1mTOdJ3SeDN8tW2UEmwBNQ1ineXgoHsou/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -23151,7 +23235,11 @@
           <t>Informe final</t>
         </is>
       </c>
-      <c r="C704" t="inlineStr"/>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>Informe final</t>
+        </is>
+      </c>
       <c r="D704" t="inlineStr">
         <is>
           <t>Sí</t>
@@ -23172,7 +23260,11 @@
           <t>Anexo</t>
         </is>
       </c>
-      <c r="C705" t="inlineStr"/>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>Anexo de definición</t>
+        </is>
+      </c>
       <c r="D705" t="inlineStr">
         <is>
           <t>Sí</t>
@@ -23193,7 +23285,11 @@
           <t>Instrumento recolección</t>
         </is>
       </c>
-      <c r="C706" t="inlineStr"/>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>Formulario sondeo</t>
+        </is>
+      </c>
       <c r="D706" t="inlineStr">
         <is>
           <t>Sí</t>
@@ -23678,7 +23774,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F324"/>
+  <dimension ref="A1:F356"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28962,19 +29058,19 @@
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B293" t="n">
         <v>1</v>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>Libro al Viento como encuentro ocasional con la lectura</t>
+          <t>Experiencia y participación cultural</t>
         </is>
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Los resultados muestran que Libro al Viento funciona principalmente como una oportunidad ocasional de encuentro con la lectura, más que como un sistema de préstamo frecuente. La mayoría de las personas que toman libros accede a pocos ejemplares y lo hace de manera puntual. Esta característica es coherente con el diseño del programa y con su presencia en el espacio público, donde el acceso es abierto, espontáneo y no mediado por trámites o registros.</t>
+          <t xml:space="preserve">El Festival Monumentum 2025 registra una experiencia altamente valorada por sus asistentes y un desempeño sólido en calidad artística. Predominan asistentes primerizos, lo que sugiere capacidad de ampliación de públicos; al mismo tiempo, se observa una alta disposición a volver y a recomendar el evento. La participación no se limita a la asistencia: aparecen prácticas asociadas de circulación y apropiación (seguimiento de contenidos, espacios formativos y socialización de la experiencia), lo que refuerza el festival como un nodo que activa participación cultural más sostenida en Bogotá D.C. </t>
         </is>
       </c>
       <c r="E293" t="inlineStr"/>
@@ -28982,21 +29078,19 @@
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B294" t="n">
         <v>2</v>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t xml:space="preserve">Experiencia de lectura, disfrute, utilidad y apropiación
-</t>
+          <t>Convivencia, identidad y orgullo por Bogotá D.C.</t>
         </is>
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t xml:space="preserve">La experiencia asociada a los libros de Libro al Viento combina el disfrute con usos prácticos. La lectura aparece vinculada principalmente a la diversión, pero también al trabajo, al aprendizaje y al enriquecimiento cultural, con variaciones según el tipo de entorno. Además, los efectos simbólicos son claros entre quienes conocen el programa: orgullo por su existencia, disfrute de la lectura y reconocimiento de que leer no es solo para especialistas. Estos impactos, aunque concentrados en un grupo reducido, son intensos y significativos.
-</t>
+          <t xml:space="preserve">Los resultados muestran que el evento se percibe como un espacio de encuentro, respeto e inclusión en el espacio público, con valoraciones favorables sobre convivencia y comportamiento durante la jornada. En el plano simbólico, se reporta una conexión fuerte con la cultura de la ciudad y con el arte como forma de transformación, junto con un componente extendido de orgullo por Bogotá D.C. y por su oferta cultural. En conjunto, el festival aparece como una experiencia urbana que fortalece sentidos de pertenencia y reconocimiento cultural. </t>
         </is>
       </c>
       <c r="E294" t="inlineStr"/>
@@ -29004,19 +29098,19 @@
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B295" t="n">
         <v>3</v>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>Presencia urbana y valor cultural del programa</t>
+          <t>Condiciones de acceso, comunicación y sostenibilidad</t>
         </is>
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Libro al Viento es percibido como un proyecto cultural con presencia en múltiples espacios de la ciudad, lo que refuerza su carácter de política cultural urbana. Su circulación por bibliotecas, parques, eventos culturales, instituciones educativas y espacios de tránsito cotidiano lo posiciona como una iniciativa accesible, cercana y reconocible, que trasciende los espacios tradicionales de lectura y se integra a la vida urbana.</t>
+          <t xml:space="preserve">En accesibilidad, la mayoría reporta facilidad para gestionar transporte de llegada, ingreso, información y aspectos logísticos generales, aunque persisten retos puntuales en seguridad y planeación del transporte de salida para una fracción del público. En mediación y comunicación, predomina el canal digital (especialmente redes), con percepciones mayoritarias de información clara, pero con margen para fortalecer la promoción. En sostenibilidad, se destaca un patrón de movilidad asociado principalmente a transporte público masivo, mientras que la percepción sobre separación de residuos es positiva pero menos contundente, lo que sugiere oportunidades de mejora en visibilidad y apropiación de acciones ambientales. </t>
         </is>
       </c>
       <c r="E295" t="inlineStr"/>
@@ -29024,19 +29118,19 @@
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B296" t="n">
         <v>4</v>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>Circulación extendida y apropiación simbólica de los libros</t>
+          <t>Efectos económicos indirectos y dinámica territorial heterogénea</t>
         </is>
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>La manera en que los libros circulan muestra que su valor no se agota en el punto de entrega ni en la regla de devolución. Al conservarlos, regalarlos o compartirlos, las personas expresan una fuerte apropiación simbólica. Esta circulación extendida refuerza la presencia del programa en la vida cotidiana y lo inscribe en trayectorias personales y sociales diversas, aunque también plantea retos para la disponibilidad y sostenibilidad del sistema de dispensadores.</t>
+          <t>El análisis económico descriptivo muestra dos señales principales: el gasto declarado por asistentes en rubros asociados a su participación y el reporte de incremento de ventas en una parte de los negocios de la zona de influencia. Sin embargo, estos efectos no son homogéneos: no todos los establecimientos perciben mejoras, y la evidencia de inversión adicional y contratación de personal es limitada. En síntesis, el festival activa dinámicas económicas locales de forma parcial y desigual, aportando indicios útiles para fortalecer estrategias de articulación territorial y aprovechamiento económico en futuras ediciones en Bogotá D.C.</t>
         </is>
       </c>
       <c r="E296" t="inlineStr"/>
@@ -29047,578 +29141,1220 @@
         <v>105</v>
       </c>
       <c r="B297" t="n">
+        <v>1</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Libro al Viento como encuentro ocasional con la lectura</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Los resultados muestran que Libro al Viento funciona principalmente como una oportunidad ocasional de encuentro con la lectura, más que como un sistema de préstamo frecuente. La mayoría de las personas que toman libros accede a pocos ejemplares y lo hace de manera puntual. Esta característica es coherente con el diseño del programa y con su presencia en el espacio público, donde el acceso es abierto, espontáneo y no mediado por trámites o registros.</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr"/>
+      <c r="F297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>105</v>
+      </c>
+      <c r="B298" t="n">
+        <v>2</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Experiencia de lectura, disfrute, utilidad y apropiación
+</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">La experiencia asociada a los libros de Libro al Viento combina el disfrute con usos prácticos. La lectura aparece vinculada principalmente a la diversión, pero también al trabajo, al aprendizaje y al enriquecimiento cultural, con variaciones según el tipo de entorno. Además, los efectos simbólicos son claros entre quienes conocen el programa: orgullo por su existencia, disfrute de la lectura y reconocimiento de que leer no es solo para especialistas. Estos impactos, aunque concentrados en un grupo reducido, son intensos y significativos.
+</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr"/>
+      <c r="F298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>105</v>
+      </c>
+      <c r="B299" t="n">
+        <v>3</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Presencia urbana y valor cultural del programa</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Libro al Viento es percibido como un proyecto cultural con presencia en múltiples espacios de la ciudad, lo que refuerza su carácter de política cultural urbana. Su circulación por bibliotecas, parques, eventos culturales, instituciones educativas y espacios de tránsito cotidiano lo posiciona como una iniciativa accesible, cercana y reconocible, que trasciende los espacios tradicionales de lectura y se integra a la vida urbana.</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr"/>
+      <c r="F299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>105</v>
+      </c>
+      <c r="B300" t="n">
+        <v>4</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Circulación extendida y apropiación simbólica de los libros</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>La manera en que los libros circulan muestra que su valor no se agota en el punto de entrega ni en la regla de devolución. Al conservarlos, regalarlos o compartirlos, las personas expresan una fuerte apropiación simbólica. Esta circulación extendida refuerza la presencia del programa en la vida cotidiana y lo inscribe en trayectorias personales y sociales diversas, aunque también plantea retos para la disponibilidad y sostenibilidad del sistema de dispensadores.</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr"/>
+      <c r="F300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>105</v>
+      </c>
+      <c r="B301" t="n">
         <v>5</v>
       </c>
-      <c r="C297" t="inlineStr">
+      <c r="C301" t="inlineStr">
         <is>
           <t xml:space="preserve">El libro como objeto social situado: inserción comunitaria y política cultural </t>
         </is>
       </c>
-      <c r="D297" t="inlineStr">
+      <c r="D301" t="inlineStr">
         <is>
           <t xml:space="preserve">Las cartografías sociales evidencian que los libros del programa Libro al Viento se integran a prácticas sociales concretas y territorialmente situadas, más allá de su simple circulación física. Los libros se insertan en dinámicas comunitarias, educativas y cotidianas, adquiriendo sentidos diversos según los contextos sociales y territoriales de cada taller. En este sentido, Libro al Viento se configura como una política cultural situada, cuyos efectos dependen de las relaciones sociales que median la apropiación del libro. Las cartografías complementan el sondeo cuantitativo al mostrar cómo los libros se anclan, circulan y se resignifican en la vida cotidiana, dando lugar a circuitos múltiples y no lineales de uso. 
 </t>
         </is>
       </c>
-      <c r="E297" t="inlineStr"/>
-      <c r="F297" t="inlineStr"/>
-    </row>
-    <row r="298">
-      <c r="A298" t="n">
+      <c r="E301" t="inlineStr"/>
+      <c r="F301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>106</v>
+      </c>
+      <c r="B302" t="n">
+        <v>1</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Experiencia altamente valorada y con fuerte fidelización</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Los resultados muestran una valoración mayoritariamente positiva del Premio Luis Caballero 2025. La calidad de los proyectos y artistas es calificada como excelente por una proporción amplia de asistentes, y se observa una muy alta disposición a recomendar y a asistir nuevamente en futuras ediciones. En conjunto, esto reafirma al premio como una plataforma sólida de circulación del arte contemporáneo, capaz de generar satisfacción y continuidad en el público. </t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr"/>
+      <c r="F302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>106</v>
+      </c>
+      <c r="B303" t="n">
+        <v>2</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Ampliación de audiencias y vínculo con la oferta cultural de la ciudad</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El premio convoca públicos con trayectorias culturales activas, pero también funciona como puerta de entrada: una mayoría de asistentes reporta estar participando por primera vez en el evento y, antes de la visita, una proporción importante no lo conocía o tenía un conocimiento limitado. Tras la experiencia, aumenta el reconocimiento del Premio como un espacio relevante y se fortalece la disposición a participar en otros eventos culturales de Bogotá D.C., lo que sugiere un efecto de “enganche” con la oferta cultural más amplia. </t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr"/>
+      <c r="F303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>106</v>
+      </c>
+      <c r="B304" t="n">
+        <v>3</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Aporte simbólico y lectura crítica del arte contemporáneo</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Más allá del disfrute, los asistentes señalan que el premio contribuye a valorar el arte y el patrimonio como formas de transformación, ampliar conocimientos sobre el entorno cultural y reconocerse como parte activa de la vida cultural. En el componente modular resalta que, para una mayoría, el premio aporta al debate sobre arte contemporáneo y promueve proyectos disruptivos, pero también se reconoce que puede reforzar ciertos discursos dominantes, mostrando que el público lo comprende como un espacio de discusión real, con tensiones propias del campo artístico. </t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr"/>
+      <c r="F304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>106</v>
+      </c>
+      <c r="B305" t="n">
+        <v>4</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Accesibilidad y mediación con percepción positiva</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>En términos de logística y acceso, se reportan percepciones favorables sobre señalización, acompañamiento del personal, fluidez en entradas y/o salidas, y condiciones de accesibilidad (incluida discapacidad), mientras que transporte y seguridad aparecen como factores centrales al decidir asistir. Por otro lado, los medios de comunicación sobre el evento se distribuyen entre internet, voz a voz y descubrimiento en el lugar, lo que sugiere una oportunidad para fortalecer la divulgación previa.</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr"/>
+      <c r="F305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>107</v>
+      </c>
+      <c r="B306" t="n">
+        <v>1</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>El circo en Bogotá: un proyecto de vida en un sector consolidado</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>El sector circense en Bogotá presenta un alto grado de madurez, caracterizado por la predominancia de artistas con más de diez años de experiencia, formación empírica y/o especializada, y desempeño en múltiples disciplinas y oficios. Esta configuración da cuenta de un campo complejo, diversificado y técnicamente autónomo. De manera significativa, una parte mayoritaria de los participantes reconoce el circo como su proyecto de vida y principal ocupación, reafirmando su condición de sector profesional y no meramente recreativo.</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr"/>
+      <c r="F306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>107</v>
+      </c>
+      <c r="B307" t="n">
+        <v>2</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Ecosistema polivalente y móvil, anclado en el espacio público</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Aunque predomina el circo contemporáneo, el social‑comunitario y el tradicional mantienen una presencia significativa, con trayectorias mixtas e hibridaciones que se desplazan entre carpas, espacio público, salas, escuelas y espacios no convencionales. El entrenamiento y la circulación se apoyan fuertemente en parques, plazas y espacios comunitarios, lo que expresa la vocación itinerante del circo, pero también la ausencia de infraestructura estable y adecuada para ensayo y presentación.</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr"/>
+      <c r="F307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>107</v>
+      </c>
+      <c r="B308" t="n">
+        <v>3</v>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Organización fuerte, sostenibilidad frágil</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>El sector muestra altos niveles de organización y articulación: cerca de dos tercios de las personas encuestadas pertenecen a redes, colectivos u organizaciones, y más del 70% ha participado en mesas, sindicatos o consejos del sector cultural. Sin embargo, la mayoría se ubica en condiciones de informalidad o semi‑formalidad laboral, con ingresos esporádicos y baja protección social, lo que tensiona la posibilidad de sostener el circo como trabajo estable pese a la fuerte capacidad asociativa</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr"/>
+      <c r="F308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>107</v>
+      </c>
+      <c r="B309" t="n">
+        <v>4</v>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Restricciones estructurales que limitan la sostenibilidad económica y la circulación</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Aunque el 59% declara vivir principalmente del circo y otro grupo importante lo ejerce como actividad complementaria o mediante proyectos, las principales dificultades para sostener la práctica son el acceso a recursos públicos, la entrada a festivales y espacios de circulación, y las restricciones para usar el espacio público. Estas barreras, sumadas a la precariedad de infraestructura y la inestabilidad de los lugares de entrenamiento y presentación, impiden traducir la experiencia acumulada en condiciones económicas más estables.</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr"/>
+      <c r="F309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>107</v>
+      </c>
+      <c r="B310" t="n">
+        <v>5</v>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Un sector formado que exige condiciones para profesionalizarse</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Alrededor del 77,6% de las personas encuestadas ha recibido formación específica en circo, combinando tradición familiar, espacios comunitarios, autoformación, instituciones técnicas, maestras y maestros particulares y, en algunos casos, procesos internacionales. Existe un consenso amplio sobre la importancia de la formación profesional circense y se priorizan como apoyos clave los recursos económicos, los espacios y condiciones adecuadas de práctica, la formación especializada, el reconocimiento profesional del oficio y el acceso a salud y protección social, delineando una agenda concreta para políticas de profesionalización del sector.</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr"/>
+      <c r="F310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
         <v>109</v>
       </c>
-      <c r="B298" t="n">
+      <c r="B311" t="n">
         <v>1</v>
       </c>
-      <c r="C298" t="inlineStr">
+      <c r="C311" t="inlineStr">
         <is>
           <t>El Festival activa dinámicas económicas y de sosenibilidad cultural</t>
         </is>
       </c>
-      <c r="D298" t="inlineStr">
+      <c r="D311" t="inlineStr">
         <is>
           <t xml:space="preserve">Aunque el apoyo a emprendimientos culturales, la compra de productos o el intercambio con melómanos no constituyen el principal motivo de asistencia en ninguno de los escenarios, sí aparecen de manera consistente en todos ellos como motivaciones complementarias. Este patrón sugiere que el Festival Centro no solo funciona como un espacio de circulación artística, sino también como un dispositivo que contribuye a la sostenibilidad económica del ecosistema cultural, al activar prácticas de consumo cultural, visibilización de agentes y circulación de bienes simbólicos asociados a la música y las artes.
 Así, se podría seguir fortaleciendo de manera estratégica los componentes de circulación económica y visibilización de emprendimientos culturales, especialmente en aquellos escenarios con mayor afluencia y diversidad de públicos, sin desdibujar el eje artístico del Festival.
 </t>
         </is>
       </c>
-      <c r="E298" t="inlineStr"/>
-      <c r="F298" t="inlineStr"/>
-    </row>
-    <row r="299">
-      <c r="A299" t="n">
+      <c r="E311" t="inlineStr"/>
+      <c r="F311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
         <v>109</v>
       </c>
-      <c r="B299" t="n">
+      <c r="B312" t="n">
         <v>2</v>
       </c>
-      <c r="C299" t="inlineStr">
+      <c r="C312" t="inlineStr">
         <is>
           <t>El Festival no genera mayores impactos negativos en el espacio público</t>
         </is>
       </c>
-      <c r="D299" t="inlineStr">
+      <c r="D312" t="inlineStr">
         <is>
           <t xml:space="preserve">En los cuatro escenarios analizados, la percepción mayoritaria de los asistentes indica que la realización del Festival no modifica sustancialmente problemáticas asociadas al espacio público, como el arrojo de basuras, el parqueo en zonas prohibidas o la contaminación auditiva y visual. 
 Por otro lado, en algunos casos, como el Muelle de la FUGA y La Media Torta, se registra una mayor percepción de incremento en la presencia de vendedores informales o en el turismo; sin embargo, estos fenómenos coexisten con una valoración positiva del evento y no se asocian a un deterioro de la convivencia en la zona.
 </t>
         </is>
       </c>
-      <c r="E299" t="inlineStr"/>
-      <c r="F299" t="inlineStr"/>
-    </row>
-    <row r="300">
-      <c r="A300" t="n">
+      <c r="E312" t="inlineStr"/>
+      <c r="F312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
         <v>109</v>
       </c>
-      <c r="B300" t="n">
+      <c r="B313" t="n">
         <v>3</v>
       </c>
-      <c r="C300" t="inlineStr">
+      <c r="C313" t="inlineStr">
         <is>
           <t>El Festival articula los desplazamientos, recorridos y consumos culturales en el centro</t>
         </is>
       </c>
-      <c r="D300" t="inlineStr">
+      <c r="D313" t="inlineStr">
         <is>
           <t>En todos los escenarios, una proporción mayoritaria de asistentes declaró haber visitado o tener previsto visitar otros espacios del centro antes o después del evento. Los recorridos se concentraron principalmente en equipamientos culturales, cafés, restaurantes, bares, teatros, salas de arte y museos, lo que evidencia una alta capacidad del Festival para articular la oferta cultural, gastronómica y comercial del centro de Bogotá. Este comportamiento refuerza el papel del Festival Centro como dinamizador territorial y como nodo de conexión entre la programación cultural pública y otras actividades económicas y simbólicas del área.</t>
         </is>
       </c>
-      <c r="E300" t="inlineStr"/>
-      <c r="F300" t="inlineStr"/>
-    </row>
-    <row r="301">
-      <c r="A301" t="n">
+      <c r="E313" t="inlineStr"/>
+      <c r="F313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
         <v>109</v>
       </c>
-      <c r="B301" t="n">
+      <c r="B314" t="n">
         <v>4</v>
       </c>
-      <c r="C301" t="inlineStr">
+      <c r="C314" t="inlineStr">
         <is>
           <t xml:space="preserve">La oferta musical y artística es el principal motivo de asistencia
 </t>
         </is>
       </c>
-      <c r="D301" t="inlineStr">
+      <c r="D314" t="inlineStr">
         <is>
           <t>En todos los escenarios, los motivos de asistencia se concentran de manera consistente en la presencia de los grupos y artistas, el interés por conocer nuevas propuestas musicales y el reconocimiento previo de algunos de los artistas participantes. El Festival Centro opera simultáneamente como un espacio de encuentro entre artistas y sus audiencias y como una plataforma para el descubrimiento de nuevas propuestas, lo que explica la coexistencia de públicos con trayectoria en el Festival y de personas que asisten por primera vez.</t>
         </is>
       </c>
-      <c r="E301" t="inlineStr"/>
-      <c r="F301" t="inlineStr"/>
-    </row>
-    <row r="302">
-      <c r="A302" t="n">
+      <c r="E314" t="inlineStr"/>
+      <c r="F314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>110</v>
+      </c>
+      <c r="B315" t="n">
+        <v>1</v>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Balance general de la experiencia</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>En la Noche de Museos y el Festival Patrimonios en Ruana se observa una valoración global muy favorable por parte de los asistentes. Predominan percepciones de alta satisfacción y de calidad en la experiencia cultural, junto con una muy alta disposición a recomendar y a asistir nuevamente en futuras ediciones. En conjunto, los resultados sugieren que ambos formatos funcionan como espacios consistentes para el disfrute del patrimonio y la cultura, con capacidad de sostener la participación en el tiempo.</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr"/>
+      <c r="F315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>110</v>
+      </c>
+      <c r="B316" t="n">
+        <v>2</v>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Públicos, motivaciones y activación cultural</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Los hallazgos muestran públicos con trayectorias culturales diversas y motivaciones centradas en hacer algo distinto, explorar la ciudad y acercarse a experiencias culturales específicas. La Noche de Museos destaca por su capacidad de atraer asistentes primerizos, mientras Patrimonios en Ruana combina ese componente con un público recurrente; en ambos casos, la vivencia del evento se asocia con un mayor interés por seguir participando en la oferta cultural de la ciudad.</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr"/>
+      <c r="F316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>110</v>
+      </c>
+      <c r="B317" t="n">
+        <v>3</v>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Encuentro ciudadano, identidad y orgullo por Bogotá D.C.</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>En ambas mediciones, los eventos aparecen como escenarios de encuentro social con percepciones mayoritarias de respeto e inclusión. Además, se reportan aportes simbólicos claros: conexión con la cultura de la ciudad, fortalecimiento de lazos sociales y comunitarios, y un sentimiento extendido de orgullo por la oferta cultural de Bogotá D.C. En conjunto, los resultados respaldan la idea de que estos eventos no solo convocan público, sino que también fortalecen sentidos compartidos de pertenencia.</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr"/>
+      <c r="F317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>110</v>
+      </c>
+      <c r="B318" t="n">
+        <v>4</v>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Condiciones de acceso, comunicación y oportunidades de mejora</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>La logística es bien evaluada en aspectos como señalización, apoyo al público y organización general; aun así, el transporte, la movilidad y la seguridad aparecen como factores determinantes para facilitar la asistencia y mejorar la experiencia. En términos de comunicación, Noche de Museos se apoya más en canales digitales, mientras Patrimonios en Ruana depende más del voz a voz, lo que abre una oportunidad para fortalecer la divulgación sin perder el componente comunitario. También se identifican mejoras puntuales en accesibilidad para personas con discapacidad y en temas logísticos asociados al desplazamiento.</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr"/>
+      <c r="F318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
         <v>112</v>
       </c>
-      <c r="B302" t="n">
+      <c r="B319" t="n">
         <v>1</v>
       </c>
-      <c r="C302" t="inlineStr">
+      <c r="C319" t="inlineStr">
         <is>
           <t xml:space="preserve">Naturaleza de la creación colectiva
 </t>
         </is>
       </c>
-      <c r="D302" t="inlineStr">
+      <c r="D319" t="inlineStr">
         <is>
           <t>La creación colectiva se caracteriza por su profunda vocación de horizontalidad, solidaridad y libertad. Más que centrarse en la obtención de un producto final, privilegia el proceso como un espacio vivo de exploración, diálogo y construcción conjunta. En este sentido, se configura como un ejercicio humano y político que desafía las jerarquías tradicionales, redistribuye el poder creativo y habilita formas alternativas de relación y producción cultural.</t>
         </is>
       </c>
-      <c r="E302" t="inlineStr"/>
-      <c r="F302" t="inlineStr"/>
-    </row>
-    <row r="303">
-      <c r="A303" t="n">
+      <c r="E319" t="inlineStr"/>
+      <c r="F319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
         <v>112</v>
       </c>
-      <c r="B303" t="n">
+      <c r="B320" t="n">
         <v>2</v>
       </c>
-      <c r="C303" t="inlineStr">
+      <c r="C320" t="inlineStr">
         <is>
           <t>Metodologías, roles y autoría</t>
         </is>
       </c>
-      <c r="D303" t="inlineStr">
+      <c r="D320" t="inlineStr">
         <is>
           <t>En los procesos de creación colectiva, las metodologías se construyen desde la participación activa y la co-decisión. Los roles no se imponen de antemano, sino que emergen en función de las necesidades y momentos del proceso, lo que promueve dinámicas más flexibles y colaborativas. El liderazgo se concibe como un acompañamiento empático y orientador, antes que como una instancia de dirección jerárquica. La dramaturgia, por su parte, surge de la investigación, la improvisación y la apertura estructural, y aunque la documentación es una herramienta valiosa, suele ser poco sistemática debido a la naturaleza orgánica del trabajo.</t>
         </is>
       </c>
-      <c r="E303" t="inlineStr"/>
-      <c r="F303" t="inlineStr"/>
-    </row>
-    <row r="304">
-      <c r="A304" t="n">
+      <c r="E320" t="inlineStr"/>
+      <c r="F320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
         <v>112</v>
       </c>
-      <c r="B304" t="n">
+      <c r="B321" t="n">
         <v>3</v>
       </c>
-      <c r="C304" t="inlineStr">
+      <c r="C321" t="inlineStr">
         <is>
           <t>Interdisciplinariedad y articulación de saberes</t>
         </is>
       </c>
-      <c r="D304" t="inlineStr">
+      <c r="D321" t="inlineStr">
         <is>
           <t>La creación colectiva se nutre de una integración natural y fluida de múltiples artes, oficios y conocimientos. La apertura metodológica facilita aportes espontáneos entre disciplinas y la incorporación de especialistas externos, enriqueciendo el proceso. La tecnología también se incorpora como recurso creativo y expresivo, privilegiando enfoques de cultura libre y acceso abierto, lo que amplía las posibilidades estéticas y fomenta la innovación en los lenguajes escénicos.</t>
         </is>
       </c>
-      <c r="E304" t="inlineStr"/>
-      <c r="F304" t="inlineStr"/>
-    </row>
-    <row r="305">
-      <c r="A305" t="n">
+      <c r="E321" t="inlineStr"/>
+      <c r="F321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
         <v>112</v>
       </c>
-      <c r="B305" t="n">
+      <c r="B322" t="n">
         <v>4</v>
       </c>
-      <c r="C305" t="inlineStr">
+      <c r="C322" t="inlineStr">
         <is>
           <t>Sostenibilidad e impacto sociocultural</t>
         </is>
       </c>
-      <c r="D305" t="inlineStr">
+      <c r="D322" t="inlineStr">
         <is>
           <t>La sostenibilidad de estos procesos depende, ante todo, de los vínculos humanos, la confianza entre los participantes y la claridad de un propósito común. En este modelo, la comunidad no es solo receptora, sino coproductora activa del proceso y sus resultados. Esta dinámica favorece transformaciones significativas tanto en el plano personal como en el territorial, fortaleciendo el sentido de pertenencia, la identidad colectiva y los procesos de memoria y cuidado de los territorios.</t>
         </is>
       </c>
-      <c r="E305" t="inlineStr"/>
-      <c r="F305" t="inlineStr"/>
-    </row>
-    <row r="306">
-      <c r="A306" t="n">
+      <c r="E322" t="inlineStr"/>
+      <c r="F322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>114</v>
+      </c>
+      <c r="B323" t="n">
+        <v>1</v>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>La FUGA: Una biblioteca-destino</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>A diferencia del patrón observado en la mayoría de las bibliotecas públicas —donde predomina el uso para estudio o trabajo—, en la Biblioteca Pública FUGA el principal motivo de visita es recorrerla por primera vez (48,6%). Este valor resulta excepcionalmente alto frente al promedio general del sistema (7,9%) y pone en evidencia su carácter monumental, simbólico y turístico, así como su rol estratégico como equipamiento cultural de alto valor patrimonial en el centro histórico de Bogotá.</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr"/>
+      <c r="F323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>114</v>
+      </c>
+      <c r="B324" t="n">
+        <v>2</v>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Un patrón de afiliación excepcional dentro de la Red</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>En la Biblioteca Pública Manuel Zapata Olivella – El Tintal, el segundo motivo más frecuente de visita es la afiliación o el uso de otros servicios (18,7%). Este porcentaje es significativamente superior al promedio de la Red, lo que evidencia un desempeño atípico y sugiere que las estrategias de afiliación, fidelización y acercamiento comunitario han tenido un impacto especialmente efectivo en su entorno territorial.</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr"/>
+      <c r="F324" t="inlineStr"/>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>114</v>
+      </c>
+      <c r="B325" t="n">
+        <v>3</v>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>La biblioteca como centro de acceso digital: El caso de Suba</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>En la Biblioteca Pública Francisco José de Caldas (Suba), el uso de computadores y otros equipos tecnológicos se configura como una motivación de visita altamente relevante, alcanzando el 18,6 % de las respuestas. Esta proporción supera ampliamente el promedio general de las bibliotecas sondeadas (7,0 %), lo que evidencia una demanda territorial específica de acceso a infraestructura tecnológica y posiciona a la biblioteca como un nodo clave para la reducción de brechas digitales en la localidad.</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr"/>
+      <c r="F325" t="inlineStr"/>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>114</v>
+      </c>
+      <c r="B326" t="n">
+        <v>4</v>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Desconocimiento que frena el uso de los servicios</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>El principal obstáculo para la vinculación de usuarios potenciales a los servicios bibliotecarios es el desconocimiento de la oferta. Entre las personas que se encuentran en los recintos pero no hacen uso de los servicios, este factor aparece de manera recurrente y con una intensidad superior al promedio del sistema. En la Biblioteca de Usaquén-Servitá, el 44,4 % de estos usuarios señala no conocer la oferta disponible, mientras que en La Peña esta proporción asciende al 50 %, cifras que superan ampliamente el promedio general (20,9 %) y evidencian una brecha crítica de información y comunicación.</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr"/>
+      <c r="F326" t="inlineStr"/>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
         <v>115</v>
       </c>
-      <c r="B306" t="n">
+      <c r="B327" t="n">
         <v>1</v>
       </c>
-      <c r="C306" t="inlineStr">
+      <c r="C327" t="inlineStr">
         <is>
           <t>Patrones de uso y acompañamiento social</t>
         </is>
       </c>
-      <c r="D306" t="inlineStr">
+      <c r="D327" t="inlineStr">
         <is>
           <t>Los resultados muestran que los parques estructurantes priorizados presentan patrones de uso regular, con predominio de visitas semanales y diarias. La asistencia se realiza mayoritariamente en compañía de familiares, y el horario de uso se concentra principalmente en la franja de la mañana. La práctica de deporte o actividad física es la actividad reportada con mayor frecuencia en todos los parques, seguida por usos asociados al acompañamiento y al tránsito cotidiano</t>
         </is>
       </c>
-      <c r="E306" t="inlineStr"/>
-      <c r="F306" t="inlineStr"/>
-    </row>
-    <row r="307">
-      <c r="A307" t="n">
+      <c r="E327" t="inlineStr"/>
+      <c r="F327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
         <v>115</v>
       </c>
-      <c r="B307" t="n">
+      <c r="B328" t="n">
         <v>2</v>
       </c>
-      <c r="C307" t="inlineStr">
+      <c r="C328" t="inlineStr">
         <is>
           <t>Valoración del estado físico y la seguridad</t>
         </is>
       </c>
-      <c r="D307" t="inlineStr">
+      <c r="D328" t="inlineStr">
         <is>
           <t xml:space="preserve">La mayoría de las personas encuestadas califica el estado físico y el mantenimiento de los parques como “bueno” o “excelente”. De igual forma, una alta proporción de usuarios manifiesta sentirse segura al visitar estos espacios. No obstante, una parte de la población reporta percepciones de inseguridad, especialmente asociadas a condiciones como la iluminación, lo que coincide con los aspectos físicos señalados como susceptibles de mejora.
 </t>
         </is>
       </c>
-      <c r="E307" t="inlineStr"/>
-      <c r="F307" t="inlineStr"/>
-    </row>
-    <row r="308">
-      <c r="A308" t="n">
+      <c r="E328" t="inlineStr"/>
+      <c r="F328" t="inlineStr"/>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
         <v>115</v>
       </c>
-      <c r="B308" t="n">
+      <c r="B329" t="n">
         <v>3</v>
       </c>
-      <c r="C308" t="inlineStr">
+      <c r="C329" t="inlineStr">
         <is>
           <t>Reconocimiento comunitario del parque</t>
         </is>
       </c>
-      <c r="D308" t="inlineStr">
+      <c r="D329" t="inlineStr">
         <is>
           <t xml:space="preserve">Los parques son reconocidos por la mayoría de los usuarios como espacios importantes para su comunidad o barrio. Este reconocimiento se presenta de manera consistente en los cinco parques analizados, lo que describe el papel de estos escenarios como referentes del entorno social y del uso cotidiano del espacio público.
 </t>
         </is>
       </c>
-      <c r="E308" t="inlineStr"/>
-      <c r="F308" t="inlineStr"/>
-    </row>
-    <row r="309">
-      <c r="A309" t="n">
+      <c r="E329" t="inlineStr"/>
+      <c r="F329" t="inlineStr"/>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
         <v>115</v>
       </c>
-      <c r="B309" t="n">
+      <c r="B330" t="n">
         <v>4</v>
       </c>
-      <c r="C309" t="inlineStr">
+      <c r="C330" t="inlineStr">
         <is>
           <t>Diferencia entre participación reportada e interés declarado</t>
         </is>
       </c>
-      <c r="D309" t="inlineStr">
+      <c r="D330" t="inlineStr">
         <is>
           <t xml:space="preserve">Los resultados evidencian que la proporción de personas que reporta haber participado en actividades organizadas en los parques es menor que la proporción de usuarios que manifiesta interés en participar en actividades deportivas, recreativas, culturales o comunitarias. Esta diferencia describe una brecha entre la participación efectiva y la disposición declarada por la ciudadanía.
 </t>
         </is>
       </c>
-      <c r="E309" t="inlineStr"/>
-      <c r="F309" t="inlineStr"/>
-    </row>
-    <row r="310">
-      <c r="A310" t="n">
+      <c r="E330" t="inlineStr"/>
+      <c r="F330" t="inlineStr"/>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
         <v>115</v>
       </c>
-      <c r="B310" t="n">
+      <c r="B331" t="n">
         <v>5</v>
       </c>
-      <c r="C310" t="inlineStr">
+      <c r="C331" t="inlineStr">
         <is>
           <t>Barreras y condiciones para el aprovechamiento</t>
         </is>
       </c>
-      <c r="D310" t="inlineStr">
+      <c r="D331" t="inlineStr">
         <is>
           <t>La falta de tiempo es la barrera más reportada para el uso y aprovechamiento de los parques, seguida por la percepción de inseguridad y la falta de información sobre la oferta de actividades. Estas barreras se presentan en todos los parques, con variaciones en su magnitud relativa según el escenario.</t>
         </is>
       </c>
-      <c r="E310" t="inlineStr"/>
-      <c r="F310" t="inlineStr"/>
-    </row>
-    <row r="311">
-      <c r="A311" t="n">
+      <c r="E331" t="inlineStr"/>
+      <c r="F331" t="inlineStr"/>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
         <v>116</v>
       </c>
-      <c r="B311" t="n">
+      <c r="B332" t="n">
         <v>1</v>
       </c>
-      <c r="C311" t="inlineStr">
+      <c r="C332" t="inlineStr">
         <is>
           <t xml:space="preserve">La motivación existe. 
 Las barreras son estructurales y de contexto
 </t>
         </is>
       </c>
-      <c r="D311" t="inlineStr">
+      <c r="D332" t="inlineStr">
         <is>
           <t xml:space="preserve">Ciclovía: la mayoría sabe montar bicicleta y reconoce beneficios claros (ahorro de tiempo/dinero, autonomía).
 Escuela de la Bici: el principal obstáculo inicial no es el desinterés, sino no saber montar, la inseguridad y la falta de confianza.
 </t>
         </is>
       </c>
-      <c r="E311" t="inlineStr"/>
-      <c r="F311" t="inlineStr"/>
-    </row>
-    <row r="312">
-      <c r="A312" t="n">
+      <c r="E332" t="inlineStr"/>
+      <c r="F332" t="inlineStr"/>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
         <v>116</v>
       </c>
-      <c r="B312" t="n">
+      <c r="B333" t="n">
         <v>2</v>
       </c>
-      <c r="C312" t="inlineStr">
+      <c r="C333" t="inlineStr">
         <is>
           <t>Los programas generan percepción de impacto, pero de forma diferenciada</t>
         </is>
       </c>
-      <c r="D312" t="inlineStr">
+      <c r="D333" t="inlineStr">
         <is>
           <t>Ciclovía: alta recurrencia y masividad; impacto percibido en actividad física, motivación semanal y uso recreativo de la bicicleta.
 Escuela de la Bici: impacto percibido en aprendizaje, confianza, bienestar emocional y cambio personal, aunque con menor uso posterior por barreras materiales.</t>
         </is>
       </c>
-      <c r="E312" t="inlineStr"/>
-      <c r="F312" t="inlineStr"/>
-    </row>
-    <row r="313">
-      <c r="A313" t="n">
+      <c r="E333" t="inlineStr"/>
+      <c r="F333" t="inlineStr"/>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
         <v>116</v>
       </c>
-      <c r="B313" t="n">
+      <c r="B334" t="n">
         <v>3</v>
       </c>
-      <c r="C313" t="inlineStr">
+      <c r="C334" t="inlineStr">
         <is>
           <t>La bicicleta transforma la vida cotidiana más que la identidad colectiva</t>
         </is>
       </c>
-      <c r="D313" t="inlineStr">
+      <c r="D334" t="inlineStr">
         <is>
           <t>La sociabilidad se expresa principalmente en vínculos cercanos (familia, amigos) más que en colectivos organizados.
 El principal beneficio percibido es práctico (ahorro de tiempo/dinero, autonomía), seguido de salud y bienestar.</t>
         </is>
       </c>
-      <c r="E313" t="inlineStr"/>
-      <c r="F313" t="inlineStr"/>
-    </row>
-    <row r="314">
-      <c r="A314" t="n">
+      <c r="E334" t="inlineStr"/>
+      <c r="F334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
         <v>117</v>
       </c>
-      <c r="B314" t="n">
+      <c r="B335" t="n">
         <v>1</v>
       </c>
-      <c r="C314" t="inlineStr">
+      <c r="C335" t="inlineStr">
         <is>
           <t>Comprender la gobernanza deportiva como un sistema complejo, multinivel y en evolución</t>
         </is>
       </c>
-      <c r="D314" t="inlineStr">
+      <c r="D335" t="inlineStr">
         <is>
           <t>Los hallazgos de esta investigación muestran que la gobernanza del deporte, la recreación y la actividad física en Bogotá debería entenderse como un sistema complejo en el que convergen actores públicos, privados, comunitarios y académicos con distintos niveles de autoridad, capacidades y responsabilidades. La revisión de literatura confirma que los modelos contemporáneos de gobernanza combinan mecanismos jerárquicos, colaborativos e híbridos, lo cual coincide con la configuración del ecosistema distrital. Esta perspectiva permite reconocer tanto el valor de las estructuras formales del Sistema Nacional del Deporte como la importancia de los vínculos territoriales, las redes sociales y las prácticas comunitarias que sostienen el funcionamiento cotidiano del sistema.</t>
         </is>
       </c>
-      <c r="E314" t="inlineStr"/>
-      <c r="F314" t="inlineStr"/>
-    </row>
-    <row r="315">
-      <c r="A315" t="n">
+      <c r="E335" t="inlineStr"/>
+      <c r="F335" t="inlineStr"/>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
         <v>117</v>
       </c>
-      <c r="B315" t="n">
+      <c r="B336" t="n">
         <v>2</v>
       </c>
-      <c r="C315" t="inlineStr">
+      <c r="C336" t="inlineStr">
         <is>
           <t>Clarificar el papel de los actores como base para mejorar la articulación y corresponsabilidad</t>
         </is>
       </c>
-      <c r="D315" t="inlineStr">
+      <c r="D336" t="inlineStr">
         <is>
           <t>Se considera necesario seguir avanzando en mecanismos que fortalezcan la corresponsabilidad entre niveles de gobierno, organizaciones deportivas, sector privado, ciudadanía y academia. La claridad en los roles y la comprensión de las relaciones entre actores son condiciones esenciales para que la política deportiva distrital evolucione hacia formas más consistentes de cooperación, planificación conjunta y toma de decisiones basada en evidencia, la tipología de actores es un punto de partida para esta definición.</t>
         </is>
       </c>
-      <c r="E315" t="inlineStr"/>
-      <c r="F315" t="inlineStr"/>
-    </row>
-    <row r="316">
-      <c r="A316" t="n">
+      <c r="E336" t="inlineStr"/>
+      <c r="F336" t="inlineStr"/>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
         <v>117</v>
       </c>
-      <c r="B316" t="n">
+      <c r="B337" t="n">
         <v>3</v>
       </c>
-      <c r="C316" t="inlineStr">
+      <c r="C337" t="inlineStr">
         <is>
           <t>Aplicar la medición para caracterizar a los actores y fortalecer el sistema de información</t>
         </is>
       </c>
-      <c r="D316" t="inlineStr">
+      <c r="D337" t="inlineStr">
         <is>
           <t>El desarrollo de las categorías analíticas, del formulario cuantitativo y de la propuesta metodológica cualitativa constituye un insumo clave para avanzar hacia un sistema de información más sólido y útil para la toma de decisiones. La aplicación de estos instrumentos permitirá caracterizar de manera rigurosa a los actores del ecosistema deportivo y facilitará una comprensión más completa, contextualizada y accionable sobre el funcionamiento real del ecosistema deportivo y sobre las oportunidades para fortalecer su gobernanza.</t>
         </is>
       </c>
-      <c r="E316" t="inlineStr"/>
-      <c r="F316" t="inlineStr"/>
-    </row>
-    <row r="317">
-      <c r="A317" t="n">
+      <c r="E337" t="inlineStr"/>
+      <c r="F337" t="inlineStr"/>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
         <v>117</v>
       </c>
-      <c r="B317" t="n">
+      <c r="B338" t="n">
         <v>4</v>
       </c>
-      <c r="C317" t="inlineStr">
+      <c r="C338" t="inlineStr">
         <is>
           <t>Usar el instrumento como herramienta progresiva para la mejora de la política pública</t>
         </is>
       </c>
-      <c r="D317" t="inlineStr">
+      <c r="D338" t="inlineStr">
         <is>
           <t xml:space="preserve">Se recomienda concebir el instrumento desarrollado no como un ejercicio aislado de levantamiento de información, sino como una herramienta estratégica de uso progresivo para el fortalecimiento de la política pública del deporte en Bogotá. Su aplicación periódica y su articulación con otros sistemas de información permitirán identificar brechas, monitorear avances en la articulación institucional y ajustar intervenciones de manera gradual. En este sentido, el instrumento ofrece una base para avanzar hacia procesos de planeación, seguimiento y evaluación más coherentes, orientados al aprendizaje institucional y a la generación de valor público en el ecosistema deportivo.
 En este marco, el instrumento constituye una base para promover procesos de aprendizaje institucional, mejorar la coordinación entre actores y fortalecer la generación de valor público en el ecosistema deportivo, a partir de decisiones informadas y basadas en evidencia.
 </t>
         </is>
       </c>
-      <c r="E317" t="inlineStr"/>
-      <c r="F317" t="inlineStr"/>
-    </row>
-    <row r="318">
-      <c r="A318" t="n">
+      <c r="E338" t="inlineStr"/>
+      <c r="F338" t="inlineStr"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>119</v>
+      </c>
+      <c r="B339" t="n">
+        <v>1</v>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Balance general y experiencia del público</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El Festival de Verano 2025 presenta una valoración mayoritariamente positiva en Bogotá D.C., con satisfacción frente a la programación y a la experiencia general de participación. Como recomendación, se sugiere mantener temas logísticos que más inciden en el disfrute de la experiencia como personal de apoyo, información clara, entre otros, especialmente en escenarios de alta afluencia. </t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr"/>
+      <c r="F339" t="inlineStr"/>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>119</v>
+      </c>
+      <c r="B340" t="n">
+        <v>2</v>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>Accesibilidad, movilidad y seguridad como factores críticos</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">La evidencia indica que la experiencia no depende solo de las actividades, sino de condiciones de acceso, circulación y permanencia. Se recomienda fortalecer la gestión de movilidad (incluida la salida) y de seguridad, con medidas preventivas y coordinación interinstitucional, priorizando los puntos y franjas horarias donde se concentran los mayores flujos. </t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr"/>
+      <c r="F340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>119</v>
+      </c>
+      <c r="B341" t="n">
+        <v>3</v>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Convivencia y gestión del entorno territorial</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">En términos de convivencia, el festival es percibido como espacio favorable para el encuentro, pero la medición a vecinos y ciudadanía muestra tensiones asociadas al entorno (parqueo indebido, residuos, ruido y otras dinámicas percibidas). Se recomienda reforzar estrategias de ordenamiento, mitigación ambiental y corresponsabilidad ciudadana en zonas de influencia, para equilibrar disfrute y bienestar barrial. </t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr"/>
+      <c r="F341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>119</v>
+      </c>
+      <c r="B342" t="n">
+        <v>4</v>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>Dinámica económica local y formalización de oportunidades</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>Los resultados sugieren una activación económica asociada al festival (ingresos reportados por vendedores informales y participación de emprendimientos), aunque con comportamientos heterogéneos. Se recomienda consolidar lineamientos de participación, articulación con emprendimientos y vendedores, y mecanismos de seguimiento que permitan aprovechar mejor el potencial económico sin perder el enfoque cultural, recreativo y de espacio público del evento.</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr"/>
+      <c r="F342" t="inlineStr"/>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>120</v>
+      </c>
+      <c r="B343" t="n">
+        <v>1</v>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>Balance general de satisfacción</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">La investigación consolida resultados de la Bienal Internacional de Arte y Ciudad BOG25, el Concurso Internacional de Violín 2025 y Navidad es Cultura 2025, donde se identifica una experiencia ampliamente positiva, con altos niveles de recomendación, orgullo y disposición a regresar en futuras ediciones, lo que sugiere una aceptación sólida de los formatos en Bogotá D.C. </t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr"/>
+      <c r="F343" t="inlineStr"/>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>120</v>
+      </c>
+      <c r="B344" t="n">
+        <v>2</v>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>Aportes culturales y formativos para los públicos</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">De forma agregada, los resultados muestran que la experiencia no se limita al disfrute: una proporción alta reporta aprendizajes, descubrimiento y reflexión, así como un incremento en el interés por seguir participando en la oferta cultural. En este sentido, se destaca el descubrimiento de nuevos artistas o discursos, la reflexión provocada por las obras y la motivación para asistir a otros eventos; además, se observa un fortalecimiento del interés por la música clásica y la formación de públicos en Bogotá D.C. </t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr"/>
+      <c r="F344" t="inlineStr"/>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>120</v>
+      </c>
+      <c r="B345" t="n">
+        <v>3</v>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>Encuentro ciudadano, identidad y orgullo por Bogotá D.C.</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">En conjunto, los eventos se perciben como espacios que favorecen el encuentro social, la convivencia y el fortalecimiento de sentidos de identidad y pertenencia. Los hallazgos también muestran un componente simbólico fuerte de orgullo por Bogotá D.C. y una lectura del arte y la cultura como herramientas que pueden reunir a personas diversas y abrir conversaciones. Adicionalmente, tras la experiencia, una parte importante de asistentes reporta mayor confianza en la articulación institucional y en el uso transparente de recursos públicos. </t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr"/>
+      <c r="F345" t="inlineStr"/>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>120</v>
+      </c>
+      <c r="B346" t="n">
+        <v>4</v>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>Acceso y comunicación: fortalezas y oportunidades de mejora</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>En términos generales, se reportan condiciones de participación mayoritariamente favorables, con énfasis en la accesibilidad física y la logística; sin embargo, los resultados sugieren un reto claro en comunicación previa (cuando una proporción de asistentes percibe información poco clara o confusa) y, en eventos desarrollados en espacio público, la mediación puede reforzarse para que más personas identifiquen que lo que observan hace parte del evento. En síntesis, el balance operativo es positivo, pero hay margen para fortalecer divulgación y mediación para ampliar alcance y mejorar la experiencia.</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr"/>
+      <c r="F346" t="inlineStr"/>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
         <v>121</v>
       </c>
-      <c r="B318" t="n">
+      <c r="B347" t="n">
         <v>4</v>
       </c>
-      <c r="C318" t="inlineStr">
+      <c r="C347" t="inlineStr">
         <is>
           <t>Mucho orgullo, confianza aún frágil</t>
         </is>
       </c>
-      <c r="D318" t="inlineStr">
+      <c r="D347" t="inlineStr">
         <is>
           <t>La encuesta muestra un considerable orgullo por Bogotá, pero una confianza interpersonal limitada: la mayoría dice poder confiar en menos de la mitad de las personas. Esta brecha sugiere que el sentido de pertenencia no se traduce automáticamente en cooperación cotidiana. Para cerrarla, los laboratorios deben priorizar mediaciones comunitarias, pedagogía de cuidado del espacio público y acciones que incrementen encuentros repetidos y seguros entre vecinos. Deporte, juego y arte son palancas idóneas para “hacer juntos” con bajas barreras de entrada. Medir confianza barrial antes y después de cada ciclo permitirá verificar si las intervenciones logran convertir orgullo en vínculos efectivos.</t>
         </is>
       </c>
-      <c r="E318" t="inlineStr"/>
-      <c r="F318" t="inlineStr"/>
-    </row>
-    <row r="319">
-      <c r="A319" t="n">
+      <c r="E347" t="inlineStr"/>
+      <c r="F347" t="inlineStr"/>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
         <v>121</v>
       </c>
-      <c r="B319" t="n">
+      <c r="B348" t="n">
         <v>5</v>
       </c>
-      <c r="C319" t="inlineStr">
+      <c r="C348" t="inlineStr">
         <is>
           <t>Gobernanza compartida con palancas culturales</t>
         </is>
       </c>
-      <c r="D319" t="inlineStr">
+      <c r="D348" t="inlineStr">
         <is>
           <t>Los hallazgos apuntan a corresponsabilidad distribuida: fuerza pública, entidades distritales, vecinos y JAL son percibidos como actores clave según el tipo de problema. Esta lectura respalda una gobernanza compartida, con roles claros y coordinación por barrio, donde cultura ciudadana, bibliotecas y arte urbano actúan como catalizadores. La priorización debe enfocarse en inseguridad y basuras, conectando intervenciones de seguridad situacional con cuidado del entorno y gestión de residuos. Diseñar participación flexible (horarios extendidos, micro-tareas, reconocimiento simbólico) reduce barreras para ese tercio que no puede involucrarse. Con tableros de seguimiento por barrio, la estrategia podrá iterar con evidencia y escalar lo que funciona.</t>
         </is>
       </c>
-      <c r="E319" t="inlineStr"/>
-      <c r="F319" t="inlineStr"/>
-    </row>
-    <row r="320">
-      <c r="A320" t="n">
+      <c r="E348" t="inlineStr"/>
+      <c r="F348" t="inlineStr"/>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>128</v>
+      </c>
+      <c r="B349" t="n">
+        <v>1</v>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>Un instrumento que lee el oficio como economía cultural</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>El nuevo formulario no solo recoge información: reconstruye la lógica productiva del oficio artesanal. Aunque mantiene seis ejes estructurales (sociodemografía, identificación, elaboración, comercialización, valor patrimonial y consentimiento), incorpora variables que permiten entender al artesano como unidad productiva inserta en dinámicas territoriales y de mercado.</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr"/>
+      <c r="F349" t="inlineStr"/>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>128</v>
+      </c>
+      <c r="B350" t="n">
+        <v>2</v>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>Georreferenciación: el espacio público como territorio productivo</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>La incorporación de georreferenciación de puntos de elaboración y venta, junto con la identificación de tipos de espacios (públicos y privados), convierte el instrumento en una herramienta de análisis territorial. Esta información permite mapear las dinámicas reales de ocupación económica del espacio público, identificar concentraciones, circuitos y patrones de uso, y generar insumos estratégicos para la gestión urbana y la toma de decisiones sobre regulación y permisos.</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr"/>
+      <c r="F350" t="inlineStr"/>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>128</v>
+      </c>
+      <c r="B351" t="n">
+        <v>3</v>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>Hacedores, creadores y comercializadores: una tipología para entender el rol de los artesanos en la cadena de valor</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>La introducción de preguntas sobre rol principal frente a las piezas, etapas del proceso en las que se participa y vínculo con la venta permitió construir una clasificación en cuatro categorías: hacedor/a, hacedor/a‑comercializador/a, creador/a y comercializador/a. Esta tipología, basada en una definición de artesano que articula medio de vida, expresión cultural y dominio técnico, ofrece un insumo clave para orientar estrategias diferenciadas de formación, visibilización y fortalecimiento según el lugar que cada persona ocupa en la cadena de valor artesanal</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr"/>
+      <c r="F351" t="inlineStr"/>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
         <v>133</v>
       </c>
-      <c r="B320" t="n">
+      <c r="B352" t="n">
         <v>1</v>
       </c>
-      <c r="C320" t="inlineStr">
+      <c r="C352" t="inlineStr">
         <is>
           <t>La violencia sexual no es un desvío, es un mandato aprendido</t>
         </is>
       </c>
-      <c r="D320" t="inlineStr">
+      <c r="D352" t="inlineStr">
         <is>
           <t>La investigación evidencia que la violencia sexual no aparece como un hecho aislado o accidental, sino como una expresión coherente de la masculinidad hegemónica aprendida en distintos entornos sociales. El ejercicio de la violencia se asocia a expectativas de poder, control, dominación y validación identitaria masculina. Estas prácticas son reforzadas por la familia, los pares, los medios y, en ocasiones, por la ausencia de una educación sexual integral. La violencia se convierte así en un mecanismo para “demostrar hombría”, más que en una desviación individual.</t>
         </is>
       </c>
-      <c r="E320" t="inlineStr"/>
-      <c r="F320" t="inlineStr"/>
-    </row>
-    <row r="321">
-      <c r="A321" t="n">
+      <c r="E352" t="inlineStr"/>
+      <c r="F352" t="inlineStr"/>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
         <v>133</v>
       </c>
-      <c r="B321" t="n">
+      <c r="B353" t="n">
         <v>2</v>
       </c>
-      <c r="C321" t="inlineStr">
+      <c r="C353" t="inlineStr">
         <is>
           <t>El hogar es el principal escenario de riesgo y silenciamiento</t>
         </is>
       </c>
-      <c r="D321" t="inlineStr">
+      <c r="D353" t="inlineStr">
         <is>
           <t>Una proporción significativa de los hechos de violencia sexual ocurre en la vivienda y es ejercida por personas cercanas a la víctima. El entorno familiar, lejos de ser siempre un espacio protector, puede funcionar como un escenario de encubrimiento, negación o minimización del daño. Esta dinámica dificulta la denuncia, la intervención temprana y la activación de rutas de protección. La naturalización del abuso dentro del hogar refuerza el silencio y perpetúa la violencia.</t>
         </is>
       </c>
-      <c r="E321" t="inlineStr"/>
-      <c r="F321" t="inlineStr"/>
-    </row>
-    <row r="322">
-      <c r="A322" t="n">
+      <c r="E353" t="inlineStr"/>
+      <c r="F353" t="inlineStr"/>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
         <v>133</v>
       </c>
-      <c r="B322" t="n">
+      <c r="B354" t="n">
         <v>3</v>
       </c>
-      <c r="C322" t="inlineStr">
+      <c r="C354" t="inlineStr">
         <is>
           <t>Negar, minimizar y justificar: la principal barrera para la responsabilidad</t>
         </is>
       </c>
-      <c r="D322" t="inlineStr">
+      <c r="D354" t="inlineStr">
         <is>
           <t>Tanto los ofensores como sus familias tienden a negar, minimizar o justificar la violencia sexual, lo que constituye una barrera estructural para los procesos de responsabilización y reparación. Estas narrativas desplazan la culpa hacia las víctimas, apelan a la cercanía afectiva o normalizan el abuso como “error” o “juego”. Esta falta de reconocimiento del daño limita la efectividad de las sanciones y de los procesos restaurativos. Sin responsabilidad no hay transformación posible.</t>
         </is>
       </c>
-      <c r="E322" t="inlineStr"/>
-      <c r="F322" t="inlineStr"/>
-    </row>
-    <row r="323">
-      <c r="A323" t="n">
+      <c r="E354" t="inlineStr"/>
+      <c r="F354" t="inlineStr"/>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
         <v>133</v>
       </c>
-      <c r="B323" t="n">
+      <c r="B355" t="n">
         <v>4</v>
       </c>
-      <c r="C323" t="inlineStr">
+      <c r="C355" t="inlineStr">
         <is>
           <t>La sexualidad se aprende sin consentimiento ni empatía</t>
         </is>
       </c>
-      <c r="D323" t="inlineStr">
+      <c r="D355" t="inlineStr">
         <is>
           <t>Los hallazgos muestran que muchos jóvenes adquieren conocimientos sobre sexualidad a través de pares, pornografía y medios, sin mediación crítica ni enfoque ético. Esto produce ideas distorsionadas sobre el consentimiento, la reciprocidad y el deseo, normalizando la cosificación y la dominación. La ausencia de educación sexual integral favorece prácticas sexuales violentas y dificulta el desarrollo de empatía hacia las víctimas. La sexualidad se configura más como ejercicio de poder que como relación.</t>
         </is>
       </c>
-      <c r="E323" t="inlineStr"/>
-      <c r="F323" t="inlineStr"/>
-    </row>
-    <row r="324">
-      <c r="A324" t="n">
+      <c r="E355" t="inlineStr"/>
+      <c r="F355" t="inlineStr"/>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
         <v>133</v>
       </c>
-      <c r="B324" t="n">
+      <c r="B356" t="n">
         <v>5</v>
       </c>
-      <c r="C324" t="inlineStr">
+      <c r="C356" t="inlineStr">
         <is>
           <t>Transformar las masculinidades es clave para prevenir la violencia</t>
         </is>
       </c>
-      <c r="D324" t="inlineStr">
+      <c r="D356" t="inlineStr">
         <is>
           <t>La erradicación de la violencia sexual requiere intervenir directamente en la construcción social de las masculinidades. El estudio muestra que trabajar únicamente sobre las víctimas o desde una lógica punitiva es insuficiente. Se necesitan estrategias preventivas, educativas, culturales y restaurativas que involucren activamente a los hombres, desde la infancia hasta la adultez. Promover masculinidades no violentas es una condición central para la justicia, la convivencia y la transformación cultural.</t>
         </is>
       </c>
-      <c r="E324" t="inlineStr"/>
-      <c r="F324" t="inlineStr"/>
+      <c r="E356" t="inlineStr"/>
+      <c r="F356" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update investigaciones, pendientes Sector Cultura, LauLozV2
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -1070,7 +1070,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Caracterización de la oferta cultural en horarios no convencionales, con énfasis en públicos, franjas horarias e impactos. Incluye un módulo sobre estímulos e hitos 24/7 del sector.
+          <t xml:space="preserve">Caracterización de la oferta y demanda cultural en horarios no convencionales, con énfasis en públicos, franjas horarias e impactos. Incluye un módulo sobre estímulos e hitos 24/7 del sector.
 </t>
         </is>
       </c>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Caracterizar las percepciones, prácticas y valoraciones de la ciudadanía frente a los Festivales al Parque, mediante técnicas cualitativas y cuantitativas, con especial énfasis en los 30 años de Rock al Parque.</t>
+          <t>La investigación se orienta a la caracterización de públicos y al análisis de percepciones asociadas a los eventos culturales de gran formato de Idartes, con el fin de evaluar los impactos culturales, sociales y económicos de los Festivales al Parque. El estudio analiza la composición y perfiles de asistencia, los niveles de satisfacción, los patrones de consumo, la percepción de marca y los aportes de los festivales al posicionamiento de Bogotá como ciudad de grandes eventos. Los resultados constituyen insumos estratégicos para la toma de decisiones, el fortalecimiento de la oferta cultural y la proyección de la ciudad a nivel nacional e internacional.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1697,12 +1697,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Noche de Museos y Noche Iberoamericana de Museos</t>
+          <t>Medición de eventos culturales de gran formato del IDPC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Investigación dirigida a caracterizar los públicos y recoger percepciones sobre los eventos culturales de gran formato del IDPC, incluyendo la Noche de Museos, la Noche Iberoamericana de Museos y el Festival de Patrimonios en Ruana.</t>
+          <t>La investigación se orienta a la caracterización de públicos y al análisis de percepciones asociadas a los eventos culturales de gran formato del IDPC, con el fin de evaluar los impactos culturales, sociales y económicos de la Noche de Museos, la Noche Iberoamericana de Museos y el Festival de Patrimonios en Ruana. El estudio analiza la composición y perfiles de asistencia, los niveles de satisfacción, los patrones de consumo, la percepción de marca y los aportes de los festivales al posicionamiento de Bogotá como ciudad de grandes eventos. Los resultados constituyen insumos estratégicos para la toma de decisiones, el fortalecimiento de la oferta cultural y la proyección de la ciudad a nivel nacional e internacional.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Evaluar el impacto cultural, social y económico de los principales eventos de gran formato organizados por la SCRD, incluyendo el Concurso Internacional de Violín, la Feria de Navidad, el Encuentro de Cultura en Iberoamérica y la Bienal de Arte y Ciudad.</t>
+          <t>La investigación se orienta a la caracterización de públicos y al análisis de percepciones asociadas a los eventos culturales de gran formato organizados por la SCRD con el fin de evaluar los impactos culturales, sociales y económicos del Concurso Internacional de Violín, la Feria de Navidad, el Encuentro de Cultura en Iberoamérica y la Bienal de Arte y Ciudad. El estudio analiza la composición y perfiles de asistencia, los niveles de satisfacción, los patrones de consumo, la percepción de marca y los aportes de los festivales al posicionamiento de Bogotá como ciudad de grandes eventos. Los resultados constituyen insumos estratégicos para la toma de decisiones, el fortalecimiento de la oferta cultural y la proyección de la ciudad a nivel nacional e internacional.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Evaluar los impactos culturales, sociales y económicos del Festival de Verano, incluyendo la caracterización de públicos, satisfacción, consumo, percepción de marca y aportes al posicionamiento de Bogotá como ciudad de grandes eventos.
+          <t xml:space="preserve">La investigación se orienta a la caracterización de públicos y al análisis de percepciones asociadas a los eventos culturales de gran formato del IDRD, con el fin de evaluar los impactos culturales, sociales y económicos del Festival de Verano. El estudio analiza la composición y perfiles de asistencia, los niveles de satisfacción, los patrones de consumo, la percepción de marca y los aportes de los festivales al posicionamiento de Bogotá como ciudad de grandes eventos. Los resultados constituyen insumos estratégicos para la toma de decisiones, el fortalecimiento de la oferta cultural y la proyección de la ciudad a nivel nacional e internacional.
 </t>
         </is>
       </c>
@@ -20083,7 +20083,7 @@
       </c>
       <c r="D550" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Sí</t>
         </is>
       </c>
       <c r="E550" t="inlineStr">
@@ -20660,7 +20660,7 @@
       </c>
       <c r="E578" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1H-gGZzkXd1x4NUFnUjlHJsbv2SNMHxa3/view?usp=drive_link</t>
+          <t>https://drive.google.com/file/d/1zSXYH6cCKPEoIcuur0PuPncZ0IaOLo8E/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -20743,10 +20743,26 @@
       <c r="A582" t="n">
         <v>104</v>
       </c>
-      <c r="B582" t="inlineStr"/>
-      <c r="C582" t="inlineStr"/>
-      <c r="D582" t="inlineStr"/>
-      <c r="E582" t="inlineStr"/>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>Formularios Festival Monumentum 2025</t>
+        </is>
+      </c>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E582" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1f8Q-GMDfGsdYbhOeIsTIlHRfCnQpw8vh/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="583">
       <c r="A583" t="n">
@@ -20979,10 +20995,26 @@
       <c r="A594" t="n">
         <v>106</v>
       </c>
-      <c r="B594" t="inlineStr"/>
-      <c r="C594" t="inlineStr"/>
-      <c r="D594" t="inlineStr"/>
-      <c r="E594" t="inlineStr"/>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>Formularios Premio Luis Caballero 2025</t>
+        </is>
+      </c>
+      <c r="D594" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E594" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1tA-OMX6rjr4wNMQ0GIEXPrZ_v1L66jet/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="595">
       <c r="A595" t="n">
@@ -21004,12 +21036,28 @@
     </row>
     <row r="597">
       <c r="A597" t="n">
-        <v>106</v>
-      </c>
-      <c r="B597" t="inlineStr"/>
-      <c r="C597" t="inlineStr"/>
-      <c r="D597" t="inlineStr"/>
-      <c r="E597" t="inlineStr"/>
+        <v>108</v>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Presentación</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>Presentación resultados Festivales al Parque 2025</t>
+        </is>
+      </c>
+      <c r="D597" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E597" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1ju-2pVTUW2-guIgxcUm7FLAnb1yNjvGX/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="598">
       <c r="A598" t="n">
@@ -21207,7 +21255,7 @@
       </c>
       <c r="E605" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1Lcu0iYLFoiXHMX8f8ivPgJPF5XDn-IYx?usp=drive_link</t>
+          <t>https://drive.google.com/drive/folders/1Lcu0iYLFoiXHMX8f8ivPgJPF5XDn-IYx?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21232,7 +21280,7 @@
       </c>
       <c r="E606" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1rccxA6SFUSsKbjgRKqWnvEbok0SpWS9t?usp=drive_link</t>
+          <t>https://drive.google.com/drive/folders/1rccxA6SFUSsKbjgRKqWnvEbok0SpWS9t?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21257,7 +21305,7 @@
       </c>
       <c r="E607" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1BchZfxR7zuYYbkgIH8qE8fdgQ1y1EYZk?usp=drive_link</t>
+          <t>https://drive.google.com/drive/folders/1BchZfxR7zuYYbkgIH8qE8fdgQ1y1EYZk?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21282,7 +21330,7 @@
       </c>
       <c r="E608" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1HBmOWH-hQDqwj0mDiTDqlVdSUVcQkhYt?usp=drive_link</t>
+          <t>https://drive.google.com/drive/folders/1HBmOWH-hQDqwj0mDiTDqlVdSUVcQkhYt?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21307,7 +21355,7 @@
       </c>
       <c r="E609" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1SSz2sXnITpz_lT4g5-n2AR3M8Ed3LsnM?usp=drive_link</t>
+          <t>https://drive.google.com/drive/folders/1SSz2sXnITpz_lT4g5-n2AR3M8Ed3LsnM?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21418,7 +21466,7 @@
       </c>
       <c r="E616" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/14CmZAQrG8eHOh7xDTf8ypS7TweGA5Df_?usp=drive_link</t>
+          <t>https://drive.google.com/drive/folders/14CmZAQrG8eHOh7xDTf8ypS7TweGA5Df_?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21443,7 +21491,7 @@
       </c>
       <c r="E617" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/19PXuTzH3C_Nfl5Gj8LO1_XHUgBfjb4b4?usp=drive_link</t>
+          <t>https://drive.google.com/drive/folders/19PXuTzH3C_Nfl5Gj8LO1_XHUgBfjb4b4?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21468,7 +21516,7 @@
       </c>
       <c r="E618" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1DwWfpUiZRNgalk9jBxS-hFLcAWPqdcap?usp=drive_link</t>
+          <t>https://drive.google.com/drive/folders/1DwWfpUiZRNgalk9jBxS-hFLcAWPqdcap?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21478,12 +21526,12 @@
       </c>
       <c r="B619" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C619" t="inlineStr">
         <is>
-          <t>Informe Festival Patrimonios en Ruana 2025</t>
+          <t>Productos finales Festival Patrimonios en Ruana 2025</t>
         </is>
       </c>
       <c r="D619" t="inlineStr">
@@ -21493,7 +21541,7 @@
       </c>
       <c r="E619" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1wvZVJDVHbqK5dHnGP3YmZgPAUOh17Dxg/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/11bbVLTsTRBTvuwOBfs-eO66V-l-ZCh3_?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21503,12 +21551,12 @@
       </c>
       <c r="B620" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C620" t="inlineStr">
         <is>
-          <t>Informe Noche de Museos 2025</t>
+          <t>Productos finales Noche de Museos 2025</t>
         </is>
       </c>
       <c r="D620" t="inlineStr">
@@ -21518,7 +21566,7 @@
       </c>
       <c r="E620" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1pFLvJdEzUI-VNyrHRMUQCrJQpZAkapIx/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/10FyRwNotpVpQk4mvg9tOUyDOFYRDlXA3?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21526,51 +21574,19 @@
       <c r="A621" t="n">
         <v>110</v>
       </c>
-      <c r="B621" t="inlineStr">
-        <is>
-          <t>Presentación</t>
-        </is>
-      </c>
-      <c r="C621" t="inlineStr">
-        <is>
-          <t>Presentación Festival Patrimonios en Ruana 2025</t>
-        </is>
-      </c>
-      <c r="D621" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="E621" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1CaHBM28hdOyauLNWrACrgLpvdPbUDqch/view?usp=sharing</t>
-        </is>
-      </c>
+      <c r="B621" t="inlineStr"/>
+      <c r="C621" t="inlineStr"/>
+      <c r="D621" t="inlineStr"/>
+      <c r="E621" t="inlineStr"/>
     </row>
     <row r="622">
       <c r="A622" t="n">
         <v>110</v>
       </c>
-      <c r="B622" t="inlineStr">
-        <is>
-          <t>Presentación</t>
-        </is>
-      </c>
-      <c r="C622" t="inlineStr">
-        <is>
-          <t>Presentación Noche de Museos 2025</t>
-        </is>
-      </c>
-      <c r="D622" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="E622" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1CaHBM28hdOyauLNWrACrgLpvdPbUDqch/view?usp=sharing</t>
-        </is>
-      </c>
+      <c r="B622" t="inlineStr"/>
+      <c r="C622" t="inlineStr"/>
+      <c r="D622" t="inlineStr"/>
+      <c r="E622" t="inlineStr"/>
     </row>
     <row r="623">
       <c r="A623" t="n">
@@ -22581,7 +22597,7 @@
       </c>
       <c r="E670" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1mTOdJ3SeDN8tW2UEmwBNQ1ineXgoHsou/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/1-uaRSsIb95aqNSXjLDLMJG0a-OjealWM/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -22589,10 +22605,26 @@
       <c r="A671" t="n">
         <v>119</v>
       </c>
-      <c r="B671" t="inlineStr"/>
-      <c r="C671" t="inlineStr"/>
-      <c r="D671" t="inlineStr"/>
-      <c r="E671" t="inlineStr"/>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Instrumento recolección</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>Formularios Festival de Verano 2025</t>
+        </is>
+      </c>
+      <c r="D671" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E671" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1mDfyDNhmr4Y0uawfGhle1_DlUiM9H9oU/view?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="672">
       <c r="A672" t="n">
@@ -22636,12 +22668,12 @@
       </c>
       <c r="B676" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C676" t="inlineStr">
         <is>
-          <t>Informe Concurso Internacional de Violín 2025</t>
+          <t>Productos finales Concurso Internacional de Violín 2025</t>
         </is>
       </c>
       <c r="D676" t="inlineStr">
@@ -22651,7 +22683,7 @@
       </c>
       <c r="E676" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1om-sh_zxWJhBidcMWVCsb1psSg8gwLXr/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/114QuIa8ZzjC_GNjRUVggtFVTN3y_zOAL?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -22661,12 +22693,12 @@
       </c>
       <c r="B677" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C677" t="inlineStr">
         <is>
-          <t>Informe Bienal Internacional de Arte y Ciudad BOG25</t>
+          <t>Productos finales Bienal Internacional de Arte y Ciudad BOG25</t>
         </is>
       </c>
       <c r="D677" t="inlineStr">
@@ -22676,7 +22708,7 @@
       </c>
       <c r="E677" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/19W6ZP0kAGHIjQJfGd3cAnFvG1Cmo4qtu/view?usp=sharing</t>
+          <t>https://drive.google.com/drive/folders/17Bi6a6nKxYmJNqTEWtIH6lYiXMxIECYi?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -23774,7 +23806,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F356"/>
+  <dimension ref="A1:F360"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29421,164 +29453,164 @@
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B311" t="n">
         <v>1</v>
       </c>
       <c r="C311" t="inlineStr">
         <is>
+          <t>Experiencia y calidad artística como eje de satisfacción</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>En los ocho Festivales al Parque 2025, el balance general converge en una valoración muy favorable de la experiencia, donde el disfrute del espectáculo, la calidad artística y la programación aparecen como el principal motor de satisfacción y como el rasgo que sostiene la reputación de los eventos. En conjunto, los eventos se consolidan como plataformas culturales del Distrito que ofrecen experiencias significativas en espacio público, con una percepción positiva sobre la organización y logística, reforzando su carácter emblemático dentro de la vida cultural de Bogotá D.C.</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr"/>
+      <c r="F311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>108</v>
+      </c>
+      <c r="B312" t="n">
+        <v>2</v>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Renovación y fidelización de públicos</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Los resultados muestran una dinámica consistente de públicos mixtos con personas que asisten por primera vez y que conviven con asistentes recurrentes, lo que sugiere simultáneamente capacidad de ampliar audiencias y de fidelizar comunidades culturales ya formadas. Esta combinación refuerza el rol de los festivales como puerta de entrada a la oferta cultural distrital y, al mismo tiempo, como un circuito de permanencia donde se sostienen trayectorias de participación. Además, se reconoce que la experiencia del evento tiende a motivar a los asistentes a explorar otras actividades culturales de la ciudad.</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr"/>
+      <c r="F312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>108</v>
+      </c>
+      <c r="B313" t="n">
+        <v>3</v>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Comunidad, convivencia e inclusión</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">De manera transversal, los festivales son percibidos como espacios de encuentro ciudadano que favorecen la convivencia y el reconocimiento mutuo entre públicos diversos. Sumado al componente musical, resalta la capacidad de los Festivales al Parque para activar vínculos sociales, fortalecer sentidos de pertenencia y producir experiencias colectivas en torno a prácticas culturales compartidas. </t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr"/>
+      <c r="F313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>108</v>
+      </c>
+      <c r="B314" t="n">
+        <v>4</v>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Identidad y orgullo por Bogotá D.C.</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Se identifica una relación entre los festivales y el fortalecimiento de la identidad cultural, tanto por el reconocimiento musical y de expresiones artísticas, como por la apropiación simbólica del espacio público, lo cual se traduce en percepciones favorables de orgullo por la ciudad y por su oferta cultural. De manera complementaria, se observan valoraciones menos homogéneas en lo que respecta a la confianza institucional y algunos componentes de la experiencia urbana, lo que sugiere un campo claro para fortalecer el vínculo entre experiencia cultural e institucionalidad.</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr"/>
+      <c r="F314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>109</v>
+      </c>
+      <c r="B315" t="n">
+        <v>1</v>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
           <t>El Festival activa dinámicas económicas y de sosenibilidad cultural</t>
         </is>
       </c>
-      <c r="D311" t="inlineStr">
+      <c r="D315" t="inlineStr">
         <is>
           <t xml:space="preserve">Aunque el apoyo a emprendimientos culturales, la compra de productos o el intercambio con melómanos no constituyen el principal motivo de asistencia en ninguno de los escenarios, sí aparecen de manera consistente en todos ellos como motivaciones complementarias. Este patrón sugiere que el Festival Centro no solo funciona como un espacio de circulación artística, sino también como un dispositivo que contribuye a la sostenibilidad económica del ecosistema cultural, al activar prácticas de consumo cultural, visibilización de agentes y circulación de bienes simbólicos asociados a la música y las artes.
 Así, se podría seguir fortaleciendo de manera estratégica los componentes de circulación económica y visibilización de emprendimientos culturales, especialmente en aquellos escenarios con mayor afluencia y diversidad de públicos, sin desdibujar el eje artístico del Festival.
 </t>
         </is>
       </c>
-      <c r="E311" t="inlineStr"/>
-      <c r="F311" t="inlineStr"/>
-    </row>
-    <row r="312">
-      <c r="A312" t="n">
+      <c r="E315" t="inlineStr"/>
+      <c r="F315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
         <v>109</v>
       </c>
-      <c r="B312" t="n">
+      <c r="B316" t="n">
         <v>2</v>
       </c>
-      <c r="C312" t="inlineStr">
+      <c r="C316" t="inlineStr">
         <is>
           <t>El Festival no genera mayores impactos negativos en el espacio público</t>
         </is>
       </c>
-      <c r="D312" t="inlineStr">
+      <c r="D316" t="inlineStr">
         <is>
           <t xml:space="preserve">En los cuatro escenarios analizados, la percepción mayoritaria de los asistentes indica que la realización del Festival no modifica sustancialmente problemáticas asociadas al espacio público, como el arrojo de basuras, el parqueo en zonas prohibidas o la contaminación auditiva y visual. 
 Por otro lado, en algunos casos, como el Muelle de la FUGA y La Media Torta, se registra una mayor percepción de incremento en la presencia de vendedores informales o en el turismo; sin embargo, estos fenómenos coexisten con una valoración positiva del evento y no se asocian a un deterioro de la convivencia en la zona.
 </t>
         </is>
       </c>
-      <c r="E312" t="inlineStr"/>
-      <c r="F312" t="inlineStr"/>
-    </row>
-    <row r="313">
-      <c r="A313" t="n">
+      <c r="E316" t="inlineStr"/>
+      <c r="F316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
         <v>109</v>
       </c>
-      <c r="B313" t="n">
+      <c r="B317" t="n">
         <v>3</v>
       </c>
-      <c r="C313" t="inlineStr">
+      <c r="C317" t="inlineStr">
         <is>
           <t>El Festival articula los desplazamientos, recorridos y consumos culturales en el centro</t>
         </is>
       </c>
-      <c r="D313" t="inlineStr">
+      <c r="D317" t="inlineStr">
         <is>
           <t>En todos los escenarios, una proporción mayoritaria de asistentes declaró haber visitado o tener previsto visitar otros espacios del centro antes o después del evento. Los recorridos se concentraron principalmente en equipamientos culturales, cafés, restaurantes, bares, teatros, salas de arte y museos, lo que evidencia una alta capacidad del Festival para articular la oferta cultural, gastronómica y comercial del centro de Bogotá. Este comportamiento refuerza el papel del Festival Centro como dinamizador territorial y como nodo de conexión entre la programación cultural pública y otras actividades económicas y simbólicas del área.</t>
         </is>
       </c>
-      <c r="E313" t="inlineStr"/>
-      <c r="F313" t="inlineStr"/>
-    </row>
-    <row r="314">
-      <c r="A314" t="n">
+      <c r="E317" t="inlineStr"/>
+      <c r="F317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
         <v>109</v>
       </c>
-      <c r="B314" t="n">
+      <c r="B318" t="n">
         <v>4</v>
       </c>
-      <c r="C314" t="inlineStr">
+      <c r="C318" t="inlineStr">
         <is>
           <t xml:space="preserve">La oferta musical y artística es el principal motivo de asistencia
 </t>
         </is>
       </c>
-      <c r="D314" t="inlineStr">
+      <c r="D318" t="inlineStr">
         <is>
           <t>En todos los escenarios, los motivos de asistencia se concentran de manera consistente en la presencia de los grupos y artistas, el interés por conocer nuevas propuestas musicales y el reconocimiento previo de algunos de los artistas participantes. El Festival Centro opera simultáneamente como un espacio de encuentro entre artistas y sus audiencias y como una plataforma para el descubrimiento de nuevas propuestas, lo que explica la coexistencia de públicos con trayectoria en el Festival y de personas que asisten por primera vez.</t>
-        </is>
-      </c>
-      <c r="E314" t="inlineStr"/>
-      <c r="F314" t="inlineStr"/>
-    </row>
-    <row r="315">
-      <c r="A315" t="n">
-        <v>110</v>
-      </c>
-      <c r="B315" t="n">
-        <v>1</v>
-      </c>
-      <c r="C315" t="inlineStr">
-        <is>
-          <t>Balance general de la experiencia</t>
-        </is>
-      </c>
-      <c r="D315" t="inlineStr">
-        <is>
-          <t>En la Noche de Museos y el Festival Patrimonios en Ruana se observa una valoración global muy favorable por parte de los asistentes. Predominan percepciones de alta satisfacción y de calidad en la experiencia cultural, junto con una muy alta disposición a recomendar y a asistir nuevamente en futuras ediciones. En conjunto, los resultados sugieren que ambos formatos funcionan como espacios consistentes para el disfrute del patrimonio y la cultura, con capacidad de sostener la participación en el tiempo.</t>
-        </is>
-      </c>
-      <c r="E315" t="inlineStr"/>
-      <c r="F315" t="inlineStr"/>
-    </row>
-    <row r="316">
-      <c r="A316" t="n">
-        <v>110</v>
-      </c>
-      <c r="B316" t="n">
-        <v>2</v>
-      </c>
-      <c r="C316" t="inlineStr">
-        <is>
-          <t>Públicos, motivaciones y activación cultural</t>
-        </is>
-      </c>
-      <c r="D316" t="inlineStr">
-        <is>
-          <t>Los hallazgos muestran públicos con trayectorias culturales diversas y motivaciones centradas en hacer algo distinto, explorar la ciudad y acercarse a experiencias culturales específicas. La Noche de Museos destaca por su capacidad de atraer asistentes primerizos, mientras Patrimonios en Ruana combina ese componente con un público recurrente; en ambos casos, la vivencia del evento se asocia con un mayor interés por seguir participando en la oferta cultural de la ciudad.</t>
-        </is>
-      </c>
-      <c r="E316" t="inlineStr"/>
-      <c r="F316" t="inlineStr"/>
-    </row>
-    <row r="317">
-      <c r="A317" t="n">
-        <v>110</v>
-      </c>
-      <c r="B317" t="n">
-        <v>3</v>
-      </c>
-      <c r="C317" t="inlineStr">
-        <is>
-          <t>Encuentro ciudadano, identidad y orgullo por Bogotá D.C.</t>
-        </is>
-      </c>
-      <c r="D317" t="inlineStr">
-        <is>
-          <t>En ambas mediciones, los eventos aparecen como escenarios de encuentro social con percepciones mayoritarias de respeto e inclusión. Además, se reportan aportes simbólicos claros: conexión con la cultura de la ciudad, fortalecimiento de lazos sociales y comunitarios, y un sentimiento extendido de orgullo por la oferta cultural de Bogotá D.C. En conjunto, los resultados respaldan la idea de que estos eventos no solo convocan público, sino que también fortalecen sentidos compartidos de pertenencia.</t>
-        </is>
-      </c>
-      <c r="E317" t="inlineStr"/>
-      <c r="F317" t="inlineStr"/>
-    </row>
-    <row r="318">
-      <c r="A318" t="n">
-        <v>110</v>
-      </c>
-      <c r="B318" t="n">
-        <v>4</v>
-      </c>
-      <c r="C318" t="inlineStr">
-        <is>
-          <t>Condiciones de acceso, comunicación y oportunidades de mejora</t>
-        </is>
-      </c>
-      <c r="D318" t="inlineStr">
-        <is>
-          <t>La logística es bien evaluada en aspectos como señalización, apoyo al público y organización general; aun así, el transporte, la movilidad y la seguridad aparecen como factores determinantes para facilitar la asistencia y mejorar la experiencia. En términos de comunicación, Noche de Museos se apoya más en canales digitales, mientras Patrimonios en Ruana depende más del voz a voz, lo que abre una oportunidad para fortalecer la divulgación sin perder el componente comunitario. También se identifican mejoras puntuales en accesibilidad para personas con discapacidad y en temas logísticos asociados al desplazamiento.</t>
         </is>
       </c>
       <c r="E318" t="inlineStr"/>
@@ -29586,100 +29618,100 @@
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B319" t="n">
         <v>1</v>
       </c>
       <c r="C319" t="inlineStr">
         <is>
+          <t>Balance general de la experiencia</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>En la Noche de Museos y el Festival Patrimonios en Ruana se observa una valoración global muy favorable por parte de los asistentes. Predominan percepciones de alta satisfacción y de calidad en la experiencia cultural, junto con una muy alta disposición a recomendar y a asistir nuevamente en futuras ediciones. En conjunto, los resultados sugieren que ambos formatos funcionan como espacios consistentes para el disfrute del patrimonio y la cultura, con capacidad de sostener la participación en el tiempo.</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr"/>
+      <c r="F319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>110</v>
+      </c>
+      <c r="B320" t="n">
+        <v>2</v>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Públicos, motivaciones y activación cultural</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Los hallazgos muestran públicos con trayectorias culturales diversas y motivaciones centradas en hacer algo distinto, explorar la ciudad y acercarse a experiencias culturales específicas. La Noche de Museos destaca por su capacidad de atraer asistentes primerizos, mientras Patrimonios en Ruana combina ese componente con un público recurrente; en ambos casos, la vivencia del evento se asocia con un mayor interés por seguir participando en la oferta cultural de la ciudad.</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr"/>
+      <c r="F320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>110</v>
+      </c>
+      <c r="B321" t="n">
+        <v>3</v>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Encuentro ciudadano, identidad y orgullo por Bogotá D.C.</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>En ambas mediciones, los eventos aparecen como escenarios de encuentro social con percepciones mayoritarias de respeto e inclusión. Además, se reportan aportes simbólicos claros: conexión con la cultura de la ciudad, fortalecimiento de lazos sociales y comunitarios, y un sentimiento extendido de orgullo por la oferta cultural de Bogotá D.C. En conjunto, los resultados respaldan la idea de que estos eventos no solo convocan público, sino que también fortalecen sentidos compartidos de pertenencia.</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr"/>
+      <c r="F321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>110</v>
+      </c>
+      <c r="B322" t="n">
+        <v>4</v>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>Condiciones de acceso, comunicación y oportunidades de mejora</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>La logística es bien evaluada en aspectos como señalización, apoyo al público y organización general; aun así, el transporte, la movilidad y la seguridad aparecen como factores determinantes para facilitar la asistencia y mejorar la experiencia. En términos de comunicación, Noche de Museos se apoya más en canales digitales, mientras Patrimonios en Ruana depende más del voz a voz, lo que abre una oportunidad para fortalecer la divulgación sin perder el componente comunitario. También se identifican mejoras puntuales en accesibilidad para personas con discapacidad y en temas logísticos asociados al desplazamiento.</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr"/>
+      <c r="F322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>112</v>
+      </c>
+      <c r="B323" t="n">
+        <v>1</v>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
           <t xml:space="preserve">Naturaleza de la creación colectiva
 </t>
         </is>
       </c>
-      <c r="D319" t="inlineStr">
+      <c r="D323" t="inlineStr">
         <is>
           <t>La creación colectiva se caracteriza por su profunda vocación de horizontalidad, solidaridad y libertad. Más que centrarse en la obtención de un producto final, privilegia el proceso como un espacio vivo de exploración, diálogo y construcción conjunta. En este sentido, se configura como un ejercicio humano y político que desafía las jerarquías tradicionales, redistribuye el poder creativo y habilita formas alternativas de relación y producción cultural.</t>
-        </is>
-      </c>
-      <c r="E319" t="inlineStr"/>
-      <c r="F319" t="inlineStr"/>
-    </row>
-    <row r="320">
-      <c r="A320" t="n">
-        <v>112</v>
-      </c>
-      <c r="B320" t="n">
-        <v>2</v>
-      </c>
-      <c r="C320" t="inlineStr">
-        <is>
-          <t>Metodologías, roles y autoría</t>
-        </is>
-      </c>
-      <c r="D320" t="inlineStr">
-        <is>
-          <t>En los procesos de creación colectiva, las metodologías se construyen desde la participación activa y la co-decisión. Los roles no se imponen de antemano, sino que emergen en función de las necesidades y momentos del proceso, lo que promueve dinámicas más flexibles y colaborativas. El liderazgo se concibe como un acompañamiento empático y orientador, antes que como una instancia de dirección jerárquica. La dramaturgia, por su parte, surge de la investigación, la improvisación y la apertura estructural, y aunque la documentación es una herramienta valiosa, suele ser poco sistemática debido a la naturaleza orgánica del trabajo.</t>
-        </is>
-      </c>
-      <c r="E320" t="inlineStr"/>
-      <c r="F320" t="inlineStr"/>
-    </row>
-    <row r="321">
-      <c r="A321" t="n">
-        <v>112</v>
-      </c>
-      <c r="B321" t="n">
-        <v>3</v>
-      </c>
-      <c r="C321" t="inlineStr">
-        <is>
-          <t>Interdisciplinariedad y articulación de saberes</t>
-        </is>
-      </c>
-      <c r="D321" t="inlineStr">
-        <is>
-          <t>La creación colectiva se nutre de una integración natural y fluida de múltiples artes, oficios y conocimientos. La apertura metodológica facilita aportes espontáneos entre disciplinas y la incorporación de especialistas externos, enriqueciendo el proceso. La tecnología también se incorpora como recurso creativo y expresivo, privilegiando enfoques de cultura libre y acceso abierto, lo que amplía las posibilidades estéticas y fomenta la innovación en los lenguajes escénicos.</t>
-        </is>
-      </c>
-      <c r="E321" t="inlineStr"/>
-      <c r="F321" t="inlineStr"/>
-    </row>
-    <row r="322">
-      <c r="A322" t="n">
-        <v>112</v>
-      </c>
-      <c r="B322" t="n">
-        <v>4</v>
-      </c>
-      <c r="C322" t="inlineStr">
-        <is>
-          <t>Sostenibilidad e impacto sociocultural</t>
-        </is>
-      </c>
-      <c r="D322" t="inlineStr">
-        <is>
-          <t>La sostenibilidad de estos procesos depende, ante todo, de los vínculos humanos, la confianza entre los participantes y la claridad de un propósito común. En este modelo, la comunidad no es solo receptora, sino coproductora activa del proceso y sus resultados. Esta dinámica favorece transformaciones significativas tanto en el plano personal como en el territorial, fortaleciendo el sentido de pertenencia, la identidad colectiva y los procesos de memoria y cuidado de los territorios.</t>
-        </is>
-      </c>
-      <c r="E322" t="inlineStr"/>
-      <c r="F322" t="inlineStr"/>
-    </row>
-    <row r="323">
-      <c r="A323" t="n">
-        <v>114</v>
-      </c>
-      <c r="B323" t="n">
-        <v>1</v>
-      </c>
-      <c r="C323" t="inlineStr">
-        <is>
-          <t>La FUGA: Una biblioteca-destino</t>
-        </is>
-      </c>
-      <c r="D323" t="inlineStr">
-        <is>
-          <t>A diferencia del patrón observado en la mayoría de las bibliotecas públicas —donde predomina el uso para estudio o trabajo—, en la Biblioteca Pública FUGA el principal motivo de visita es recorrerla por primera vez (48,6%). Este valor resulta excepcionalmente alto frente al promedio general del sistema (7,9%) y pone en evidencia su carácter monumental, simbólico y turístico, así como su rol estratégico como equipamiento cultural de alto valor patrimonial en el centro histórico de Bogotá.</t>
         </is>
       </c>
       <c r="E323" t="inlineStr"/>
@@ -29687,19 +29719,19 @@
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B324" t="n">
         <v>2</v>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>Un patrón de afiliación excepcional dentro de la Red</t>
+          <t>Metodologías, roles y autoría</t>
         </is>
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>En la Biblioteca Pública Manuel Zapata Olivella – El Tintal, el segundo motivo más frecuente de visita es la afiliación o el uso de otros servicios (18,7%). Este porcentaje es significativamente superior al promedio de la Red, lo que evidencia un desempeño atípico y sugiere que las estrategias de afiliación, fidelización y acercamiento comunitario han tenido un impacto especialmente efectivo en su entorno territorial.</t>
+          <t>En los procesos de creación colectiva, las metodologías se construyen desde la participación activa y la co-decisión. Los roles no se imponen de antemano, sino que emergen en función de las necesidades y momentos del proceso, lo que promueve dinámicas más flexibles y colaborativas. El liderazgo se concibe como un acompañamiento empático y orientador, antes que como una instancia de dirección jerárquica. La dramaturgia, por su parte, surge de la investigación, la improvisación y la apertura estructural, y aunque la documentación es una herramienta valiosa, suele ser poco sistemática debido a la naturaleza orgánica del trabajo.</t>
         </is>
       </c>
       <c r="E324" t="inlineStr"/>
@@ -29707,19 +29739,19 @@
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B325" t="n">
         <v>3</v>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>La biblioteca como centro de acceso digital: El caso de Suba</t>
+          <t>Interdisciplinariedad y articulación de saberes</t>
         </is>
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>En la Biblioteca Pública Francisco José de Caldas (Suba), el uso de computadores y otros equipos tecnológicos se configura como una motivación de visita altamente relevante, alcanzando el 18,6 % de las respuestas. Esta proporción supera ampliamente el promedio general de las bibliotecas sondeadas (7,0 %), lo que evidencia una demanda territorial específica de acceso a infraestructura tecnológica y posiciona a la biblioteca como un nodo clave para la reducción de brechas digitales en la localidad.</t>
+          <t>La creación colectiva se nutre de una integración natural y fluida de múltiples artes, oficios y conocimientos. La apertura metodológica facilita aportes espontáneos entre disciplinas y la incorporación de especialistas externos, enriqueciendo el proceso. La tecnología también se incorpora como recurso creativo y expresivo, privilegiando enfoques de cultura libre y acceso abierto, lo que amplía las posibilidades estéticas y fomenta la innovación en los lenguajes escénicos.</t>
         </is>
       </c>
       <c r="E325" t="inlineStr"/>
@@ -29727,19 +29759,19 @@
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B326" t="n">
         <v>4</v>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>Desconocimiento que frena el uso de los servicios</t>
+          <t>Sostenibilidad e impacto sociocultural</t>
         </is>
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>El principal obstáculo para la vinculación de usuarios potenciales a los servicios bibliotecarios es el desconocimiento de la oferta. Entre las personas que se encuentran en los recintos pero no hacen uso de los servicios, este factor aparece de manera recurrente y con una intensidad superior al promedio del sistema. En la Biblioteca de Usaquén-Servitá, el 44,4 % de estos usuarios señala no conocer la oferta disponible, mientras que en La Peña esta proporción asciende al 50 %, cifras que superan ampliamente el promedio general (20,9 %) y evidencian una brecha crítica de información y comunicación.</t>
+          <t>La sostenibilidad de estos procesos depende, ante todo, de los vínculos humanos, la confianza entre los participantes y la claridad de un propósito común. En este modelo, la comunidad no es solo receptora, sino coproductora activa del proceso y sus resultados. Esta dinámica favorece transformaciones significativas tanto en el plano personal como en el territorial, fortaleciendo el sentido de pertenencia, la identidad colectiva y los procesos de memoria y cuidado de los territorios.</t>
         </is>
       </c>
       <c r="E326" t="inlineStr"/>
@@ -29747,19 +29779,19 @@
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B327" t="n">
         <v>1</v>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>Patrones de uso y acompañamiento social</t>
+          <t>La FUGA: Una biblioteca-destino</t>
         </is>
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Los resultados muestran que los parques estructurantes priorizados presentan patrones de uso regular, con predominio de visitas semanales y diarias. La asistencia se realiza mayoritariamente en compañía de familiares, y el horario de uso se concentra principalmente en la franja de la mañana. La práctica de deporte o actividad física es la actividad reportada con mayor frecuencia en todos los parques, seguida por usos asociados al acompañamiento y al tránsito cotidiano</t>
+          <t>A diferencia del patrón observado en la mayoría de las bibliotecas públicas —donde predomina el uso para estudio o trabajo—, en la Biblioteca Pública FUGA el principal motivo de visita es recorrerla por primera vez (48,6%). Este valor resulta excepcionalmente alto frente al promedio general del sistema (7,9%) y pone en evidencia su carácter monumental, simbólico y turístico, así como su rol estratégico como equipamiento cultural de alto valor patrimonial en el centro histórico de Bogotá.</t>
         </is>
       </c>
       <c r="E327" t="inlineStr"/>
@@ -29767,20 +29799,19 @@
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B328" t="n">
         <v>2</v>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>Valoración del estado físico y la seguridad</t>
+          <t>Un patrón de afiliación excepcional dentro de la Red</t>
         </is>
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t xml:space="preserve">La mayoría de las personas encuestadas califica el estado físico y el mantenimiento de los parques como “bueno” o “excelente”. De igual forma, una alta proporción de usuarios manifiesta sentirse segura al visitar estos espacios. No obstante, una parte de la población reporta percepciones de inseguridad, especialmente asociadas a condiciones como la iluminación, lo que coincide con los aspectos físicos señalados como susceptibles de mejora.
-</t>
+          <t>En la Biblioteca Pública Manuel Zapata Olivella – El Tintal, el segundo motivo más frecuente de visita es la afiliación o el uso de otros servicios (18,7%). Este porcentaje es significativamente superior al promedio de la Red, lo que evidencia un desempeño atípico y sugiere que las estrategias de afiliación, fidelización y acercamiento comunitario han tenido un impacto especialmente efectivo en su entorno territorial.</t>
         </is>
       </c>
       <c r="E328" t="inlineStr"/>
@@ -29788,20 +29819,19 @@
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B329" t="n">
         <v>3</v>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>Reconocimiento comunitario del parque</t>
+          <t>La biblioteca como centro de acceso digital: El caso de Suba</t>
         </is>
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t xml:space="preserve">Los parques son reconocidos por la mayoría de los usuarios como espacios importantes para su comunidad o barrio. Este reconocimiento se presenta de manera consistente en los cinco parques analizados, lo que describe el papel de estos escenarios como referentes del entorno social y del uso cotidiano del espacio público.
-</t>
+          <t>En la Biblioteca Pública Francisco José de Caldas (Suba), el uso de computadores y otros equipos tecnológicos se configura como una motivación de visita altamente relevante, alcanzando el 18,6 % de las respuestas. Esta proporción supera ampliamente el promedio general de las bibliotecas sondeadas (7,0 %), lo que evidencia una demanda territorial específica de acceso a infraestructura tecnológica y posiciona a la biblioteca como un nodo clave para la reducción de brechas digitales en la localidad.</t>
         </is>
       </c>
       <c r="E329" t="inlineStr"/>
@@ -29809,20 +29839,19 @@
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B330" t="n">
         <v>4</v>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>Diferencia entre participación reportada e interés declarado</t>
+          <t>Desconocimiento que frena el uso de los servicios</t>
         </is>
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t xml:space="preserve">Los resultados evidencian que la proporción de personas que reporta haber participado en actividades organizadas en los parques es menor que la proporción de usuarios que manifiesta interés en participar en actividades deportivas, recreativas, culturales o comunitarias. Esta diferencia describe una brecha entre la participación efectiva y la disposición declarada por la ciudadanía.
-</t>
+          <t>El principal obstáculo para la vinculación de usuarios potenciales a los servicios bibliotecarios es el desconocimiento de la oferta. Entre las personas que se encuentran en los recintos pero no hacen uso de los servicios, este factor aparece de manera recurrente y con una intensidad superior al promedio del sistema. En la Biblioteca de Usaquén-Servitá, el 44,4 % de estos usuarios señala no conocer la oferta disponible, mientras que en La Peña esta proporción asciende al 50 %, cifras que superan ampliamente el promedio general (20,9 %) y evidencian una brecha crítica de información y comunicación.</t>
         </is>
       </c>
       <c r="E330" t="inlineStr"/>
@@ -29833,16 +29862,16 @@
         <v>115</v>
       </c>
       <c r="B331" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>Barreras y condiciones para el aprovechamiento</t>
+          <t>Patrones de uso y acompañamiento social</t>
         </is>
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>La falta de tiempo es la barrera más reportada para el uso y aprovechamiento de los parques, seguida por la percepción de inseguridad y la falta de información sobre la oferta de actividades. Estas barreras se presentan en todos los parques, con variaciones en su magnitud relativa según el escenario.</t>
+          <t>Los resultados muestran que los parques estructurantes priorizados presentan patrones de uso regular, con predominio de visitas semanales y diarias. La asistencia se realiza mayoritariamente en compañía de familiares, y el horario de uso se concentra principalmente en la franja de la mañana. La práctica de deporte o actividad física es la actividad reportada con mayor frecuencia en todos los parques, seguida por usos asociados al acompañamiento y al tránsito cotidiano</t>
         </is>
       </c>
       <c r="E331" t="inlineStr"/>
@@ -29850,247 +29879,250 @@
     </row>
     <row r="332">
       <c r="A332" t="n">
+        <v>115</v>
+      </c>
+      <c r="B332" t="n">
+        <v>2</v>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Valoración del estado físico y la seguridad</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">La mayoría de las personas encuestadas califica el estado físico y el mantenimiento de los parques como “bueno” o “excelente”. De igual forma, una alta proporción de usuarios manifiesta sentirse segura al visitar estos espacios. No obstante, una parte de la población reporta percepciones de inseguridad, especialmente asociadas a condiciones como la iluminación, lo que coincide con los aspectos físicos señalados como susceptibles de mejora.
+</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr"/>
+      <c r="F332" t="inlineStr"/>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>115</v>
+      </c>
+      <c r="B333" t="n">
+        <v>3</v>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>Reconocimiento comunitario del parque</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Los parques son reconocidos por la mayoría de los usuarios como espacios importantes para su comunidad o barrio. Este reconocimiento se presenta de manera consistente en los cinco parques analizados, lo que describe el papel de estos escenarios como referentes del entorno social y del uso cotidiano del espacio público.
+</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr"/>
+      <c r="F333" t="inlineStr"/>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>115</v>
+      </c>
+      <c r="B334" t="n">
+        <v>4</v>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Diferencia entre participación reportada e interés declarado</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Los resultados evidencian que la proporción de personas que reporta haber participado en actividades organizadas en los parques es menor que la proporción de usuarios que manifiesta interés en participar en actividades deportivas, recreativas, culturales o comunitarias. Esta diferencia describe una brecha entre la participación efectiva y la disposición declarada por la ciudadanía.
+</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr"/>
+      <c r="F334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>115</v>
+      </c>
+      <c r="B335" t="n">
+        <v>5</v>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Barreras y condiciones para el aprovechamiento</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>La falta de tiempo es la barrera más reportada para el uso y aprovechamiento de los parques, seguida por la percepción de inseguridad y la falta de información sobre la oferta de actividades. Estas barreras se presentan en todos los parques, con variaciones en su magnitud relativa según el escenario.</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr"/>
+      <c r="F335" t="inlineStr"/>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
         <v>116</v>
       </c>
-      <c r="B332" t="n">
+      <c r="B336" t="n">
         <v>1</v>
       </c>
-      <c r="C332" t="inlineStr">
+      <c r="C336" t="inlineStr">
         <is>
           <t xml:space="preserve">La motivación existe. 
 Las barreras son estructurales y de contexto
 </t>
         </is>
       </c>
-      <c r="D332" t="inlineStr">
+      <c r="D336" t="inlineStr">
         <is>
           <t xml:space="preserve">Ciclovía: la mayoría sabe montar bicicleta y reconoce beneficios claros (ahorro de tiempo/dinero, autonomía).
 Escuela de la Bici: el principal obstáculo inicial no es el desinterés, sino no saber montar, la inseguridad y la falta de confianza.
 </t>
         </is>
       </c>
-      <c r="E332" t="inlineStr"/>
-      <c r="F332" t="inlineStr"/>
-    </row>
-    <row r="333">
-      <c r="A333" t="n">
+      <c r="E336" t="inlineStr"/>
+      <c r="F336" t="inlineStr"/>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
         <v>116</v>
       </c>
-      <c r="B333" t="n">
+      <c r="B337" t="n">
         <v>2</v>
       </c>
-      <c r="C333" t="inlineStr">
+      <c r="C337" t="inlineStr">
         <is>
           <t>Los programas generan percepción de impacto, pero de forma diferenciada</t>
         </is>
       </c>
-      <c r="D333" t="inlineStr">
+      <c r="D337" t="inlineStr">
         <is>
           <t>Ciclovía: alta recurrencia y masividad; impacto percibido en actividad física, motivación semanal y uso recreativo de la bicicleta.
 Escuela de la Bici: impacto percibido en aprendizaje, confianza, bienestar emocional y cambio personal, aunque con menor uso posterior por barreras materiales.</t>
         </is>
       </c>
-      <c r="E333" t="inlineStr"/>
-      <c r="F333" t="inlineStr"/>
-    </row>
-    <row r="334">
-      <c r="A334" t="n">
+      <c r="E337" t="inlineStr"/>
+      <c r="F337" t="inlineStr"/>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
         <v>116</v>
       </c>
-      <c r="B334" t="n">
+      <c r="B338" t="n">
         <v>3</v>
       </c>
-      <c r="C334" t="inlineStr">
+      <c r="C338" t="inlineStr">
         <is>
           <t>La bicicleta transforma la vida cotidiana más que la identidad colectiva</t>
         </is>
       </c>
-      <c r="D334" t="inlineStr">
+      <c r="D338" t="inlineStr">
         <is>
           <t>La sociabilidad se expresa principalmente en vínculos cercanos (familia, amigos) más que en colectivos organizados.
 El principal beneficio percibido es práctico (ahorro de tiempo/dinero, autonomía), seguido de salud y bienestar.</t>
         </is>
       </c>
-      <c r="E334" t="inlineStr"/>
-      <c r="F334" t="inlineStr"/>
-    </row>
-    <row r="335">
-      <c r="A335" t="n">
+      <c r="E338" t="inlineStr"/>
+      <c r="F338" t="inlineStr"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
         <v>117</v>
       </c>
-      <c r="B335" t="n">
+      <c r="B339" t="n">
         <v>1</v>
       </c>
-      <c r="C335" t="inlineStr">
+      <c r="C339" t="inlineStr">
         <is>
           <t>Comprender la gobernanza deportiva como un sistema complejo, multinivel y en evolución</t>
         </is>
       </c>
-      <c r="D335" t="inlineStr">
+      <c r="D339" t="inlineStr">
         <is>
           <t>Los hallazgos de esta investigación muestran que la gobernanza del deporte, la recreación y la actividad física en Bogotá debería entenderse como un sistema complejo en el que convergen actores públicos, privados, comunitarios y académicos con distintos niveles de autoridad, capacidades y responsabilidades. La revisión de literatura confirma que los modelos contemporáneos de gobernanza combinan mecanismos jerárquicos, colaborativos e híbridos, lo cual coincide con la configuración del ecosistema distrital. Esta perspectiva permite reconocer tanto el valor de las estructuras formales del Sistema Nacional del Deporte como la importancia de los vínculos territoriales, las redes sociales y las prácticas comunitarias que sostienen el funcionamiento cotidiano del sistema.</t>
         </is>
       </c>
-      <c r="E335" t="inlineStr"/>
-      <c r="F335" t="inlineStr"/>
-    </row>
-    <row r="336">
-      <c r="A336" t="n">
+      <c r="E339" t="inlineStr"/>
+      <c r="F339" t="inlineStr"/>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
         <v>117</v>
       </c>
-      <c r="B336" t="n">
+      <c r="B340" t="n">
         <v>2</v>
       </c>
-      <c r="C336" t="inlineStr">
+      <c r="C340" t="inlineStr">
         <is>
           <t>Clarificar el papel de los actores como base para mejorar la articulación y corresponsabilidad</t>
         </is>
       </c>
-      <c r="D336" t="inlineStr">
+      <c r="D340" t="inlineStr">
         <is>
           <t>Se considera necesario seguir avanzando en mecanismos que fortalezcan la corresponsabilidad entre niveles de gobierno, organizaciones deportivas, sector privado, ciudadanía y academia. La claridad en los roles y la comprensión de las relaciones entre actores son condiciones esenciales para que la política deportiva distrital evolucione hacia formas más consistentes de cooperación, planificación conjunta y toma de decisiones basada en evidencia, la tipología de actores es un punto de partida para esta definición.</t>
         </is>
       </c>
-      <c r="E336" t="inlineStr"/>
-      <c r="F336" t="inlineStr"/>
-    </row>
-    <row r="337">
-      <c r="A337" t="n">
+      <c r="E340" t="inlineStr"/>
+      <c r="F340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
         <v>117</v>
       </c>
-      <c r="B337" t="n">
+      <c r="B341" t="n">
         <v>3</v>
       </c>
-      <c r="C337" t="inlineStr">
+      <c r="C341" t="inlineStr">
         <is>
           <t>Aplicar la medición para caracterizar a los actores y fortalecer el sistema de información</t>
         </is>
       </c>
-      <c r="D337" t="inlineStr">
+      <c r="D341" t="inlineStr">
         <is>
           <t>El desarrollo de las categorías analíticas, del formulario cuantitativo y de la propuesta metodológica cualitativa constituye un insumo clave para avanzar hacia un sistema de información más sólido y útil para la toma de decisiones. La aplicación de estos instrumentos permitirá caracterizar de manera rigurosa a los actores del ecosistema deportivo y facilitará una comprensión más completa, contextualizada y accionable sobre el funcionamiento real del ecosistema deportivo y sobre las oportunidades para fortalecer su gobernanza.</t>
         </is>
       </c>
-      <c r="E337" t="inlineStr"/>
-      <c r="F337" t="inlineStr"/>
-    </row>
-    <row r="338">
-      <c r="A338" t="n">
+      <c r="E341" t="inlineStr"/>
+      <c r="F341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
         <v>117</v>
       </c>
-      <c r="B338" t="n">
+      <c r="B342" t="n">
         <v>4</v>
       </c>
-      <c r="C338" t="inlineStr">
+      <c r="C342" t="inlineStr">
         <is>
           <t>Usar el instrumento como herramienta progresiva para la mejora de la política pública</t>
         </is>
       </c>
-      <c r="D338" t="inlineStr">
+      <c r="D342" t="inlineStr">
         <is>
           <t xml:space="preserve">Se recomienda concebir el instrumento desarrollado no como un ejercicio aislado de levantamiento de información, sino como una herramienta estratégica de uso progresivo para el fortalecimiento de la política pública del deporte en Bogotá. Su aplicación periódica y su articulación con otros sistemas de información permitirán identificar brechas, monitorear avances en la articulación institucional y ajustar intervenciones de manera gradual. En este sentido, el instrumento ofrece una base para avanzar hacia procesos de planeación, seguimiento y evaluación más coherentes, orientados al aprendizaje institucional y a la generación de valor público en el ecosistema deportivo.
 En este marco, el instrumento constituye una base para promover procesos de aprendizaje institucional, mejorar la coordinación entre actores y fortalecer la generación de valor público en el ecosistema deportivo, a partir de decisiones informadas y basadas en evidencia.
 </t>
         </is>
       </c>
-      <c r="E338" t="inlineStr"/>
-      <c r="F338" t="inlineStr"/>
-    </row>
-    <row r="339">
-      <c r="A339" t="n">
-        <v>119</v>
-      </c>
-      <c r="B339" t="n">
-        <v>1</v>
-      </c>
-      <c r="C339" t="inlineStr">
-        <is>
-          <t>Balance general y experiencia del público</t>
-        </is>
-      </c>
-      <c r="D339" t="inlineStr">
-        <is>
-          <t xml:space="preserve">El Festival de Verano 2025 presenta una valoración mayoritariamente positiva en Bogotá D.C., con satisfacción frente a la programación y a la experiencia general de participación. Como recomendación, se sugiere mantener temas logísticos que más inciden en el disfrute de la experiencia como personal de apoyo, información clara, entre otros, especialmente en escenarios de alta afluencia. </t>
-        </is>
-      </c>
-      <c r="E339" t="inlineStr"/>
-      <c r="F339" t="inlineStr"/>
-    </row>
-    <row r="340">
-      <c r="A340" t="n">
-        <v>119</v>
-      </c>
-      <c r="B340" t="n">
-        <v>2</v>
-      </c>
-      <c r="C340" t="inlineStr">
-        <is>
-          <t>Accesibilidad, movilidad y seguridad como factores críticos</t>
-        </is>
-      </c>
-      <c r="D340" t="inlineStr">
-        <is>
-          <t xml:space="preserve">La evidencia indica que la experiencia no depende solo de las actividades, sino de condiciones de acceso, circulación y permanencia. Se recomienda fortalecer la gestión de movilidad (incluida la salida) y de seguridad, con medidas preventivas y coordinación interinstitucional, priorizando los puntos y franjas horarias donde se concentran los mayores flujos. </t>
-        </is>
-      </c>
-      <c r="E340" t="inlineStr"/>
-      <c r="F340" t="inlineStr"/>
-    </row>
-    <row r="341">
-      <c r="A341" t="n">
-        <v>119</v>
-      </c>
-      <c r="B341" t="n">
-        <v>3</v>
-      </c>
-      <c r="C341" t="inlineStr">
-        <is>
-          <t>Convivencia y gestión del entorno territorial</t>
-        </is>
-      </c>
-      <c r="D341" t="inlineStr">
-        <is>
-          <t xml:space="preserve">En términos de convivencia, el festival es percibido como espacio favorable para el encuentro, pero la medición a vecinos y ciudadanía muestra tensiones asociadas al entorno (parqueo indebido, residuos, ruido y otras dinámicas percibidas). Se recomienda reforzar estrategias de ordenamiento, mitigación ambiental y corresponsabilidad ciudadana en zonas de influencia, para equilibrar disfrute y bienestar barrial. </t>
-        </is>
-      </c>
-      <c r="E341" t="inlineStr"/>
-      <c r="F341" t="inlineStr"/>
-    </row>
-    <row r="342">
-      <c r="A342" t="n">
-        <v>119</v>
-      </c>
-      <c r="B342" t="n">
-        <v>4</v>
-      </c>
-      <c r="C342" t="inlineStr">
-        <is>
-          <t>Dinámica económica local y formalización de oportunidades</t>
-        </is>
-      </c>
-      <c r="D342" t="inlineStr">
-        <is>
-          <t>Los resultados sugieren una activación económica asociada al festival (ingresos reportados por vendedores informales y participación de emprendimientos), aunque con comportamientos heterogéneos. Se recomienda consolidar lineamientos de participación, articulación con emprendimientos y vendedores, y mecanismos de seguimiento que permitan aprovechar mejor el potencial económico sin perder el enfoque cultural, recreativo y de espacio público del evento.</t>
-        </is>
-      </c>
       <c r="E342" t="inlineStr"/>
       <c r="F342" t="inlineStr"/>
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B343" t="n">
         <v>1</v>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>Balance general de satisfacción</t>
+          <t>Balance general y experiencia del público</t>
         </is>
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t xml:space="preserve">La investigación consolida resultados de la Bienal Internacional de Arte y Ciudad BOG25, el Concurso Internacional de Violín 2025 y Navidad es Cultura 2025, donde se identifica una experiencia ampliamente positiva, con altos niveles de recomendación, orgullo y disposición a regresar en futuras ediciones, lo que sugiere una aceptación sólida de los formatos en Bogotá D.C. </t>
+          <t xml:space="preserve">El Festival de Verano 2025 presenta una valoración mayoritariamente positiva en Bogotá D.C., con satisfacción frente a la programación y a la experiencia general de participación. Como recomendación, se sugiere mantener temas logísticos que más inciden en el disfrute de la experiencia como personal de apoyo, información clara, entre otros, especialmente en escenarios de alta afluencia. </t>
         </is>
       </c>
       <c r="E343" t="inlineStr"/>
@@ -30098,19 +30130,19 @@
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B344" t="n">
         <v>2</v>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>Aportes culturales y formativos para los públicos</t>
+          <t>Accesibilidad, movilidad y seguridad como factores críticos</t>
         </is>
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t xml:space="preserve">De forma agregada, los resultados muestran que la experiencia no se limita al disfrute: una proporción alta reporta aprendizajes, descubrimiento y reflexión, así como un incremento en el interés por seguir participando en la oferta cultural. En este sentido, se destaca el descubrimiento de nuevos artistas o discursos, la reflexión provocada por las obras y la motivación para asistir a otros eventos; además, se observa un fortalecimiento del interés por la música clásica y la formación de públicos en Bogotá D.C. </t>
+          <t xml:space="preserve">La evidencia indica que la experiencia no depende solo de las actividades, sino de condiciones de acceso, circulación y permanencia. Se recomienda fortalecer la gestión de movilidad (incluida la salida) y de seguridad, con medidas preventivas y coordinación interinstitucional, priorizando los puntos y franjas horarias donde se concentran los mayores flujos. </t>
         </is>
       </c>
       <c r="E344" t="inlineStr"/>
@@ -30118,19 +30150,19 @@
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B345" t="n">
         <v>3</v>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>Encuentro ciudadano, identidad y orgullo por Bogotá D.C.</t>
+          <t>Convivencia y gestión del entorno territorial</t>
         </is>
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t xml:space="preserve">En conjunto, los eventos se perciben como espacios que favorecen el encuentro social, la convivencia y el fortalecimiento de sentidos de identidad y pertenencia. Los hallazgos también muestran un componente simbólico fuerte de orgullo por Bogotá D.C. y una lectura del arte y la cultura como herramientas que pueden reunir a personas diversas y abrir conversaciones. Adicionalmente, tras la experiencia, una parte importante de asistentes reporta mayor confianza en la articulación institucional y en el uso transparente de recursos públicos. </t>
+          <t xml:space="preserve">En términos de convivencia, el festival es percibido como espacio favorable para el encuentro, pero la medición a vecinos y ciudadanía muestra tensiones asociadas al entorno (parqueo indebido, residuos, ruido y otras dinámicas percibidas). Se recomienda reforzar estrategias de ordenamiento, mitigación ambiental y corresponsabilidad ciudadana en zonas de influencia, para equilibrar disfrute y bienestar barrial. </t>
         </is>
       </c>
       <c r="E345" t="inlineStr"/>
@@ -30138,19 +30170,19 @@
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B346" t="n">
         <v>4</v>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>Acceso y comunicación: fortalezas y oportunidades de mejora</t>
+          <t>Dinámica económica local y formalización de oportunidades</t>
         </is>
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>En términos generales, se reportan condiciones de participación mayoritariamente favorables, con énfasis en la accesibilidad física y la logística; sin embargo, los resultados sugieren un reto claro en comunicación previa (cuando una proporción de asistentes percibe información poco clara o confusa) y, en eventos desarrollados en espacio público, la mediación puede reforzarse para que más personas identifiquen que lo que observan hace parte del evento. En síntesis, el balance operativo es positivo, pero hay margen para fortalecer divulgación y mediación para ampliar alcance y mejorar la experiencia.</t>
+          <t>Los resultados sugieren una activación económica asociada al festival (ingresos reportados por vendedores informales y participación de emprendimientos), aunque con comportamientos heterogéneos. Se recomienda consolidar lineamientos de participación, articulación con emprendimientos y vendedores, y mecanismos de seguimiento que permitan aprovechar mejor el potencial económico sin perder el enfoque cultural, recreativo y de espacio público del evento.</t>
         </is>
       </c>
       <c r="E346" t="inlineStr"/>
@@ -30158,19 +30190,19 @@
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B347" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>Mucho orgullo, confianza aún frágil</t>
+          <t>Balance general de satisfacción</t>
         </is>
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>La encuesta muestra un considerable orgullo por Bogotá, pero una confianza interpersonal limitada: la mayoría dice poder confiar en menos de la mitad de las personas. Esta brecha sugiere que el sentido de pertenencia no se traduce automáticamente en cooperación cotidiana. Para cerrarla, los laboratorios deben priorizar mediaciones comunitarias, pedagogía de cuidado del espacio público y acciones que incrementen encuentros repetidos y seguros entre vecinos. Deporte, juego y arte son palancas idóneas para “hacer juntos” con bajas barreras de entrada. Medir confianza barrial antes y después de cada ciclo permitirá verificar si las intervenciones logran convertir orgullo en vínculos efectivos.</t>
+          <t xml:space="preserve">La investigación consolida resultados de la Bienal Internacional de Arte y Ciudad BOG25, el Concurso Internacional de Violín 2025 y Navidad es Cultura 2025, donde se identifica una experiencia ampliamente positiva, con altos niveles de recomendación, orgullo y disposición a regresar en futuras ediciones, lo que sugiere una aceptación sólida de los formatos en Bogotá D.C. </t>
         </is>
       </c>
       <c r="E347" t="inlineStr"/>
@@ -30178,19 +30210,19 @@
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B348" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>Gobernanza compartida con palancas culturales</t>
+          <t>Aportes culturales y formativos para los públicos</t>
         </is>
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>Los hallazgos apuntan a corresponsabilidad distribuida: fuerza pública, entidades distritales, vecinos y JAL son percibidos como actores clave según el tipo de problema. Esta lectura respalda una gobernanza compartida, con roles claros y coordinación por barrio, donde cultura ciudadana, bibliotecas y arte urbano actúan como catalizadores. La priorización debe enfocarse en inseguridad y basuras, conectando intervenciones de seguridad situacional con cuidado del entorno y gestión de residuos. Diseñar participación flexible (horarios extendidos, micro-tareas, reconocimiento simbólico) reduce barreras para ese tercio que no puede involucrarse. Con tableros de seguimiento por barrio, la estrategia podrá iterar con evidencia y escalar lo que funciona.</t>
+          <t xml:space="preserve">De forma agregada, los resultados muestran que la experiencia no se limita al disfrute: una proporción alta reporta aprendizajes, descubrimiento y reflexión, así como un incremento en el interés por seguir participando en la oferta cultural. En este sentido, se destaca el descubrimiento de nuevos artistas o discursos, la reflexión provocada por las obras y la motivación para asistir a otros eventos; además, se observa un fortalecimiento del interés por la música clásica y la formación de públicos en Bogotá D.C. </t>
         </is>
       </c>
       <c r="E348" t="inlineStr"/>
@@ -30198,19 +30230,19 @@
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B349" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>Un instrumento que lee el oficio como economía cultural</t>
+          <t>Encuentro ciudadano, identidad y orgullo por Bogotá D.C.</t>
         </is>
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>El nuevo formulario no solo recoge información: reconstruye la lógica productiva del oficio artesanal. Aunque mantiene seis ejes estructurales (sociodemografía, identificación, elaboración, comercialización, valor patrimonial y consentimiento), incorpora variables que permiten entender al artesano como unidad productiva inserta en dinámicas territoriales y de mercado.</t>
+          <t xml:space="preserve">En conjunto, los eventos se perciben como espacios que favorecen el encuentro social, la convivencia y el fortalecimiento de sentidos de identidad y pertenencia. Los hallazgos también muestran un componente simbólico fuerte de orgullo por Bogotá D.C. y una lectura del arte y la cultura como herramientas que pueden reunir a personas diversas y abrir conversaciones. Adicionalmente, tras la experiencia, una parte importante de asistentes reporta mayor confianza en la articulación institucional y en el uso transparente de recursos públicos. </t>
         </is>
       </c>
       <c r="E349" t="inlineStr"/>
@@ -30218,19 +30250,19 @@
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B350" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>Georreferenciación: el espacio público como territorio productivo</t>
+          <t>Acceso y comunicación: fortalezas y oportunidades de mejora</t>
         </is>
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>La incorporación de georreferenciación de puntos de elaboración y venta, junto con la identificación de tipos de espacios (públicos y privados), convierte el instrumento en una herramienta de análisis territorial. Esta información permite mapear las dinámicas reales de ocupación económica del espacio público, identificar concentraciones, circuitos y patrones de uso, y generar insumos estratégicos para la gestión urbana y la toma de decisiones sobre regulación y permisos.</t>
+          <t>En términos generales, se reportan condiciones de participación mayoritariamente favorables, con énfasis en la accesibilidad física y la logística; sin embargo, los resultados sugieren un reto claro en comunicación previa (cuando una proporción de asistentes percibe información poco clara o confusa) y, en eventos desarrollados en espacio público, la mediación puede reforzarse para que más personas identifiquen que lo que observan hace parte del evento. En síntesis, el balance operativo es positivo, pero hay margen para fortalecer divulgación y mediación para ampliar alcance y mejorar la experiencia.</t>
         </is>
       </c>
       <c r="E350" t="inlineStr"/>
@@ -30238,19 +30270,19 @@
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B351" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>Hacedores, creadores y comercializadores: una tipología para entender el rol de los artesanos en la cadena de valor</t>
+          <t>Mucho orgullo, confianza aún frágil</t>
         </is>
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>La introducción de preguntas sobre rol principal frente a las piezas, etapas del proceso en las que se participa y vínculo con la venta permitió construir una clasificación en cuatro categorías: hacedor/a, hacedor/a‑comercializador/a, creador/a y comercializador/a. Esta tipología, basada en una definición de artesano que articula medio de vida, expresión cultural y dominio técnico, ofrece un insumo clave para orientar estrategias diferenciadas de formación, visibilización y fortalecimiento según el lugar que cada persona ocupa en la cadena de valor artesanal</t>
+          <t>La encuesta muestra un considerable orgullo por Bogotá, pero una confianza interpersonal limitada: la mayoría dice poder confiar en menos de la mitad de las personas. Esta brecha sugiere que el sentido de pertenencia no se traduce automáticamente en cooperación cotidiana. Para cerrarla, los laboratorios deben priorizar mediaciones comunitarias, pedagogía de cuidado del espacio público y acciones que incrementen encuentros repetidos y seguros entre vecinos. Deporte, juego y arte son palancas idóneas para “hacer juntos” con bajas barreras de entrada. Medir confianza barrial antes y después de cada ciclo permitirá verificar si las intervenciones logran convertir orgullo en vínculos efectivos.</t>
         </is>
       </c>
       <c r="E351" t="inlineStr"/>
@@ -30258,19 +30290,19 @@
     </row>
     <row r="352">
       <c r="A352" t="n">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B352" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>La violencia sexual no es un desvío, es un mandato aprendido</t>
+          <t>Gobernanza compartida con palancas culturales</t>
         </is>
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>La investigación evidencia que la violencia sexual no aparece como un hecho aislado o accidental, sino como una expresión coherente de la masculinidad hegemónica aprendida en distintos entornos sociales. El ejercicio de la violencia se asocia a expectativas de poder, control, dominación y validación identitaria masculina. Estas prácticas son reforzadas por la familia, los pares, los medios y, en ocasiones, por la ausencia de una educación sexual integral. La violencia se convierte así en un mecanismo para “demostrar hombría”, más que en una desviación individual.</t>
+          <t>Los hallazgos apuntan a corresponsabilidad distribuida: fuerza pública, entidades distritales, vecinos y JAL son percibidos como actores clave según el tipo de problema. Esta lectura respalda una gobernanza compartida, con roles claros y coordinación por barrio, donde cultura ciudadana, bibliotecas y arte urbano actúan como catalizadores. La priorización debe enfocarse en inseguridad y basuras, conectando intervenciones de seguridad situacional con cuidado del entorno y gestión de residuos. Diseñar participación flexible (horarios extendidos, micro-tareas, reconocimiento simbólico) reduce barreras para ese tercio que no puede involucrarse. Con tableros de seguimiento por barrio, la estrategia podrá iterar con evidencia y escalar lo que funciona.</t>
         </is>
       </c>
       <c r="E352" t="inlineStr"/>
@@ -30278,19 +30310,19 @@
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B353" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>El hogar es el principal escenario de riesgo y silenciamiento</t>
+          <t>Un instrumento que lee el oficio como economía cultural</t>
         </is>
       </c>
       <c r="D353" t="inlineStr">
         <is>
-          <t>Una proporción significativa de los hechos de violencia sexual ocurre en la vivienda y es ejercida por personas cercanas a la víctima. El entorno familiar, lejos de ser siempre un espacio protector, puede funcionar como un escenario de encubrimiento, negación o minimización del daño. Esta dinámica dificulta la denuncia, la intervención temprana y la activación de rutas de protección. La naturalización del abuso dentro del hogar refuerza el silencio y perpetúa la violencia.</t>
+          <t>El nuevo formulario no solo recoge información: reconstruye la lógica productiva del oficio artesanal. Aunque mantiene seis ejes estructurales (sociodemografía, identificación, elaboración, comercialización, valor patrimonial y consentimiento), incorpora variables que permiten entender al artesano como unidad productiva inserta en dinámicas territoriales y de mercado.</t>
         </is>
       </c>
       <c r="E353" t="inlineStr"/>
@@ -30298,19 +30330,19 @@
     </row>
     <row r="354">
       <c r="A354" t="n">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B354" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>Negar, minimizar y justificar: la principal barrera para la responsabilidad</t>
+          <t>Georreferenciación: el espacio público como territorio productivo</t>
         </is>
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>Tanto los ofensores como sus familias tienden a negar, minimizar o justificar la violencia sexual, lo que constituye una barrera estructural para los procesos de responsabilización y reparación. Estas narrativas desplazan la culpa hacia las víctimas, apelan a la cercanía afectiva o normalizan el abuso como “error” o “juego”. Esta falta de reconocimiento del daño limita la efectividad de las sanciones y de los procesos restaurativos. Sin responsabilidad no hay transformación posible.</t>
+          <t>La incorporación de georreferenciación de puntos de elaboración y venta, junto con la identificación de tipos de espacios (públicos y privados), convierte el instrumento en una herramienta de análisis territorial. Esta información permite mapear las dinámicas reales de ocupación económica del espacio público, identificar concentraciones, circuitos y patrones de uso, y generar insumos estratégicos para la gestión urbana y la toma de decisiones sobre regulación y permisos.</t>
         </is>
       </c>
       <c r="E354" t="inlineStr"/>
@@ -30318,19 +30350,19 @@
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B355" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>La sexualidad se aprende sin consentimiento ni empatía</t>
+          <t>Hacedores, creadores y comercializadores: una tipología para entender el rol de los artesanos en la cadena de valor</t>
         </is>
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>Los hallazgos muestran que muchos jóvenes adquieren conocimientos sobre sexualidad a través de pares, pornografía y medios, sin mediación crítica ni enfoque ético. Esto produce ideas distorsionadas sobre el consentimiento, la reciprocidad y el deseo, normalizando la cosificación y la dominación. La ausencia de educación sexual integral favorece prácticas sexuales violentas y dificulta el desarrollo de empatía hacia las víctimas. La sexualidad se configura más como ejercicio de poder que como relación.</t>
+          <t>La introducción de preguntas sobre rol principal frente a las piezas, etapas del proceso en las que se participa y vínculo con la venta permitió construir una clasificación en cuatro categorías: hacedor/a, hacedor/a‑comercializador/a, creador/a y comercializador/a. Esta tipología, basada en una definición de artesano que articula medio de vida, expresión cultural y dominio técnico, ofrece un insumo clave para orientar estrategias diferenciadas de formación, visibilización y fortalecimiento según el lugar que cada persona ocupa en la cadena de valor artesanal</t>
         </is>
       </c>
       <c r="E355" t="inlineStr"/>
@@ -30341,20 +30373,100 @@
         <v>133</v>
       </c>
       <c r="B356" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>Transformar las masculinidades es clave para prevenir la violencia</t>
+          <t>La violencia sexual no es un desvío, es un mandato aprendido</t>
         </is>
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>La erradicación de la violencia sexual requiere intervenir directamente en la construcción social de las masculinidades. El estudio muestra que trabajar únicamente sobre las víctimas o desde una lógica punitiva es insuficiente. Se necesitan estrategias preventivas, educativas, culturales y restaurativas que involucren activamente a los hombres, desde la infancia hasta la adultez. Promover masculinidades no violentas es una condición central para la justicia, la convivencia y la transformación cultural.</t>
+          <t>La investigación evidencia que la violencia sexual no aparece como un hecho aislado o accidental, sino como una expresión coherente de la masculinidad hegemónica aprendida en distintos entornos sociales. El ejercicio de la violencia se asocia a expectativas de poder, control, dominación y validación identitaria masculina. Estas prácticas son reforzadas por la familia, los pares, los medios y, en ocasiones, por la ausencia de una educación sexual integral. La violencia se convierte así en un mecanismo para “demostrar hombría”, más que en una desviación individual.</t>
         </is>
       </c>
       <c r="E356" t="inlineStr"/>
       <c r="F356" t="inlineStr"/>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>133</v>
+      </c>
+      <c r="B357" t="n">
+        <v>2</v>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>El hogar es el principal escenario de riesgo y silenciamiento</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>Una proporción significativa de los hechos de violencia sexual ocurre en la vivienda y es ejercida por personas cercanas a la víctima. El entorno familiar, lejos de ser siempre un espacio protector, puede funcionar como un escenario de encubrimiento, negación o minimización del daño. Esta dinámica dificulta la denuncia, la intervención temprana y la activación de rutas de protección. La naturalización del abuso dentro del hogar refuerza el silencio y perpetúa la violencia.</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr"/>
+      <c r="F357" t="inlineStr"/>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>133</v>
+      </c>
+      <c r="B358" t="n">
+        <v>3</v>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>Negar, minimizar y justificar: la principal barrera para la responsabilidad</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>Tanto los ofensores como sus familias tienden a negar, minimizar o justificar la violencia sexual, lo que constituye una barrera estructural para los procesos de responsabilización y reparación. Estas narrativas desplazan la culpa hacia las víctimas, apelan a la cercanía afectiva o normalizan el abuso como “error” o “juego”. Esta falta de reconocimiento del daño limita la efectividad de las sanciones y de los procesos restaurativos. Sin responsabilidad no hay transformación posible.</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr"/>
+      <c r="F358" t="inlineStr"/>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>133</v>
+      </c>
+      <c r="B359" t="n">
+        <v>4</v>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>La sexualidad se aprende sin consentimiento ni empatía</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>Los hallazgos muestran que muchos jóvenes adquieren conocimientos sobre sexualidad a través de pares, pornografía y medios, sin mediación crítica ni enfoque ético. Esto produce ideas distorsionadas sobre el consentimiento, la reciprocidad y el deseo, normalizando la cosificación y la dominación. La ausencia de educación sexual integral favorece prácticas sexuales violentas y dificulta el desarrollo de empatía hacia las víctimas. La sexualidad se configura más como ejercicio de poder que como relación.</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr"/>
+      <c r="F359" t="inlineStr"/>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>133</v>
+      </c>
+      <c r="B360" t="n">
+        <v>5</v>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>Transformar las masculinidades es clave para prevenir la violencia</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>La erradicación de la violencia sexual requiere intervenir directamente en la construcción social de las masculinidades. El estudio muestra que trabajar únicamente sobre las víctimas o desde una lógica punitiva es insuficiente. Se necesitan estrategias preventivas, educativas, culturales y restaurativas que involucren activamente a los hombres, desde la infancia hasta la adultez. Promover masculinidades no violentas es una condición central para la justicia, la convivencia y la transformación cultural.</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr"/>
+      <c r="F360" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update investigaciones, pendientes Sector Cultura, LauLozV3
</commit_message>
<xml_diff>
--- a/content/data/investigaciones/investigaciones.xlsx
+++ b/content/data/investigaciones/investigaciones.xlsx
@@ -20038,7 +20038,7 @@
       </c>
       <c r="E548" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1V2LcYxrrvtQrwyVv-PxQ9jHBnJp-Q5lX/view?usp=drive_link</t>
+          <t>https://drive.google.com/file/d/10rcFV4zkdfiV5hJwwOk1Ns5T-GuJe4XH/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -20533,11 +20533,7 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="E573" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1QIL_a1eOSFhjpKgln0XgVpFeVcFhCG1n/view?usp=drive_link</t>
-        </is>
-      </c>
+      <c r="E573" t="inlineStr"/>
     </row>
     <row r="574">
       <c r="A574" t="n">
@@ -20685,7 +20681,7 @@
       </c>
       <c r="E579" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1zSXYH6cCKPEoIcuur0PuPncZ0IaOLo8E/view?usp=drive_link</t>
+          <t>https://drive.google.com/file/d/1tbs8mCFLp3B8oB1k6wusfvYA4GtfgQ3D/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -20710,7 +20706,7 @@
       </c>
       <c r="E580" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1VNIkQ3a3hetNE0tCChMkmlcdGIUJ_ttA/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/1UVUUqWPRqoC9-J_3rJPCiwC_FLLGKNPY/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -20735,7 +20731,7 @@
       </c>
       <c r="E581" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1xJO1lFA1uh52DD5A-mAYv6s-glGlN2jZ/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/1Xe170cnqUJe0L75fIRULax6fAtG4DoW9/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -20760,7 +20756,7 @@
       </c>
       <c r="E582" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1f8Q-GMDfGsdYbhOeIsTIlHRfCnQpw8vh/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/1gnrVe2NjozYAHQCAlLTR23iZjIlgxno0/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -20812,7 +20808,7 @@
       </c>
       <c r="E586" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1gEDdQ_9ggb2qbkisdnS3h-SixumLgwVD/view?usp=drive_link</t>
+          <t>https://drive.google.com/file/d/1vrgSbr3C0hKpepJciOdwbINqKkhfQCDx/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -20927,7 +20923,7 @@
       </c>
       <c r="C591" t="inlineStr">
         <is>
-          <t>Guía metodológica Talleres Consumo Audiovisual de Audiencias Infantiles</t>
+          <t>Guía metodológica Cartografía Social</t>
         </is>
       </c>
       <c r="D591" t="inlineStr">
@@ -20962,7 +20958,7 @@
       </c>
       <c r="E592" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1bwHUP2WQlU55fpvnMYn6gs-02lHoYDrR/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/18QKMBaJoy4nqZQlFRNYvsZzoo_sFJDIT/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -20987,7 +20983,7 @@
       </c>
       <c r="E593" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1RJzTRw-lxF_ZvQ08fhfsIohq1XHwRm7J/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/1hqNl-FukfRsmkLFkKFbhRMjbCi_keQVa/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21012,7 +21008,7 @@
       </c>
       <c r="E594" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1tA-OMX6rjr4wNMQ0GIEXPrZ_v1L66jet/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/1yzZXgr7VzlUbRtj5fNNi_JyDWjan8aNY/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -21055,7 +21051,7 @@
       </c>
       <c r="E597" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1ju-2pVTUW2-guIgxcUm7FLAnb1yNjvGX/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/1uvPcjC3VFFwdTN4LKTZqQa4dd_mt6aRq/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21105,7 +21101,7 @@
       </c>
       <c r="E599" t="inlineStr">
         <is>
-          <t>https://docs.google.com/spreadsheets/d/1B55s6qmoQu8Bya1h17h2RlICtcbL17Ns/edit?usp=drive_link&amp;ouid=105090632649587320414&amp;rtpof=true&amp;sd=true</t>
+          <t>https://drive.google.com/file/d/1PnmpSnkkyh4bJVzxfL-RkYnrgoOycMXn/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -21240,7 +21236,7 @@
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C605" t="inlineStr">
@@ -21265,7 +21261,7 @@
       </c>
       <c r="B606" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C606" t="inlineStr">
@@ -21290,7 +21286,7 @@
       </c>
       <c r="B607" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C607" t="inlineStr">
@@ -21315,7 +21311,7 @@
       </c>
       <c r="B608" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C608" t="inlineStr">
@@ -21340,7 +21336,7 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C609" t="inlineStr">
@@ -21451,7 +21447,7 @@
       </c>
       <c r="B616" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C616" t="inlineStr">
@@ -21476,7 +21472,7 @@
       </c>
       <c r="B617" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C617" t="inlineStr">
@@ -21501,7 +21497,7 @@
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>Informe final</t>
+          <t>Carpeta archivos</t>
         </is>
       </c>
       <c r="C618" t="inlineStr">
@@ -22082,11 +22078,7 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="E646" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/file/d/1d3w0unHW47dgfCZ6IMcGCLINTQKRglPO/view?usp=drive_link</t>
-        </is>
-      </c>
+      <c r="E646" t="inlineStr"/>
     </row>
     <row r="647">
       <c r="A647" t="n">
@@ -22243,7 +22235,7 @@
       </c>
       <c r="E653" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1vW5sSAFWII3dQByOxN53S71Rj_aNYBgG/view?usp=drive_link</t>
+          <t>https://drive.google.com/file/d/1ml0N-5tIACWRSjSXde5tKA2Q9Wn_J-9k/view?usp=drive_link</t>
         </is>
       </c>
     </row>
@@ -22368,7 +22360,7 @@
       </c>
       <c r="E658" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1h8ZkIRLLynb8caE2rR8zZagF76_ChE1P/view?usp=drive_link</t>
+          <t>https://drive.google.com/file/d/1aRQvwNu04n8HAXbE9o69GhoBogD2Uqj6/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -22597,7 +22589,7 @@
       </c>
       <c r="E670" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1-uaRSsIb95aqNSXjLDLMJG0a-OjealWM/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/1flNJJ6CFGtqXgQG3sAJJHbyuCFh8RuOs/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -22622,7 +22614,7 @@
       </c>
       <c r="E671" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1mDfyDNhmr4Y0uawfGhle1_DlUiM9H9oU/view?usp=sharing</t>
+          <t>https://drive.google.com/file/d/1syhJzh5ipnYrYWpHmXhOuq1UKOuyL5FQ/view?usp=sharing</t>
         </is>
       </c>
     </row>
@@ -22716,10 +22708,26 @@
       <c r="A678" t="n">
         <v>120</v>
       </c>
-      <c r="B678" t="inlineStr"/>
-      <c r="C678" t="inlineStr"/>
-      <c r="D678" t="inlineStr"/>
-      <c r="E678" t="inlineStr"/>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Carpeta archivos</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>Productos finales Navidad es Cultura 2025</t>
+        </is>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="E678" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1rb7lrObK-r5g1iF6SsaYKbR-J_K7nLy-?usp=sharing</t>
+        </is>
+      </c>
     </row>
     <row r="679">
       <c r="A679" t="n">

</xml_diff>